<commit_message>
Move datasets to datasets folder
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -427,7 +427,7 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2">
-        <v>8.3828239041679176</v>
+        <v>8.7272994732618372</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -438,7 +438,7 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2">
-        <v>8.7004537499730183</v>
+        <v>8.8713044592641381</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -449,7 +449,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2">
-        <v>8.9886037581756923</v>
+        <v>8.9807986369439288</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -460,7 +460,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2">
-        <v>8.8874508024503704</v>
+        <v>9.0347167337631706</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -471,7 +471,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2">
-        <v>9.2106651776660584</v>
+        <v>8.5716512513415886</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -482,7 +482,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2">
-        <v>8.9236378622304144</v>
+        <v>9.5480007528572859</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -493,7 +493,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2">
-        <v>8.3282199705814186</v>
+        <v>8.7869830802510869</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -504,7 +504,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2">
-        <v>8.1017350214363173</v>
+        <v>8.7725819126343403</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -515,7 +515,7 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2">
-        <v>8.7700138845602496</v>
+        <v>8.8113209078371622</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -526,7 +526,7 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2">
-        <v>8.2831029857151321</v>
+        <v>9.0037973860483405</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -537,7 +537,7 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2">
-        <v>8.8433263104502569</v>
+        <v>8.4906799961212869</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -548,7 +548,7 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2">
-        <v>9.0853880788483377</v>
+        <v>9.0767993752222438</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -559,7 +559,7 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2">
-        <v>8.6251962854748587</v>
+        <v>8.7284712144319112</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -570,7 +570,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2">
-        <v>7.5747810269945584</v>
+        <v>8.3948351859006376</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -581,7 +581,7 @@
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2">
-        <v>8.4548125737755981</v>
+        <v>9.0974352946121737</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -592,7 +592,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2">
-        <v>8.8717555566615278</v>
+        <v>9.0979560942739841</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -603,7 +603,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2">
-        <v>9.1642897508062244</v>
+        <v>8.4329159565046048</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -614,7 +614,7 @@
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2">
-        <v>9.1851177671832041</v>
+        <v>8.7689500062657544</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -625,7 +625,7 @@
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2">
-        <v>8.3031999481143419</v>
+        <v>8.9935463856686138</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -636,7 +636,7 @@
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2">
-        <v>8.8165382220417623</v>
+        <v>7.7772980565447316</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -647,7 +647,7 @@
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2">
-        <v>8.8534769714437722</v>
+        <v>8.2697901223039132</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -658,7 +658,7 @@
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2">
-        <v>8.4620982651786836</v>
+        <v>8.9071050250692902</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -669,7 +669,7 @@
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2">
-        <v>8.3620771668415728</v>
+        <v>8.6623127103451516</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -680,7 +680,7 @@
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2">
-        <v>9.2265704984223582</v>
+        <v>9.2504418853263459</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2">
-        <v>8.7871620184156338</v>
+        <v>8.8537487961303434</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -702,7 +702,7 @@
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2">
-        <v>8.5668138424876759</v>
+        <v>9.2121167605214591</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -713,7 +713,7 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2">
-        <v>8.730328450984441</v>
+        <v>8.8348827489786732</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -724,7 +724,7 @@
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2">
-        <v>9.3372501459533908</v>
+        <v>8.4923938877342167</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -735,7 +735,7 @@
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2">
-        <v>8.5330043810294605</v>
+        <v>7.8719462995498724</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -746,7 +746,7 @@
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2">
-        <v>8.095792878292837</v>
+        <v>8.04433558508922</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -801,7 +801,7 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2">
-        <v>2.7141156262348605</v>
+        <v>2.8046452083940321</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -812,7 +812,7 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2">
-        <v>2.3107976071630074</v>
+        <v>2.3012554823722984</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -823,7 +823,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2">
-        <v>2.1608181665757265</v>
+        <v>2.2665946875564686</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -834,7 +834,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2">
-        <v>2.1735717087475979</v>
+        <v>2.0835451486535574</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -845,7 +845,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2">
-        <v>2.3073912050936047</v>
+        <v>2.5590333655686379</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -856,7 +856,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2">
-        <v>2.0723354182186418</v>
+        <v>1.478997732558665</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -867,7 +867,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2">
-        <v>2.724018320255575</v>
+        <v>2.31094501463518</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -878,7 +878,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2">
-        <v>3.1860334914610724</v>
+        <v>2.3666078405007402</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -889,7 +889,7 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2">
-        <v>2.4792081371791892</v>
+        <v>2.2241977574036911</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -900,7 +900,7 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2">
-        <v>3.0775017165753504</v>
+        <v>2.3794238705716801</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -911,7 +911,7 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2">
-        <v>2.3255120238118918</v>
+        <v>2.6550008250783965</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -922,7 +922,7 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2">
-        <v>2.1574035415144324</v>
+        <v>1.9362067712192452</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -933,7 +933,7 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2">
-        <v>2.6325505267572398</v>
+        <v>2.4552689442158728</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -944,7 +944,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2">
-        <v>3.5958046138733364</v>
+        <v>2.7361406871608085</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -955,7 +955,7 @@
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2">
-        <v>2.6679935580915095</v>
+        <v>2.1302024511560829</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -966,7 +966,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2">
-        <v>2.3187103809014062</v>
+        <v>2.0763356439577834</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -977,7 +977,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2">
-        <v>1.920959572190877</v>
+        <v>2.5467484154309701</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -988,7 +988,7 @@
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2">
-        <v>1.9492571840118789</v>
+        <v>2.2960869811848337</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2">
-        <v>2.8640437714706719</v>
+        <v>2.0149185853374294</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1010,7 +1010,7 @@
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2">
-        <v>2.174207204657018</v>
+        <v>3.3024855448894441</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2">
-        <v>2.3816412001350971</v>
+        <v>2.7011095309845063</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1032,7 +1032,7 @@
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2">
-        <v>2.5548707198891645</v>
+        <v>2.4999117094730487</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2">
-        <v>2.5984395178602631</v>
+        <v>2.5911977094757055</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2">
-        <v>2.0345081620777474</v>
+        <v>1.8430918121201039</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1065,7 +1065,7 @@
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2">
-        <v>2.4448250968011456</v>
+        <v>2.3641153681864919</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1076,7 +1076,7 @@
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2">
-        <v>2.6490171037199164</v>
+        <v>1.9285430587232832</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2">
-        <v>2.3695838647359411</v>
+        <v>2.1981783220057078</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1098,7 +1098,7 @@
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2">
-        <v>1.8621684832384169</v>
+        <v>2.5246228731548328</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1109,7 +1109,7 @@
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2">
-        <v>2.5649544839829956</v>
+        <v>3.1860394748015062</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1120,7 +1120,7 @@
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2">
-        <v>3.1103021011704088</v>
+        <v>3.0010430663772905</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>

</xml_diff>

<commit_message>
Add c oncrete compressive strength dataset
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="15255" windowHeight="6165"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="15255" windowHeight="6165" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="9">
   <si>
     <t>Slump Test</t>
   </si>
@@ -41,6 +41,9 @@
   <si>
     <t>O-ring Dataset</t>
   </si>
+  <si>
+    <t>Concrete Compressive Strength Dataset</t>
+  </si>
 </sst>
 </file>
 
@@ -63,7 +66,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -86,11 +89,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -100,6 +140,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -396,38 +448,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:Q34"/>
+  <dimension ref="A3:W34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5:O34"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5:U34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:23">
       <c r="A3" s="2"/>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="S3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="8"/>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -473,8 +532,23 @@
       <c r="Q4" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="S4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -508,8 +582,19 @@
         <v>34.333337836390733</v>
       </c>
       <c r="Q5" s="2"/>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="S5" s="2">
+        <v>1</v>
+      </c>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2">
+        <v>87.344039495134368</v>
+      </c>
+      <c r="V5" s="2">
+        <v>34.333337836390733</v>
+      </c>
+      <c r="W5" s="2"/>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -543,8 +628,19 @@
         <v>35.238292636577022</v>
       </c>
       <c r="Q6" s="2"/>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="S6" s="2">
+        <v>2</v>
+      </c>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2">
+        <v>90.389974169207917</v>
+      </c>
+      <c r="V6" s="2">
+        <v>35.238292636577022</v>
+      </c>
+      <c r="W6" s="2"/>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -578,8 +674,19 @@
         <v>33.414195951190571</v>
       </c>
       <c r="Q7" s="2"/>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="S7" s="2">
+        <v>3</v>
+      </c>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2">
+        <v>88.764916371290127</v>
+      </c>
+      <c r="V7" s="2">
+        <v>33.414195951190571</v>
+      </c>
+      <c r="W7" s="2"/>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -613,8 +720,19 @@
         <v>33.10390321886964</v>
       </c>
       <c r="Q8" s="2"/>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="S8" s="2">
+        <v>4</v>
+      </c>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2">
+        <v>88.900635432109382</v>
+      </c>
+      <c r="V8" s="2">
+        <v>33.10390321886964</v>
+      </c>
+      <c r="W8" s="2"/>
+    </row>
+    <row r="9" spans="1:23">
       <c r="A9" s="2">
         <v>5</v>
       </c>
@@ -648,8 +766,19 @@
         <v>34.532627902761824</v>
       </c>
       <c r="Q9" s="2"/>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="S9" s="2">
+        <v>5</v>
+      </c>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2">
+        <v>89.156182929271282</v>
+      </c>
+      <c r="V9" s="2">
+        <v>34.532627902761824</v>
+      </c>
+      <c r="W9" s="2"/>
+    </row>
+    <row r="10" spans="1:23">
       <c r="A10" s="2">
         <v>6</v>
       </c>
@@ -683,8 +812,19 @@
         <v>33.954393269315474</v>
       </c>
       <c r="Q10" s="2"/>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="S10" s="2">
+        <v>6</v>
+      </c>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2">
+        <v>90.560128155756473</v>
+      </c>
+      <c r="V10" s="2">
+        <v>33.954393269315474</v>
+      </c>
+      <c r="W10" s="2"/>
+    </row>
+    <row r="11" spans="1:23">
       <c r="A11" s="2">
         <v>7</v>
       </c>
@@ -718,8 +858,19 @@
         <v>34.188286916042344</v>
       </c>
       <c r="Q11" s="2"/>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="S11" s="2">
+        <v>7</v>
+      </c>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2">
+        <v>87.985253243016643</v>
+      </c>
+      <c r="V11" s="2">
+        <v>34.188286916042344</v>
+      </c>
+      <c r="W11" s="2"/>
+    </row>
+    <row r="12" spans="1:23">
       <c r="A12" s="2">
         <v>8</v>
       </c>
@@ -753,8 +904,19 @@
         <v>35.225941225370008</v>
       </c>
       <c r="Q12" s="2"/>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="S12" s="2">
+        <v>8</v>
+      </c>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2">
+        <v>87.90024205594537</v>
+      </c>
+      <c r="V12" s="2">
+        <v>35.225941225370008</v>
+      </c>
+      <c r="W12" s="2"/>
+    </row>
+    <row r="13" spans="1:23">
       <c r="A13" s="2">
         <v>9</v>
       </c>
@@ -788,8 +950,19 @@
         <v>32.822205520592874</v>
       </c>
       <c r="Q13" s="2"/>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="S13" s="2">
+        <v>9</v>
+      </c>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2">
+        <v>89.44969605081809</v>
+      </c>
+      <c r="V13" s="2">
+        <v>32.822205520592874</v>
+      </c>
+      <c r="W13" s="2"/>
+    </row>
+    <row r="14" spans="1:23">
       <c r="A14" s="2">
         <v>10</v>
       </c>
@@ -823,8 +996,19 @@
         <v>34.406714412746496</v>
       </c>
       <c r="Q14" s="2"/>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="S14" s="2">
+        <v>10</v>
+      </c>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2">
+        <v>89.85584362099965</v>
+      </c>
+      <c r="V14" s="2">
+        <v>34.406714412746496</v>
+      </c>
+      <c r="W14" s="2"/>
+    </row>
+    <row r="15" spans="1:23">
       <c r="A15" s="2">
         <v>11</v>
       </c>
@@ -858,8 +1042,19 @@
         <v>35.754307256723955</v>
       </c>
       <c r="Q15" s="2"/>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="S15" s="2">
+        <v>11</v>
+      </c>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2">
+        <v>89.346589288574776</v>
+      </c>
+      <c r="V15" s="2">
+        <v>35.754307256723955</v>
+      </c>
+      <c r="W15" s="2"/>
+    </row>
+    <row r="16" spans="1:23">
       <c r="A16" s="2">
         <v>12</v>
       </c>
@@ -893,8 +1088,19 @@
         <v>35.07667385668708</v>
       </c>
       <c r="Q16" s="2"/>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="S16" s="2">
+        <v>12</v>
+      </c>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2">
+        <v>89.169665431178501</v>
+      </c>
+      <c r="V16" s="2">
+        <v>35.07667385668708</v>
+      </c>
+      <c r="W16" s="2"/>
+    </row>
+    <row r="17" spans="1:23">
       <c r="A17" s="2">
         <v>13</v>
       </c>
@@ -928,8 +1134,19 @@
         <v>35.26457661466717</v>
       </c>
       <c r="Q17" s="2"/>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="S17" s="2">
+        <v>13</v>
+      </c>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2">
+        <v>87.555155671271748</v>
+      </c>
+      <c r="V17" s="2">
+        <v>35.26457661466717</v>
+      </c>
+      <c r="W17" s="2"/>
+    </row>
+    <row r="18" spans="1:23">
       <c r="A18" s="2">
         <v>14</v>
       </c>
@@ -963,8 +1180,19 @@
         <v>34.990444301090378</v>
       </c>
       <c r="Q18" s="2"/>
-    </row>
-    <row r="19" spans="1:17">
+      <c r="S18" s="2">
+        <v>14</v>
+      </c>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2">
+        <v>90.04644667510091</v>
+      </c>
+      <c r="V18" s="2">
+        <v>34.990444301090378</v>
+      </c>
+      <c r="W18" s="2"/>
+    </row>
+    <row r="19" spans="1:23">
       <c r="A19" s="2">
         <v>15</v>
       </c>
@@ -998,8 +1226,19 @@
         <v>33.652591405527673</v>
       </c>
       <c r="Q19" s="2"/>
-    </row>
-    <row r="20" spans="1:17">
+      <c r="S19" s="2">
+        <v>15</v>
+      </c>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2">
+        <v>88.926150708891043</v>
+      </c>
+      <c r="V19" s="2">
+        <v>33.652591405527673</v>
+      </c>
+      <c r="W19" s="2"/>
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20" s="2">
         <v>16</v>
       </c>
@@ -1033,8 +1272,19 @@
         <v>35.493750234388799</v>
       </c>
       <c r="Q20" s="2"/>
-    </row>
-    <row r="21" spans="1:17">
+      <c r="S20" s="2">
+        <v>16</v>
+      </c>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2">
+        <v>89.387721575792241</v>
+      </c>
+      <c r="V20" s="2">
+        <v>35.493750234388799</v>
+      </c>
+      <c r="W20" s="2"/>
+    </row>
+    <row r="21" spans="1:23">
       <c r="A21" s="2">
         <v>17</v>
       </c>
@@ -1068,8 +1318,19 @@
         <v>35.392234789709974</v>
       </c>
       <c r="Q21" s="2"/>
-    </row>
-    <row r="22" spans="1:17">
+      <c r="S21" s="2">
+        <v>17</v>
+      </c>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2">
+        <v>90.146626768418074</v>
+      </c>
+      <c r="V21" s="2">
+        <v>35.392234789709974</v>
+      </c>
+      <c r="W21" s="2"/>
+    </row>
+    <row r="22" spans="1:23">
       <c r="A22" s="2">
         <v>18</v>
       </c>
@@ -1103,8 +1364,19 @@
         <v>33.091644786556117</v>
       </c>
       <c r="Q22" s="2"/>
-    </row>
-    <row r="23" spans="1:17">
+      <c r="S22" s="2">
+        <v>18</v>
+      </c>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2">
+        <v>89.464820368026892</v>
+      </c>
+      <c r="V22" s="2">
+        <v>33.091644786556117</v>
+      </c>
+      <c r="W22" s="2"/>
+    </row>
+    <row r="23" spans="1:23">
       <c r="A23" s="2">
         <v>19</v>
       </c>
@@ -1138,8 +1410,19 @@
         <v>33.55428817370008</v>
       </c>
       <c r="Q23" s="2"/>
-    </row>
-    <row r="24" spans="1:17">
+      <c r="S23" s="2">
+        <v>19</v>
+      </c>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2">
+        <v>89.56632859934129</v>
+      </c>
+      <c r="V23" s="2">
+        <v>33.55428817370008</v>
+      </c>
+      <c r="W23" s="2"/>
+    </row>
+    <row r="24" spans="1:23">
       <c r="A24" s="2">
         <v>20</v>
       </c>
@@ -1173,8 +1456,19 @@
         <v>35.097837416371704</v>
       </c>
       <c r="Q24" s="2"/>
-    </row>
-    <row r="25" spans="1:17">
+      <c r="S24" s="2">
+        <v>20</v>
+      </c>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2">
+        <v>86.912890552886637</v>
+      </c>
+      <c r="V24" s="2">
+        <v>35.097837416371704</v>
+      </c>
+      <c r="W24" s="2"/>
+    </row>
+    <row r="25" spans="1:23">
       <c r="A25" s="2">
         <v>21</v>
       </c>
@@ -1208,8 +1502,19 @@
         <v>34.77114772163079</v>
       </c>
       <c r="Q25" s="2"/>
-    </row>
-    <row r="26" spans="1:17">
+      <c r="S25" s="2">
+        <v>21</v>
+      </c>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2">
+        <v>90.789054445727288</v>
+      </c>
+      <c r="V25" s="2">
+        <v>34.77114772163079</v>
+      </c>
+      <c r="W25" s="2"/>
+    </row>
+    <row r="26" spans="1:23">
       <c r="A26" s="2">
         <v>22</v>
       </c>
@@ -1243,8 +1548,19 @@
         <v>34.534131615866343</v>
       </c>
       <c r="Q26" s="2"/>
-    </row>
-    <row r="27" spans="1:17">
+      <c r="S26" s="2">
+        <v>22</v>
+      </c>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2">
+        <v>89.846985300502752</v>
+      </c>
+      <c r="V26" s="2">
+        <v>34.534131615866343</v>
+      </c>
+      <c r="W26" s="2"/>
+    </row>
+    <row r="27" spans="1:23">
       <c r="A27" s="2">
         <v>23</v>
       </c>
@@ -1278,8 +1594,19 @@
         <v>34.8012231046376</v>
       </c>
       <c r="Q27" s="2"/>
-    </row>
-    <row r="28" spans="1:17">
+      <c r="S27" s="2">
+        <v>23</v>
+      </c>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2">
+        <v>88.847283856599674</v>
+      </c>
+      <c r="V27" s="2">
+        <v>34.8012231046376</v>
+      </c>
+      <c r="W27" s="2"/>
+    </row>
+    <row r="28" spans="1:23">
       <c r="A28" s="2">
         <v>24</v>
       </c>
@@ -1313,8 +1640,19 @@
         <v>34.8817732783168</v>
       </c>
       <c r="Q28" s="2"/>
-    </row>
-    <row r="29" spans="1:17">
+      <c r="S28" s="2">
+        <v>24</v>
+      </c>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2">
+        <v>88.962835804286385</v>
+      </c>
+      <c r="V28" s="2">
+        <v>34.8817732783168</v>
+      </c>
+      <c r="W28" s="2"/>
+    </row>
+    <row r="29" spans="1:23">
       <c r="A29" s="2">
         <v>25</v>
       </c>
@@ -1348,8 +1686,19 @@
         <v>35.31663119471223</v>
       </c>
       <c r="Q29" s="2"/>
-    </row>
-    <row r="30" spans="1:17">
+      <c r="S29" s="2">
+        <v>25</v>
+      </c>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2">
+        <v>87.705174165305394</v>
+      </c>
+      <c r="V29" s="2">
+        <v>35.31663119471223</v>
+      </c>
+      <c r="W29" s="2"/>
+    </row>
+    <row r="30" spans="1:23">
       <c r="A30" s="2">
         <v>26</v>
       </c>
@@ -1383,8 +1732,19 @@
         <v>33.223220903760506</v>
       </c>
       <c r="Q30" s="2"/>
-    </row>
-    <row r="31" spans="1:17">
+      <c r="S30" s="2">
+        <v>26</v>
+      </c>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2">
+        <v>87.895151208688048</v>
+      </c>
+      <c r="V30" s="2">
+        <v>33.223220903760506</v>
+      </c>
+      <c r="W30" s="2"/>
+    </row>
+    <row r="31" spans="1:23">
       <c r="A31" s="2">
         <v>27</v>
       </c>
@@ -1418,8 +1778,19 @@
         <v>34.493444677833068</v>
       </c>
       <c r="Q31" s="2"/>
-    </row>
-    <row r="32" spans="1:17">
+      <c r="S31" s="2">
+        <v>27</v>
+      </c>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2">
+        <v>88.938586359584733</v>
+      </c>
+      <c r="V31" s="2">
+        <v>34.493444677833068</v>
+      </c>
+      <c r="W31" s="2"/>
+    </row>
+    <row r="32" spans="1:23">
       <c r="A32" s="2">
         <v>28</v>
       </c>
@@ -1453,8 +1824,19 @@
         <v>35.315221026153679</v>
       </c>
       <c r="Q32" s="2"/>
-    </row>
-    <row r="33" spans="1:17">
+      <c r="S32" s="2">
+        <v>28</v>
+      </c>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2">
+        <v>89.895509451736373</v>
+      </c>
+      <c r="V32" s="2">
+        <v>35.315221026153679</v>
+      </c>
+      <c r="W32" s="2"/>
+    </row>
+    <row r="33" spans="1:23">
       <c r="A33" s="2">
         <v>29</v>
       </c>
@@ -1488,8 +1870,19 @@
         <v>35.734482719855279</v>
       </c>
       <c r="Q33" s="2"/>
-    </row>
-    <row r="34" spans="1:17">
+      <c r="S33" s="2">
+        <v>29</v>
+      </c>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2">
+        <v>89.053092467741266</v>
+      </c>
+      <c r="V33" s="2">
+        <v>35.734482719855279</v>
+      </c>
+      <c r="W33" s="2"/>
+    </row>
+    <row r="34" spans="1:23">
       <c r="A34" s="2">
         <v>30</v>
       </c>
@@ -1523,12 +1916,24 @@
         <v>34.400667023288385</v>
       </c>
       <c r="Q34" s="2"/>
+      <c r="S34" s="2">
+        <v>30</v>
+      </c>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2">
+        <v>90.016858318820184</v>
+      </c>
+      <c r="V34" s="2">
+        <v>34.400667023288385</v>
+      </c>
+      <c r="W34" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="S3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1536,38 +1941,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:Q34"/>
+  <dimension ref="A3:W34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5:O34"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5:U34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:23">
       <c r="A3" s="2"/>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="S3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="8"/>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1613,8 +2025,23 @@
       <c r="Q4" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="S4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -1648,8 +2075,19 @@
         <v>34.333337836390733</v>
       </c>
       <c r="Q5" s="2"/>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="S5" s="2">
+        <v>1</v>
+      </c>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2">
+        <v>23.816540005628696</v>
+      </c>
+      <c r="V5" s="2">
+        <v>34.333337836390733</v>
+      </c>
+      <c r="W5" s="2"/>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -1683,8 +2121,19 @@
         <v>35.238292636577022</v>
       </c>
       <c r="Q6" s="2"/>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="S6" s="2">
+        <v>2</v>
+      </c>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2">
+        <v>21.062510619807334</v>
+      </c>
+      <c r="V6" s="2">
+        <v>35.238292636577022</v>
+      </c>
+      <c r="W6" s="2"/>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -1718,8 +2167,19 @@
         <v>33.414195951190571</v>
       </c>
       <c r="Q7" s="2"/>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="S7" s="2">
+        <v>3</v>
+      </c>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2">
+        <v>22.489920708993097</v>
+      </c>
+      <c r="V7" s="2">
+        <v>33.414195951190571</v>
+      </c>
+      <c r="W7" s="2"/>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -1753,8 +2213,19 @@
         <v>33.10390321886964</v>
       </c>
       <c r="Q8" s="2"/>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="S8" s="2">
+        <v>4</v>
+      </c>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2">
+        <v>23.358995173572225</v>
+      </c>
+      <c r="V8" s="2">
+        <v>33.10390321886964</v>
+      </c>
+      <c r="W8" s="2"/>
+    </row>
+    <row r="9" spans="1:23">
       <c r="A9" s="2">
         <v>5</v>
       </c>
@@ -1788,8 +2259,19 @@
         <v>34.532627902761824</v>
       </c>
       <c r="Q9" s="2"/>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="S9" s="2">
+        <v>5</v>
+      </c>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2">
+        <v>22.450261199604128</v>
+      </c>
+      <c r="V9" s="2">
+        <v>34.532627902761824</v>
+      </c>
+      <c r="W9" s="2"/>
+    </row>
+    <row r="10" spans="1:23">
       <c r="A10" s="2">
         <v>6</v>
       </c>
@@ -1823,8 +2305,19 @@
         <v>33.954393269315474</v>
       </c>
       <c r="Q10" s="2"/>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="S10" s="2">
+        <v>6</v>
+      </c>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2">
+        <v>21.119194594032759</v>
+      </c>
+      <c r="V10" s="2">
+        <v>33.954393269315474</v>
+      </c>
+      <c r="W10" s="2"/>
+    </row>
+    <row r="11" spans="1:23">
       <c r="A11" s="2">
         <v>7</v>
       </c>
@@ -1858,8 +2351,19 @@
         <v>34.188286916042344</v>
       </c>
       <c r="Q11" s="2"/>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="S11" s="2">
+        <v>7</v>
+      </c>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2">
+        <v>23.427504001608462</v>
+      </c>
+      <c r="V11" s="2">
+        <v>34.188286916042344</v>
+      </c>
+      <c r="W11" s="2"/>
+    </row>
+    <row r="12" spans="1:23">
       <c r="A12" s="2">
         <v>8</v>
       </c>
@@ -1893,8 +2397,19 @@
         <v>35.225941225370008</v>
       </c>
       <c r="Q12" s="2"/>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="S12" s="2">
+        <v>8</v>
+      </c>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2">
+        <v>23.069164002306078</v>
+      </c>
+      <c r="V12" s="2">
+        <v>35.225941225370008</v>
+      </c>
+      <c r="W12" s="2"/>
+    </row>
+    <row r="13" spans="1:23">
       <c r="A13" s="2">
         <v>9</v>
       </c>
@@ -1928,8 +2443,19 @@
         <v>32.822205520592874</v>
       </c>
       <c r="Q13" s="2"/>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="S13" s="2">
+        <v>9</v>
+      </c>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2">
+        <v>22.098123677287976</v>
+      </c>
+      <c r="V13" s="2">
+        <v>32.822205520592874</v>
+      </c>
+      <c r="W13" s="2"/>
+    </row>
+    <row r="14" spans="1:23">
       <c r="A14" s="2">
         <v>10</v>
       </c>
@@ -1963,8 +2489,19 @@
         <v>34.406714412746496</v>
       </c>
       <c r="Q14" s="2"/>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="S14" s="2">
+        <v>10</v>
+      </c>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2">
+        <v>21.782262998149125</v>
+      </c>
+      <c r="V14" s="2">
+        <v>34.406714412746496</v>
+      </c>
+      <c r="W14" s="2"/>
+    </row>
+    <row r="15" spans="1:23">
       <c r="A15" s="2">
         <v>11</v>
       </c>
@@ -1998,8 +2535,19 @@
         <v>35.754307256723955</v>
       </c>
       <c r="Q15" s="2"/>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="S15" s="2">
+        <v>11</v>
+      </c>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2">
+        <v>21.974414232170737</v>
+      </c>
+      <c r="V15" s="2">
+        <v>35.754307256723955</v>
+      </c>
+      <c r="W15" s="2"/>
+    </row>
+    <row r="16" spans="1:23">
       <c r="A16" s="2">
         <v>12</v>
       </c>
@@ -2033,8 +2581,19 @@
         <v>35.07667385668708</v>
       </c>
       <c r="Q16" s="2"/>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="S16" s="2">
+        <v>12</v>
+      </c>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2">
+        <v>22.689493934089398</v>
+      </c>
+      <c r="V16" s="2">
+        <v>35.07667385668708</v>
+      </c>
+      <c r="W16" s="2"/>
+    </row>
+    <row r="17" spans="1:23">
       <c r="A17" s="2">
         <v>13</v>
       </c>
@@ -2068,8 +2627,19 @@
         <v>35.26457661466717</v>
       </c>
       <c r="Q17" s="2"/>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="S17" s="2">
+        <v>13</v>
+      </c>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2">
+        <v>23.653509015870476</v>
+      </c>
+      <c r="V17" s="2">
+        <v>35.26457661466717</v>
+      </c>
+      <c r="W17" s="2"/>
+    </row>
+    <row r="18" spans="1:23">
       <c r="A18" s="2">
         <v>14</v>
       </c>
@@ -2103,8 +2673,19 @@
         <v>34.990444301090378</v>
       </c>
       <c r="Q18" s="2"/>
-    </row>
-    <row r="19" spans="1:17">
+      <c r="S18" s="2">
+        <v>14</v>
+      </c>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2">
+        <v>21.095518848878051</v>
+      </c>
+      <c r="V18" s="2">
+        <v>34.990444301090378</v>
+      </c>
+      <c r="W18" s="2"/>
+    </row>
+    <row r="19" spans="1:23">
       <c r="A19" s="2">
         <v>15</v>
       </c>
@@ -2138,8 +2719,19 @@
         <v>33.652591405527673</v>
       </c>
       <c r="Q19" s="2"/>
-    </row>
-    <row r="20" spans="1:17">
+      <c r="S19" s="2">
+        <v>15</v>
+      </c>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2">
+        <v>22.496500773223126</v>
+      </c>
+      <c r="V19" s="2">
+        <v>33.652591405527673</v>
+      </c>
+      <c r="W19" s="2"/>
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20" s="2">
         <v>16</v>
       </c>
@@ -2173,8 +2765,19 @@
         <v>35.493750234388799</v>
       </c>
       <c r="Q20" s="2"/>
-    </row>
-    <row r="21" spans="1:17">
+      <c r="S20" s="2">
+        <v>16</v>
+      </c>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2">
+        <v>22.291452607418648</v>
+      </c>
+      <c r="V20" s="2">
+        <v>35.493750234388799</v>
+      </c>
+      <c r="W20" s="2"/>
+    </row>
+    <row r="21" spans="1:23">
       <c r="A21" s="2">
         <v>17</v>
       </c>
@@ -2208,8 +2811,19 @@
         <v>35.392234789709974</v>
       </c>
       <c r="Q21" s="2"/>
-    </row>
-    <row r="22" spans="1:17">
+      <c r="S21" s="2">
+        <v>17</v>
+      </c>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2">
+        <v>21.205964757693188</v>
+      </c>
+      <c r="V21" s="2">
+        <v>35.392234789709974</v>
+      </c>
+      <c r="W21" s="2"/>
+    </row>
+    <row r="22" spans="1:23">
       <c r="A22" s="2">
         <v>18</v>
       </c>
@@ -2243,8 +2857,19 @@
         <v>33.091644786556117</v>
       </c>
       <c r="Q22" s="2"/>
-    </row>
-    <row r="23" spans="1:17">
+      <c r="S22" s="2">
+        <v>18</v>
+      </c>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2">
+        <v>22.337749860051932</v>
+      </c>
+      <c r="V22" s="2">
+        <v>33.091644786556117</v>
+      </c>
+      <c r="W22" s="2"/>
+    </row>
+    <row r="23" spans="1:23">
       <c r="A23" s="2">
         <v>19</v>
       </c>
@@ -2278,8 +2903,19 @@
         <v>33.55428817370008</v>
       </c>
       <c r="Q23" s="2"/>
-    </row>
-    <row r="24" spans="1:17">
+      <c r="S23" s="2">
+        <v>19</v>
+      </c>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2">
+        <v>22.108330905423241</v>
+      </c>
+      <c r="V23" s="2">
+        <v>33.55428817370008</v>
+      </c>
+      <c r="W23" s="2"/>
+    </row>
+    <row r="24" spans="1:23">
       <c r="A24" s="2">
         <v>20</v>
       </c>
@@ -2313,8 +2949,19 @@
         <v>35.097837416371704</v>
       </c>
       <c r="Q24" s="2"/>
-    </row>
-    <row r="25" spans="1:17">
+      <c r="S24" s="2">
+        <v>20</v>
+      </c>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2">
+        <v>24.206796555777544</v>
+      </c>
+      <c r="V24" s="2">
+        <v>35.097837416371704</v>
+      </c>
+      <c r="W24" s="2"/>
+    </row>
+    <row r="25" spans="1:23">
       <c r="A25" s="2">
         <v>21</v>
       </c>
@@ -2348,8 +2995,19 @@
         <v>34.77114772163079</v>
       </c>
       <c r="Q25" s="2"/>
-    </row>
-    <row r="26" spans="1:17">
+      <c r="S25" s="2">
+        <v>21</v>
+      </c>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2">
+        <v>20.931393195616486</v>
+      </c>
+      <c r="V25" s="2">
+        <v>34.77114772163079</v>
+      </c>
+      <c r="W25" s="2"/>
+    </row>
+    <row r="26" spans="1:23">
       <c r="A26" s="2">
         <v>22</v>
       </c>
@@ -2383,8 +3041,19 @@
         <v>34.534131615866343</v>
       </c>
       <c r="Q26" s="2"/>
-    </row>
-    <row r="27" spans="1:17">
+      <c r="S26" s="2">
+        <v>22</v>
+      </c>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2">
+        <v>21.710597899909828</v>
+      </c>
+      <c r="V26" s="2">
+        <v>34.534131615866343</v>
+      </c>
+      <c r="W26" s="2"/>
+    </row>
+    <row r="27" spans="1:23">
       <c r="A27" s="2">
         <v>23</v>
       </c>
@@ -2418,8 +3087,19 @@
         <v>34.8012231046376</v>
       </c>
       <c r="Q27" s="2"/>
-    </row>
-    <row r="28" spans="1:17">
+      <c r="S27" s="2">
+        <v>23</v>
+      </c>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2">
+        <v>22.695345479298329</v>
+      </c>
+      <c r="V27" s="2">
+        <v>34.8012231046376</v>
+      </c>
+      <c r="W27" s="2"/>
+    </row>
+    <row r="28" spans="1:23">
       <c r="A28" s="2">
         <v>24</v>
       </c>
@@ -2453,8 +3133,19 @@
         <v>34.8817732783168</v>
       </c>
       <c r="Q28" s="2"/>
-    </row>
-    <row r="29" spans="1:17">
+      <c r="S28" s="2">
+        <v>24</v>
+      </c>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2">
+        <v>22.638792879778123</v>
+      </c>
+      <c r="V28" s="2">
+        <v>34.8817732783168</v>
+      </c>
+      <c r="W28" s="2"/>
+    </row>
+    <row r="29" spans="1:23">
       <c r="A29" s="2">
         <v>25</v>
       </c>
@@ -2488,8 +3179,19 @@
         <v>35.31663119471223</v>
       </c>
       <c r="Q29" s="2"/>
-    </row>
-    <row r="30" spans="1:17">
+      <c r="S29" s="2">
+        <v>25</v>
+      </c>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2">
+        <v>24.094856504004955</v>
+      </c>
+      <c r="V29" s="2">
+        <v>35.31663119471223</v>
+      </c>
+      <c r="W29" s="2"/>
+    </row>
+    <row r="30" spans="1:23">
       <c r="A30" s="2">
         <v>26</v>
       </c>
@@ -2523,8 +3225,19 @@
         <v>33.223220903760506</v>
       </c>
       <c r="Q30" s="2"/>
-    </row>
-    <row r="31" spans="1:17">
+      <c r="S30" s="2">
+        <v>26</v>
+      </c>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2">
+        <v>23.588018165020323</v>
+      </c>
+      <c r="V30" s="2">
+        <v>33.223220903760506</v>
+      </c>
+      <c r="W30" s="2"/>
+    </row>
+    <row r="31" spans="1:23">
       <c r="A31" s="2">
         <v>27</v>
       </c>
@@ -2558,8 +3271,19 @@
         <v>34.493444677833068</v>
       </c>
       <c r="Q31" s="2"/>
-    </row>
-    <row r="32" spans="1:17">
+      <c r="S31" s="2">
+        <v>27</v>
+      </c>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2">
+        <v>22.721295785868691</v>
+      </c>
+      <c r="V31" s="2">
+        <v>34.493444677833068</v>
+      </c>
+      <c r="W31" s="2"/>
+    </row>
+    <row r="32" spans="1:23">
       <c r="A32" s="2">
         <v>28</v>
       </c>
@@ -2593,8 +3317,19 @@
         <v>35.315221026153679</v>
       </c>
       <c r="Q32" s="2"/>
-    </row>
-    <row r="33" spans="1:17">
+      <c r="S32" s="2">
+        <v>28</v>
+      </c>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2">
+        <v>21.463995271108104</v>
+      </c>
+      <c r="V32" s="2">
+        <v>35.315221026153679</v>
+      </c>
+      <c r="W32" s="2"/>
+    </row>
+    <row r="33" spans="1:23">
       <c r="A33" s="2">
         <v>29</v>
       </c>
@@ -2628,8 +3363,19 @@
         <v>35.734482719855279</v>
       </c>
       <c r="Q33" s="2"/>
-    </row>
-    <row r="34" spans="1:17">
+      <c r="S33" s="2">
+        <v>29</v>
+      </c>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2">
+        <v>22.757353908794084</v>
+      </c>
+      <c r="V33" s="2">
+        <v>35.734482719855279</v>
+      </c>
+      <c r="W33" s="2"/>
+    </row>
+    <row r="34" spans="1:23">
       <c r="A34" s="2">
         <v>30</v>
       </c>
@@ -2663,12 +3409,24 @@
         <v>34.400667023288385</v>
       </c>
       <c r="Q34" s="2"/>
+      <c r="S34" s="2">
+        <v>30</v>
+      </c>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2">
+        <v>22.017175124018618</v>
+      </c>
+      <c r="V34" s="2">
+        <v>34.400667023288385</v>
+      </c>
+      <c r="W34" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="S3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add red wine quality to runPSO
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="15255" windowHeight="6165" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="15255" windowHeight="6165"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="11">
   <si>
     <t>Slump Test</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Concrete Compressive Strength Dataset</t>
+  </si>
+  <si>
+    <t>Red Wine Quality</t>
+  </si>
+  <si>
+    <t>White Wine Quality</t>
   </si>
 </sst>
 </file>
@@ -130,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -152,6 +158,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -448,36 +457,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:W34"/>
+  <dimension ref="A3:AI34"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5:U34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:35">
       <c r="A3" s="2"/>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
       <c r="S3" s="6" t="s">
         <v>8</v>
       </c>
@@ -485,8 +494,22 @@
       <c r="U3" s="7"/>
       <c r="V3" s="7"/>
       <c r="W3" s="8"/>
-    </row>
-    <row r="4" spans="1:23">
+      <c r="Y3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="8"/>
+      <c r="AE3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF3" s="7"/>
+      <c r="AG3" s="7"/>
+      <c r="AH3" s="7"/>
+      <c r="AI3" s="8"/>
+    </row>
+    <row r="4" spans="1:35">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -547,8 +570,38 @@
       <c r="W4" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:23">
+      <c r="Y4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI4" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -556,9 +609,7 @@
       <c r="C5" s="2">
         <v>8.8570241628233184</v>
       </c>
-      <c r="D5" s="2">
-        <v>34.333337836390733</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="G5" s="2">
         <v>1</v>
@@ -567,9 +618,7 @@
       <c r="I5" s="2">
         <v>34.855482580164256</v>
       </c>
-      <c r="J5" s="2">
-        <v>34.333337836390733</v>
-      </c>
+      <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="M5" s="2">
         <v>1</v>
@@ -578,9 +627,7 @@
       <c r="O5" s="2">
         <v>25.371197018440967</v>
       </c>
-      <c r="P5" s="2">
-        <v>34.333337836390733</v>
-      </c>
+      <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="S5" s="2">
         <v>1</v>
@@ -589,12 +636,28 @@
       <c r="U5" s="2">
         <v>87.344039495134368</v>
       </c>
-      <c r="V5" s="2">
-        <v>34.333337836390733</v>
-      </c>
+      <c r="V5" s="2"/>
       <c r="W5" s="2"/>
-    </row>
-    <row r="6" spans="1:23">
+      <c r="Y5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2">
+        <v>818.7710536659115</v>
+      </c>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AE5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2">
+        <v>424.58585828211886</v>
+      </c>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+    </row>
+    <row r="6" spans="1:35">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -602,9 +665,7 @@
       <c r="C6" s="2">
         <v>9.161164934202203</v>
       </c>
-      <c r="D6" s="2">
-        <v>35.238292636577022</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="G6" s="2">
         <v>2</v>
@@ -613,9 +674,7 @@
       <c r="I6" s="2">
         <v>33.841742498805409</v>
       </c>
-      <c r="J6" s="2">
-        <v>35.238292636577022</v>
-      </c>
+      <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="M6" s="2">
         <v>2</v>
@@ -624,9 +683,7 @@
       <c r="O6" s="2">
         <v>19.199319641827845</v>
       </c>
-      <c r="P6" s="2">
-        <v>35.238292636577022</v>
-      </c>
+      <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="S6" s="2">
         <v>2</v>
@@ -635,12 +692,28 @@
       <c r="U6" s="2">
         <v>90.389974169207917</v>
       </c>
-      <c r="V6" s="2">
-        <v>35.238292636577022</v>
-      </c>
+      <c r="V6" s="2"/>
       <c r="W6" s="2"/>
-    </row>
-    <row r="7" spans="1:23">
+      <c r="Y6" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2">
+        <v>814.48000578482788</v>
+      </c>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AE6" s="2">
+        <v>2</v>
+      </c>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2">
+        <v>413.03417428185338</v>
+      </c>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+    </row>
+    <row r="7" spans="1:35">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -648,9 +721,7 @@
       <c r="C7" s="2">
         <v>8.7527460644814088</v>
       </c>
-      <c r="D7" s="2">
-        <v>33.414195951190571</v>
-      </c>
+      <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="G7" s="2">
         <v>3</v>
@@ -659,9 +730,7 @@
       <c r="I7" s="2">
         <v>32.465087426973874</v>
       </c>
-      <c r="J7" s="2">
-        <v>33.414195951190571</v>
-      </c>
+      <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="M7" s="2">
         <v>3</v>
@@ -670,9 +739,7 @@
       <c r="O7" s="2">
         <v>23.074386864512853</v>
       </c>
-      <c r="P7" s="2">
-        <v>33.414195951190571</v>
-      </c>
+      <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="S7" s="2">
         <v>3</v>
@@ -681,12 +748,28 @@
       <c r="U7" s="2">
         <v>88.764916371290127</v>
       </c>
-      <c r="V7" s="2">
-        <v>33.414195951190571</v>
-      </c>
+      <c r="V7" s="2"/>
       <c r="W7" s="2"/>
-    </row>
-    <row r="8" spans="1:23">
+      <c r="Y7" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2">
+        <v>812.23428932003458</v>
+      </c>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AE7" s="2">
+        <v>3</v>
+      </c>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2">
+        <v>419.5255114260471</v>
+      </c>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+    </row>
+    <row r="8" spans="1:35">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -694,9 +777,7 @@
       <c r="C8" s="2">
         <v>8.8082906792446956</v>
       </c>
-      <c r="D8" s="2">
-        <v>33.10390321886964</v>
-      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="G8" s="2">
         <v>4</v>
@@ -705,9 +786,7 @@
       <c r="I8" s="2">
         <v>35.460499005783397</v>
       </c>
-      <c r="J8" s="2">
-        <v>33.10390321886964</v>
-      </c>
+      <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="M8" s="2">
         <v>4</v>
@@ -716,9 +795,7 @@
       <c r="O8" s="2">
         <v>17.708531393706885</v>
       </c>
-      <c r="P8" s="2">
-        <v>33.10390321886964</v>
-      </c>
+      <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="S8" s="2">
         <v>4</v>
@@ -727,12 +804,28 @@
       <c r="U8" s="2">
         <v>88.900635432109382</v>
       </c>
-      <c r="V8" s="2">
-        <v>33.10390321886964</v>
-      </c>
+      <c r="V8" s="2"/>
       <c r="W8" s="2"/>
-    </row>
-    <row r="9" spans="1:23">
+      <c r="Y8" s="2">
+        <v>4</v>
+      </c>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2">
+        <v>811.73937971337125</v>
+      </c>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AE8" s="2">
+        <v>4</v>
+      </c>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2">
+        <v>422.67560304195183</v>
+      </c>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+    </row>
+    <row r="9" spans="1:35">
       <c r="A9" s="2">
         <v>5</v>
       </c>
@@ -740,9 +833,7 @@
       <c r="C9" s="2">
         <v>8.9565860324539575</v>
       </c>
-      <c r="D9" s="2">
-        <v>34.532627902761824</v>
-      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="G9" s="2">
         <v>5</v>
@@ -751,9 +842,7 @@
       <c r="I9" s="2">
         <v>33.453129314424281</v>
       </c>
-      <c r="J9" s="2">
-        <v>34.532627902761824</v>
-      </c>
+      <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="M9" s="2">
         <v>5</v>
@@ -762,9 +851,7 @@
       <c r="O9" s="2">
         <v>20.912293649444411</v>
       </c>
-      <c r="P9" s="2">
-        <v>34.532627902761824</v>
-      </c>
+      <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="S9" s="2">
         <v>5</v>
@@ -773,12 +860,28 @@
       <c r="U9" s="2">
         <v>89.156182929271282</v>
       </c>
-      <c r="V9" s="2">
-        <v>34.532627902761824</v>
-      </c>
+      <c r="V9" s="2"/>
       <c r="W9" s="2"/>
-    </row>
-    <row r="10" spans="1:23">
+      <c r="Y9" s="2">
+        <v>5</v>
+      </c>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2">
+        <v>809.38094825166468</v>
+      </c>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AE9" s="2">
+        <v>5</v>
+      </c>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2">
+        <v>426.76671774352894</v>
+      </c>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="2"/>
+    </row>
+    <row r="10" spans="1:35">
       <c r="A10" s="2">
         <v>6</v>
       </c>
@@ -786,9 +889,7 @@
       <c r="C10" s="2">
         <v>9.0439585333186283</v>
       </c>
-      <c r="D10" s="2">
-        <v>33.954393269315474</v>
-      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="G10" s="2">
         <v>6</v>
@@ -797,9 +898,7 @@
       <c r="I10" s="2">
         <v>34.124926790775881</v>
       </c>
-      <c r="J10" s="2">
-        <v>33.954393269315474</v>
-      </c>
+      <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="M10" s="2">
         <v>6</v>
@@ -808,9 +907,7 @@
       <c r="O10" s="2">
         <v>20.048862798086571</v>
       </c>
-      <c r="P10" s="2">
-        <v>33.954393269315474</v>
-      </c>
+      <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="S10" s="2">
         <v>6</v>
@@ -819,12 +916,28 @@
       <c r="U10" s="2">
         <v>90.560128155756473</v>
       </c>
-      <c r="V10" s="2">
-        <v>33.954393269315474</v>
-      </c>
+      <c r="V10" s="2"/>
       <c r="W10" s="2"/>
-    </row>
-    <row r="11" spans="1:23">
+      <c r="Y10" s="2">
+        <v>6</v>
+      </c>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2">
+        <v>820.36724361717665</v>
+      </c>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
+      <c r="AE10" s="2">
+        <v>6</v>
+      </c>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="2">
+        <v>414.17008911382715</v>
+      </c>
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="2"/>
+    </row>
+    <row r="11" spans="1:35">
       <c r="A11" s="2">
         <v>7</v>
       </c>
@@ -832,9 +945,7 @@
       <c r="C11" s="2">
         <v>7.991795208482527</v>
       </c>
-      <c r="D11" s="2">
-        <v>34.188286916042344</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="G11" s="2">
         <v>7</v>
@@ -843,9 +954,7 @@
       <c r="I11" s="2">
         <v>36.171814283210111</v>
       </c>
-      <c r="J11" s="2">
-        <v>34.188286916042344</v>
-      </c>
+      <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="M11" s="2">
         <v>7</v>
@@ -854,9 +963,7 @@
       <c r="O11" s="2">
         <v>25.58484696044728</v>
       </c>
-      <c r="P11" s="2">
-        <v>34.188286916042344</v>
-      </c>
+      <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="S11" s="2">
         <v>7</v>
@@ -865,12 +972,28 @@
       <c r="U11" s="2">
         <v>87.985253243016643</v>
       </c>
-      <c r="V11" s="2">
-        <v>34.188286916042344</v>
-      </c>
+      <c r="V11" s="2"/>
       <c r="W11" s="2"/>
-    </row>
-    <row r="12" spans="1:23">
+      <c r="Y11" s="2">
+        <v>7</v>
+      </c>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2">
+        <v>820.40904802852674</v>
+      </c>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AE11" s="2">
+        <v>7</v>
+      </c>
+      <c r="AF11" s="2"/>
+      <c r="AG11" s="2">
+        <v>423.02220302402208</v>
+      </c>
+      <c r="AH11" s="2"/>
+      <c r="AI11" s="2"/>
+    </row>
+    <row r="12" spans="1:35">
       <c r="A12" s="2">
         <v>8</v>
       </c>
@@ -878,9 +1001,7 @@
       <c r="C12" s="2">
         <v>8.7258167293044</v>
       </c>
-      <c r="D12" s="2">
-        <v>35.225941225370008</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="G12" s="2">
         <v>8</v>
@@ -889,9 +1010,7 @@
       <c r="I12" s="2">
         <v>34.242574376967504</v>
       </c>
-      <c r="J12" s="2">
-        <v>35.225941225370008</v>
-      </c>
+      <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="M12" s="2">
         <v>8</v>
@@ -900,9 +1019,7 @@
       <c r="O12" s="2">
         <v>22.171037946605658</v>
       </c>
-      <c r="P12" s="2">
-        <v>35.225941225370008</v>
-      </c>
+      <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="S12" s="2">
         <v>8</v>
@@ -911,12 +1028,28 @@
       <c r="U12" s="2">
         <v>87.90024205594537</v>
       </c>
-      <c r="V12" s="2">
-        <v>35.225941225370008</v>
-      </c>
+      <c r="V12" s="2"/>
       <c r="W12" s="2"/>
-    </row>
-    <row r="13" spans="1:23">
+      <c r="Y12" s="2">
+        <v>8</v>
+      </c>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2">
+        <v>811.48577541751661</v>
+      </c>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AE12" s="2">
+        <v>8</v>
+      </c>
+      <c r="AF12" s="2"/>
+      <c r="AG12" s="2">
+        <v>424.99890930556256</v>
+      </c>
+      <c r="AH12" s="2"/>
+      <c r="AI12" s="2"/>
+    </row>
+    <row r="13" spans="1:35">
       <c r="A13" s="2">
         <v>9</v>
       </c>
@@ -924,9 +1057,7 @@
       <c r="C13" s="2">
         <v>8.6683224770388314</v>
       </c>
-      <c r="D13" s="2">
-        <v>32.822205520592874</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="G13" s="2">
         <v>9</v>
@@ -935,9 +1066,7 @@
       <c r="I13" s="2">
         <v>35.52983282923654</v>
       </c>
-      <c r="J13" s="2">
-        <v>32.822205520592874</v>
-      </c>
+      <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="M13" s="2">
         <v>9</v>
@@ -946,9 +1075,7 @@
       <c r="O13" s="2">
         <v>25.013346312937355</v>
       </c>
-      <c r="P13" s="2">
-        <v>32.822205520592874</v>
-      </c>
+      <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="S13" s="2">
         <v>9</v>
@@ -957,12 +1084,28 @@
       <c r="U13" s="2">
         <v>89.44969605081809</v>
       </c>
-      <c r="V13" s="2">
-        <v>32.822205520592874</v>
-      </c>
+      <c r="V13" s="2"/>
       <c r="W13" s="2"/>
-    </row>
-    <row r="14" spans="1:23">
+      <c r="Y13" s="2">
+        <v>9</v>
+      </c>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2">
+        <v>825.52009883417236</v>
+      </c>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AE13" s="2">
+        <v>9</v>
+      </c>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="2">
+        <v>422.97709245578886</v>
+      </c>
+      <c r="AH13" s="2"/>
+      <c r="AI13" s="2"/>
+    </row>
+    <row r="14" spans="1:35">
       <c r="A14" s="2">
         <v>10</v>
       </c>
@@ -970,9 +1113,7 @@
       <c r="C14" s="2">
         <v>8.8591766192163455</v>
       </c>
-      <c r="D14" s="2">
-        <v>34.406714412746496</v>
-      </c>
+      <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="G14" s="2">
         <v>10</v>
@@ -981,9 +1122,7 @@
       <c r="I14" s="2">
         <v>33.857234033497136</v>
       </c>
-      <c r="J14" s="2">
-        <v>34.406714412746496</v>
-      </c>
+      <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="M14" s="2">
         <v>10</v>
@@ -992,9 +1131,7 @@
       <c r="O14" s="2">
         <v>22.702045493559762</v>
       </c>
-      <c r="P14" s="2">
-        <v>34.406714412746496</v>
-      </c>
+      <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="S14" s="2">
         <v>10</v>
@@ -1003,12 +1140,28 @@
       <c r="U14" s="2">
         <v>89.85584362099965</v>
       </c>
-      <c r="V14" s="2">
-        <v>34.406714412746496</v>
-      </c>
+      <c r="V14" s="2"/>
       <c r="W14" s="2"/>
-    </row>
-    <row r="15" spans="1:23">
+      <c r="Y14" s="2">
+        <v>10</v>
+      </c>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2">
+        <v>812.90675909780009</v>
+      </c>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AE14" s="2">
+        <v>10</v>
+      </c>
+      <c r="AF14" s="2"/>
+      <c r="AG14" s="2">
+        <v>424.18716868500258</v>
+      </c>
+      <c r="AH14" s="2"/>
+      <c r="AI14" s="2"/>
+    </row>
+    <row r="15" spans="1:35">
       <c r="A15" s="2">
         <v>11</v>
       </c>
@@ -1016,9 +1169,7 @@
       <c r="C15" s="2">
         <v>9.0088313483942351</v>
       </c>
-      <c r="D15" s="2">
-        <v>35.754307256723955</v>
-      </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="G15" s="2">
         <v>11</v>
@@ -1027,9 +1178,7 @@
       <c r="I15" s="2">
         <v>33.968154030631965</v>
       </c>
-      <c r="J15" s="2">
-        <v>35.754307256723955</v>
-      </c>
+      <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="M15" s="2">
         <v>11</v>
@@ -1038,9 +1187,7 @@
       <c r="O15" s="2">
         <v>22.033482987701852</v>
       </c>
-      <c r="P15" s="2">
-        <v>35.754307256723955</v>
-      </c>
+      <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="S15" s="2">
         <v>11</v>
@@ -1049,12 +1196,28 @@
       <c r="U15" s="2">
         <v>89.346589288574776</v>
       </c>
-      <c r="V15" s="2">
-        <v>35.754307256723955</v>
-      </c>
+      <c r="V15" s="2"/>
       <c r="W15" s="2"/>
-    </row>
-    <row r="16" spans="1:23">
+      <c r="Y15" s="2">
+        <v>11</v>
+      </c>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2">
+        <v>817.95724324851381</v>
+      </c>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AE15" s="2">
+        <v>11</v>
+      </c>
+      <c r="AF15" s="2"/>
+      <c r="AG15" s="2">
+        <v>420.9134437837501</v>
+      </c>
+      <c r="AH15" s="2"/>
+      <c r="AI15" s="2"/>
+    </row>
+    <row r="16" spans="1:35">
       <c r="A16" s="2">
         <v>12</v>
       </c>
@@ -1062,9 +1225,7 @@
       <c r="C16" s="2">
         <v>8.4288989027471448</v>
       </c>
-      <c r="D16" s="2">
-        <v>35.07667385668708</v>
-      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="G16" s="2">
         <v>12</v>
@@ -1073,9 +1234,7 @@
       <c r="I16" s="2">
         <v>35.219756203838827</v>
       </c>
-      <c r="J16" s="2">
-        <v>35.07667385668708</v>
-      </c>
+      <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="M16" s="2">
         <v>12</v>
@@ -1084,9 +1243,7 @@
       <c r="O16" s="2">
         <v>21.452720065004726</v>
       </c>
-      <c r="P16" s="2">
-        <v>35.07667385668708</v>
-      </c>
+      <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="S16" s="2">
         <v>12</v>
@@ -1095,12 +1252,28 @@
       <c r="U16" s="2">
         <v>89.169665431178501</v>
       </c>
-      <c r="V16" s="2">
-        <v>35.07667385668708</v>
-      </c>
+      <c r="V16" s="2"/>
       <c r="W16" s="2"/>
-    </row>
-    <row r="17" spans="1:23">
+      <c r="Y16" s="2">
+        <v>12</v>
+      </c>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2">
+        <v>804.79886146046283</v>
+      </c>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AE16" s="2">
+        <v>12</v>
+      </c>
+      <c r="AF16" s="2"/>
+      <c r="AG16" s="2">
+        <v>423.15290887450993</v>
+      </c>
+      <c r="AH16" s="2"/>
+      <c r="AI16" s="2"/>
+    </row>
+    <row r="17" spans="1:35">
       <c r="A17" s="2">
         <v>13</v>
       </c>
@@ -1108,9 +1281,7 @@
       <c r="C17" s="2">
         <v>8.6018563724973021</v>
       </c>
-      <c r="D17" s="2">
-        <v>35.26457661466717</v>
-      </c>
+      <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="G17" s="2">
         <v>13</v>
@@ -1119,9 +1290,7 @@
       <c r="I17" s="2">
         <v>34.197487420032651</v>
       </c>
-      <c r="J17" s="2">
-        <v>35.26457661466717</v>
-      </c>
+      <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="M17" s="2">
         <v>13</v>
@@ -1130,9 +1299,7 @@
       <c r="O17" s="2">
         <v>24.284514860292166</v>
       </c>
-      <c r="P17" s="2">
-        <v>35.26457661466717</v>
-      </c>
+      <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="S17" s="2">
         <v>13</v>
@@ -1141,12 +1308,28 @@
       <c r="U17" s="2">
         <v>87.555155671271748</v>
       </c>
-      <c r="V17" s="2">
-        <v>35.26457661466717</v>
-      </c>
+      <c r="V17" s="2"/>
       <c r="W17" s="2"/>
-    </row>
-    <row r="18" spans="1:23">
+      <c r="Y17" s="2">
+        <v>13</v>
+      </c>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2">
+        <v>804.11017053529758</v>
+      </c>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AE17" s="2">
+        <v>13</v>
+      </c>
+      <c r="AF17" s="2"/>
+      <c r="AG17" s="2">
+        <v>415.91938324453645</v>
+      </c>
+      <c r="AH17" s="2"/>
+      <c r="AI17" s="2"/>
+    </row>
+    <row r="18" spans="1:35">
       <c r="A18" s="2">
         <v>14</v>
       </c>
@@ -1154,9 +1337,7 @@
       <c r="C18" s="2">
         <v>8.473699395860617</v>
       </c>
-      <c r="D18" s="2">
-        <v>34.990444301090378</v>
-      </c>
+      <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="G18" s="2">
         <v>14</v>
@@ -1165,9 +1346,7 @@
       <c r="I18" s="2">
         <v>34.534323513622475</v>
       </c>
-      <c r="J18" s="2">
-        <v>34.990444301090378</v>
-      </c>
+      <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="M18" s="2">
         <v>14</v>
@@ -1176,9 +1355,7 @@
       <c r="O18" s="2">
         <v>25.891413586064644</v>
       </c>
-      <c r="P18" s="2">
-        <v>34.990444301090378</v>
-      </c>
+      <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="S18" s="2">
         <v>14</v>
@@ -1187,12 +1364,28 @@
       <c r="U18" s="2">
         <v>90.04644667510091</v>
       </c>
-      <c r="V18" s="2">
-        <v>34.990444301090378</v>
-      </c>
+      <c r="V18" s="2"/>
       <c r="W18" s="2"/>
-    </row>
-    <row r="19" spans="1:23">
+      <c r="Y18" s="2">
+        <v>14</v>
+      </c>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2">
+        <v>796.49228697130002</v>
+      </c>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AE18" s="2">
+        <v>14</v>
+      </c>
+      <c r="AF18" s="2"/>
+      <c r="AG18" s="2">
+        <v>421.19809395949756</v>
+      </c>
+      <c r="AH18" s="2"/>
+      <c r="AI18" s="2"/>
+    </row>
+    <row r="19" spans="1:35">
       <c r="A19" s="2">
         <v>15</v>
       </c>
@@ -1200,9 +1393,7 @@
       <c r="C19" s="2">
         <v>8.56792558766948</v>
       </c>
-      <c r="D19" s="2">
-        <v>33.652591405527673</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="G19" s="2">
         <v>15</v>
@@ -1211,9 +1402,7 @@
       <c r="I19" s="2">
         <v>34.665393028275631</v>
       </c>
-      <c r="J19" s="2">
-        <v>33.652591405527673</v>
-      </c>
+      <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="M19" s="2">
         <v>15</v>
@@ -1222,9 +1411,7 @@
       <c r="O19" s="2">
         <v>22.507639934291475</v>
       </c>
-      <c r="P19" s="2">
-        <v>33.652591405527673</v>
-      </c>
+      <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="S19" s="2">
         <v>15</v>
@@ -1233,12 +1420,28 @@
       <c r="U19" s="2">
         <v>88.926150708891043</v>
       </c>
-      <c r="V19" s="2">
-        <v>33.652591405527673</v>
-      </c>
+      <c r="V19" s="2"/>
       <c r="W19" s="2"/>
-    </row>
-    <row r="20" spans="1:23">
+      <c r="Y19" s="2">
+        <v>15</v>
+      </c>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2">
+        <v>817.51012257642628</v>
+      </c>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AE19" s="2">
+        <v>15</v>
+      </c>
+      <c r="AF19" s="2"/>
+      <c r="AG19" s="2">
+        <v>421.24423479257405</v>
+      </c>
+      <c r="AH19" s="2"/>
+      <c r="AI19" s="2"/>
+    </row>
+    <row r="20" spans="1:35">
       <c r="A20" s="2">
         <v>16</v>
       </c>
@@ -1246,9 +1449,7 @@
       <c r="C20" s="2">
         <v>8.8399753241941941</v>
       </c>
-      <c r="D20" s="2">
-        <v>35.493750234388799</v>
-      </c>
+      <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="G20" s="2">
         <v>16</v>
@@ -1257,9 +1458,7 @@
       <c r="I20" s="2">
         <v>34.235351458733184</v>
       </c>
-      <c r="J20" s="2">
-        <v>35.493750234388799</v>
-      </c>
+      <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="M20" s="2">
         <v>16</v>
@@ -1268,9 +1467,7 @@
       <c r="O20" s="2">
         <v>24.707347173049023</v>
       </c>
-      <c r="P20" s="2">
-        <v>35.493750234388799</v>
-      </c>
+      <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="S20" s="2">
         <v>16</v>
@@ -1279,12 +1476,28 @@
       <c r="U20" s="2">
         <v>89.387721575792241</v>
       </c>
-      <c r="V20" s="2">
-        <v>35.493750234388799</v>
-      </c>
+      <c r="V20" s="2"/>
       <c r="W20" s="2"/>
-    </row>
-    <row r="21" spans="1:23">
+      <c r="Y20" s="2">
+        <v>16</v>
+      </c>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2">
+        <v>804.15125188653644</v>
+      </c>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="2"/>
+      <c r="AE20" s="2">
+        <v>16</v>
+      </c>
+      <c r="AF20" s="2"/>
+      <c r="AG20" s="2">
+        <v>419.95919613565798</v>
+      </c>
+      <c r="AH20" s="2"/>
+      <c r="AI20" s="2"/>
+    </row>
+    <row r="21" spans="1:35">
       <c r="A21" s="2">
         <v>17</v>
       </c>
@@ -1292,9 +1505,7 @@
       <c r="C21" s="2">
         <v>9.2748385582093729</v>
       </c>
-      <c r="D21" s="2">
-        <v>35.392234789709974</v>
-      </c>
+      <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="G21" s="2">
         <v>17</v>
@@ -1303,9 +1514,7 @@
       <c r="I21" s="2">
         <v>35.068867181003313</v>
       </c>
-      <c r="J21" s="2">
-        <v>35.392234789709974</v>
-      </c>
+      <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="M21" s="2">
         <v>17</v>
@@ -1314,9 +1523,7 @@
       <c r="O21" s="2">
         <v>19.979692594762451</v>
       </c>
-      <c r="P21" s="2">
-        <v>35.392234789709974</v>
-      </c>
+      <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="S21" s="2">
         <v>17</v>
@@ -1325,12 +1532,28 @@
       <c r="U21" s="2">
         <v>90.146626768418074</v>
       </c>
-      <c r="V21" s="2">
-        <v>35.392234789709974</v>
-      </c>
+      <c r="V21" s="2"/>
       <c r="W21" s="2"/>
-    </row>
-    <row r="22" spans="1:23">
+      <c r="Y21" s="2">
+        <v>17</v>
+      </c>
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="2">
+        <v>822.12664092970385</v>
+      </c>
+      <c r="AB21" s="2"/>
+      <c r="AC21" s="2"/>
+      <c r="AE21" s="2">
+        <v>17</v>
+      </c>
+      <c r="AF21" s="2"/>
+      <c r="AG21" s="2">
+        <v>424.82387835376556</v>
+      </c>
+      <c r="AH21" s="2"/>
+      <c r="AI21" s="2"/>
+    </row>
+    <row r="22" spans="1:35">
       <c r="A22" s="2">
         <v>18</v>
       </c>
@@ -1338,9 +1561,7 @@
       <c r="C22" s="2">
         <v>8.9328016740605456</v>
       </c>
-      <c r="D22" s="2">
-        <v>33.091644786556117</v>
-      </c>
+      <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="G22" s="2">
         <v>18</v>
@@ -1349,9 +1570,7 @@
       <c r="I22" s="2">
         <v>35.187536616426883</v>
       </c>
-      <c r="J22" s="2">
-        <v>33.091644786556117</v>
-      </c>
+      <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="M22" s="2">
         <v>18</v>
@@ -1360,9 +1579,7 @@
       <c r="O22" s="2">
         <v>22.598230862597269</v>
       </c>
-      <c r="P22" s="2">
-        <v>33.091644786556117</v>
-      </c>
+      <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="S22" s="2">
         <v>18</v>
@@ -1371,12 +1588,28 @@
       <c r="U22" s="2">
         <v>89.464820368026892</v>
       </c>
-      <c r="V22" s="2">
-        <v>33.091644786556117</v>
-      </c>
+      <c r="V22" s="2"/>
       <c r="W22" s="2"/>
-    </row>
-    <row r="23" spans="1:23">
+      <c r="Y22" s="2">
+        <v>18</v>
+      </c>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2">
+        <v>814.7148137267053</v>
+      </c>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="2"/>
+      <c r="AE22" s="2">
+        <v>18</v>
+      </c>
+      <c r="AF22" s="2"/>
+      <c r="AG22" s="2">
+        <v>412.2645061494153</v>
+      </c>
+      <c r="AH22" s="2"/>
+      <c r="AI22" s="2"/>
+    </row>
+    <row r="23" spans="1:35">
       <c r="A23" s="2">
         <v>19</v>
       </c>
@@ -1384,9 +1617,7 @@
       <c r="C23" s="2">
         <v>8.2299771406344977</v>
       </c>
-      <c r="D23" s="2">
-        <v>33.55428817370008</v>
-      </c>
+      <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="G23" s="2">
         <v>19</v>
@@ -1395,9 +1626,7 @@
       <c r="I23" s="2">
         <v>35.462226184029277</v>
       </c>
-      <c r="J23" s="2">
-        <v>33.55428817370008</v>
-      </c>
+      <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="M23" s="2">
         <v>19</v>
@@ -1406,9 +1635,7 @@
       <c r="O23" s="2">
         <v>25.131508956082868</v>
       </c>
-      <c r="P23" s="2">
-        <v>33.55428817370008</v>
-      </c>
+      <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="S23" s="2">
         <v>19</v>
@@ -1417,12 +1644,28 @@
       <c r="U23" s="2">
         <v>89.56632859934129</v>
       </c>
-      <c r="V23" s="2">
-        <v>33.55428817370008</v>
-      </c>
+      <c r="V23" s="2"/>
       <c r="W23" s="2"/>
-    </row>
-    <row r="24" spans="1:23">
+      <c r="Y23" s="2">
+        <v>19</v>
+      </c>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2">
+        <v>819.73802257117381</v>
+      </c>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AE23" s="2">
+        <v>19</v>
+      </c>
+      <c r="AF23" s="2"/>
+      <c r="AG23" s="2">
+        <v>423.08425508064676</v>
+      </c>
+      <c r="AH23" s="2"/>
+      <c r="AI23" s="2"/>
+    </row>
+    <row r="24" spans="1:35">
       <c r="A24" s="2">
         <v>20</v>
       </c>
@@ -1430,9 +1673,7 @@
       <c r="C24" s="2">
         <v>8.6500203105041038</v>
       </c>
-      <c r="D24" s="2">
-        <v>35.097837416371704</v>
-      </c>
+      <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="G24" s="2">
         <v>20</v>
@@ -1441,9 +1682,7 @@
       <c r="I24" s="2">
         <v>35.947208224593012</v>
       </c>
-      <c r="J24" s="2">
-        <v>35.097837416371704</v>
-      </c>
+      <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="M24" s="2">
         <v>20</v>
@@ -1452,9 +1691,7 @@
       <c r="O24" s="2">
         <v>24.248422655977393</v>
       </c>
-      <c r="P24" s="2">
-        <v>35.097837416371704</v>
-      </c>
+      <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="S24" s="2">
         <v>20</v>
@@ -1463,12 +1700,28 @@
       <c r="U24" s="2">
         <v>86.912890552886637</v>
       </c>
-      <c r="V24" s="2">
-        <v>35.097837416371704</v>
-      </c>
+      <c r="V24" s="2"/>
       <c r="W24" s="2"/>
-    </row>
-    <row r="25" spans="1:23">
+      <c r="Y24" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2">
+        <v>820.42129475210504</v>
+      </c>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="2"/>
+      <c r="AE24" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF24" s="2"/>
+      <c r="AG24" s="2">
+        <v>422.36600999776476</v>
+      </c>
+      <c r="AH24" s="2"/>
+      <c r="AI24" s="2"/>
+    </row>
+    <row r="25" spans="1:35">
       <c r="A25" s="2">
         <v>21</v>
       </c>
@@ -1476,9 +1729,7 @@
       <c r="C25" s="2">
         <v>8.9496800403291648</v>
       </c>
-      <c r="D25" s="2">
-        <v>34.77114772163079</v>
-      </c>
+      <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="G25" s="2">
         <v>21</v>
@@ -1487,9 +1738,7 @@
       <c r="I25" s="2">
         <v>34.410879788425561</v>
       </c>
-      <c r="J25" s="2">
-        <v>34.77114772163079</v>
-      </c>
+      <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="M25" s="2">
         <v>21</v>
@@ -1498,9 +1747,7 @@
       <c r="O25" s="2">
         <v>20.22789187414957</v>
       </c>
-      <c r="P25" s="2">
-        <v>34.77114772163079</v>
-      </c>
+      <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
       <c r="S25" s="2">
         <v>21</v>
@@ -1509,12 +1756,28 @@
       <c r="U25" s="2">
         <v>90.789054445727288</v>
       </c>
-      <c r="V25" s="2">
-        <v>34.77114772163079</v>
-      </c>
+      <c r="V25" s="2"/>
       <c r="W25" s="2"/>
-    </row>
-    <row r="26" spans="1:23">
+      <c r="Y25" s="2">
+        <v>21</v>
+      </c>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="2">
+        <v>818.26821956257299</v>
+      </c>
+      <c r="AB25" s="2"/>
+      <c r="AC25" s="2"/>
+      <c r="AE25" s="2">
+        <v>21</v>
+      </c>
+      <c r="AF25" s="2"/>
+      <c r="AG25" s="2">
+        <v>413.46351582774236</v>
+      </c>
+      <c r="AH25" s="2"/>
+      <c r="AI25" s="2"/>
+    </row>
+    <row r="26" spans="1:35">
       <c r="A26" s="2">
         <v>22</v>
       </c>
@@ -1522,9 +1785,7 @@
       <c r="C26" s="2">
         <v>9.5189105735240975</v>
       </c>
-      <c r="D26" s="2">
-        <v>34.534131615866343</v>
-      </c>
+      <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="G26" s="2">
         <v>22</v>
@@ -1533,9 +1794,7 @@
       <c r="I26" s="2">
         <v>35.321314744284848</v>
       </c>
-      <c r="J26" s="2">
-        <v>34.534131615866343</v>
-      </c>
+      <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="M26" s="2">
         <v>22</v>
@@ -1544,9 +1803,7 @@
       <c r="O26" s="2">
         <v>20.9701913726153</v>
       </c>
-      <c r="P26" s="2">
-        <v>34.534131615866343</v>
-      </c>
+      <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="S26" s="2">
         <v>22</v>
@@ -1555,12 +1812,28 @@
       <c r="U26" s="2">
         <v>89.846985300502752</v>
       </c>
-      <c r="V26" s="2">
-        <v>34.534131615866343</v>
-      </c>
+      <c r="V26" s="2"/>
       <c r="W26" s="2"/>
-    </row>
-    <row r="27" spans="1:23">
+      <c r="Y26" s="2">
+        <v>22</v>
+      </c>
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="2">
+        <v>803.98323825681348</v>
+      </c>
+      <c r="AB26" s="2"/>
+      <c r="AC26" s="2"/>
+      <c r="AE26" s="2">
+        <v>22</v>
+      </c>
+      <c r="AF26" s="2"/>
+      <c r="AG26" s="2">
+        <v>421.53615684308005</v>
+      </c>
+      <c r="AH26" s="2"/>
+      <c r="AI26" s="2"/>
+    </row>
+    <row r="27" spans="1:35">
       <c r="A27" s="2">
         <v>23</v>
       </c>
@@ -1568,9 +1841,7 @@
       <c r="C27" s="2">
         <v>8.4218825512814117</v>
       </c>
-      <c r="D27" s="2">
-        <v>34.8012231046376</v>
-      </c>
+      <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="G27" s="2">
         <v>23</v>
@@ -1579,9 +1850,7 @@
       <c r="I27" s="2">
         <v>34.348009505853561</v>
       </c>
-      <c r="J27" s="2">
-        <v>34.8012231046376</v>
-      </c>
+      <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="M27" s="2">
         <v>23</v>
@@ -1590,9 +1859,7 @@
       <c r="O27" s="2">
         <v>23.733788622342718</v>
       </c>
-      <c r="P27" s="2">
-        <v>34.8012231046376</v>
-      </c>
+      <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="S27" s="2">
         <v>23</v>
@@ -1601,12 +1868,28 @@
       <c r="U27" s="2">
         <v>88.847283856599674</v>
       </c>
-      <c r="V27" s="2">
-        <v>34.8012231046376</v>
-      </c>
+      <c r="V27" s="2"/>
       <c r="W27" s="2"/>
-    </row>
-    <row r="28" spans="1:23">
+      <c r="Y27" s="2">
+        <v>23</v>
+      </c>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="2">
+        <v>822.44484749864978</v>
+      </c>
+      <c r="AB27" s="2"/>
+      <c r="AC27" s="2"/>
+      <c r="AE27" s="2">
+        <v>23</v>
+      </c>
+      <c r="AF27" s="2"/>
+      <c r="AG27" s="2">
+        <v>415.38873002619226</v>
+      </c>
+      <c r="AH27" s="2"/>
+      <c r="AI27" s="2"/>
+    </row>
+    <row r="28" spans="1:35">
       <c r="A28" s="2">
         <v>24</v>
       </c>
@@ -1614,9 +1897,7 @@
       <c r="C28" s="2">
         <v>8.9132030055737772</v>
       </c>
-      <c r="D28" s="2">
-        <v>34.8817732783168</v>
-      </c>
+      <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="G28" s="2">
         <v>24</v>
@@ -1625,9 +1906,7 @@
       <c r="I28" s="2">
         <v>34.474826855154689</v>
       </c>
-      <c r="J28" s="2">
-        <v>34.8817732783168</v>
-      </c>
+      <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="M28" s="2">
         <v>24</v>
@@ -1636,9 +1915,7 @@
       <c r="O28" s="2">
         <v>20.461081438199216</v>
       </c>
-      <c r="P28" s="2">
-        <v>34.8817732783168</v>
-      </c>
+      <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
       <c r="S28" s="2">
         <v>24</v>
@@ -1647,12 +1924,28 @@
       <c r="U28" s="2">
         <v>88.962835804286385</v>
       </c>
-      <c r="V28" s="2">
-        <v>34.8817732783168</v>
-      </c>
+      <c r="V28" s="2"/>
       <c r="W28" s="2"/>
-    </row>
-    <row r="29" spans="1:23">
+      <c r="Y28" s="2">
+        <v>24</v>
+      </c>
+      <c r="Z28" s="2"/>
+      <c r="AA28" s="2">
+        <v>801.03783010516361</v>
+      </c>
+      <c r="AB28" s="2"/>
+      <c r="AC28" s="2"/>
+      <c r="AE28" s="2">
+        <v>24</v>
+      </c>
+      <c r="AF28" s="2"/>
+      <c r="AG28" s="2">
+        <v>409.10006242320122</v>
+      </c>
+      <c r="AH28" s="2"/>
+      <c r="AI28" s="2"/>
+    </row>
+    <row r="29" spans="1:35">
       <c r="A29" s="2">
         <v>25</v>
       </c>
@@ -1660,9 +1953,7 @@
       <c r="C29" s="2">
         <v>8.9839470830440025</v>
       </c>
-      <c r="D29" s="2">
-        <v>35.31663119471223</v>
-      </c>
+      <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="G29" s="2">
         <v>25</v>
@@ -1671,9 +1962,7 @@
       <c r="I29" s="2">
         <v>33.913138898204615</v>
       </c>
-      <c r="J29" s="2">
-        <v>35.31663119471223</v>
-      </c>
+      <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="M29" s="2">
         <v>25</v>
@@ -1682,9 +1971,7 @@
       <c r="O29" s="2">
         <v>19.559688451555957</v>
       </c>
-      <c r="P29" s="2">
-        <v>35.31663119471223</v>
-      </c>
+      <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="S29" s="2">
         <v>25</v>
@@ -1693,12 +1980,28 @@
       <c r="U29" s="2">
         <v>87.705174165305394</v>
       </c>
-      <c r="V29" s="2">
-        <v>35.31663119471223</v>
-      </c>
+      <c r="V29" s="2"/>
       <c r="W29" s="2"/>
-    </row>
-    <row r="30" spans="1:23">
+      <c r="Y29" s="2">
+        <v>25</v>
+      </c>
+      <c r="Z29" s="2"/>
+      <c r="AA29" s="2">
+        <v>804.06161071377949</v>
+      </c>
+      <c r="AB29" s="2"/>
+      <c r="AC29" s="2"/>
+      <c r="AE29" s="2">
+        <v>25</v>
+      </c>
+      <c r="AF29" s="2"/>
+      <c r="AG29" s="2">
+        <v>420.44599692575139</v>
+      </c>
+      <c r="AH29" s="2"/>
+      <c r="AI29" s="2"/>
+    </row>
+    <row r="30" spans="1:35">
       <c r="A30" s="2">
         <v>26</v>
       </c>
@@ -1706,9 +2009,7 @@
       <c r="C30" s="2">
         <v>9.1085264713126861</v>
       </c>
-      <c r="D30" s="2">
-        <v>33.223220903760506</v>
-      </c>
+      <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="G30" s="2">
         <v>26</v>
@@ -1717,9 +2018,7 @@
       <c r="I30" s="2">
         <v>34.755769438695815</v>
       </c>
-      <c r="J30" s="2">
-        <v>33.223220903760506</v>
-      </c>
+      <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="M30" s="2">
         <v>26</v>
@@ -1728,9 +2027,7 @@
       <c r="O30" s="2">
         <v>24.474464196559435</v>
       </c>
-      <c r="P30" s="2">
-        <v>33.223220903760506</v>
-      </c>
+      <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="S30" s="2">
         <v>26</v>
@@ -1739,12 +2036,28 @@
       <c r="U30" s="2">
         <v>87.895151208688048</v>
       </c>
-      <c r="V30" s="2">
-        <v>33.223220903760506</v>
-      </c>
+      <c r="V30" s="2"/>
       <c r="W30" s="2"/>
-    </row>
-    <row r="31" spans="1:23">
+      <c r="Y30" s="2">
+        <v>26</v>
+      </c>
+      <c r="Z30" s="2"/>
+      <c r="AA30" s="2">
+        <v>817.80934096247961</v>
+      </c>
+      <c r="AB30" s="2"/>
+      <c r="AC30" s="2"/>
+      <c r="AE30" s="2">
+        <v>26</v>
+      </c>
+      <c r="AF30" s="2"/>
+      <c r="AG30" s="2">
+        <v>418.54674246274936</v>
+      </c>
+      <c r="AH30" s="2"/>
+      <c r="AI30" s="2"/>
+    </row>
+    <row r="31" spans="1:35">
       <c r="A31" s="2">
         <v>27</v>
       </c>
@@ -1752,9 +2065,7 @@
       <c r="C31" s="2">
         <v>9.2041399964108503</v>
       </c>
-      <c r="D31" s="2">
-        <v>34.493444677833068</v>
-      </c>
+      <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="G31" s="2">
         <v>27</v>
@@ -1763,9 +2074,7 @@
       <c r="I31" s="2">
         <v>34.510931467172433</v>
       </c>
-      <c r="J31" s="2">
-        <v>34.493444677833068</v>
-      </c>
+      <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="M31" s="2">
         <v>27</v>
@@ -1774,9 +2083,7 @@
       <c r="O31" s="2">
         <v>24.347055943562715</v>
       </c>
-      <c r="P31" s="2">
-        <v>34.493444677833068</v>
-      </c>
+      <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="S31" s="2">
         <v>27</v>
@@ -1785,12 +2092,28 @@
       <c r="U31" s="2">
         <v>88.938586359584733</v>
       </c>
-      <c r="V31" s="2">
-        <v>34.493444677833068</v>
-      </c>
+      <c r="V31" s="2"/>
       <c r="W31" s="2"/>
-    </row>
-    <row r="32" spans="1:23">
+      <c r="Y31" s="2">
+        <v>27</v>
+      </c>
+      <c r="Z31" s="2"/>
+      <c r="AA31" s="2">
+        <v>816.68998211606993</v>
+      </c>
+      <c r="AB31" s="2"/>
+      <c r="AC31" s="2"/>
+      <c r="AE31" s="2">
+        <v>27</v>
+      </c>
+      <c r="AF31" s="2"/>
+      <c r="AG31" s="2">
+        <v>423.62002660480431</v>
+      </c>
+      <c r="AH31" s="2"/>
+      <c r="AI31" s="2"/>
+    </row>
+    <row r="32" spans="1:35">
       <c r="A32" s="2">
         <v>28</v>
       </c>
@@ -1798,9 +2121,7 @@
       <c r="C32" s="2">
         <v>8.8662335375863162</v>
       </c>
-      <c r="D32" s="2">
-        <v>35.315221026153679</v>
-      </c>
+      <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="G32" s="2">
         <v>28</v>
@@ -1809,9 +2130,7 @@
       <c r="I32" s="2">
         <v>35.013769055962264</v>
       </c>
-      <c r="J32" s="2">
-        <v>35.315221026153679</v>
-      </c>
+      <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="M32" s="2">
         <v>28</v>
@@ -1820,9 +2139,7 @@
       <c r="O32" s="2">
         <v>23.895397823502083</v>
       </c>
-      <c r="P32" s="2">
-        <v>35.315221026153679</v>
-      </c>
+      <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="S32" s="2">
         <v>28</v>
@@ -1831,12 +2148,28 @@
       <c r="U32" s="2">
         <v>89.895509451736373</v>
       </c>
-      <c r="V32" s="2">
-        <v>35.315221026153679</v>
-      </c>
+      <c r="V32" s="2"/>
       <c r="W32" s="2"/>
-    </row>
-    <row r="33" spans="1:23">
+      <c r="Y32" s="2">
+        <v>28</v>
+      </c>
+      <c r="Z32" s="2"/>
+      <c r="AA32" s="2">
+        <v>812.27664413261652</v>
+      </c>
+      <c r="AB32" s="2"/>
+      <c r="AC32" s="2"/>
+      <c r="AE32" s="2">
+        <v>28</v>
+      </c>
+      <c r="AF32" s="2"/>
+      <c r="AG32" s="2">
+        <v>421.03533894639946</v>
+      </c>
+      <c r="AH32" s="2"/>
+      <c r="AI32" s="2"/>
+    </row>
+    <row r="33" spans="1:35">
       <c r="A33" s="2">
         <v>29</v>
       </c>
@@ -1844,9 +2177,7 @@
       <c r="C33" s="2">
         <v>9.0619523391388146</v>
       </c>
-      <c r="D33" s="2">
-        <v>35.734482719855279</v>
-      </c>
+      <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="G33" s="2">
         <v>29</v>
@@ -1855,9 +2186,7 @@
       <c r="I33" s="2">
         <v>34.862596235722023</v>
       </c>
-      <c r="J33" s="2">
-        <v>35.734482719855279</v>
-      </c>
+      <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="M33" s="2">
         <v>29</v>
@@ -1866,9 +2195,7 @@
       <c r="O33" s="2">
         <v>18.331055401938414</v>
       </c>
-      <c r="P33" s="2">
-        <v>35.734482719855279</v>
-      </c>
+      <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
       <c r="S33" s="2">
         <v>29</v>
@@ -1877,12 +2204,28 @@
       <c r="U33" s="2">
         <v>89.053092467741266</v>
       </c>
-      <c r="V33" s="2">
-        <v>35.734482719855279</v>
-      </c>
+      <c r="V33" s="2"/>
       <c r="W33" s="2"/>
-    </row>
-    <row r="34" spans="1:23">
+      <c r="Y33" s="2">
+        <v>29</v>
+      </c>
+      <c r="Z33" s="2"/>
+      <c r="AA33" s="2">
+        <v>809.23454073675077</v>
+      </c>
+      <c r="AB33" s="2"/>
+      <c r="AC33" s="2"/>
+      <c r="AE33" s="2">
+        <v>29</v>
+      </c>
+      <c r="AF33" s="2"/>
+      <c r="AG33" s="2">
+        <v>425.30652482686997</v>
+      </c>
+      <c r="AH33" s="2"/>
+      <c r="AI33" s="2"/>
+    </row>
+    <row r="34" spans="1:35">
       <c r="A34" s="2">
         <v>30</v>
       </c>
@@ -1890,9 +2233,7 @@
       <c r="C34" s="2">
         <v>8.5162341599070928</v>
       </c>
-      <c r="D34" s="2">
-        <v>34.400667023288385</v>
-      </c>
+      <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="G34" s="2">
         <v>30</v>
@@ -1901,9 +2242,7 @@
       <c r="I34" s="2">
         <v>35.23601959002962</v>
       </c>
-      <c r="J34" s="2">
-        <v>34.400667023288385</v>
-      </c>
+      <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="M34" s="2">
         <v>30</v>
@@ -1912,9 +2251,7 @@
       <c r="O34" s="2">
         <v>20.120940418779071</v>
       </c>
-      <c r="P34" s="2">
-        <v>34.400667023288385</v>
-      </c>
+      <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
       <c r="S34" s="2">
         <v>30</v>
@@ -1923,17 +2260,35 @@
       <c r="U34" s="2">
         <v>90.016858318820184</v>
       </c>
-      <c r="V34" s="2">
-        <v>34.400667023288385</v>
-      </c>
+      <c r="V34" s="2"/>
       <c r="W34" s="2"/>
+      <c r="Y34" s="2">
+        <v>30</v>
+      </c>
+      <c r="Z34" s="2"/>
+      <c r="AA34" s="2">
+        <v>821.13294182594564</v>
+      </c>
+      <c r="AB34" s="2"/>
+      <c r="AC34" s="2"/>
+      <c r="AE34" s="2">
+        <v>30</v>
+      </c>
+      <c r="AF34" s="2"/>
+      <c r="AG34" s="2">
+        <v>420.42601369956316</v>
+      </c>
+      <c r="AH34" s="2"/>
+      <c r="AI34" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="AE3:AI3"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="N3:Q3"/>
     <mergeCell ref="S3:W3"/>
+    <mergeCell ref="Y3:AC3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1941,36 +2296,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:W34"/>
+  <dimension ref="A3:AI34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5:U34"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AE18" sqref="AE18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:35">
       <c r="A3" s="2"/>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
       <c r="S3" s="6" t="s">
         <v>8</v>
       </c>
@@ -1978,8 +2333,22 @@
       <c r="U3" s="7"/>
       <c r="V3" s="7"/>
       <c r="W3" s="8"/>
-    </row>
-    <row r="4" spans="1:23">
+      <c r="Y3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="8"/>
+      <c r="AE3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF3" s="7"/>
+      <c r="AG3" s="7"/>
+      <c r="AH3" s="7"/>
+      <c r="AI3" s="8"/>
+    </row>
+    <row r="4" spans="1:35">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -2040,8 +2409,38 @@
       <c r="W4" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:23">
+      <c r="Y4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI4" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -2049,9 +2448,7 @@
       <c r="C5" s="2">
         <v>2.1334945306560704</v>
       </c>
-      <c r="D5" s="2">
-        <v>9.4788485990828093</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="G5" s="2">
         <v>1</v>
@@ -2060,9 +2457,7 @@
       <c r="I5" s="2">
         <v>8.3318691318502953</v>
       </c>
-      <c r="J5" s="2">
-        <v>34.333337836390733</v>
-      </c>
+      <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="M5" s="2">
         <v>1</v>
@@ -2071,9 +2466,7 @@
       <c r="O5" s="2">
         <v>4.7143768259831491</v>
       </c>
-      <c r="P5" s="2">
-        <v>34.333337836390733</v>
-      </c>
+      <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="S5" s="2">
         <v>1</v>
@@ -2082,12 +2475,28 @@
       <c r="U5" s="2">
         <v>23.816540005628696</v>
       </c>
-      <c r="V5" s="2">
-        <v>34.333337836390733</v>
-      </c>
+      <c r="V5" s="2"/>
       <c r="W5" s="2"/>
-    </row>
-    <row r="6" spans="1:23">
+      <c r="Y5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2">
+        <v>198.77011387302639</v>
+      </c>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AE5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2">
+        <v>102.47796774420222</v>
+      </c>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+    </row>
+    <row r="6" spans="1:35">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -2095,9 +2504,7 @@
       <c r="C6" s="2">
         <v>1.9559903967612584</v>
       </c>
-      <c r="D6" s="2">
-        <v>8.3559987878404076</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="G6" s="2">
         <v>2</v>
@@ -2106,9 +2513,7 @@
       <c r="I6" s="2">
         <v>9.9055743149702025</v>
       </c>
-      <c r="J6" s="2">
-        <v>35.238292636577022</v>
-      </c>
+      <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="M6" s="2">
         <v>2</v>
@@ -2117,9 +2522,7 @@
       <c r="O6" s="2">
         <v>9.4124225566013742</v>
       </c>
-      <c r="P6" s="2">
-        <v>35.238292636577022</v>
-      </c>
+      <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="S6" s="2">
         <v>2</v>
@@ -2128,12 +2531,28 @@
       <c r="U6" s="2">
         <v>21.062510619807334</v>
       </c>
-      <c r="V6" s="2">
-        <v>35.238292636577022</v>
-      </c>
+      <c r="V6" s="2"/>
       <c r="W6" s="2"/>
-    </row>
-    <row r="7" spans="1:23">
+      <c r="Y6" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2">
+        <v>200.33957767873807</v>
+      </c>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AE6" s="2">
+        <v>2</v>
+      </c>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2">
+        <v>107.61390464803897</v>
+      </c>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+    </row>
+    <row r="7" spans="1:35">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -2141,9 +2560,7 @@
       <c r="C7" s="2">
         <v>2.3193518377696054</v>
       </c>
-      <c r="D7" s="2">
-        <v>9.9390650521741097</v>
-      </c>
+      <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="G7" s="2">
         <v>3</v>
@@ -2152,9 +2569,7 @@
       <c r="I7" s="2">
         <v>10.724345788325733</v>
       </c>
-      <c r="J7" s="2">
-        <v>33.414195951190571</v>
-      </c>
+      <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="M7" s="2">
         <v>3</v>
@@ -2163,9 +2578,7 @@
       <c r="O7" s="2">
         <v>6.6218519952512649</v>
       </c>
-      <c r="P7" s="2">
-        <v>33.414195951190571</v>
-      </c>
+      <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="S7" s="2">
         <v>3</v>
@@ -2174,12 +2587,28 @@
       <c r="U7" s="2">
         <v>22.489920708993097</v>
       </c>
-      <c r="V7" s="2">
-        <v>33.414195951190571</v>
-      </c>
+      <c r="V7" s="2"/>
       <c r="W7" s="2"/>
-    </row>
-    <row r="8" spans="1:23">
+      <c r="Y7" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2">
+        <v>203.99343786852498</v>
+      </c>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AE7" s="2">
+        <v>3</v>
+      </c>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2">
+        <v>108.0136212258269</v>
+      </c>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+    </row>
+    <row r="8" spans="1:35">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -2187,9 +2616,7 @@
       <c r="C8" s="2">
         <v>2.4345907539627509</v>
       </c>
-      <c r="D8" s="2">
-        <v>10.036514213751724</v>
-      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="G8" s="2">
         <v>4</v>
@@ -2198,9 +2625,7 @@
       <c r="I8" s="2">
         <v>8.1404903472824284</v>
       </c>
-      <c r="J8" s="2">
-        <v>33.10390321886964</v>
-      </c>
+      <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="M8" s="2">
         <v>4</v>
@@ -2209,9 +2634,7 @@
       <c r="O8" s="2">
         <v>11.055272461204169</v>
       </c>
-      <c r="P8" s="2">
-        <v>33.10390321886964</v>
-      </c>
+      <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="S8" s="2">
         <v>4</v>
@@ -2220,12 +2643,28 @@
       <c r="U8" s="2">
         <v>23.358995173572225</v>
       </c>
-      <c r="V8" s="2">
-        <v>33.10390321886964</v>
-      </c>
+      <c r="V8" s="2"/>
       <c r="W8" s="2"/>
-    </row>
-    <row r="9" spans="1:23">
+      <c r="Y8" s="2">
+        <v>4</v>
+      </c>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2">
+        <v>204.96588516299761</v>
+      </c>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AE8" s="2">
+        <v>4</v>
+      </c>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2">
+        <v>104.37391191855824</v>
+      </c>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+    </row>
+    <row r="9" spans="1:35">
       <c r="A9" s="2">
         <v>5</v>
       </c>
@@ -2233,9 +2672,7 @@
       <c r="C9" s="2">
         <v>2.1922969949641571</v>
       </c>
-      <c r="D9" s="2">
-        <v>8.7880365878879907</v>
-      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="G9" s="2">
         <v>5</v>
@@ -2244,9 +2681,7 @@
       <c r="I9" s="2">
         <v>9.6525497232356905</v>
       </c>
-      <c r="J9" s="2">
-        <v>34.532627902761824</v>
-      </c>
+      <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="M9" s="2">
         <v>5</v>
@@ -2255,9 +2690,7 @@
       <c r="O9" s="2">
         <v>7.9966623820057681</v>
       </c>
-      <c r="P9" s="2">
-        <v>34.532627902761824</v>
-      </c>
+      <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="S9" s="2">
         <v>5</v>
@@ -2266,12 +2699,28 @@
       <c r="U9" s="2">
         <v>22.450261199604128</v>
       </c>
-      <c r="V9" s="2">
-        <v>34.532627902761824</v>
-      </c>
+      <c r="V9" s="2"/>
       <c r="W9" s="2"/>
-    </row>
-    <row r="10" spans="1:23">
+      <c r="Y9" s="2">
+        <v>5</v>
+      </c>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2">
+        <v>207.18175273589034</v>
+      </c>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AE9" s="2">
+        <v>5</v>
+      </c>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2">
+        <v>99.743194434835203</v>
+      </c>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="2"/>
+    </row>
+    <row r="10" spans="1:35">
       <c r="A10" s="2">
         <v>6</v>
       </c>
@@ -2279,9 +2728,7 @@
       <c r="C10" s="2">
         <v>2.0560844437447612</v>
       </c>
-      <c r="D10" s="2">
-        <v>9.5860166865935845</v>
-      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="G10" s="2">
         <v>6</v>
@@ -2290,9 +2737,7 @@
       <c r="I10" s="2">
         <v>9.5431094062838024</v>
       </c>
-      <c r="J10" s="2">
-        <v>33.954393269315474</v>
-      </c>
+      <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="M10" s="2">
         <v>6</v>
@@ -2301,9 +2746,7 @@
       <c r="O10" s="2">
         <v>8.5404459724334885</v>
       </c>
-      <c r="P10" s="2">
-        <v>33.954393269315474</v>
-      </c>
+      <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="S10" s="2">
         <v>6</v>
@@ -2312,12 +2755,28 @@
       <c r="U10" s="2">
         <v>21.119194594032759</v>
       </c>
-      <c r="V10" s="2">
-        <v>33.954393269315474</v>
-      </c>
+      <c r="V10" s="2"/>
       <c r="W10" s="2"/>
-    </row>
-    <row r="11" spans="1:23">
+      <c r="Y10" s="2">
+        <v>6</v>
+      </c>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2">
+        <v>195.97459150383708</v>
+      </c>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
+      <c r="AE10" s="2">
+        <v>6</v>
+      </c>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="2">
+        <v>106.51793835975624</v>
+      </c>
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="2"/>
+    </row>
+    <row r="11" spans="1:35">
       <c r="A11" s="2">
         <v>7</v>
       </c>
@@ -2325,9 +2784,7 @@
       <c r="C11" s="2">
         <v>3.0706354486114908</v>
       </c>
-      <c r="D11" s="2">
-        <v>9.0291950806512595</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="G11" s="2">
         <v>7</v>
@@ -2336,9 +2793,7 @@
       <c r="I11" s="2">
         <v>7.9794403338394542</v>
       </c>
-      <c r="J11" s="2">
-        <v>34.188286916042344</v>
-      </c>
+      <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="M11" s="2">
         <v>7</v>
@@ -2347,9 +2802,7 @@
       <c r="O11" s="2">
         <v>3.2503455891247208</v>
       </c>
-      <c r="P11" s="2">
-        <v>34.188286916042344</v>
-      </c>
+      <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="S11" s="2">
         <v>7</v>
@@ -2358,12 +2811,28 @@
       <c r="U11" s="2">
         <v>23.427504001608462</v>
       </c>
-      <c r="V11" s="2">
-        <v>34.188286916042344</v>
-      </c>
+      <c r="V11" s="2"/>
       <c r="W11" s="2"/>
-    </row>
-    <row r="12" spans="1:23">
+      <c r="Y11" s="2">
+        <v>7</v>
+      </c>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2">
+        <v>192.67582669311869</v>
+      </c>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AE11" s="2">
+        <v>7</v>
+      </c>
+      <c r="AF11" s="2"/>
+      <c r="AG11" s="2">
+        <v>104.66443389121832</v>
+      </c>
+      <c r="AH11" s="2"/>
+      <c r="AI11" s="2"/>
+    </row>
+    <row r="12" spans="1:35">
       <c r="A12" s="2">
         <v>8</v>
       </c>
@@ -2371,9 +2840,7 @@
       <c r="C12" s="2">
         <v>2.3044975126198559</v>
       </c>
-      <c r="D12" s="2">
-        <v>8.007796895628168</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="G12" s="2">
         <v>8</v>
@@ -2382,9 +2849,7 @@
       <c r="I12" s="2">
         <v>9.3293501851619904</v>
       </c>
-      <c r="J12" s="2">
-        <v>35.225941225370008</v>
-      </c>
+      <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="M12" s="2">
         <v>8</v>
@@ -2393,9 +2858,7 @@
       <c r="O12" s="2">
         <v>7.1672572560075034</v>
       </c>
-      <c r="P12" s="2">
-        <v>35.225941225370008</v>
-      </c>
+      <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="S12" s="2">
         <v>8</v>
@@ -2404,12 +2867,28 @@
       <c r="U12" s="2">
         <v>23.069164002306078</v>
       </c>
-      <c r="V12" s="2">
-        <v>35.225941225370008</v>
-      </c>
+      <c r="V12" s="2"/>
       <c r="W12" s="2"/>
-    </row>
-    <row r="13" spans="1:23">
+      <c r="Y12" s="2">
+        <v>8</v>
+      </c>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2">
+        <v>204.89799099761626</v>
+      </c>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AE12" s="2">
+        <v>8</v>
+      </c>
+      <c r="AF12" s="2"/>
+      <c r="AG12" s="2">
+        <v>102.04192054989677</v>
+      </c>
+      <c r="AH12" s="2"/>
+      <c r="AI12" s="2"/>
+    </row>
+    <row r="13" spans="1:35">
       <c r="A13" s="2">
         <v>9</v>
       </c>
@@ -2417,9 +2896,7 @@
       <c r="C13" s="2">
         <v>2.688593883069414</v>
       </c>
-      <c r="D13" s="2">
-        <v>9.9176598764727579</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="G13" s="2">
         <v>9</v>
@@ -2428,9 +2905,7 @@
       <c r="I13" s="2">
         <v>8.70887912290166</v>
       </c>
-      <c r="J13" s="2">
-        <v>32.822205520592874</v>
-      </c>
+      <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="M13" s="2">
         <v>9</v>
@@ -2439,9 +2914,7 @@
       <c r="O13" s="2">
         <v>4.6750588016008674</v>
       </c>
-      <c r="P13" s="2">
-        <v>32.822205520592874</v>
-      </c>
+      <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="S13" s="2">
         <v>9</v>
@@ -2450,12 +2923,28 @@
       <c r="U13" s="2">
         <v>22.098123677287976</v>
       </c>
-      <c r="V13" s="2">
-        <v>32.822205520592874</v>
-      </c>
+      <c r="V13" s="2"/>
       <c r="W13" s="2"/>
-    </row>
-    <row r="14" spans="1:23">
+      <c r="Y13" s="2">
+        <v>9</v>
+      </c>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2">
+        <v>191.15766210796346</v>
+      </c>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AE13" s="2">
+        <v>9</v>
+      </c>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="2">
+        <v>104.6097553119202</v>
+      </c>
+      <c r="AH13" s="2"/>
+      <c r="AI13" s="2"/>
+    </row>
+    <row r="14" spans="1:35">
       <c r="A14" s="2">
         <v>10</v>
       </c>
@@ -2463,9 +2952,7 @@
       <c r="C14" s="2">
         <v>2.1515681707542798</v>
       </c>
-      <c r="D14" s="2">
-        <v>9.1049348917492825</v>
-      </c>
+      <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="G14" s="2">
         <v>10</v>
@@ -2474,9 +2961,7 @@
       <c r="I14" s="2">
         <v>9.1404875716195839</v>
       </c>
-      <c r="J14" s="2">
-        <v>34.406714412746496</v>
-      </c>
+      <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="M14" s="2">
         <v>10</v>
@@ -2485,9 +2970,7 @@
       <c r="O14" s="2">
         <v>7.768264107197556</v>
       </c>
-      <c r="P14" s="2">
-        <v>34.406714412746496</v>
-      </c>
+      <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="S14" s="2">
         <v>10</v>
@@ -2496,12 +2979,28 @@
       <c r="U14" s="2">
         <v>21.782262998149125</v>
       </c>
-      <c r="V14" s="2">
-        <v>34.406714412746496</v>
-      </c>
+      <c r="V14" s="2"/>
       <c r="W14" s="2"/>
-    </row>
-    <row r="15" spans="1:23">
+      <c r="Y14" s="2">
+        <v>10</v>
+      </c>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2">
+        <v>204.84184006911516</v>
+      </c>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AE14" s="2">
+        <v>10</v>
+      </c>
+      <c r="AF14" s="2"/>
+      <c r="AG14" s="2">
+        <v>103.17879716664456</v>
+      </c>
+      <c r="AH14" s="2"/>
+      <c r="AI14" s="2"/>
+    </row>
+    <row r="15" spans="1:35">
       <c r="A15" s="2">
         <v>11</v>
       </c>
@@ -2509,9 +3008,7 @@
       <c r="C15" s="2">
         <v>2.0508703222527038</v>
       </c>
-      <c r="D15" s="2">
-        <v>7.8845716016306202</v>
-      </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="G15" s="2">
         <v>11</v>
@@ -2520,9 +3017,7 @@
       <c r="I15" s="2">
         <v>9.3059809150041097</v>
       </c>
-      <c r="J15" s="2">
-        <v>35.754307256723955</v>
-      </c>
+      <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="M15" s="2">
         <v>11</v>
@@ -2531,9 +3026,7 @@
       <c r="O15" s="2">
         <v>7.8617358841656051</v>
       </c>
-      <c r="P15" s="2">
-        <v>35.754307256723955</v>
-      </c>
+      <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="S15" s="2">
         <v>11</v>
@@ -2542,12 +3035,28 @@
       <c r="U15" s="2">
         <v>21.974414232170737</v>
       </c>
-      <c r="V15" s="2">
-        <v>35.754307256723955</v>
-      </c>
+      <c r="V15" s="2"/>
       <c r="W15" s="2"/>
-    </row>
-    <row r="16" spans="1:23">
+      <c r="Y15" s="2">
+        <v>11</v>
+      </c>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2">
+        <v>198.17163437267089</v>
+      </c>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AE15" s="2">
+        <v>11</v>
+      </c>
+      <c r="AF15" s="2"/>
+      <c r="AG15" s="2">
+        <v>106.38231921844385</v>
+      </c>
+      <c r="AH15" s="2"/>
+      <c r="AI15" s="2"/>
+    </row>
+    <row r="16" spans="1:35">
       <c r="A16" s="2">
         <v>12</v>
       </c>
@@ -2555,9 +3064,7 @@
       <c r="C16" s="2">
         <v>2.5874983376243779</v>
       </c>
-      <c r="D16" s="2">
-        <v>8.2530564885301807</v>
-      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="G16" s="2">
         <v>12</v>
@@ -2566,9 +3073,7 @@
       <c r="I16" s="2">
         <v>8.3888187058648782</v>
       </c>
-      <c r="J16" s="2">
-        <v>35.07667385668708</v>
-      </c>
+      <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="M16" s="2">
         <v>12</v>
@@ -2577,9 +3082,7 @@
       <c r="O16" s="2">
         <v>7.2521409844709108</v>
       </c>
-      <c r="P16" s="2">
-        <v>35.07667385668708</v>
-      </c>
+      <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="S16" s="2">
         <v>12</v>
@@ -2588,12 +3091,28 @@
       <c r="U16" s="2">
         <v>22.689493934089398</v>
       </c>
-      <c r="V16" s="2">
-        <v>35.07667385668708</v>
-      </c>
+      <c r="V16" s="2"/>
       <c r="W16" s="2"/>
-    </row>
-    <row r="17" spans="1:23">
+      <c r="Y16" s="2">
+        <v>12</v>
+      </c>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2">
+        <v>214.8929925884087</v>
+      </c>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AE16" s="2">
+        <v>12</v>
+      </c>
+      <c r="AF16" s="2"/>
+      <c r="AG16" s="2">
+        <v>102.17313478600889</v>
+      </c>
+      <c r="AH16" s="2"/>
+      <c r="AI16" s="2"/>
+    </row>
+    <row r="17" spans="1:35">
       <c r="A17" s="2">
         <v>13</v>
       </c>
@@ -2601,9 +3120,7 @@
       <c r="C17" s="2">
         <v>2.3488104340313982</v>
       </c>
-      <c r="D17" s="2">
-        <v>8.2911420220333749</v>
-      </c>
+      <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="G17" s="2">
         <v>13</v>
@@ -2612,9 +3129,7 @@
       <c r="I17" s="2">
         <v>8.9347557701884384</v>
       </c>
-      <c r="J17" s="2">
-        <v>35.26457661466717</v>
-      </c>
+      <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="M17" s="2">
         <v>13</v>
@@ -2623,9 +3138,7 @@
       <c r="O17" s="2">
         <v>4.8630719321585296</v>
       </c>
-      <c r="P17" s="2">
-        <v>35.26457661466717</v>
-      </c>
+      <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="S17" s="2">
         <v>13</v>
@@ -2634,12 +3147,28 @@
       <c r="U17" s="2">
         <v>23.653509015870476</v>
       </c>
-      <c r="V17" s="2">
-        <v>35.26457661466717</v>
-      </c>
+      <c r="V17" s="2"/>
       <c r="W17" s="2"/>
-    </row>
-    <row r="18" spans="1:23">
+      <c r="Y17" s="2">
+        <v>13</v>
+      </c>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2">
+        <v>208.82593323104095</v>
+      </c>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AE17" s="2">
+        <v>13</v>
+      </c>
+      <c r="AF17" s="2"/>
+      <c r="AG17" s="2">
+        <v>110.3551587127657</v>
+      </c>
+      <c r="AH17" s="2"/>
+      <c r="AI17" s="2"/>
+    </row>
+    <row r="18" spans="1:35">
       <c r="A18" s="2">
         <v>14</v>
       </c>
@@ -2647,9 +3176,7 @@
       <c r="C18" s="2">
         <v>2.7376548885108725</v>
       </c>
-      <c r="D18" s="2">
-        <v>9.0911527113668846</v>
-      </c>
+      <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="G18" s="2">
         <v>14</v>
@@ -2658,9 +3185,7 @@
       <c r="I18" s="2">
         <v>8.7714162531669544</v>
       </c>
-      <c r="J18" s="2">
-        <v>34.990444301090378</v>
-      </c>
+      <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="M18" s="2">
         <v>14</v>
@@ -2669,9 +3194,7 @@
       <c r="O18" s="2">
         <v>3.5388177535866356</v>
       </c>
-      <c r="P18" s="2">
-        <v>34.990444301090378</v>
-      </c>
+      <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="S18" s="2">
         <v>14</v>
@@ -2680,12 +3203,28 @@
       <c r="U18" s="2">
         <v>21.095518848878051</v>
       </c>
-      <c r="V18" s="2">
-        <v>34.990444301090378</v>
-      </c>
+      <c r="V18" s="2"/>
       <c r="W18" s="2"/>
-    </row>
-    <row r="19" spans="1:23">
+      <c r="Y18" s="2">
+        <v>14</v>
+      </c>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2">
+        <v>216.47644209257226</v>
+      </c>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AE18" s="2">
+        <v>14</v>
+      </c>
+      <c r="AF18" s="2"/>
+      <c r="AG18" s="2">
+        <v>106.92960024690026</v>
+      </c>
+      <c r="AH18" s="2"/>
+      <c r="AI18" s="2"/>
+    </row>
+    <row r="19" spans="1:35">
       <c r="A19" s="2">
         <v>15</v>
       </c>
@@ -2693,9 +3232,7 @@
       <c r="C19" s="2">
         <v>2.6269802804504918</v>
       </c>
-      <c r="D19" s="2">
-        <v>9.960935131986874</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="G19" s="2">
         <v>15</v>
@@ -2704,9 +3241,7 @@
       <c r="I19" s="2">
         <v>8.6695442507978981</v>
       </c>
-      <c r="J19" s="2">
-        <v>33.652591405527673</v>
-      </c>
+      <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="M19" s="2">
         <v>15</v>
@@ -2715,9 +3250,7 @@
       <c r="O19" s="2">
         <v>7.0222861133328642</v>
       </c>
-      <c r="P19" s="2">
-        <v>33.652591405527673</v>
-      </c>
+      <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="S19" s="2">
         <v>15</v>
@@ -2726,12 +3259,28 @@
       <c r="U19" s="2">
         <v>22.496500773223126</v>
       </c>
-      <c r="V19" s="2">
-        <v>33.652591405527673</v>
-      </c>
+      <c r="V19" s="2"/>
       <c r="W19" s="2"/>
-    </row>
-    <row r="20" spans="1:23">
+      <c r="Y19" s="2">
+        <v>15</v>
+      </c>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2">
+        <v>197.98739714269823</v>
+      </c>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AE19" s="2">
+        <v>15</v>
+      </c>
+      <c r="AF19" s="2"/>
+      <c r="AG19" s="2">
+        <v>106.39883906294124</v>
+      </c>
+      <c r="AH19" s="2"/>
+      <c r="AI19" s="2"/>
+    </row>
+    <row r="20" spans="1:35">
       <c r="A20" s="2">
         <v>16</v>
       </c>
@@ -2739,9 +3288,7 @@
       <c r="C20" s="2">
         <v>2.2667773262884929</v>
       </c>
-      <c r="D20" s="2">
-        <v>8.2931088905432766</v>
-      </c>
+      <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="G20" s="2">
         <v>16</v>
@@ -2750,9 +3297,7 @@
       <c r="I20" s="2">
         <v>8.8372254096689637</v>
       </c>
-      <c r="J20" s="2">
-        <v>35.493750234388799</v>
-      </c>
+      <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="M20" s="2">
         <v>16</v>
@@ -2761,9 +3306,7 @@
       <c r="O20" s="2">
         <v>4.9155578335342058</v>
       </c>
-      <c r="P20" s="2">
-        <v>35.493750234388799</v>
-      </c>
+      <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="S20" s="2">
         <v>16</v>
@@ -2772,12 +3315,28 @@
       <c r="U20" s="2">
         <v>22.291452607418648</v>
       </c>
-      <c r="V20" s="2">
-        <v>35.493750234388799</v>
-      </c>
+      <c r="V20" s="2"/>
       <c r="W20" s="2"/>
-    </row>
-    <row r="21" spans="1:23">
+      <c r="Y20" s="2">
+        <v>16</v>
+      </c>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2">
+        <v>210.42331277904398</v>
+      </c>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="2"/>
+      <c r="AE20" s="2">
+        <v>16</v>
+      </c>
+      <c r="AF20" s="2"/>
+      <c r="AG20" s="2">
+        <v>106.94148534571694</v>
+      </c>
+      <c r="AH20" s="2"/>
+      <c r="AI20" s="2"/>
+    </row>
+    <row r="21" spans="1:35">
       <c r="A21" s="2">
         <v>17</v>
       </c>
@@ -2785,9 +3344,7 @@
       <c r="C21" s="2">
         <v>1.9193421394683214</v>
       </c>
-      <c r="D21" s="2">
-        <v>8.7778337246606082</v>
-      </c>
+      <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="G21" s="2">
         <v>17</v>
@@ -2796,9 +3353,7 @@
       <c r="I21" s="2">
         <v>8.606359315948378</v>
       </c>
-      <c r="J21" s="2">
-        <v>35.392234789709974</v>
-      </c>
+      <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="M21" s="2">
         <v>17</v>
@@ -2807,9 +3362,7 @@
       <c r="O21" s="2">
         <v>8.8147844954531855</v>
       </c>
-      <c r="P21" s="2">
-        <v>35.392234789709974</v>
-      </c>
+      <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="S21" s="2">
         <v>17</v>
@@ -2818,12 +3371,28 @@
       <c r="U21" s="2">
         <v>21.205964757693188</v>
       </c>
-      <c r="V21" s="2">
-        <v>35.392234789709974</v>
-      </c>
+      <c r="V21" s="2"/>
       <c r="W21" s="2"/>
-    </row>
-    <row r="22" spans="1:23">
+      <c r="Y21" s="2">
+        <v>17</v>
+      </c>
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="2">
+        <v>191.53291444194909</v>
+      </c>
+      <c r="AB21" s="2"/>
+      <c r="AC21" s="2"/>
+      <c r="AE21" s="2">
+        <v>17</v>
+      </c>
+      <c r="AF21" s="2"/>
+      <c r="AG21" s="2">
+        <v>103.24169601533083</v>
+      </c>
+      <c r="AH21" s="2"/>
+      <c r="AI21" s="2"/>
+    </row>
+    <row r="22" spans="1:35">
       <c r="A22" s="2">
         <v>18</v>
       </c>
@@ -2831,9 +3400,7 @@
       <c r="C22" s="2">
         <v>2.3136043230608241</v>
       </c>
-      <c r="D22" s="2">
-        <v>10.593530018213807</v>
-      </c>
+      <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="G22" s="2">
         <v>18</v>
@@ -2842,9 +3409,7 @@
       <c r="I22" s="2">
         <v>9.721964134553545</v>
       </c>
-      <c r="J22" s="2">
-        <v>33.091644786556117</v>
-      </c>
+      <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="M22" s="2">
         <v>18</v>
@@ -2853,9 +3418,7 @@
       <c r="O22" s="2">
         <v>6.629396187751988</v>
       </c>
-      <c r="P22" s="2">
-        <v>33.091644786556117</v>
-      </c>
+      <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="S22" s="2">
         <v>18</v>
@@ -2864,12 +3427,28 @@
       <c r="U22" s="2">
         <v>22.337749860051932</v>
       </c>
-      <c r="V22" s="2">
-        <v>33.091644786556117</v>
-      </c>
+      <c r="V22" s="2"/>
       <c r="W22" s="2"/>
-    </row>
-    <row r="23" spans="1:23">
+      <c r="Y22" s="2">
+        <v>18</v>
+      </c>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2">
+        <v>199.60090656428403</v>
+      </c>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="2"/>
+      <c r="AE22" s="2">
+        <v>18</v>
+      </c>
+      <c r="AF22" s="2"/>
+      <c r="AG22" s="2">
+        <v>108.12630157182934</v>
+      </c>
+      <c r="AH22" s="2"/>
+      <c r="AI22" s="2"/>
+    </row>
+    <row r="23" spans="1:35">
       <c r="A23" s="2">
         <v>19</v>
       </c>
@@ -2877,9 +3456,7 @@
       <c r="C23" s="2">
         <v>3.0784333801850732</v>
       </c>
-      <c r="D23" s="2">
-        <v>9.0963217451470566</v>
-      </c>
+      <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="G23" s="2">
         <v>19</v>
@@ -2888,9 +3465,7 @@
       <c r="I23" s="2">
         <v>7.9945526578383195</v>
       </c>
-      <c r="J23" s="2">
-        <v>33.55428817370008</v>
-      </c>
+      <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="M23" s="2">
         <v>19</v>
@@ -2899,9 +3474,7 @@
       <c r="O23" s="2">
         <v>3.7555606090788878</v>
       </c>
-      <c r="P23" s="2">
-        <v>33.55428817370008</v>
-      </c>
+      <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="S23" s="2">
         <v>19</v>
@@ -2910,12 +3483,28 @@
       <c r="U23" s="2">
         <v>22.108330905423241</v>
       </c>
-      <c r="V23" s="2">
-        <v>33.55428817370008</v>
-      </c>
+      <c r="V23" s="2"/>
       <c r="W23" s="2"/>
-    </row>
-    <row r="24" spans="1:23">
+      <c r="Y23" s="2">
+        <v>19</v>
+      </c>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2">
+        <v>193.32762177356909</v>
+      </c>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AE23" s="2">
+        <v>19</v>
+      </c>
+      <c r="AF23" s="2"/>
+      <c r="AG23" s="2">
+        <v>104.29985733966535</v>
+      </c>
+      <c r="AH23" s="2"/>
+      <c r="AI23" s="2"/>
+    </row>
+    <row r="24" spans="1:35">
       <c r="A24" s="2">
         <v>20</v>
       </c>
@@ -2923,9 +3512,7 @@
       <c r="C24" s="2">
         <v>2.5169192873482058</v>
       </c>
-      <c r="D24" s="2">
-        <v>8.6201480665153092</v>
-      </c>
+      <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="G24" s="2">
         <v>20</v>
@@ -2934,9 +3521,7 @@
       <c r="I24" s="2">
         <v>8.0836699445677667</v>
       </c>
-      <c r="J24" s="2">
-        <v>35.097837416371704</v>
-      </c>
+      <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="M24" s="2">
         <v>20</v>
@@ -2945,9 +3530,7 @@
       <c r="O24" s="2">
         <v>5.5036927820527817</v>
       </c>
-      <c r="P24" s="2">
-        <v>35.097837416371704</v>
-      </c>
+      <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="S24" s="2">
         <v>20</v>
@@ -2956,12 +3539,28 @@
       <c r="U24" s="2">
         <v>24.206796555777544</v>
       </c>
-      <c r="V24" s="2">
-        <v>35.097837416371704</v>
-      </c>
+      <c r="V24" s="2"/>
       <c r="W24" s="2"/>
-    </row>
-    <row r="25" spans="1:23">
+      <c r="Y24" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2">
+        <v>193.38172796442498</v>
+      </c>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="2"/>
+      <c r="AE24" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF24" s="2"/>
+      <c r="AG24" s="2">
+        <v>105.2727078088794</v>
+      </c>
+      <c r="AH24" s="2"/>
+      <c r="AI24" s="2"/>
+    </row>
+    <row r="25" spans="1:35">
       <c r="A25" s="2">
         <v>21</v>
       </c>
@@ -2969,9 +3568,7 @@
       <c r="C25" s="2">
         <v>2.0630056814983515</v>
       </c>
-      <c r="D25" s="2">
-        <v>8.9274676363201699</v>
-      </c>
+      <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="G25" s="2">
         <v>21</v>
@@ -2980,9 +3577,7 @@
       <c r="I25" s="2">
         <v>8.8308274530219144</v>
       </c>
-      <c r="J25" s="2">
-        <v>34.77114772163079</v>
-      </c>
+      <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="M25" s="2">
         <v>21</v>
@@ -2991,9 +3586,7 @@
       <c r="O25" s="2">
         <v>8.4233850914329693</v>
       </c>
-      <c r="P25" s="2">
-        <v>34.77114772163079</v>
-      </c>
+      <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
       <c r="S25" s="2">
         <v>21</v>
@@ -3002,12 +3595,28 @@
       <c r="U25" s="2">
         <v>20.931393195616486</v>
       </c>
-      <c r="V25" s="2">
-        <v>34.77114772163079</v>
-      </c>
+      <c r="V25" s="2"/>
       <c r="W25" s="2"/>
-    </row>
-    <row r="26" spans="1:23">
+      <c r="Y25" s="2">
+        <v>21</v>
+      </c>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="2">
+        <v>198.91708535275748</v>
+      </c>
+      <c r="AB25" s="2"/>
+      <c r="AC25" s="2"/>
+      <c r="AE25" s="2">
+        <v>21</v>
+      </c>
+      <c r="AF25" s="2"/>
+      <c r="AG25" s="2">
+        <v>107.12371888737583</v>
+      </c>
+      <c r="AH25" s="2"/>
+      <c r="AI25" s="2"/>
+    </row>
+    <row r="26" spans="1:35">
       <c r="A26" s="2">
         <v>22</v>
       </c>
@@ -3015,9 +3624,7 @@
       <c r="C26" s="2">
         <v>1.5963423619509298</v>
       </c>
-      <c r="D26" s="2">
-        <v>9.1123796386283153</v>
-      </c>
+      <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="G26" s="2">
         <v>22</v>
@@ -3026,9 +3633,7 @@
       <c r="I26" s="2">
         <v>8.4105912727021899</v>
       </c>
-      <c r="J26" s="2">
-        <v>34.534131615866343</v>
-      </c>
+      <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="M26" s="2">
         <v>22</v>
@@ -3037,9 +3642,7 @@
       <c r="O26" s="2">
         <v>9.9500108676513932</v>
       </c>
-      <c r="P26" s="2">
-        <v>34.534131615866343</v>
-      </c>
+      <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="S26" s="2">
         <v>22</v>
@@ -3048,12 +3651,28 @@
       <c r="U26" s="2">
         <v>21.710597899909828</v>
       </c>
-      <c r="V26" s="2">
-        <v>34.534131615866343</v>
-      </c>
+      <c r="V26" s="2"/>
       <c r="W26" s="2"/>
-    </row>
-    <row r="27" spans="1:23">
+      <c r="Y26" s="2">
+        <v>22</v>
+      </c>
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="2">
+        <v>213.13670347253424</v>
+      </c>
+      <c r="AB26" s="2"/>
+      <c r="AC26" s="2"/>
+      <c r="AE26" s="2">
+        <v>22</v>
+      </c>
+      <c r="AF26" s="2"/>
+      <c r="AG26" s="2">
+        <v>105.8077346138512</v>
+      </c>
+      <c r="AH26" s="2"/>
+      <c r="AI26" s="2"/>
+    </row>
+    <row r="27" spans="1:35">
       <c r="A27" s="2">
         <v>23</v>
       </c>
@@ -3061,9 +3680,7 @@
       <c r="C27" s="2">
         <v>2.5921794742509143</v>
       </c>
-      <c r="D27" s="2">
-        <v>8.5283002544562976</v>
-      </c>
+      <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="G27" s="2">
         <v>23</v>
@@ -3072,9 +3689,7 @@
       <c r="I27" s="2">
         <v>8.4141679203618924</v>
       </c>
-      <c r="J27" s="2">
-        <v>34.8012231046376</v>
-      </c>
+      <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="M27" s="2">
         <v>23</v>
@@ -3083,9 +3698,7 @@
       <c r="O27" s="2">
         <v>5.8717369400446371</v>
       </c>
-      <c r="P27" s="2">
-        <v>34.8012231046376</v>
-      </c>
+      <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="S27" s="2">
         <v>23</v>
@@ -3094,12 +3707,28 @@
       <c r="U27" s="2">
         <v>22.695345479298329</v>
       </c>
-      <c r="V27" s="2">
-        <v>34.8012231046376</v>
-      </c>
+      <c r="V27" s="2"/>
       <c r="W27" s="2"/>
-    </row>
-    <row r="28" spans="1:23">
+      <c r="Y27" s="2">
+        <v>23</v>
+      </c>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="2">
+        <v>193.20808311066634</v>
+      </c>
+      <c r="AB27" s="2"/>
+      <c r="AC27" s="2"/>
+      <c r="AE27" s="2">
+        <v>23</v>
+      </c>
+      <c r="AF27" s="2"/>
+      <c r="AG27" s="2">
+        <v>110.15500946087421</v>
+      </c>
+      <c r="AH27" s="2"/>
+      <c r="AI27" s="2"/>
+    </row>
+    <row r="28" spans="1:35">
       <c r="A28" s="2">
         <v>24</v>
       </c>
@@ -3107,9 +3736,7 @@
       <c r="C28" s="2">
         <v>2.1745976981089723</v>
       </c>
-      <c r="D28" s="2">
-        <v>9.0201699212193489</v>
-      </c>
+      <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="G28" s="2">
         <v>24</v>
@@ -3118,9 +3745,7 @@
       <c r="I28" s="2">
         <v>9.3802430641210819</v>
       </c>
-      <c r="J28" s="2">
-        <v>34.8817732783168</v>
-      </c>
+      <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="M28" s="2">
         <v>24</v>
@@ -3129,9 +3754,7 @@
       <c r="O28" s="2">
         <v>9.0265898645780354</v>
       </c>
-      <c r="P28" s="2">
-        <v>34.8817732783168</v>
-      </c>
+      <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
       <c r="S28" s="2">
         <v>24</v>
@@ -3140,12 +3763,28 @@
       <c r="U28" s="2">
         <v>22.638792879778123</v>
       </c>
-      <c r="V28" s="2">
-        <v>34.8817732783168</v>
-      </c>
+      <c r="V28" s="2"/>
       <c r="W28" s="2"/>
-    </row>
-    <row r="29" spans="1:23">
+      <c r="Y28" s="2">
+        <v>24</v>
+      </c>
+      <c r="Z28" s="2"/>
+      <c r="AA28" s="2">
+        <v>213.97601440574869</v>
+      </c>
+      <c r="AB28" s="2"/>
+      <c r="AC28" s="2"/>
+      <c r="AE28" s="2">
+        <v>24</v>
+      </c>
+      <c r="AF28" s="2"/>
+      <c r="AG28" s="2">
+        <v>111.04272446477889</v>
+      </c>
+      <c r="AH28" s="2"/>
+      <c r="AI28" s="2"/>
+    </row>
+    <row r="29" spans="1:35">
       <c r="A29" s="2">
         <v>25</v>
       </c>
@@ -3153,9 +3792,7 @@
       <c r="C29" s="2">
         <v>2.3897209605092868</v>
       </c>
-      <c r="D29" s="2">
-        <v>8.4231753656245214</v>
-      </c>
+      <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="G29" s="2">
         <v>25</v>
@@ -3164,9 +3801,7 @@
       <c r="I29" s="2">
         <v>9.0705311255470242</v>
       </c>
-      <c r="J29" s="2">
-        <v>35.31663119471223</v>
-      </c>
+      <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="M29" s="2">
         <v>25</v>
@@ -3175,9 +3810,7 @@
       <c r="O29" s="2">
         <v>11.469723382335658</v>
       </c>
-      <c r="P29" s="2">
-        <v>35.31663119471223</v>
-      </c>
+      <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="S29" s="2">
         <v>25</v>
@@ -3186,12 +3819,28 @@
       <c r="U29" s="2">
         <v>24.094856504004955</v>
       </c>
-      <c r="V29" s="2">
-        <v>35.31663119471223</v>
-      </c>
+      <c r="V29" s="2"/>
       <c r="W29" s="2"/>
-    </row>
-    <row r="30" spans="1:23">
+      <c r="Y29" s="2">
+        <v>25</v>
+      </c>
+      <c r="Z29" s="2"/>
+      <c r="AA29" s="2">
+        <v>210.68444317396879</v>
+      </c>
+      <c r="AB29" s="2"/>
+      <c r="AC29" s="2"/>
+      <c r="AE29" s="2">
+        <v>25</v>
+      </c>
+      <c r="AF29" s="2"/>
+      <c r="AG29" s="2">
+        <v>106.93338402998995</v>
+      </c>
+      <c r="AH29" s="2"/>
+      <c r="AI29" s="2"/>
+    </row>
+    <row r="30" spans="1:35">
       <c r="A30" s="2">
         <v>26</v>
       </c>
@@ -3199,9 +3848,7 @@
       <c r="C30" s="2">
         <v>2.1443395041110906</v>
       </c>
-      <c r="D30" s="2">
-        <v>10.112412359848996</v>
-      </c>
+      <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="G30" s="2">
         <v>26</v>
@@ -3210,9 +3857,7 @@
       <c r="I30" s="2">
         <v>9.0631893525410678</v>
       </c>
-      <c r="J30" s="2">
-        <v>33.223220903760506</v>
-      </c>
+      <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="M30" s="2">
         <v>26</v>
@@ -3221,9 +3866,7 @@
       <c r="O30" s="2">
         <v>4.8166469359106241</v>
       </c>
-      <c r="P30" s="2">
-        <v>33.223220903760506</v>
-      </c>
+      <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="S30" s="2">
         <v>26</v>
@@ -3232,12 +3875,28 @@
       <c r="U30" s="2">
         <v>23.588018165020323</v>
       </c>
-      <c r="V30" s="2">
-        <v>33.223220903760506</v>
-      </c>
+      <c r="V30" s="2"/>
       <c r="W30" s="2"/>
-    </row>
-    <row r="31" spans="1:23">
+      <c r="Y30" s="2">
+        <v>26</v>
+      </c>
+      <c r="Z30" s="2"/>
+      <c r="AA30" s="2">
+        <v>198.89925821112618</v>
+      </c>
+      <c r="AB30" s="2"/>
+      <c r="AC30" s="2"/>
+      <c r="AE30" s="2">
+        <v>26</v>
+      </c>
+      <c r="AF30" s="2"/>
+      <c r="AG30" s="2">
+        <v>109.55641331869832</v>
+      </c>
+      <c r="AH30" s="2"/>
+      <c r="AI30" s="2"/>
+    </row>
+    <row r="31" spans="1:35">
       <c r="A31" s="2">
         <v>27</v>
       </c>
@@ -3245,9 +3904,7 @@
       <c r="C31" s="2">
         <v>2.0995880716170108</v>
       </c>
-      <c r="D31" s="2">
-        <v>9.3572309433914551</v>
-      </c>
+      <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="G31" s="2">
         <v>27</v>
@@ -3256,9 +3913,7 @@
       <c r="I31" s="2">
         <v>9.0367328795794393</v>
       </c>
-      <c r="J31" s="2">
-        <v>34.493444677833068</v>
-      </c>
+      <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="M31" s="2">
         <v>27</v>
@@ -3267,9 +3922,7 @@
       <c r="O31" s="2">
         <v>4.7675297848696649</v>
       </c>
-      <c r="P31" s="2">
-        <v>34.493444677833068</v>
-      </c>
+      <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="S31" s="2">
         <v>27</v>
@@ -3278,12 +3931,28 @@
       <c r="U31" s="2">
         <v>22.721295785868691</v>
       </c>
-      <c r="V31" s="2">
-        <v>34.493444677833068</v>
-      </c>
+      <c r="V31" s="2"/>
       <c r="W31" s="2"/>
-    </row>
-    <row r="32" spans="1:23">
+      <c r="Y31" s="2">
+        <v>27</v>
+      </c>
+      <c r="Z31" s="2"/>
+      <c r="AA31" s="2">
+        <v>198.46279014601186</v>
+      </c>
+      <c r="AB31" s="2"/>
+      <c r="AC31" s="2"/>
+      <c r="AE31" s="2">
+        <v>27</v>
+      </c>
+      <c r="AF31" s="2"/>
+      <c r="AG31" s="2">
+        <v>103.44817046418551</v>
+      </c>
+      <c r="AH31" s="2"/>
+      <c r="AI31" s="2"/>
+    </row>
+    <row r="32" spans="1:35">
       <c r="A32" s="2">
         <v>28</v>
       </c>
@@ -3291,9 +3960,7 @@
       <c r="C32" s="2">
         <v>2.2054085790808453</v>
       </c>
-      <c r="D32" s="2">
-        <v>8.0927307482542989</v>
-      </c>
+      <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="G32" s="2">
         <v>28</v>
@@ -3302,9 +3969,7 @@
       <c r="I32" s="2">
         <v>8.4273273067991479</v>
       </c>
-      <c r="J32" s="2">
-        <v>35.315221026153679</v>
-      </c>
+      <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="M32" s="2">
         <v>28</v>
@@ -3313,9 +3978,7 @@
       <c r="O32" s="2">
         <v>5.2579874748026674</v>
       </c>
-      <c r="P32" s="2">
-        <v>35.315221026153679</v>
-      </c>
+      <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="S32" s="2">
         <v>28</v>
@@ -3324,12 +3987,28 @@
       <c r="U32" s="2">
         <v>21.463995271108104</v>
       </c>
-      <c r="V32" s="2">
-        <v>35.315221026153679</v>
-      </c>
+      <c r="V32" s="2"/>
       <c r="W32" s="2"/>
-    </row>
-    <row r="33" spans="1:23">
+      <c r="Y32" s="2">
+        <v>28</v>
+      </c>
+      <c r="Z32" s="2"/>
+      <c r="AA32" s="2">
+        <v>201.60846263253529</v>
+      </c>
+      <c r="AB32" s="2"/>
+      <c r="AC32" s="2"/>
+      <c r="AE32" s="2">
+        <v>28</v>
+      </c>
+      <c r="AF32" s="2"/>
+      <c r="AG32" s="2">
+        <v>105.48759724999562</v>
+      </c>
+      <c r="AH32" s="2"/>
+      <c r="AI32" s="2"/>
+    </row>
+    <row r="33" spans="1:35">
       <c r="A33" s="2">
         <v>29</v>
       </c>
@@ -3337,9 +4016,7 @@
       <c r="C33" s="2">
         <v>2.1553752240718347</v>
       </c>
-      <c r="D33" s="2">
-        <v>8.1410857493942128</v>
-      </c>
+      <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="G33" s="2">
         <v>29</v>
@@ -3348,9 +4025,7 @@
       <c r="I33" s="2">
         <v>9.0399894935119942</v>
       </c>
-      <c r="J33" s="2">
-        <v>35.734482719855279</v>
-      </c>
+      <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="M33" s="2">
         <v>29</v>
@@ -3359,9 +4034,7 @@
       <c r="O33" s="2">
         <v>11.841397821370636</v>
       </c>
-      <c r="P33" s="2">
-        <v>35.734482719855279</v>
-      </c>
+      <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
       <c r="S33" s="2">
         <v>29</v>
@@ -3370,12 +4043,28 @@
       <c r="U33" s="2">
         <v>22.757353908794084</v>
       </c>
-      <c r="V33" s="2">
-        <v>35.734482719855279</v>
-      </c>
+      <c r="V33" s="2"/>
       <c r="W33" s="2"/>
-    </row>
-    <row r="34" spans="1:23">
+      <c r="Y33" s="2">
+        <v>29</v>
+      </c>
+      <c r="Z33" s="2"/>
+      <c r="AA33" s="2">
+        <v>206.22407315554497</v>
+      </c>
+      <c r="AB33" s="2"/>
+      <c r="AC33" s="2"/>
+      <c r="AE33" s="2">
+        <v>29</v>
+      </c>
+      <c r="AF33" s="2"/>
+      <c r="AG33" s="2">
+        <v>102.89257973197172</v>
+      </c>
+      <c r="AH33" s="2"/>
+      <c r="AI33" s="2"/>
+    </row>
+    <row r="34" spans="1:35">
       <c r="A34" s="2">
         <v>30</v>
       </c>
@@ -3383,9 +4072,7 @@
       <c r="C34" s="2">
         <v>2.483397283609714</v>
       </c>
-      <c r="D34" s="2">
-        <v>9.0481217459332957</v>
-      </c>
+      <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="G34" s="2">
         <v>30</v>
@@ -3394,9 +4081,7 @@
       <c r="I34" s="2">
         <v>8.4894781385281188</v>
       </c>
-      <c r="J34" s="2">
-        <v>34.400667023288385</v>
-      </c>
+      <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="M34" s="2">
         <v>30</v>
@@ -3405,9 +4090,7 @@
       <c r="O34" s="2">
         <v>10.255152768080059</v>
       </c>
-      <c r="P34" s="2">
-        <v>34.400667023288385</v>
-      </c>
+      <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
       <c r="S34" s="2">
         <v>30</v>
@@ -3416,17 +4099,35 @@
       <c r="U34" s="2">
         <v>22.017175124018618</v>
       </c>
-      <c r="V34" s="2">
-        <v>34.400667023288385</v>
-      </c>
+      <c r="V34" s="2"/>
       <c r="W34" s="2"/>
+      <c r="Y34" s="2">
+        <v>30</v>
+      </c>
+      <c r="Z34" s="2"/>
+      <c r="AA34" s="2">
+        <v>198.24188993153453</v>
+      </c>
+      <c r="AB34" s="2"/>
+      <c r="AC34" s="2"/>
+      <c r="AE34" s="2">
+        <v>30</v>
+      </c>
+      <c r="AF34" s="2"/>
+      <c r="AG34" s="2">
+        <v>106.78690780920147</v>
+      </c>
+      <c r="AH34" s="2"/>
+      <c r="AI34" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="AE3:AI3"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="N3:Q3"/>
     <mergeCell ref="S3:W3"/>
+    <mergeCell ref="Y3:AC3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Differential Evolution algo, not yet correct
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="15255" windowHeight="6165"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="15255" windowHeight="6165" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="1" r:id="rId1"/>
@@ -459,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:AI34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="AF5" sqref="AF5:AF34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -605,7 +605,9 @@
       <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>2.3609519194424142</v>
+      </c>
       <c r="C5" s="2">
         <v>8.8570241628233184</v>
       </c>
@@ -614,7 +616,9 @@
       <c r="G5" s="2">
         <v>1</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="2">
+        <v>3.1895708999498449E+103</v>
+      </c>
       <c r="I5" s="2">
         <v>34.855482580164256</v>
       </c>
@@ -623,7 +627,9 @@
       <c r="M5" s="2">
         <v>1</v>
       </c>
-      <c r="N5" s="2"/>
+      <c r="N5" s="2">
+        <v>1.9676893394837691E-4</v>
+      </c>
       <c r="O5" s="2">
         <v>25.371197018440967</v>
       </c>
@@ -632,7 +638,9 @@
       <c r="S5" s="2">
         <v>1</v>
       </c>
-      <c r="T5" s="2"/>
+      <c r="T5" s="2">
+        <v>84.792551732279847</v>
+      </c>
       <c r="U5" s="2">
         <v>87.344039495134368</v>
       </c>
@@ -641,7 +649,9 @@
       <c r="Y5" s="2">
         <v>1</v>
       </c>
-      <c r="Z5" s="2"/>
+      <c r="Z5" s="2">
+        <v>124.88283170519293</v>
+      </c>
       <c r="AA5" s="2">
         <v>818.7710536659115</v>
       </c>
@@ -650,7 +660,9 @@
       <c r="AE5" s="2">
         <v>1</v>
       </c>
-      <c r="AF5" s="2"/>
+      <c r="AF5" s="2">
+        <v>383.8529931931908</v>
+      </c>
       <c r="AG5" s="2">
         <v>424.58585828211886</v>
       </c>
@@ -661,7 +673,9 @@
       <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <v>1.9955912540922323</v>
+      </c>
       <c r="C6" s="2">
         <v>9.161164934202203</v>
       </c>
@@ -670,7 +684,9 @@
       <c r="G6" s="2">
         <v>2</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="2">
+        <v>6.9482632674886248E+204</v>
+      </c>
       <c r="I6" s="2">
         <v>33.841742498805409</v>
       </c>
@@ -679,7 +695,9 @@
       <c r="M6" s="2">
         <v>2</v>
       </c>
-      <c r="N6" s="2"/>
+      <c r="N6" s="2">
+        <v>1.4707105755462635E-8</v>
+      </c>
       <c r="O6" s="2">
         <v>19.199319641827845</v>
       </c>
@@ -688,7 +706,9 @@
       <c r="S6" s="2">
         <v>2</v>
       </c>
-      <c r="T6" s="2"/>
+      <c r="T6" s="2">
+        <v>84.466228034195581</v>
+      </c>
       <c r="U6" s="2">
         <v>90.389974169207917</v>
       </c>
@@ -697,7 +717,9 @@
       <c r="Y6" s="2">
         <v>2</v>
       </c>
-      <c r="Z6" s="2"/>
+      <c r="Z6" s="2">
+        <v>127.15950852175722</v>
+      </c>
       <c r="AA6" s="2">
         <v>814.48000578482788</v>
       </c>
@@ -706,7 +728,9 @@
       <c r="AE6" s="2">
         <v>2</v>
       </c>
-      <c r="AF6" s="2"/>
+      <c r="AF6" s="2">
+        <v>384.54908599537174</v>
+      </c>
       <c r="AG6" s="2">
         <v>413.03417428185338</v>
       </c>
@@ -717,7 +741,9 @@
       <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <v>2.1643287842626147</v>
+      </c>
       <c r="C7" s="2">
         <v>8.7527460644814088</v>
       </c>
@@ -726,7 +752,9 @@
       <c r="G7" s="2">
         <v>3</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2">
+        <v>1.5081293579749544E+306</v>
+      </c>
       <c r="I7" s="2">
         <v>32.465087426973874</v>
       </c>
@@ -735,7 +763,9 @@
       <c r="M7" s="2">
         <v>3</v>
       </c>
-      <c r="N7" s="2"/>
+      <c r="N7" s="2">
+        <v>1.5081269566508126E-12</v>
+      </c>
       <c r="O7" s="2">
         <v>23.074386864512853</v>
       </c>
@@ -744,7 +774,9 @@
       <c r="S7" s="2">
         <v>3</v>
       </c>
-      <c r="T7" s="2"/>
+      <c r="T7" s="2">
+        <v>83.344928087766888</v>
+      </c>
       <c r="U7" s="2">
         <v>88.764916371290127</v>
       </c>
@@ -753,7 +785,9 @@
       <c r="Y7" s="2">
         <v>3</v>
       </c>
-      <c r="Z7" s="2"/>
+      <c r="Z7" s="2">
+        <v>128.36881942822254</v>
+      </c>
       <c r="AA7" s="2">
         <v>812.23428932003458</v>
       </c>
@@ -762,7 +796,9 @@
       <c r="AE7" s="2">
         <v>3</v>
       </c>
-      <c r="AF7" s="2"/>
+      <c r="AF7" s="2">
+        <v>387.57797057813042</v>
+      </c>
       <c r="AG7" s="2">
         <v>419.5255114260471</v>
       </c>
@@ -773,7 +809,9 @@
       <c r="A8" s="2">
         <v>4</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <v>2.1715164622136522</v>
+      </c>
       <c r="C8" s="2">
         <v>8.8082906792446956</v>
       </c>
@@ -791,7 +829,9 @@
       <c r="M8" s="2">
         <v>4</v>
       </c>
-      <c r="N8" s="2"/>
+      <c r="N8" s="2">
+        <v>7.1054273576010019E-15</v>
+      </c>
       <c r="O8" s="2">
         <v>17.708531393706885</v>
       </c>
@@ -800,7 +840,9 @@
       <c r="S8" s="2">
         <v>4</v>
       </c>
-      <c r="T8" s="2"/>
+      <c r="T8" s="2">
+        <v>84.235823017778969</v>
+      </c>
       <c r="U8" s="2">
         <v>88.900635432109382</v>
       </c>
@@ -809,7 +851,9 @@
       <c r="Y8" s="2">
         <v>4</v>
       </c>
-      <c r="Z8" s="2"/>
+      <c r="Z8" s="2">
+        <v>127.94780802578123</v>
+      </c>
       <c r="AA8" s="2">
         <v>811.73937971337125</v>
       </c>
@@ -818,7 +862,9 @@
       <c r="AE8" s="2">
         <v>4</v>
       </c>
-      <c r="AF8" s="2"/>
+      <c r="AF8" s="2">
+        <v>388.34744779879958</v>
+      </c>
       <c r="AG8" s="2">
         <v>422.67560304195183</v>
       </c>
@@ -829,7 +875,9 @@
       <c r="A9" s="2">
         <v>5</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2">
+        <v>1.9199898219705387</v>
+      </c>
       <c r="C9" s="2">
         <v>8.9565860324539575</v>
       </c>
@@ -847,7 +895,9 @@
       <c r="M9" s="2">
         <v>5</v>
       </c>
-      <c r="N9" s="2"/>
+      <c r="N9" s="2">
+        <v>1.1546319456101628E-14</v>
+      </c>
       <c r="O9" s="2">
         <v>20.912293649444411</v>
       </c>
@@ -856,7 +906,9 @@
       <c r="S9" s="2">
         <v>5</v>
       </c>
-      <c r="T9" s="2"/>
+      <c r="T9" s="2">
+        <v>83.653184258742556</v>
+      </c>
       <c r="U9" s="2">
         <v>89.156182929271282</v>
       </c>
@@ -865,7 +917,9 @@
       <c r="Y9" s="2">
         <v>5</v>
       </c>
-      <c r="Z9" s="2"/>
+      <c r="Z9" s="2">
+        <v>131.40394256779297</v>
+      </c>
       <c r="AA9" s="2">
         <v>809.38094825166468</v>
       </c>
@@ -874,7 +928,9 @@
       <c r="AE9" s="2">
         <v>5</v>
       </c>
-      <c r="AF9" s="2"/>
+      <c r="AF9" s="2">
+        <v>381.0138657703817</v>
+      </c>
       <c r="AG9" s="2">
         <v>426.76671774352894</v>
       </c>
@@ -885,7 +941,9 @@
       <c r="A10" s="2">
         <v>6</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2">
+        <v>2.164394893478375</v>
+      </c>
       <c r="C10" s="2">
         <v>9.0439585333186283</v>
       </c>
@@ -903,7 +961,9 @@
       <c r="M10" s="2">
         <v>6</v>
       </c>
-      <c r="N10" s="2"/>
+      <c r="N10" s="2">
+        <v>7.1054273576010019E-15</v>
+      </c>
       <c r="O10" s="2">
         <v>20.048862798086571</v>
       </c>
@@ -912,7 +972,9 @@
       <c r="S10" s="2">
         <v>6</v>
       </c>
-      <c r="T10" s="2"/>
+      <c r="T10" s="2">
+        <v>85.078700191119182</v>
+      </c>
       <c r="U10" s="2">
         <v>90.560128155756473</v>
       </c>
@@ -921,7 +983,9 @@
       <c r="Y10" s="2">
         <v>6</v>
       </c>
-      <c r="Z10" s="2"/>
+      <c r="Z10" s="2">
+        <v>126.59720791642741</v>
+      </c>
       <c r="AA10" s="2">
         <v>820.36724361717665</v>
       </c>
@@ -930,7 +994,9 @@
       <c r="AE10" s="2">
         <v>6</v>
       </c>
-      <c r="AF10" s="2"/>
+      <c r="AF10" s="2">
+        <v>379.82379085512065</v>
+      </c>
       <c r="AG10" s="2">
         <v>414.17008911382715</v>
       </c>
@@ -941,7 +1007,9 @@
       <c r="A11" s="2">
         <v>7</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <v>2.0859855211289386</v>
+      </c>
       <c r="C11" s="2">
         <v>7.991795208482527</v>
       </c>
@@ -959,7 +1027,9 @@
       <c r="M11" s="2">
         <v>7</v>
       </c>
-      <c r="N11" s="2"/>
+      <c r="N11" s="2">
+        <v>1.3322676295501878E-14</v>
+      </c>
       <c r="O11" s="2">
         <v>25.58484696044728</v>
       </c>
@@ -968,7 +1038,9 @@
       <c r="S11" s="2">
         <v>7</v>
       </c>
-      <c r="T11" s="2"/>
+      <c r="T11" s="2">
+        <v>84.093538493890819</v>
+      </c>
       <c r="U11" s="2">
         <v>87.985253243016643</v>
       </c>
@@ -977,7 +1049,9 @@
       <c r="Y11" s="2">
         <v>7</v>
       </c>
-      <c r="Z11" s="2"/>
+      <c r="Z11" s="2">
+        <v>126.53143234421671</v>
+      </c>
       <c r="AA11" s="2">
         <v>820.40904802852674</v>
       </c>
@@ -986,7 +1060,9 @@
       <c r="AE11" s="2">
         <v>7</v>
       </c>
-      <c r="AF11" s="2"/>
+      <c r="AF11" s="2">
+        <v>381.32991246400024</v>
+      </c>
       <c r="AG11" s="2">
         <v>423.02220302402208</v>
       </c>
@@ -997,7 +1073,9 @@
       <c r="A12" s="2">
         <v>8</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2">
+        <v>2.1210707588841338</v>
+      </c>
       <c r="C12" s="2">
         <v>8.7258167293044</v>
       </c>
@@ -1015,7 +1093,9 @@
       <c r="M12" s="2">
         <v>8</v>
       </c>
-      <c r="N12" s="2"/>
+      <c r="N12" s="2">
+        <v>1.2434497875801753E-14</v>
+      </c>
       <c r="O12" s="2">
         <v>22.171037946605658</v>
       </c>
@@ -1024,7 +1104,9 @@
       <c r="S12" s="2">
         <v>8</v>
       </c>
-      <c r="T12" s="2"/>
+      <c r="T12" s="2">
+        <v>85.011579957861827</v>
+      </c>
       <c r="U12" s="2">
         <v>87.90024205594537</v>
       </c>
@@ -1033,7 +1115,9 @@
       <c r="Y12" s="2">
         <v>8</v>
       </c>
-      <c r="Z12" s="2"/>
+      <c r="Z12" s="2">
+        <v>128.52713573103497</v>
+      </c>
       <c r="AA12" s="2">
         <v>811.48577541751661</v>
       </c>
@@ -1042,7 +1126,9 @@
       <c r="AE12" s="2">
         <v>8</v>
       </c>
-      <c r="AF12" s="2"/>
+      <c r="AF12" s="2">
+        <v>380.99776718174951</v>
+      </c>
       <c r="AG12" s="2">
         <v>424.99890930556256</v>
       </c>
@@ -1053,7 +1139,9 @@
       <c r="A13" s="2">
         <v>9</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2">
+        <v>2.2492133955587712</v>
+      </c>
       <c r="C13" s="2">
         <v>8.6683224770388314</v>
       </c>
@@ -1071,7 +1159,9 @@
       <c r="M13" s="2">
         <v>9</v>
       </c>
-      <c r="N13" s="2"/>
+      <c r="N13" s="2">
+        <v>1.2434497875801753E-14</v>
+      </c>
       <c r="O13" s="2">
         <v>25.013346312937355</v>
       </c>
@@ -1080,7 +1170,9 @@
       <c r="S13" s="2">
         <v>9</v>
       </c>
-      <c r="T13" s="2"/>
+      <c r="T13" s="2">
+        <v>82.91759986560875</v>
+      </c>
       <c r="U13" s="2">
         <v>89.44969605081809</v>
       </c>
@@ -1089,7 +1181,9 @@
       <c r="Y13" s="2">
         <v>9</v>
       </c>
-      <c r="Z13" s="2"/>
+      <c r="Z13" s="2">
+        <v>130.12985616708124</v>
+      </c>
       <c r="AA13" s="2">
         <v>825.52009883417236</v>
       </c>
@@ -1098,7 +1192,9 @@
       <c r="AE13" s="2">
         <v>9</v>
       </c>
-      <c r="AF13" s="2"/>
+      <c r="AF13" s="2">
+        <v>380.99608985671671</v>
+      </c>
       <c r="AG13" s="2">
         <v>422.97709245578886</v>
       </c>
@@ -1109,7 +1205,9 @@
       <c r="A14" s="2">
         <v>10</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2">
+        <v>2.1414520813578757</v>
+      </c>
       <c r="C14" s="2">
         <v>8.8591766192163455</v>
       </c>
@@ -1127,7 +1225,9 @@
       <c r="M14" s="2">
         <v>10</v>
       </c>
-      <c r="N14" s="2"/>
+      <c r="N14" s="2">
+        <v>1.3322676295501878E-14</v>
+      </c>
       <c r="O14" s="2">
         <v>22.702045493559762</v>
       </c>
@@ -1136,7 +1236,9 @@
       <c r="S14" s="2">
         <v>10</v>
       </c>
-      <c r="T14" s="2"/>
+      <c r="T14" s="2">
+        <v>86.197366327197983</v>
+      </c>
       <c r="U14" s="2">
         <v>89.85584362099965</v>
       </c>
@@ -1145,7 +1247,9 @@
       <c r="Y14" s="2">
         <v>10</v>
       </c>
-      <c r="Z14" s="2"/>
+      <c r="Z14" s="2">
+        <v>126.06533136114327</v>
+      </c>
       <c r="AA14" s="2">
         <v>812.90675909780009</v>
       </c>
@@ -1154,7 +1258,9 @@
       <c r="AE14" s="2">
         <v>10</v>
       </c>
-      <c r="AF14" s="2"/>
+      <c r="AF14" s="2">
+        <v>382.65618082304417</v>
+      </c>
       <c r="AG14" s="2">
         <v>424.18716868500258</v>
       </c>
@@ -1165,7 +1271,9 @@
       <c r="A15" s="2">
         <v>11</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2">
+        <v>2.2432026024857494</v>
+      </c>
       <c r="C15" s="2">
         <v>9.0088313483942351</v>
       </c>
@@ -1183,7 +1291,9 @@
       <c r="M15" s="2">
         <v>11</v>
       </c>
-      <c r="N15" s="2"/>
+      <c r="N15" s="2">
+        <v>1.3322676295501878E-14</v>
+      </c>
       <c r="O15" s="2">
         <v>22.033482987701852</v>
       </c>
@@ -1192,7 +1302,9 @@
       <c r="S15" s="2">
         <v>11</v>
       </c>
-      <c r="T15" s="2"/>
+      <c r="T15" s="2">
+        <v>84.336324771508359</v>
+      </c>
       <c r="U15" s="2">
         <v>89.346589288574776</v>
       </c>
@@ -1201,7 +1313,9 @@
       <c r="Y15" s="2">
         <v>11</v>
       </c>
-      <c r="Z15" s="2"/>
+      <c r="Z15" s="2">
+        <v>127.20452661271655</v>
+      </c>
       <c r="AA15" s="2">
         <v>817.95724324851381</v>
       </c>
@@ -1210,7 +1324,9 @@
       <c r="AE15" s="2">
         <v>11</v>
       </c>
-      <c r="AF15" s="2"/>
+      <c r="AF15" s="2">
+        <v>383.35463116384915</v>
+      </c>
       <c r="AG15" s="2">
         <v>420.9134437837501</v>
       </c>
@@ -1221,7 +1337,9 @@
       <c r="A16" s="2">
         <v>12</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2">
+        <v>2.1345253575072523</v>
+      </c>
       <c r="C16" s="2">
         <v>8.4288989027471448</v>
       </c>
@@ -1239,7 +1357,9 @@
       <c r="M16" s="2">
         <v>12</v>
       </c>
-      <c r="N16" s="2"/>
+      <c r="N16" s="2">
+        <v>7.9936057773011271E-15</v>
+      </c>
       <c r="O16" s="2">
         <v>21.452720065004726</v>
       </c>
@@ -1248,7 +1368,9 @@
       <c r="S16" s="2">
         <v>12</v>
       </c>
-      <c r="T16" s="2"/>
+      <c r="T16" s="2">
+        <v>85.560549343887232</v>
+      </c>
       <c r="U16" s="2">
         <v>89.169665431178501</v>
       </c>
@@ -1257,7 +1379,9 @@
       <c r="Y16" s="2">
         <v>12</v>
       </c>
-      <c r="Z16" s="2"/>
+      <c r="Z16" s="2">
+        <v>127.05443768176572</v>
+      </c>
       <c r="AA16" s="2">
         <v>804.79886146046283</v>
       </c>
@@ -1266,7 +1390,9 @@
       <c r="AE16" s="2">
         <v>12</v>
       </c>
-      <c r="AF16" s="2"/>
+      <c r="AF16" s="2">
+        <v>377.04381974631411</v>
+      </c>
       <c r="AG16" s="2">
         <v>423.15290887450993</v>
       </c>
@@ -1277,7 +1403,9 @@
       <c r="A17" s="2">
         <v>13</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2">
+        <v>2.2125777818801406</v>
+      </c>
       <c r="C17" s="2">
         <v>8.6018563724973021</v>
       </c>
@@ -1295,7 +1423,9 @@
       <c r="M17" s="2">
         <v>13</v>
       </c>
-      <c r="N17" s="2"/>
+      <c r="N17" s="2">
+        <v>1.3322676295501878E-14</v>
+      </c>
       <c r="O17" s="2">
         <v>24.284514860292166</v>
       </c>
@@ -1304,7 +1434,9 @@
       <c r="S17" s="2">
         <v>13</v>
       </c>
-      <c r="T17" s="2"/>
+      <c r="T17" s="2">
+        <v>83.601963078857764</v>
+      </c>
       <c r="U17" s="2">
         <v>87.555155671271748</v>
       </c>
@@ -1313,7 +1445,9 @@
       <c r="Y17" s="2">
         <v>13</v>
       </c>
-      <c r="Z17" s="2"/>
+      <c r="Z17" s="2">
+        <v>129.98481288879461</v>
+      </c>
       <c r="AA17" s="2">
         <v>804.11017053529758</v>
       </c>
@@ -1322,7 +1456,9 @@
       <c r="AE17" s="2">
         <v>13</v>
       </c>
-      <c r="AF17" s="2"/>
+      <c r="AF17" s="2">
+        <v>386.58630753958363</v>
+      </c>
       <c r="AG17" s="2">
         <v>415.91938324453645</v>
       </c>
@@ -1333,7 +1469,9 @@
       <c r="A18" s="2">
         <v>14</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2">
+        <v>2.0916317933866719</v>
+      </c>
       <c r="C18" s="2">
         <v>8.473699395860617</v>
       </c>
@@ -1351,7 +1489,9 @@
       <c r="M18" s="2">
         <v>14</v>
       </c>
-      <c r="N18" s="2"/>
+      <c r="N18" s="2">
+        <v>1.2434497875801753E-14</v>
+      </c>
       <c r="O18" s="2">
         <v>25.891413586064644</v>
       </c>
@@ -1360,7 +1500,9 @@
       <c r="S18" s="2">
         <v>14</v>
       </c>
-      <c r="T18" s="2"/>
+      <c r="T18" s="2">
+        <v>83.187552547471029</v>
+      </c>
       <c r="U18" s="2">
         <v>90.04644667510091</v>
       </c>
@@ -1369,7 +1511,9 @@
       <c r="Y18" s="2">
         <v>14</v>
       </c>
-      <c r="Z18" s="2"/>
+      <c r="Z18" s="2">
+        <v>126.91626952479541</v>
+      </c>
       <c r="AA18" s="2">
         <v>796.49228697130002</v>
       </c>
@@ -1378,7 +1522,9 @@
       <c r="AE18" s="2">
         <v>14</v>
       </c>
-      <c r="AF18" s="2"/>
+      <c r="AF18" s="2">
+        <v>380.47003015729541</v>
+      </c>
       <c r="AG18" s="2">
         <v>421.19809395949756</v>
       </c>
@@ -1389,7 +1535,9 @@
       <c r="A19" s="2">
         <v>15</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2">
+        <v>2.2716785240169037</v>
+      </c>
       <c r="C19" s="2">
         <v>8.56792558766948</v>
       </c>
@@ -1407,7 +1555,9 @@
       <c r="M19" s="2">
         <v>15</v>
       </c>
-      <c r="N19" s="2"/>
+      <c r="N19" s="2">
+        <v>1.1546319456101628E-14</v>
+      </c>
       <c r="O19" s="2">
         <v>22.507639934291475</v>
       </c>
@@ -1416,7 +1566,9 @@
       <c r="S19" s="2">
         <v>15</v>
       </c>
-      <c r="T19" s="2"/>
+      <c r="T19" s="2">
+        <v>85.568590012834335</v>
+      </c>
       <c r="U19" s="2">
         <v>88.926150708891043</v>
       </c>
@@ -1425,7 +1577,9 @@
       <c r="Y19" s="2">
         <v>15</v>
       </c>
-      <c r="Z19" s="2"/>
+      <c r="Z19" s="2">
+        <v>128.15962554629888</v>
+      </c>
       <c r="AA19" s="2">
         <v>817.51012257642628</v>
       </c>
@@ -1434,7 +1588,9 @@
       <c r="AE19" s="2">
         <v>15</v>
       </c>
-      <c r="AF19" s="2"/>
+      <c r="AF19" s="2">
+        <v>383.52198688354355</v>
+      </c>
       <c r="AG19" s="2">
         <v>421.24423479257405</v>
       </c>
@@ -1445,7 +1601,9 @@
       <c r="A20" s="2">
         <v>16</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2">
+        <v>2.222620044233564</v>
+      </c>
       <c r="C20" s="2">
         <v>8.8399753241941941</v>
       </c>
@@ -1463,7 +1621,9 @@
       <c r="M20" s="2">
         <v>16</v>
       </c>
-      <c r="N20" s="2"/>
+      <c r="N20" s="2">
+        <v>9.7699626167013776E-15</v>
+      </c>
       <c r="O20" s="2">
         <v>24.707347173049023</v>
       </c>
@@ -1472,7 +1632,9 @@
       <c r="S20" s="2">
         <v>16</v>
       </c>
-      <c r="T20" s="2"/>
+      <c r="T20" s="2">
+        <v>83.127344407031714</v>
+      </c>
       <c r="U20" s="2">
         <v>89.387721575792241</v>
       </c>
@@ -1481,7 +1643,9 @@
       <c r="Y20" s="2">
         <v>16</v>
       </c>
-      <c r="Z20" s="2"/>
+      <c r="Z20" s="2">
+        <v>128.07447562862748</v>
+      </c>
       <c r="AA20" s="2">
         <v>804.15125188653644</v>
       </c>
@@ -1490,7 +1654,9 @@
       <c r="AE20" s="2">
         <v>16</v>
       </c>
-      <c r="AF20" s="2"/>
+      <c r="AF20" s="2">
+        <v>381.41575196622858</v>
+      </c>
       <c r="AG20" s="2">
         <v>419.95919613565798</v>
       </c>
@@ -1501,7 +1667,9 @@
       <c r="A21" s="2">
         <v>17</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2">
+        <v>2.1745469239469255</v>
+      </c>
       <c r="C21" s="2">
         <v>9.2748385582093729</v>
       </c>
@@ -1519,7 +1687,9 @@
       <c r="M21" s="2">
         <v>17</v>
       </c>
-      <c r="N21" s="2"/>
+      <c r="N21" s="2">
+        <v>1.2434497875801753E-14</v>
+      </c>
       <c r="O21" s="2">
         <v>19.979692594762451</v>
       </c>
@@ -1528,7 +1698,9 @@
       <c r="S21" s="2">
         <v>17</v>
       </c>
-      <c r="T21" s="2"/>
+      <c r="T21" s="2">
+        <v>84.71953902484799</v>
+      </c>
       <c r="U21" s="2">
         <v>90.146626768418074</v>
       </c>
@@ -1537,7 +1709,9 @@
       <c r="Y21" s="2">
         <v>17</v>
       </c>
-      <c r="Z21" s="2"/>
+      <c r="Z21" s="2">
+        <v>125.74019212054678</v>
+      </c>
       <c r="AA21" s="2">
         <v>822.12664092970385</v>
       </c>
@@ -1546,7 +1720,9 @@
       <c r="AE21" s="2">
         <v>17</v>
       </c>
-      <c r="AF21" s="2"/>
+      <c r="AF21" s="2">
+        <v>386.17297202575133</v>
+      </c>
       <c r="AG21" s="2">
         <v>424.82387835376556</v>
       </c>
@@ -1557,7 +1733,9 @@
       <c r="A22" s="2">
         <v>18</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2">
+        <v>2.2620340142476256</v>
+      </c>
       <c r="C22" s="2">
         <v>8.9328016740605456</v>
       </c>
@@ -1575,7 +1753,9 @@
       <c r="M22" s="2">
         <v>18</v>
       </c>
-      <c r="N22" s="2"/>
+      <c r="N22" s="2">
+        <v>1.1546319456101628E-14</v>
+      </c>
       <c r="O22" s="2">
         <v>22.598230862597269</v>
       </c>
@@ -1584,7 +1764,9 @@
       <c r="S22" s="2">
         <v>18</v>
       </c>
-      <c r="T22" s="2"/>
+      <c r="T22" s="2">
+        <v>84.991000453002272</v>
+      </c>
       <c r="U22" s="2">
         <v>89.464820368026892</v>
       </c>
@@ -1593,7 +1775,9 @@
       <c r="Y22" s="2">
         <v>18</v>
       </c>
-      <c r="Z22" s="2"/>
+      <c r="Z22" s="2">
+        <v>127.16844074729542</v>
+      </c>
       <c r="AA22" s="2">
         <v>814.7148137267053</v>
       </c>
@@ -1602,7 +1786,9 @@
       <c r="AE22" s="2">
         <v>18</v>
       </c>
-      <c r="AF22" s="2"/>
+      <c r="AF22" s="2">
+        <v>382.79695514597501</v>
+      </c>
       <c r="AG22" s="2">
         <v>412.2645061494153</v>
       </c>
@@ -1613,7 +1799,9 @@
       <c r="A23" s="2">
         <v>19</v>
       </c>
-      <c r="B23" s="2"/>
+      <c r="B23" s="2">
+        <v>2.0456938486602976</v>
+      </c>
       <c r="C23" s="2">
         <v>8.2299771406344977</v>
       </c>
@@ -1631,7 +1819,9 @@
       <c r="M23" s="2">
         <v>19</v>
       </c>
-      <c r="N23" s="2"/>
+      <c r="N23" s="2">
+        <v>6.2172489379008766E-15</v>
+      </c>
       <c r="O23" s="2">
         <v>25.131508956082868</v>
       </c>
@@ -1640,7 +1830,9 @@
       <c r="S23" s="2">
         <v>19</v>
       </c>
-      <c r="T23" s="2"/>
+      <c r="T23" s="2">
+        <v>84.16751187340013</v>
+      </c>
       <c r="U23" s="2">
         <v>89.56632859934129</v>
       </c>
@@ -1649,7 +1841,9 @@
       <c r="Y23" s="2">
         <v>19</v>
       </c>
-      <c r="Z23" s="2"/>
+      <c r="Z23" s="2">
+        <v>126.93938723204757</v>
+      </c>
       <c r="AA23" s="2">
         <v>819.73802257117381</v>
       </c>
@@ -1658,7 +1852,9 @@
       <c r="AE23" s="2">
         <v>19</v>
       </c>
-      <c r="AF23" s="2"/>
+      <c r="AF23" s="2">
+        <v>384.62148377126709</v>
+      </c>
       <c r="AG23" s="2">
         <v>423.08425508064676</v>
       </c>
@@ -1669,7 +1865,9 @@
       <c r="A24" s="2">
         <v>20</v>
       </c>
-      <c r="B24" s="2"/>
+      <c r="B24" s="2">
+        <v>2.2130826823810614</v>
+      </c>
       <c r="C24" s="2">
         <v>8.6500203105041038</v>
       </c>
@@ -1687,7 +1885,9 @@
       <c r="M24" s="2">
         <v>20</v>
       </c>
-      <c r="N24" s="2"/>
+      <c r="N24" s="2">
+        <v>5.3290705182007514E-15</v>
+      </c>
       <c r="O24" s="2">
         <v>24.248422655977393</v>
       </c>
@@ -1696,7 +1896,9 @@
       <c r="S24" s="2">
         <v>20</v>
       </c>
-      <c r="T24" s="2"/>
+      <c r="T24" s="2">
+        <v>85.138768495165692</v>
+      </c>
       <c r="U24" s="2">
         <v>86.912890552886637</v>
       </c>
@@ -1705,7 +1907,9 @@
       <c r="Y24" s="2">
         <v>20</v>
       </c>
-      <c r="Z24" s="2"/>
+      <c r="Z24" s="2">
+        <v>129.59475407667114</v>
+      </c>
       <c r="AA24" s="2">
         <v>820.42129475210504</v>
       </c>
@@ -1714,7 +1918,9 @@
       <c r="AE24" s="2">
         <v>20</v>
       </c>
-      <c r="AF24" s="2"/>
+      <c r="AF24" s="2">
+        <v>379.22135270126938</v>
+      </c>
       <c r="AG24" s="2">
         <v>422.36600999776476</v>
       </c>
@@ -1725,7 +1931,9 @@
       <c r="A25" s="2">
         <v>21</v>
       </c>
-      <c r="B25" s="2"/>
+      <c r="B25" s="2">
+        <v>2.224634099419216</v>
+      </c>
       <c r="C25" s="2">
         <v>8.9496800403291648</v>
       </c>
@@ -1743,7 +1951,9 @@
       <c r="M25" s="2">
         <v>21</v>
       </c>
-      <c r="N25" s="2"/>
+      <c r="N25" s="2">
+        <v>1.2434497875801753E-14</v>
+      </c>
       <c r="O25" s="2">
         <v>20.22789187414957</v>
       </c>
@@ -1752,7 +1962,9 @@
       <c r="S25" s="2">
         <v>21</v>
       </c>
-      <c r="T25" s="2"/>
+      <c r="T25" s="2">
+        <v>84.646004189310588</v>
+      </c>
       <c r="U25" s="2">
         <v>90.789054445727288</v>
       </c>
@@ -1761,7 +1973,9 @@
       <c r="Y25" s="2">
         <v>21</v>
       </c>
-      <c r="Z25" s="2"/>
+      <c r="Z25" s="2">
+        <v>126.99569753671341</v>
+      </c>
       <c r="AA25" s="2">
         <v>818.26821956257299</v>
       </c>
@@ -1770,7 +1984,9 @@
       <c r="AE25" s="2">
         <v>21</v>
       </c>
-      <c r="AF25" s="2"/>
+      <c r="AF25" s="2">
+        <v>381.79259712060559</v>
+      </c>
       <c r="AG25" s="2">
         <v>413.46351582774236</v>
       </c>
@@ -1781,7 +1997,9 @@
       <c r="A26" s="2">
         <v>22</v>
       </c>
-      <c r="B26" s="2"/>
+      <c r="B26" s="2">
+        <v>2.3088033578074647</v>
+      </c>
       <c r="C26" s="2">
         <v>9.5189105735240975</v>
       </c>
@@ -1799,7 +2017,9 @@
       <c r="M26" s="2">
         <v>22</v>
       </c>
-      <c r="N26" s="2"/>
+      <c r="N26" s="2">
+        <v>1.3322676295501878E-14</v>
+      </c>
       <c r="O26" s="2">
         <v>20.9701913726153</v>
       </c>
@@ -1808,7 +2028,9 @@
       <c r="S26" s="2">
         <v>22</v>
       </c>
-      <c r="T26" s="2"/>
+      <c r="T26" s="2">
+        <v>85.724228480960548</v>
+      </c>
       <c r="U26" s="2">
         <v>89.846985300502752</v>
       </c>
@@ -1817,7 +2039,9 @@
       <c r="Y26" s="2">
         <v>22</v>
       </c>
-      <c r="Z26" s="2"/>
+      <c r="Z26" s="2">
+        <v>130.48089783449456</v>
+      </c>
       <c r="AA26" s="2">
         <v>803.98323825681348</v>
       </c>
@@ -1826,7 +2050,9 @@
       <c r="AE26" s="2">
         <v>22</v>
       </c>
-      <c r="AF26" s="2"/>
+      <c r="AF26" s="2">
+        <v>378.88320176699347</v>
+      </c>
       <c r="AG26" s="2">
         <v>421.53615684308005</v>
       </c>
@@ -1837,7 +2063,9 @@
       <c r="A27" s="2">
         <v>23</v>
       </c>
-      <c r="B27" s="2"/>
+      <c r="B27" s="2">
+        <v>2.2497126213934124</v>
+      </c>
       <c r="C27" s="2">
         <v>8.4218825512814117</v>
       </c>
@@ -1855,7 +2083,9 @@
       <c r="M27" s="2">
         <v>23</v>
       </c>
-      <c r="N27" s="2"/>
+      <c r="N27" s="2">
+        <v>1.0658141036401503E-14</v>
+      </c>
       <c r="O27" s="2">
         <v>23.733788622342718</v>
       </c>
@@ -1864,7 +2094,9 @@
       <c r="S27" s="2">
         <v>23</v>
       </c>
-      <c r="T27" s="2"/>
+      <c r="T27" s="2">
+        <v>84.74739927078295</v>
+      </c>
       <c r="U27" s="2">
         <v>88.847283856599674</v>
       </c>
@@ -1873,7 +2105,9 @@
       <c r="Y27" s="2">
         <v>23</v>
       </c>
-      <c r="Z27" s="2"/>
+      <c r="Z27" s="2">
+        <v>130.01340120085305</v>
+      </c>
       <c r="AA27" s="2">
         <v>822.44484749864978</v>
       </c>
@@ -1882,7 +2116,9 @@
       <c r="AE27" s="2">
         <v>23</v>
       </c>
-      <c r="AF27" s="2"/>
+      <c r="AF27" s="2">
+        <v>378.54936518654455</v>
+      </c>
       <c r="AG27" s="2">
         <v>415.38873002619226</v>
       </c>
@@ -1893,7 +2129,9 @@
       <c r="A28" s="2">
         <v>24</v>
       </c>
-      <c r="B28" s="2"/>
+      <c r="B28" s="2">
+        <v>2.2180901713539063</v>
+      </c>
       <c r="C28" s="2">
         <v>8.9132030055737772</v>
       </c>
@@ -1911,7 +2149,9 @@
       <c r="M28" s="2">
         <v>24</v>
       </c>
-      <c r="N28" s="2"/>
+      <c r="N28" s="2">
+        <v>1.2434497875801753E-14</v>
+      </c>
       <c r="O28" s="2">
         <v>20.461081438199216</v>
       </c>
@@ -1920,7 +2160,9 @@
       <c r="S28" s="2">
         <v>24</v>
       </c>
-      <c r="T28" s="2"/>
+      <c r="T28" s="2">
+        <v>84.343863182263107</v>
+      </c>
       <c r="U28" s="2">
         <v>88.962835804286385</v>
       </c>
@@ -1929,7 +2171,9 @@
       <c r="Y28" s="2">
         <v>24</v>
       </c>
-      <c r="Z28" s="2"/>
+      <c r="Z28" s="2">
+        <v>128.23811019775465</v>
+      </c>
       <c r="AA28" s="2">
         <v>801.03783010516361</v>
       </c>
@@ -1938,7 +2182,9 @@
       <c r="AE28" s="2">
         <v>24</v>
       </c>
-      <c r="AF28" s="2"/>
+      <c r="AF28" s="2">
+        <v>380.67020237084358</v>
+      </c>
       <c r="AG28" s="2">
         <v>409.10006242320122</v>
       </c>
@@ -1949,7 +2195,9 @@
       <c r="A29" s="2">
         <v>25</v>
       </c>
-      <c r="B29" s="2"/>
+      <c r="B29" s="2">
+        <v>2.0473505852314684</v>
+      </c>
       <c r="C29" s="2">
         <v>8.9839470830440025</v>
       </c>
@@ -1967,7 +2215,9 @@
       <c r="M29" s="2">
         <v>25</v>
       </c>
-      <c r="N29" s="2"/>
+      <c r="N29" s="2">
+        <v>1.0658141036401503E-14</v>
+      </c>
       <c r="O29" s="2">
         <v>19.559688451555957</v>
       </c>
@@ -1976,7 +2226,9 @@
       <c r="S29" s="2">
         <v>25</v>
       </c>
-      <c r="T29" s="2"/>
+      <c r="T29" s="2">
+        <v>84.60112158912699</v>
+      </c>
       <c r="U29" s="2">
         <v>87.705174165305394</v>
       </c>
@@ -1985,7 +2237,9 @@
       <c r="Y29" s="2">
         <v>25</v>
       </c>
-      <c r="Z29" s="2"/>
+      <c r="Z29" s="2">
+        <v>128.3589900037326</v>
+      </c>
       <c r="AA29" s="2">
         <v>804.06161071377949</v>
       </c>
@@ -1994,7 +2248,9 @@
       <c r="AE29" s="2">
         <v>25</v>
       </c>
-      <c r="AF29" s="2"/>
+      <c r="AF29" s="2">
+        <v>382.31212848452469</v>
+      </c>
       <c r="AG29" s="2">
         <v>420.44599692575139</v>
       </c>
@@ -2005,7 +2261,9 @@
       <c r="A30" s="2">
         <v>26</v>
       </c>
-      <c r="B30" s="2"/>
+      <c r="B30" s="2">
+        <v>2.0599947434392609</v>
+      </c>
       <c r="C30" s="2">
         <v>9.1085264713126861</v>
       </c>
@@ -2023,7 +2281,9 @@
       <c r="M30" s="2">
         <v>26</v>
       </c>
-      <c r="N30" s="2"/>
+      <c r="N30" s="2">
+        <v>1.2434497875801753E-14</v>
+      </c>
       <c r="O30" s="2">
         <v>24.474464196559435</v>
       </c>
@@ -2032,7 +2292,9 @@
       <c r="S30" s="2">
         <v>26</v>
       </c>
-      <c r="T30" s="2"/>
+      <c r="T30" s="2">
+        <v>84.917259225159214</v>
+      </c>
       <c r="U30" s="2">
         <v>87.895151208688048</v>
       </c>
@@ -2041,7 +2303,9 @@
       <c r="Y30" s="2">
         <v>26</v>
       </c>
-      <c r="Z30" s="2"/>
+      <c r="Z30" s="2">
+        <v>128.8712605460961</v>
+      </c>
       <c r="AA30" s="2">
         <v>817.80934096247961</v>
       </c>
@@ -2050,7 +2314,9 @@
       <c r="AE30" s="2">
         <v>26</v>
       </c>
-      <c r="AF30" s="2"/>
+      <c r="AF30" s="2">
+        <v>379.45983182503358</v>
+      </c>
       <c r="AG30" s="2">
         <v>418.54674246274936</v>
       </c>
@@ -2061,7 +2327,9 @@
       <c r="A31" s="2">
         <v>27</v>
       </c>
-      <c r="B31" s="2"/>
+      <c r="B31" s="2">
+        <v>2.1142877866278944</v>
+      </c>
       <c r="C31" s="2">
         <v>9.2041399964108503</v>
       </c>
@@ -2079,7 +2347,9 @@
       <c r="M31" s="2">
         <v>27</v>
       </c>
-      <c r="N31" s="2"/>
+      <c r="N31" s="2">
+        <v>1.1546319456101628E-14</v>
+      </c>
       <c r="O31" s="2">
         <v>24.347055943562715</v>
       </c>
@@ -2088,7 +2358,9 @@
       <c r="S31" s="2">
         <v>27</v>
       </c>
-      <c r="T31" s="2"/>
+      <c r="T31" s="2">
+        <v>82.266656170144955</v>
+      </c>
       <c r="U31" s="2">
         <v>88.938586359584733</v>
       </c>
@@ -2097,7 +2369,9 @@
       <c r="Y31" s="2">
         <v>27</v>
       </c>
-      <c r="Z31" s="2"/>
+      <c r="Z31" s="2">
+        <v>127.97341703401057</v>
+      </c>
       <c r="AA31" s="2">
         <v>816.68998211606993</v>
       </c>
@@ -2106,7 +2380,9 @@
       <c r="AE31" s="2">
         <v>27</v>
       </c>
-      <c r="AF31" s="2"/>
+      <c r="AF31" s="2">
+        <v>384.23892986730561</v>
+      </c>
       <c r="AG31" s="2">
         <v>423.62002660480431</v>
       </c>
@@ -2117,7 +2393,9 @@
       <c r="A32" s="2">
         <v>28</v>
       </c>
-      <c r="B32" s="2"/>
+      <c r="B32" s="2">
+        <v>2.1056068993419821</v>
+      </c>
       <c r="C32" s="2">
         <v>8.8662335375863162</v>
       </c>
@@ -2135,7 +2413,9 @@
       <c r="M32" s="2">
         <v>28</v>
       </c>
-      <c r="N32" s="2"/>
+      <c r="N32" s="2">
+        <v>1.0658141036401503E-14</v>
+      </c>
       <c r="O32" s="2">
         <v>23.895397823502083</v>
       </c>
@@ -2144,7 +2424,9 @@
       <c r="S32" s="2">
         <v>28</v>
       </c>
-      <c r="T32" s="2"/>
+      <c r="T32" s="2">
+        <v>84.046243981716472</v>
+      </c>
       <c r="U32" s="2">
         <v>89.895509451736373</v>
       </c>
@@ -2153,7 +2435,9 @@
       <c r="Y32" s="2">
         <v>28</v>
       </c>
-      <c r="Z32" s="2"/>
+      <c r="Z32" s="2">
+        <v>130.54051593244293</v>
+      </c>
       <c r="AA32" s="2">
         <v>812.27664413261652</v>
       </c>
@@ -2162,7 +2446,9 @@
       <c r="AE32" s="2">
         <v>28</v>
       </c>
-      <c r="AF32" s="2"/>
+      <c r="AF32" s="2">
+        <v>380.09994821182164</v>
+      </c>
       <c r="AG32" s="2">
         <v>421.03533894639946</v>
       </c>
@@ -2173,7 +2459,9 @@
       <c r="A33" s="2">
         <v>29</v>
       </c>
-      <c r="B33" s="2"/>
+      <c r="B33" s="2">
+        <v>2.0923256723834798</v>
+      </c>
       <c r="C33" s="2">
         <v>9.0619523391388146</v>
       </c>
@@ -2191,7 +2479,9 @@
       <c r="M33" s="2">
         <v>29</v>
       </c>
-      <c r="N33" s="2"/>
+      <c r="N33" s="2">
+        <v>6.2172489379008766E-15</v>
+      </c>
       <c r="O33" s="2">
         <v>18.331055401938414</v>
       </c>
@@ -2200,7 +2490,9 @@
       <c r="S33" s="2">
         <v>29</v>
       </c>
-      <c r="T33" s="2"/>
+      <c r="T33" s="2">
+        <v>84.855702888828773</v>
+      </c>
       <c r="U33" s="2">
         <v>89.053092467741266</v>
       </c>
@@ -2209,7 +2501,9 @@
       <c r="Y33" s="2">
         <v>29</v>
       </c>
-      <c r="Z33" s="2"/>
+      <c r="Z33" s="2">
+        <v>127.30391295803156</v>
+      </c>
       <c r="AA33" s="2">
         <v>809.23454073675077</v>
       </c>
@@ -2218,7 +2512,9 @@
       <c r="AE33" s="2">
         <v>29</v>
       </c>
-      <c r="AF33" s="2"/>
+      <c r="AF33" s="2">
+        <v>380.96045180890587</v>
+      </c>
       <c r="AG33" s="2">
         <v>425.30652482686997</v>
       </c>
@@ -2229,7 +2525,9 @@
       <c r="A34" s="2">
         <v>30</v>
       </c>
-      <c r="B34" s="2"/>
+      <c r="B34" s="2">
+        <v>1.987655686176137</v>
+      </c>
       <c r="C34" s="2">
         <v>8.5162341599070928</v>
       </c>
@@ -2247,7 +2545,9 @@
       <c r="M34" s="2">
         <v>30</v>
       </c>
-      <c r="N34" s="2"/>
+      <c r="N34" s="2">
+        <v>5.3290705182007514E-15</v>
+      </c>
       <c r="O34" s="2">
         <v>20.120940418779071</v>
       </c>
@@ -2256,7 +2556,9 @@
       <c r="S34" s="2">
         <v>30</v>
       </c>
-      <c r="T34" s="2"/>
+      <c r="T34" s="2">
+        <v>85.272569034910845</v>
+      </c>
       <c r="U34" s="2">
         <v>90.016858318820184</v>
       </c>
@@ -2265,7 +2567,9 @@
       <c r="Y34" s="2">
         <v>30</v>
       </c>
-      <c r="Z34" s="2"/>
+      <c r="Z34" s="2">
+        <v>127.54866499712246</v>
+      </c>
       <c r="AA34" s="2">
         <v>821.13294182594564</v>
       </c>
@@ -2274,7 +2578,9 @@
       <c r="AE34" s="2">
         <v>30</v>
       </c>
-      <c r="AF34" s="2"/>
+      <c r="AF34" s="2">
+        <v>382.63502731789112</v>
+      </c>
       <c r="AG34" s="2">
         <v>420.42601369956316</v>
       </c>
@@ -2298,8 +2604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:AI34"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AE18" sqref="AE18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2444,7 +2750,9 @@
       <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>0.46990651464057659</v>
+      </c>
       <c r="C5" s="2">
         <v>2.1334945306560704</v>
       </c>
@@ -2453,7 +2761,9 @@
       <c r="G5" s="2">
         <v>1</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="2">
+        <v>8.1922995169022838E+102</v>
+      </c>
       <c r="I5" s="2">
         <v>8.3318691318502953</v>
       </c>
@@ -2462,7 +2772,9 @@
       <c r="M5" s="2">
         <v>1</v>
       </c>
-      <c r="N5" s="2"/>
+      <c r="N5" s="2">
+        <v>1.6411227628410074E-5</v>
+      </c>
       <c r="O5" s="2">
         <v>4.7143768259831491</v>
       </c>
@@ -2471,7 +2783,9 @@
       <c r="S5" s="2">
         <v>1</v>
       </c>
-      <c r="T5" s="2"/>
+      <c r="T5" s="2">
+        <v>21.117881215194927</v>
+      </c>
       <c r="U5" s="2">
         <v>23.816540005628696</v>
       </c>
@@ -2480,7 +2794,9 @@
       <c r="Y5" s="2">
         <v>1</v>
       </c>
-      <c r="Z5" s="2"/>
+      <c r="Z5" s="2">
+        <v>35.264187704334361</v>
+      </c>
       <c r="AA5" s="2">
         <v>198.77011387302639</v>
       </c>
@@ -2489,7 +2805,9 @@
       <c r="AE5" s="2">
         <v>1</v>
       </c>
-      <c r="AF5" s="2"/>
+      <c r="AF5" s="2">
+        <v>95.191734251414161</v>
+      </c>
       <c r="AG5" s="2">
         <v>102.47796774420222</v>
       </c>
@@ -2500,7 +2818,9 @@
       <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <v>0.68665458312868477</v>
+      </c>
       <c r="C6" s="2">
         <v>1.9559903967612584</v>
       </c>
@@ -2509,7 +2829,9 @@
       <c r="G6" s="2">
         <v>2</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="2">
+        <v>1.7489707571789854E+204</v>
+      </c>
       <c r="I6" s="2">
         <v>9.9055743149702025</v>
       </c>
@@ -2518,7 +2840,9 @@
       <c r="M6" s="2">
         <v>2</v>
       </c>
-      <c r="N6" s="2"/>
+      <c r="N6" s="2">
+        <v>4.4738381888009826E-9</v>
+      </c>
       <c r="O6" s="2">
         <v>9.4124225566013742</v>
       </c>
@@ -2527,7 +2851,9 @@
       <c r="S6" s="2">
         <v>2</v>
       </c>
-      <c r="T6" s="2"/>
+      <c r="T6" s="2">
+        <v>21.232322109381911</v>
+      </c>
       <c r="U6" s="2">
         <v>21.062510619807334</v>
       </c>
@@ -2536,7 +2862,9 @@
       <c r="Y6" s="2">
         <v>2</v>
       </c>
-      <c r="Z6" s="2"/>
+      <c r="Z6" s="2">
+        <v>32.906784911250057</v>
+      </c>
       <c r="AA6" s="2">
         <v>200.33957767873807</v>
       </c>
@@ -2545,7 +2873,9 @@
       <c r="AE6" s="2">
         <v>2</v>
       </c>
-      <c r="AF6" s="2"/>
+      <c r="AF6" s="2">
+        <v>93.916777413154307</v>
+      </c>
       <c r="AG6" s="2">
         <v>107.61390464803897</v>
       </c>
@@ -2556,7 +2886,9 @@
       <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <v>0.50446056395766203</v>
+      </c>
       <c r="C7" s="2">
         <v>2.3193518377696054</v>
       </c>
@@ -2565,7 +2897,9 @@
       <c r="G7" s="2">
         <v>3</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2">
+        <v>3.7876606235726671E+305</v>
+      </c>
       <c r="I7" s="2">
         <v>10.724345788325733</v>
       </c>
@@ -2574,7 +2908,9 @@
       <c r="M7" s="2">
         <v>3</v>
       </c>
-      <c r="N7" s="2"/>
+      <c r="N7" s="2">
+        <v>2.1938006966593093E-13</v>
+      </c>
       <c r="O7" s="2">
         <v>6.6218519952512649</v>
       </c>
@@ -2583,7 +2919,9 @@
       <c r="S7" s="2">
         <v>3</v>
       </c>
-      <c r="T7" s="2"/>
+      <c r="T7" s="2">
+        <v>22.235941902760686</v>
+      </c>
       <c r="U7" s="2">
         <v>22.489920708993097</v>
       </c>
@@ -2592,7 +2930,9 @@
       <c r="Y7" s="2">
         <v>3</v>
       </c>
-      <c r="Z7" s="2"/>
+      <c r="Z7" s="2">
+        <v>31.683380133359119</v>
+      </c>
       <c r="AA7" s="2">
         <v>203.99343786852498</v>
       </c>
@@ -2601,7 +2941,9 @@
       <c r="AE7" s="2">
         <v>3</v>
       </c>
-      <c r="AF7" s="2"/>
+      <c r="AF7" s="2">
+        <v>90.615663595104692</v>
+      </c>
       <c r="AG7" s="2">
         <v>108.0136212258269</v>
       </c>
@@ -2612,7 +2954,9 @@
       <c r="A8" s="2">
         <v>4</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <v>0.4938289724878433</v>
+      </c>
       <c r="C8" s="2">
         <v>2.4345907539627509</v>
       </c>
@@ -2630,7 +2974,9 @@
       <c r="M8" s="2">
         <v>4</v>
       </c>
-      <c r="N8" s="2"/>
+      <c r="N8" s="2">
+        <v>8.8817841970012523E-16</v>
+      </c>
       <c r="O8" s="2">
         <v>11.055272461204169</v>
       </c>
@@ -2639,7 +2985,9 @@
       <c r="S8" s="2">
         <v>4</v>
       </c>
-      <c r="T8" s="2"/>
+      <c r="T8" s="2">
+        <v>21.279414555074883</v>
+      </c>
       <c r="U8" s="2">
         <v>23.358995173572225</v>
       </c>
@@ -2648,7 +2996,9 @@
       <c r="Y8" s="2">
         <v>4</v>
       </c>
-      <c r="Z8" s="2"/>
+      <c r="Z8" s="2">
+        <v>32.104299478582952</v>
+      </c>
       <c r="AA8" s="2">
         <v>204.96588516299761</v>
       </c>
@@ -2657,7 +3007,9 @@
       <c r="AE8" s="2">
         <v>4</v>
       </c>
-      <c r="AF8" s="2"/>
+      <c r="AF8" s="2">
+        <v>89.652498340194356</v>
+      </c>
       <c r="AG8" s="2">
         <v>104.37391191855824</v>
       </c>
@@ -2668,7 +3020,9 @@
       <c r="A9" s="2">
         <v>5</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2">
+        <v>0.74409099132849876</v>
+      </c>
       <c r="C9" s="2">
         <v>2.1922969949641571</v>
       </c>
@@ -2686,7 +3040,9 @@
       <c r="M9" s="2">
         <v>5</v>
       </c>
-      <c r="N9" s="2"/>
+      <c r="N9" s="2">
+        <v>2.6645352591003757E-15</v>
+      </c>
       <c r="O9" s="2">
         <v>7.9966623820057681</v>
       </c>
@@ -2695,7 +3051,9 @@
       <c r="S9" s="2">
         <v>5</v>
       </c>
-      <c r="T9" s="2"/>
+      <c r="T9" s="2">
+        <v>21.820801696953545</v>
+      </c>
       <c r="U9" s="2">
         <v>22.450261199604128</v>
       </c>
@@ -2704,7 +3062,9 @@
       <c r="Y9" s="2">
         <v>5</v>
       </c>
-      <c r="Z9" s="2"/>
+      <c r="Z9" s="2">
+        <v>28.650192924419056</v>
+      </c>
       <c r="AA9" s="2">
         <v>207.18175273589034</v>
       </c>
@@ -2713,7 +3073,9 @@
       <c r="AE9" s="2">
         <v>5</v>
       </c>
-      <c r="AF9" s="2"/>
+      <c r="AF9" s="2">
+        <v>96.822680217666587</v>
+      </c>
       <c r="AG9" s="2">
         <v>99.743194434835203</v>
       </c>
@@ -2724,7 +3086,9 @@
       <c r="A10" s="2">
         <v>6</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2">
+        <v>0.49926842811161881</v>
+      </c>
       <c r="C10" s="2">
         <v>2.0560844437447612</v>
       </c>
@@ -2742,7 +3106,9 @@
       <c r="M10" s="2">
         <v>6</v>
       </c>
-      <c r="N10" s="2"/>
+      <c r="N10" s="2">
+        <v>8.8817841970012523E-16</v>
+      </c>
       <c r="O10" s="2">
         <v>8.5404459724334885</v>
       </c>
@@ -2751,7 +3117,9 @@
       <c r="S10" s="2">
         <v>6</v>
       </c>
-      <c r="T10" s="2"/>
+      <c r="T10" s="2">
+        <v>20.369900900781747</v>
+      </c>
       <c r="U10" s="2">
         <v>21.119194594032759</v>
       </c>
@@ -2760,7 +3128,9 @@
       <c r="Y10" s="2">
         <v>6</v>
       </c>
-      <c r="Z10" s="2"/>
+      <c r="Z10" s="2">
+        <v>33.458173659664034</v>
+      </c>
       <c r="AA10" s="2">
         <v>195.97459150383708</v>
       </c>
@@ -2769,7 +3139,9 @@
       <c r="AE10" s="2">
         <v>6</v>
       </c>
-      <c r="AF10" s="2"/>
+      <c r="AF10" s="2">
+        <v>97.872219520114385</v>
+      </c>
       <c r="AG10" s="2">
         <v>106.51793835975624</v>
       </c>
@@ -2780,7 +3152,9 @@
       <c r="A11" s="2">
         <v>7</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <v>0.57754302067258456</v>
+      </c>
       <c r="C11" s="2">
         <v>3.0706354486114908</v>
       </c>
@@ -2798,7 +3172,9 @@
       <c r="M11" s="2">
         <v>7</v>
       </c>
-      <c r="N11" s="2"/>
+      <c r="N11" s="2">
+        <v>8.8817841970012523E-16</v>
+      </c>
       <c r="O11" s="2">
         <v>3.2503455891247208</v>
       </c>
@@ -2807,7 +3183,9 @@
       <c r="S11" s="2">
         <v>7</v>
       </c>
-      <c r="T11" s="2"/>
+      <c r="T11" s="2">
+        <v>21.338903009773187</v>
+      </c>
       <c r="U11" s="2">
         <v>23.427504001608462</v>
       </c>
@@ -2816,7 +3194,9 @@
       <c r="Y11" s="2">
         <v>7</v>
       </c>
-      <c r="Z11" s="2"/>
+      <c r="Z11" s="2">
+        <v>33.52459957247391</v>
+      </c>
       <c r="AA11" s="2">
         <v>192.67582669311869</v>
       </c>
@@ -2825,7 +3205,9 @@
       <c r="AE11" s="2">
         <v>7</v>
       </c>
-      <c r="AF11" s="2"/>
+      <c r="AF11" s="2">
+        <v>96.24113757311153</v>
+      </c>
       <c r="AG11" s="2">
         <v>104.66443389121832</v>
       </c>
@@ -2836,7 +3218,9 @@
       <c r="A12" s="2">
         <v>8</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2">
+        <v>0.54241449448574286</v>
+      </c>
       <c r="C12" s="2">
         <v>2.3044975126198559</v>
       </c>
@@ -2854,7 +3238,9 @@
       <c r="M12" s="2">
         <v>8</v>
       </c>
-      <c r="N12" s="2"/>
+      <c r="N12" s="2">
+        <v>8.8817841970012523E-16</v>
+      </c>
       <c r="O12" s="2">
         <v>7.1672572560075034</v>
       </c>
@@ -2863,7 +3249,9 @@
       <c r="S12" s="2">
         <v>8</v>
       </c>
-      <c r="T12" s="2"/>
+      <c r="T12" s="2">
+        <v>20.410551525703255</v>
+      </c>
       <c r="U12" s="2">
         <v>23.069164002306078</v>
       </c>
@@ -2872,7 +3260,9 @@
       <c r="Y12" s="2">
         <v>8</v>
       </c>
-      <c r="Z12" s="2"/>
+      <c r="Z12" s="2">
+        <v>31.529225474152849</v>
+      </c>
       <c r="AA12" s="2">
         <v>204.89799099761626</v>
       </c>
@@ -2881,7 +3271,9 @@
       <c r="AE12" s="2">
         <v>8</v>
       </c>
-      <c r="AF12" s="2"/>
+      <c r="AF12" s="2">
+        <v>96.459748904317536</v>
+      </c>
       <c r="AG12" s="2">
         <v>102.04192054989677</v>
       </c>
@@ -2892,7 +3284,9 @@
       <c r="A13" s="2">
         <v>9</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2">
+        <v>0.41425797117593016</v>
+      </c>
       <c r="C13" s="2">
         <v>2.688593883069414</v>
       </c>
@@ -2910,7 +3304,9 @@
       <c r="M13" s="2">
         <v>9</v>
       </c>
-      <c r="N13" s="2"/>
+      <c r="N13" s="2">
+        <v>1.7763568394002505E-15</v>
+      </c>
       <c r="O13" s="2">
         <v>4.6750588016008674</v>
       </c>
@@ -2919,7 +3315,9 @@
       <c r="S13" s="2">
         <v>9</v>
       </c>
-      <c r="T13" s="2"/>
+      <c r="T13" s="2">
+        <v>22.497929510320489</v>
+      </c>
       <c r="U13" s="2">
         <v>22.098123677287976</v>
       </c>
@@ -2928,7 +3326,9 @@
       <c r="Y13" s="2">
         <v>9</v>
       </c>
-      <c r="Z13" s="2"/>
+      <c r="Z13" s="2">
+        <v>29.926670021363798</v>
+      </c>
       <c r="AA13" s="2">
         <v>191.15766210796346</v>
       </c>
@@ -2937,7 +3337,9 @@
       <c r="AE13" s="2">
         <v>9</v>
       </c>
-      <c r="AF13" s="2"/>
+      <c r="AF13" s="2">
+        <v>96.359669042831499</v>
+      </c>
       <c r="AG13" s="2">
         <v>104.6097553119202</v>
       </c>
@@ -2948,7 +3350,9 @@
       <c r="A14" s="2">
         <v>10</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2">
+        <v>0.52201483189672904</v>
+      </c>
       <c r="C14" s="2">
         <v>2.1515681707542798</v>
       </c>
@@ -2966,7 +3370,9 @@
       <c r="M14" s="2">
         <v>10</v>
       </c>
-      <c r="N14" s="2"/>
+      <c r="N14" s="2">
+        <v>2.6645352591003757E-15</v>
+      </c>
       <c r="O14" s="2">
         <v>7.768264107197556</v>
       </c>
@@ -2975,7 +3381,9 @@
       <c r="S14" s="2">
         <v>10</v>
       </c>
-      <c r="T14" s="2"/>
+      <c r="T14" s="2">
+        <v>19.213936833838673</v>
+      </c>
       <c r="U14" s="2">
         <v>21.782262998149125</v>
       </c>
@@ -2984,7 +3392,9 @@
       <c r="Y14" s="2">
         <v>10</v>
       </c>
-      <c r="Z14" s="2"/>
+      <c r="Z14" s="2">
+        <v>33.991277179705712</v>
+      </c>
       <c r="AA14" s="2">
         <v>204.84184006911516</v>
       </c>
@@ -2993,7 +3403,9 @@
       <c r="AE14" s="2">
         <v>10</v>
       </c>
-      <c r="AF14" s="2"/>
+      <c r="AF14" s="2">
+        <v>94.607323571186654</v>
+      </c>
       <c r="AG14" s="2">
         <v>103.17879716664456</v>
       </c>
@@ -3004,7 +3416,9 @@
       <c r="A15" s="2">
         <v>11</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2">
+        <v>0.42026288262111894</v>
+      </c>
       <c r="C15" s="2">
         <v>2.0508703222527038</v>
       </c>
@@ -3022,7 +3436,9 @@
       <c r="M15" s="2">
         <v>11</v>
       </c>
-      <c r="N15" s="2"/>
+      <c r="N15" s="2">
+        <v>8.8817841970012523E-16</v>
+      </c>
       <c r="O15" s="2">
         <v>7.8617358841656051</v>
       </c>
@@ -3031,7 +3447,9 @@
       <c r="S15" s="2">
         <v>11</v>
       </c>
-      <c r="T15" s="2"/>
+      <c r="T15" s="2">
+        <v>21.072329186337729</v>
+      </c>
       <c r="U15" s="2">
         <v>21.974414232170737</v>
       </c>
@@ -3040,7 +3458,9 @@
       <c r="Y15" s="2">
         <v>11</v>
       </c>
-      <c r="Z15" s="2"/>
+      <c r="Z15" s="2">
+        <v>32.852122979613938</v>
+      </c>
       <c r="AA15" s="2">
         <v>198.17163437267089</v>
       </c>
@@ -3049,7 +3469,9 @@
       <c r="AE15" s="2">
         <v>11</v>
       </c>
-      <c r="AF15" s="2"/>
+      <c r="AF15" s="2">
+        <v>93.824551743650318</v>
+      </c>
       <c r="AG15" s="2">
         <v>106.38231921844385</v>
       </c>
@@ -3060,7 +3482,9 @@
       <c r="A16" s="2">
         <v>12</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2">
+        <v>0.52893966962652073</v>
+      </c>
       <c r="C16" s="2">
         <v>2.5874983376243779</v>
       </c>
@@ -3078,7 +3502,9 @@
       <c r="M16" s="2">
         <v>12</v>
       </c>
-      <c r="N16" s="2"/>
+      <c r="N16" s="2">
+        <v>0</v>
+      </c>
       <c r="O16" s="2">
         <v>7.2521409844709108</v>
       </c>
@@ -3087,7 +3513,9 @@
       <c r="S16" s="2">
         <v>12</v>
       </c>
-      <c r="T16" s="2"/>
+      <c r="T16" s="2">
+        <v>19.846408174529383</v>
+      </c>
       <c r="U16" s="2">
         <v>22.689493934089398</v>
       </c>
@@ -3096,7 +3524,9 @@
       <c r="Y16" s="2">
         <v>12</v>
       </c>
-      <c r="Z16" s="2"/>
+      <c r="Z16" s="2">
+        <v>33.002232364231965</v>
+      </c>
       <c r="AA16" s="2">
         <v>214.8929925884087</v>
       </c>
@@ -3105,7 +3535,9 @@
       <c r="AE16" s="2">
         <v>12</v>
       </c>
-      <c r="AF16" s="2"/>
+      <c r="AF16" s="2">
+        <v>100.05803823263889</v>
+      </c>
       <c r="AG16" s="2">
         <v>102.17313478600889</v>
       </c>
@@ -3116,7 +3548,9 @@
       <c r="A17" s="2">
         <v>13</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2">
+        <v>0.4508870983930745</v>
+      </c>
       <c r="C17" s="2">
         <v>2.3488104340313982</v>
       </c>
@@ -3134,7 +3568,9 @@
       <c r="M17" s="2">
         <v>13</v>
       </c>
-      <c r="N17" s="2"/>
+      <c r="N17" s="2">
+        <v>8.8817841970012523E-16</v>
+      </c>
       <c r="O17" s="2">
         <v>4.8630719321585296</v>
       </c>
@@ -3143,7 +3579,9 @@
       <c r="S17" s="2">
         <v>13</v>
       </c>
-      <c r="T17" s="2"/>
+      <c r="T17" s="2">
+        <v>21.803908110375762</v>
+      </c>
       <c r="U17" s="2">
         <v>23.653509015870476</v>
       </c>
@@ -3152,7 +3590,9 @@
       <c r="Y17" s="2">
         <v>13</v>
       </c>
-      <c r="Z17" s="2"/>
+      <c r="Z17" s="2">
+        <v>30.071867346349226</v>
+      </c>
       <c r="AA17" s="2">
         <v>208.82593323104095</v>
       </c>
@@ -3161,7 +3601,9 @@
       <c r="AE17" s="2">
         <v>13</v>
       </c>
-      <c r="AF17" s="2"/>
+      <c r="AF17" s="2">
+        <v>90.446251864221566</v>
+      </c>
       <c r="AG17" s="2">
         <v>110.3551587127657</v>
       </c>
@@ -3172,7 +3614,9 @@
       <c r="A18" s="2">
         <v>14</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2">
+        <v>0.57183303979206235</v>
+      </c>
       <c r="C18" s="2">
         <v>2.7376548885108725</v>
       </c>
@@ -3190,7 +3634,9 @@
       <c r="M18" s="2">
         <v>14</v>
       </c>
-      <c r="N18" s="2"/>
+      <c r="N18" s="2">
+        <v>2.6645352591003757E-15</v>
+      </c>
       <c r="O18" s="2">
         <v>3.5388177535866356</v>
       </c>
@@ -3199,7 +3645,9 @@
       <c r="S18" s="2">
         <v>14</v>
       </c>
-      <c r="T18" s="2"/>
+      <c r="T18" s="2">
+        <v>22.217623001780805</v>
+      </c>
       <c r="U18" s="2">
         <v>21.095518848878051</v>
       </c>
@@ -3208,7 +3656,9 @@
       <c r="Y18" s="2">
         <v>14</v>
       </c>
-      <c r="Z18" s="2"/>
+      <c r="Z18" s="2">
+        <v>33.140415785828047</v>
+      </c>
       <c r="AA18" s="2">
         <v>216.47644209257226</v>
       </c>
@@ -3217,7 +3667,9 @@
       <c r="AE18" s="2">
         <v>14</v>
       </c>
-      <c r="AF18" s="2"/>
+      <c r="AF18" s="2">
+        <v>96.498410915697633</v>
+      </c>
       <c r="AG18" s="2">
         <v>106.92960024690026</v>
       </c>
@@ -3228,7 +3680,9 @@
       <c r="A19" s="2">
         <v>15</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2">
+        <v>0.39178629405981014</v>
+      </c>
       <c r="C19" s="2">
         <v>2.6269802804504918</v>
       </c>
@@ -3246,7 +3700,9 @@
       <c r="M19" s="2">
         <v>15</v>
       </c>
-      <c r="N19" s="2"/>
+      <c r="N19" s="2">
+        <v>2.6645352591003757E-15</v>
+      </c>
       <c r="O19" s="2">
         <v>7.0222861133328642</v>
       </c>
@@ -3255,7 +3711,9 @@
       <c r="S19" s="2">
         <v>15</v>
       </c>
-      <c r="T19" s="2"/>
+      <c r="T19" s="2">
+        <v>19.836140077534697</v>
+      </c>
       <c r="U19" s="2">
         <v>22.496500773223126</v>
       </c>
@@ -3264,7 +3722,9 @@
       <c r="Y19" s="2">
         <v>15</v>
       </c>
-      <c r="Z19" s="2"/>
+      <c r="Z19" s="2">
+        <v>31.897062292496127</v>
+      </c>
       <c r="AA19" s="2">
         <v>197.98739714269823</v>
       </c>
@@ -3273,7 +3733,9 @@
       <c r="AE19" s="2">
         <v>15</v>
       </c>
-      <c r="AF19" s="2"/>
+      <c r="AF19" s="2">
+        <v>93.391685194185044</v>
+      </c>
       <c r="AG19" s="2">
         <v>106.39883906294124</v>
       </c>
@@ -3284,7 +3746,9 @@
       <c r="A20" s="2">
         <v>16</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2">
+        <v>0.44084476900031899</v>
+      </c>
       <c r="C20" s="2">
         <v>2.2667773262884929</v>
       </c>
@@ -3302,7 +3766,9 @@
       <c r="M20" s="2">
         <v>16</v>
       </c>
-      <c r="N20" s="2"/>
+      <c r="N20" s="2">
+        <v>3.5527136788005009E-15</v>
+      </c>
       <c r="O20" s="2">
         <v>4.9155578335342058</v>
       </c>
@@ -3311,7 +3777,9 @@
       <c r="S20" s="2">
         <v>16</v>
       </c>
-      <c r="T20" s="2"/>
+      <c r="T20" s="2">
+        <v>22.277100430014471</v>
+      </c>
       <c r="U20" s="2">
         <v>22.291452607418648</v>
       </c>
@@ -3320,7 +3788,9 @@
       <c r="Y20" s="2">
         <v>16</v>
       </c>
-      <c r="Z20" s="2"/>
+      <c r="Z20" s="2">
+        <v>31.982213469476516</v>
+      </c>
       <c r="AA20" s="2">
         <v>210.42331277904398</v>
       </c>
@@ -3329,7 +3799,9 @@
       <c r="AE20" s="2">
         <v>16</v>
       </c>
-      <c r="AF20" s="2"/>
+      <c r="AF20" s="2">
+        <v>95.451452028340483</v>
+      </c>
       <c r="AG20" s="2">
         <v>106.94148534571694</v>
       </c>
@@ -3340,7 +3812,9 @@
       <c r="A21" s="2">
         <v>17</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2">
+        <v>0.48891788773397832</v>
+      </c>
       <c r="C21" s="2">
         <v>1.9193421394683214</v>
       </c>
@@ -3358,7 +3832,9 @@
       <c r="M21" s="2">
         <v>17</v>
       </c>
-      <c r="N21" s="2"/>
+      <c r="N21" s="2">
+        <v>1.7763568394002505E-15</v>
+      </c>
       <c r="O21" s="2">
         <v>8.8147844954531855</v>
       </c>
@@ -3367,7 +3843,9 @@
       <c r="S21" s="2">
         <v>17</v>
       </c>
-      <c r="T21" s="2"/>
+      <c r="T21" s="2">
+        <v>20.684723147846306</v>
+      </c>
       <c r="U21" s="2">
         <v>21.205964757693188</v>
       </c>
@@ -3376,7 +3854,9 @@
       <c r="Y21" s="2">
         <v>17</v>
       </c>
-      <c r="Z21" s="2"/>
+      <c r="Z21" s="2">
+        <v>34.316497604830758</v>
+      </c>
       <c r="AA21" s="2">
         <v>191.53291444194909</v>
       </c>
@@ -3385,7 +3865,9 @@
       <c r="AE21" s="2">
         <v>17</v>
       </c>
-      <c r="AF21" s="2"/>
+      <c r="AF21" s="2">
+        <v>90.652770175116743</v>
+      </c>
       <c r="AG21" s="2">
         <v>103.24169601533083</v>
       </c>
@@ -3396,7 +3878,9 @@
       <c r="A22" s="2">
         <v>18</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2">
+        <v>0.40143079693527967</v>
+      </c>
       <c r="C22" s="2">
         <v>2.3136043230608241</v>
       </c>
@@ -3414,7 +3898,9 @@
       <c r="M22" s="2">
         <v>18</v>
       </c>
-      <c r="N22" s="2"/>
+      <c r="N22" s="2">
+        <v>2.6645352591003757E-15</v>
+      </c>
       <c r="O22" s="2">
         <v>6.629396187751988</v>
       </c>
@@ -3423,7 +3909,9 @@
       <c r="S22" s="2">
         <v>18</v>
       </c>
-      <c r="T22" s="2"/>
+      <c r="T22" s="2">
+        <v>20.413144749045738</v>
+      </c>
       <c r="U22" s="2">
         <v>22.337749860051932</v>
       </c>
@@ -3432,7 +3920,9 @@
       <c r="Y22" s="2">
         <v>18</v>
       </c>
-      <c r="Z22" s="2"/>
+      <c r="Z22" s="2">
+        <v>32.888249290532542</v>
+      </c>
       <c r="AA22" s="2">
         <v>199.60090656428403</v>
       </c>
@@ -3441,7 +3931,9 @@
       <c r="AE22" s="2">
         <v>18</v>
       </c>
-      <c r="AF22" s="2"/>
+      <c r="AF22" s="2">
+        <v>93.990233789151745</v>
+      </c>
       <c r="AG22" s="2">
         <v>108.12630157182934</v>
       </c>
@@ -3452,7 +3944,9 @@
       <c r="A23" s="2">
         <v>19</v>
       </c>
-      <c r="B23" s="2"/>
+      <c r="B23" s="2">
+        <v>0.6177709623629144</v>
+      </c>
       <c r="C23" s="2">
         <v>3.0784333801850732</v>
       </c>
@@ -3470,7 +3964,9 @@
       <c r="M23" s="2">
         <v>19</v>
       </c>
-      <c r="N23" s="2"/>
+      <c r="N23" s="2">
+        <v>1.7763568394002505E-15</v>
+      </c>
       <c r="O23" s="2">
         <v>3.7555606090788878</v>
       </c>
@@ -3479,7 +3975,9 @@
       <c r="S23" s="2">
         <v>19</v>
       </c>
-      <c r="T23" s="2"/>
+      <c r="T23" s="2">
+        <v>21.236558425515749</v>
+      </c>
       <c r="U23" s="2">
         <v>22.108330905423241</v>
       </c>
@@ -3488,7 +3986,9 @@
       <c r="Y23" s="2">
         <v>19</v>
       </c>
-      <c r="Z23" s="2"/>
+      <c r="Z23" s="2">
+        <v>33.117302961414545</v>
+      </c>
       <c r="AA23" s="2">
         <v>193.32762177356909</v>
       </c>
@@ -3497,7 +3997,9 @@
       <c r="AE23" s="2">
         <v>19</v>
       </c>
-      <c r="AF23" s="2"/>
+      <c r="AF23" s="2">
+        <v>92.130756182400049</v>
+      </c>
       <c r="AG23" s="2">
         <v>104.29985733966535</v>
       </c>
@@ -3508,7 +4010,9 @@
       <c r="A24" s="2">
         <v>20</v>
       </c>
-      <c r="B24" s="2"/>
+      <c r="B24" s="2">
+        <v>0.45038212859093851</v>
+      </c>
       <c r="C24" s="2">
         <v>2.5169192873482058</v>
       </c>
@@ -3526,7 +4030,9 @@
       <c r="M24" s="2">
         <v>20</v>
       </c>
-      <c r="N24" s="2"/>
+      <c r="N24" s="2">
+        <v>2.6645352591003757E-15</v>
+      </c>
       <c r="O24" s="2">
         <v>5.5036927820527817</v>
       </c>
@@ -3535,7 +4041,9 @@
       <c r="S24" s="2">
         <v>20</v>
       </c>
-      <c r="T24" s="2"/>
+      <c r="T24" s="2">
+        <v>20.26525383890289</v>
+      </c>
       <c r="U24" s="2">
         <v>24.206796555777544</v>
       </c>
@@ -3544,7 +4052,9 @@
       <c r="Y24" s="2">
         <v>20</v>
       </c>
-      <c r="Z24" s="2"/>
+      <c r="Z24" s="2">
+        <v>30.461936194313928</v>
+      </c>
       <c r="AA24" s="2">
         <v>193.38172796442498</v>
       </c>
@@ -3553,7 +4063,9 @@
       <c r="AE24" s="2">
         <v>20</v>
       </c>
-      <c r="AF24" s="2"/>
+      <c r="AF24" s="2">
+        <v>97.498769771543664</v>
+      </c>
       <c r="AG24" s="2">
         <v>105.2727078088794</v>
       </c>
@@ -3564,7 +4076,9 @@
       <c r="A25" s="2">
         <v>21</v>
       </c>
-      <c r="B25" s="2"/>
+      <c r="B25" s="2">
+        <v>0.43883071153636133</v>
+      </c>
       <c r="C25" s="2">
         <v>2.0630056814983515</v>
       </c>
@@ -3582,7 +4096,9 @@
       <c r="M25" s="2">
         <v>21</v>
       </c>
-      <c r="N25" s="2"/>
+      <c r="N25" s="2">
+        <v>8.8817841970012523E-16</v>
+      </c>
       <c r="O25" s="2">
         <v>8.4233850914329693</v>
       </c>
@@ -3591,7 +4107,9 @@
       <c r="S25" s="2">
         <v>21</v>
       </c>
-      <c r="T25" s="2"/>
+      <c r="T25" s="2">
+        <v>20.757987430066862</v>
+      </c>
       <c r="U25" s="2">
         <v>20.931393195616486</v>
       </c>
@@ -3600,7 +4118,9 @@
       <c r="Y25" s="2">
         <v>21</v>
       </c>
-      <c r="Z25" s="2"/>
+      <c r="Z25" s="2">
+        <v>33.060992772886216</v>
+      </c>
       <c r="AA25" s="2">
         <v>198.91708535275748</v>
       </c>
@@ -3609,7 +4129,9 @@
       <c r="AE25" s="2">
         <v>21</v>
       </c>
-      <c r="AF25" s="2"/>
+      <c r="AF25" s="2">
+        <v>94.899469303058808</v>
+      </c>
       <c r="AG25" s="2">
         <v>107.12371888737583</v>
       </c>
@@ -3620,7 +4142,9 @@
       <c r="A26" s="2">
         <v>22</v>
       </c>
-      <c r="B26" s="2"/>
+      <c r="B26" s="2">
+        <v>0.35466145314283187</v>
+      </c>
       <c r="C26" s="2">
         <v>1.5963423619509298</v>
       </c>
@@ -3638,7 +4162,9 @@
       <c r="M26" s="2">
         <v>22</v>
       </c>
-      <c r="N26" s="2"/>
+      <c r="N26" s="2">
+        <v>8.8817841970012523E-16</v>
+      </c>
       <c r="O26" s="2">
         <v>9.9500108676513932</v>
       </c>
@@ -3647,7 +4173,9 @@
       <c r="S26" s="2">
         <v>22</v>
       </c>
-      <c r="T26" s="2"/>
+      <c r="T26" s="2">
+        <v>19.67974347000731</v>
+      </c>
       <c r="U26" s="2">
         <v>21.710597899909828</v>
       </c>
@@ -3656,7 +4184,9 @@
       <c r="Y26" s="2">
         <v>22</v>
       </c>
-      <c r="Z26" s="2"/>
+      <c r="Z26" s="2">
+        <v>29.575792494339588</v>
+      </c>
       <c r="AA26" s="2">
         <v>213.13670347253424</v>
       </c>
@@ -3665,7 +4195,9 @@
       <c r="AE26" s="2">
         <v>22</v>
       </c>
-      <c r="AF26" s="2"/>
+      <c r="AF26" s="2">
+        <v>97.784745635834895</v>
+      </c>
       <c r="AG26" s="2">
         <v>105.8077346138512</v>
       </c>
@@ -3676,7 +4208,9 @@
       <c r="A27" s="2">
         <v>23</v>
       </c>
-      <c r="B27" s="2"/>
+      <c r="B27" s="2">
+        <v>0.41375218955521093</v>
+      </c>
       <c r="C27" s="2">
         <v>2.5921794742509143</v>
       </c>
@@ -3694,7 +4228,9 @@
       <c r="M27" s="2">
         <v>23</v>
       </c>
-      <c r="N27" s="2"/>
+      <c r="N27" s="2">
+        <v>2.6645352591003757E-15</v>
+      </c>
       <c r="O27" s="2">
         <v>5.8717369400446371</v>
       </c>
@@ -3703,7 +4239,9 @@
       <c r="S27" s="2">
         <v>23</v>
       </c>
-      <c r="T27" s="2"/>
+      <c r="T27" s="2">
+        <v>20.65656008535419</v>
+      </c>
       <c r="U27" s="2">
         <v>22.695345479298329</v>
       </c>
@@ -3712,7 +4250,9 @@
       <c r="Y27" s="2">
         <v>23</v>
       </c>
-      <c r="Z27" s="2"/>
+      <c r="Z27" s="2">
+        <v>30.04328913756159</v>
+      </c>
       <c r="AA27" s="2">
         <v>193.20808311066634</v>
       </c>
@@ -3721,7 +4261,9 @@
       <c r="AE27" s="2">
         <v>23</v>
       </c>
-      <c r="AF27" s="2"/>
+      <c r="AF27" s="2">
+        <v>98.097263654402013</v>
+      </c>
       <c r="AG27" s="2">
         <v>110.15500946087421</v>
       </c>
@@ -3732,7 +4274,9 @@
       <c r="A28" s="2">
         <v>24</v>
       </c>
-      <c r="B28" s="2"/>
+      <c r="B28" s="2">
+        <v>0.44537463959417639</v>
+      </c>
       <c r="C28" s="2">
         <v>2.1745976981089723</v>
       </c>
@@ -3750,7 +4294,9 @@
       <c r="M28" s="2">
         <v>24</v>
       </c>
-      <c r="N28" s="2"/>
+      <c r="N28" s="2">
+        <v>1.7763568394002505E-15</v>
+      </c>
       <c r="O28" s="2">
         <v>9.0265898645780354</v>
       </c>
@@ -3759,7 +4305,9 @@
       <c r="S28" s="2">
         <v>24</v>
       </c>
-      <c r="T28" s="2"/>
+      <c r="T28" s="2">
+        <v>21.060088108668911</v>
+      </c>
       <c r="U28" s="2">
         <v>22.638792879778123</v>
       </c>
@@ -3768,7 +4316,9 @@
       <c r="Y28" s="2">
         <v>24</v>
       </c>
-      <c r="Z28" s="2"/>
+      <c r="Z28" s="2">
+        <v>31.818580145432158</v>
+      </c>
       <c r="AA28" s="2">
         <v>213.97601440574869</v>
       </c>
@@ -3777,7 +4327,9 @@
       <c r="AE28" s="2">
         <v>24</v>
       </c>
-      <c r="AF28" s="2"/>
+      <c r="AF28" s="2">
+        <v>95.957736331045808</v>
+      </c>
       <c r="AG28" s="2">
         <v>111.04272446477889</v>
       </c>
@@ -3788,7 +4340,9 @@
       <c r="A29" s="2">
         <v>25</v>
       </c>
-      <c r="B29" s="2"/>
+      <c r="B29" s="2">
+        <v>0.61611422571641328</v>
+      </c>
       <c r="C29" s="2">
         <v>2.3897209605092868</v>
       </c>
@@ -3806,7 +4360,9 @@
       <c r="M29" s="2">
         <v>25</v>
       </c>
-      <c r="N29" s="2"/>
+      <c r="N29" s="2">
+        <v>3.5527136788005009E-15</v>
+      </c>
       <c r="O29" s="2">
         <v>11.469723382335658</v>
       </c>
@@ -3815,7 +4371,9 @@
       <c r="S29" s="2">
         <v>25</v>
       </c>
-      <c r="T29" s="2"/>
+      <c r="T29" s="2">
+        <v>20.802824537183454</v>
+      </c>
       <c r="U29" s="2">
         <v>24.094856504004955</v>
       </c>
@@ -3824,7 +4382,9 @@
       <c r="Y29" s="2">
         <v>25</v>
       </c>
-      <c r="Z29" s="2"/>
+      <c r="Z29" s="2">
+        <v>31.697700341831581</v>
+      </c>
       <c r="AA29" s="2">
         <v>210.68444317396879</v>
       </c>
@@ -3833,7 +4393,9 @@
       <c r="AE29" s="2">
         <v>25</v>
       </c>
-      <c r="AF29" s="2"/>
+      <c r="AF29" s="2">
+        <v>94.298804716898474</v>
+      </c>
       <c r="AG29" s="2">
         <v>106.93338402998995</v>
       </c>
@@ -3844,7 +4406,9 @@
       <c r="A30" s="2">
         <v>26</v>
       </c>
-      <c r="B30" s="2"/>
+      <c r="B30" s="2">
+        <v>0.60347006750856569</v>
+      </c>
       <c r="C30" s="2">
         <v>2.1443395041110906</v>
       </c>
@@ -3862,7 +4426,9 @@
       <c r="M30" s="2">
         <v>26</v>
       </c>
-      <c r="N30" s="2"/>
+      <c r="N30" s="2">
+        <v>1.7763568394002505E-15</v>
+      </c>
       <c r="O30" s="2">
         <v>4.8166469359106241</v>
       </c>
@@ -3871,7 +4437,9 @@
       <c r="S30" s="2">
         <v>26</v>
       </c>
-      <c r="T30" s="2"/>
+      <c r="T30" s="2">
+        <v>20.486683593942569</v>
+      </c>
       <c r="U30" s="2">
         <v>23.588018165020323</v>
       </c>
@@ -3880,7 +4448,9 @@
       <c r="Y30" s="2">
         <v>26</v>
       </c>
-      <c r="Z30" s="2"/>
+      <c r="Z30" s="2">
+        <v>31.185429800652116</v>
+      </c>
       <c r="AA30" s="2">
         <v>198.89925821112618</v>
       </c>
@@ -3889,7 +4459,9 @@
       <c r="AE30" s="2">
         <v>26</v>
       </c>
-      <c r="AF30" s="2"/>
+      <c r="AF30" s="2">
+        <v>97.135576875997387</v>
+      </c>
       <c r="AG30" s="2">
         <v>109.55641331869832</v>
       </c>
@@ -3900,7 +4472,9 @@
       <c r="A31" s="2">
         <v>27</v>
       </c>
-      <c r="B31" s="2"/>
+      <c r="B31" s="2">
+        <v>0.54917702431992721</v>
+      </c>
       <c r="C31" s="2">
         <v>2.0995880716170108</v>
       </c>
@@ -3918,7 +4492,9 @@
       <c r="M31" s="2">
         <v>27</v>
       </c>
-      <c r="N31" s="2"/>
+      <c r="N31" s="2">
+        <v>2.6645352591003757E-15</v>
+      </c>
       <c r="O31" s="2">
         <v>4.7675297848696649</v>
       </c>
@@ -3927,7 +4503,9 @@
       <c r="S31" s="2">
         <v>27</v>
       </c>
-      <c r="T31" s="2"/>
+      <c r="T31" s="2">
+        <v>23.137284531158084</v>
+      </c>
       <c r="U31" s="2">
         <v>22.721295785868691</v>
       </c>
@@ -3936,7 +4514,9 @@
       <c r="Y31" s="2">
         <v>27</v>
       </c>
-      <c r="Z31" s="2"/>
+      <c r="Z31" s="2">
+        <v>32.083273313327204</v>
+      </c>
       <c r="AA31" s="2">
         <v>198.46279014601186</v>
       </c>
@@ -3945,7 +4525,9 @@
       <c r="AE31" s="2">
         <v>27</v>
       </c>
-      <c r="AF31" s="2"/>
+      <c r="AF31" s="2">
+        <v>92.344147249510357</v>
+      </c>
       <c r="AG31" s="2">
         <v>103.44817046418551</v>
       </c>
@@ -3956,7 +4538,9 @@
       <c r="A32" s="2">
         <v>28</v>
       </c>
-      <c r="B32" s="2"/>
+      <c r="B32" s="2">
+        <v>0.55785791160583931</v>
+      </c>
       <c r="C32" s="2">
         <v>2.2054085790808453</v>
       </c>
@@ -3974,7 +4558,9 @@
       <c r="M32" s="2">
         <v>28</v>
       </c>
-      <c r="N32" s="2"/>
+      <c r="N32" s="2">
+        <v>4.4408920985006262E-15</v>
+      </c>
       <c r="O32" s="2">
         <v>5.2579874748026674</v>
       </c>
@@ -3983,7 +4569,9 @@
       <c r="S32" s="2">
         <v>28</v>
       </c>
-      <c r="T32" s="2"/>
+      <c r="T32" s="2">
+        <v>21.357695363436314</v>
+      </c>
       <c r="U32" s="2">
         <v>21.463995271108104</v>
       </c>
@@ -3992,7 +4580,9 @@
       <c r="Y32" s="2">
         <v>28</v>
       </c>
-      <c r="Z32" s="2"/>
+      <c r="Z32" s="2">
+        <v>29.516174415188772</v>
+      </c>
       <c r="AA32" s="2">
         <v>201.60846263253529</v>
       </c>
@@ -4001,7 +4591,9 @@
       <c r="AE32" s="2">
         <v>28</v>
       </c>
-      <c r="AF32" s="2"/>
+      <c r="AF32" s="2">
+        <v>96.471843074972909</v>
+      </c>
       <c r="AG32" s="2">
         <v>105.48759724999562</v>
       </c>
@@ -4012,7 +4604,9 @@
       <c r="A33" s="2">
         <v>29</v>
       </c>
-      <c r="B33" s="2"/>
+      <c r="B33" s="2">
+        <v>0.57113913856434184</v>
+      </c>
       <c r="C33" s="2">
         <v>2.1553752240718347</v>
       </c>
@@ -4030,7 +4624,9 @@
       <c r="M33" s="2">
         <v>29</v>
       </c>
-      <c r="N33" s="2"/>
+      <c r="N33" s="2">
+        <v>1.7763568394002505E-15</v>
+      </c>
       <c r="O33" s="2">
         <v>11.841397821370636</v>
       </c>
@@ -4039,7 +4635,9 @@
       <c r="S33" s="2">
         <v>29</v>
       </c>
-      <c r="T33" s="2"/>
+      <c r="T33" s="2">
+        <v>20.548235587901921</v>
+      </c>
       <c r="U33" s="2">
         <v>22.757353908794084</v>
       </c>
@@ -4048,7 +4646,9 @@
       <c r="Y33" s="2">
         <v>29</v>
       </c>
-      <c r="Z33" s="2"/>
+      <c r="Z33" s="2">
+        <v>32.752777389746768</v>
+      </c>
       <c r="AA33" s="2">
         <v>206.22407315554497</v>
       </c>
@@ -4057,7 +4657,9 @@
       <c r="AE33" s="2">
         <v>29</v>
       </c>
-      <c r="AF33" s="2"/>
+      <c r="AF33" s="2">
+        <v>95.600660905130681</v>
+      </c>
       <c r="AG33" s="2">
         <v>102.89257973197172</v>
       </c>
@@ -4068,7 +4670,9 @@
       <c r="A34" s="2">
         <v>30</v>
       </c>
-      <c r="B34" s="2"/>
+      <c r="B34" s="2">
+        <v>0.67580912477168475</v>
+      </c>
       <c r="C34" s="2">
         <v>2.483397283609714</v>
       </c>
@@ -4086,7 +4690,9 @@
       <c r="M34" s="2">
         <v>30</v>
       </c>
-      <c r="N34" s="2"/>
+      <c r="N34" s="2">
+        <v>2.6645352591003757E-15</v>
+      </c>
       <c r="O34" s="2">
         <v>10.255152768080059</v>
       </c>
@@ -4095,7 +4701,9 @@
       <c r="S34" s="2">
         <v>30</v>
       </c>
-      <c r="T34" s="2"/>
+      <c r="T34" s="2">
+        <v>20.131368885718572</v>
+      </c>
       <c r="U34" s="2">
         <v>22.017175124018618</v>
       </c>
@@ -4104,7 +4712,9 @@
       <c r="Y34" s="2">
         <v>30</v>
       </c>
-      <c r="Z34" s="2"/>
+      <c r="Z34" s="2">
+        <v>32.508025350728609</v>
+      </c>
       <c r="AA34" s="2">
         <v>198.24188993153453</v>
       </c>
@@ -4113,7 +4723,9 @@
       <c r="AE34" s="2">
         <v>30</v>
       </c>
-      <c r="AF34" s="2"/>
+      <c r="AF34" s="2">
+        <v>93.915981342076222</v>
+      </c>
       <c r="AG34" s="2">
         <v>106.78690780920147</v>
       </c>

</xml_diff>

<commit_message>
Update results of Gradient Descent for oring, concrete dataset
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -61,8 +61,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -137,7 +138,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -148,6 +149,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -169,8 +174,8 @@
   </sheetPr>
   <dimension ref="A3:AI34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y6" activeCellId="0" sqref="Y6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -332,7 +337,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>3.18957089994984E+103</v>
+        <v>28.7502199064544</v>
       </c>
       <c r="I5" s="1" t="n">
         <v>34.8554825801643</v>
@@ -345,7 +350,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="1" t="n">
-        <v>0.000196768933948377</v>
+        <v>0.683775269185438</v>
       </c>
       <c r="O5" s="1" t="n">
         <v>25.371197018441</v>
@@ -412,7 +417,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>6.94826326748863E+204</v>
+        <v>27.7379710394112</v>
       </c>
       <c r="I6" s="1" t="n">
         <v>33.8417424988054</v>
@@ -425,7 +430,7 @@
         <v>2</v>
       </c>
       <c r="N6" s="1" t="n">
-        <v>1.47071057554626E-008</v>
+        <v>0.0754791347784796</v>
       </c>
       <c r="O6" s="1" t="n">
         <v>19.1993196418278</v>
@@ -492,7 +497,7 @@
         <v>3</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>1.50812935797495E+306</v>
+        <v>29.0883571456205</v>
       </c>
       <c r="I7" s="1" t="n">
         <v>32.4650874269739</v>
@@ -505,7 +510,7 @@
         <v>3</v>
       </c>
       <c r="N7" s="1" t="n">
-        <v>1.50812695665081E-012</v>
+        <v>0.0191422014380791</v>
       </c>
       <c r="O7" s="1" t="n">
         <v>23.0743868645129</v>
@@ -571,7 +576,9 @@
       <c r="G8" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1" t="n">
+        <v>28.1587920798967</v>
+      </c>
       <c r="I8" s="1" t="n">
         <v>35.4604990057834</v>
       </c>
@@ -583,7 +590,7 @@
         <v>4</v>
       </c>
       <c r="N8" s="1" t="n">
-        <v>7.105427357601E-015</v>
+        <v>0.00412492597107317</v>
       </c>
       <c r="O8" s="1" t="n">
         <v>17.7085313937069</v>
@@ -649,7 +656,9 @@
       <c r="G9" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1" t="n">
+        <v>29.7983011122313</v>
+      </c>
       <c r="I9" s="1" t="n">
         <v>33.4531293144243</v>
       </c>
@@ -661,7 +670,7 @@
         <v>5</v>
       </c>
       <c r="N9" s="1" t="n">
-        <v>1.15463194561016E-014</v>
+        <v>0.000810118408143268</v>
       </c>
       <c r="O9" s="1" t="n">
         <v>20.9122936494444</v>
@@ -727,7 +736,9 @@
       <c r="G10" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1" t="n">
+        <v>30.2796926792741</v>
+      </c>
       <c r="I10" s="1" t="n">
         <v>34.1249267907759</v>
       </c>
@@ -739,7 +750,7 @@
         <v>6</v>
       </c>
       <c r="N10" s="1" t="n">
-        <v>7.105427357601E-015</v>
+        <v>0.000183121113486173</v>
       </c>
       <c r="O10" s="1" t="n">
         <v>20.0488627980866</v>
@@ -805,7 +816,9 @@
       <c r="G11" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1" t="n">
+        <v>30.2541813576962</v>
+      </c>
       <c r="I11" s="1" t="n">
         <v>36.1718142832101</v>
       </c>
@@ -816,8 +829,8 @@
       <c r="M11" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="N11" s="1" t="n">
-        <v>1.33226762955019E-014</v>
+      <c r="N11" s="3" t="n">
+        <v>3.82182597142844E-005</v>
       </c>
       <c r="O11" s="1" t="n">
         <v>25.5848469604473</v>
@@ -883,7 +896,9 @@
       <c r="G12" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1" t="n">
+        <v>30.8576932721133</v>
+      </c>
       <c r="I12" s="1" t="n">
         <v>34.2425743769675</v>
       </c>
@@ -894,8 +909,8 @@
       <c r="M12" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="N12" s="1" t="n">
-        <v>1.24344978758018E-014</v>
+      <c r="N12" s="3" t="n">
+        <v>8.15631812667306E-006</v>
       </c>
       <c r="O12" s="1" t="n">
         <v>22.1710379466057</v>
@@ -961,7 +976,9 @@
       <c r="G13" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="H13" s="1"/>
+      <c r="H13" s="1" t="n">
+        <v>29.8724775886003</v>
+      </c>
       <c r="I13" s="1" t="n">
         <v>35.5298328292365</v>
       </c>
@@ -972,8 +989,8 @@
       <c r="M13" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="N13" s="1" t="n">
-        <v>1.24344978758018E-014</v>
+      <c r="N13" s="3" t="n">
+        <v>1.88356080688123E-006</v>
       </c>
       <c r="O13" s="1" t="n">
         <v>25.0133463129374</v>
@@ -1039,7 +1056,9 @@
       <c r="G14" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="H14" s="1"/>
+      <c r="H14" s="1" t="n">
+        <v>29.0291828604987</v>
+      </c>
       <c r="I14" s="1" t="n">
         <v>33.8572340334971</v>
       </c>
@@ -1050,8 +1069,8 @@
       <c r="M14" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="N14" s="1" t="n">
-        <v>1.33226762955019E-014</v>
+      <c r="N14" s="3" t="n">
+        <v>3.90604867561706E-007</v>
       </c>
       <c r="O14" s="1" t="n">
         <v>22.7020454935598</v>
@@ -1117,7 +1136,9 @@
       <c r="G15" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="H15" s="1"/>
+      <c r="H15" s="1" t="n">
+        <v>29.345917666297</v>
+      </c>
       <c r="I15" s="1" t="n">
         <v>33.968154030632</v>
       </c>
@@ -1128,8 +1149,8 @@
       <c r="M15" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="N15" s="1" t="n">
-        <v>1.33226762955019E-014</v>
+      <c r="N15" s="3" t="n">
+        <v>7.9968856425694E-008</v>
       </c>
       <c r="O15" s="1" t="n">
         <v>22.0334829877019</v>
@@ -1195,7 +1216,9 @@
       <c r="G16" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1" t="n">
+        <v>30.3423174912047</v>
+      </c>
       <c r="I16" s="1" t="n">
         <v>35.2197562038388</v>
       </c>
@@ -1206,8 +1229,8 @@
       <c r="M16" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="N16" s="1" t="n">
-        <v>7.99360577730113E-015</v>
+      <c r="N16" s="3" t="n">
+        <v>1.6677090819428E-008</v>
       </c>
       <c r="O16" s="1" t="n">
         <v>21.4527200650047</v>
@@ -1273,7 +1296,9 @@
       <c r="G17" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="H17" s="1"/>
+      <c r="H17" s="1" t="n">
+        <v>28.8366993340129</v>
+      </c>
       <c r="I17" s="1" t="n">
         <v>34.1974874200327</v>
       </c>
@@ -1284,8 +1309,8 @@
       <c r="M17" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="N17" s="1" t="n">
-        <v>1.33226762955019E-014</v>
+      <c r="N17" s="3" t="n">
+        <v>4.12143386085972E-009</v>
       </c>
       <c r="O17" s="1" t="n">
         <v>24.2845148602922</v>
@@ -1351,7 +1376,9 @@
       <c r="G18" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="H18" s="1"/>
+      <c r="H18" s="1" t="n">
+        <v>29.715606669602</v>
+      </c>
       <c r="I18" s="1" t="n">
         <v>34.5343235136225</v>
       </c>
@@ -1362,8 +1389,8 @@
       <c r="M18" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="N18" s="1" t="n">
-        <v>1.24344978758018E-014</v>
+      <c r="N18" s="3" t="n">
+        <v>7.47130357581227E-010</v>
       </c>
       <c r="O18" s="1" t="n">
         <v>25.8914135860646</v>
@@ -1429,7 +1456,9 @@
       <c r="G19" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="H19" s="1"/>
+      <c r="H19" s="1" t="n">
+        <v>30.0026568334558</v>
+      </c>
       <c r="I19" s="1" t="n">
         <v>34.6653930282756</v>
       </c>
@@ -1440,8 +1469,8 @@
       <c r="M19" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="N19" s="1" t="n">
-        <v>1.15463194561016E-014</v>
+      <c r="N19" s="3" t="n">
+        <v>1.7809487218301E-010</v>
       </c>
       <c r="O19" s="1" t="n">
         <v>22.5076399342915</v>
@@ -1507,7 +1536,9 @@
       <c r="G20" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="H20" s="1"/>
+      <c r="H20" s="1" t="n">
+        <v>30.0667090245848</v>
+      </c>
       <c r="I20" s="1" t="n">
         <v>34.2353514587332</v>
       </c>
@@ -1518,8 +1549,8 @@
       <c r="M20" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="N20" s="1" t="n">
-        <v>9.76996261670138E-015</v>
+      <c r="N20" s="3" t="n">
+        <v>3.82485154659662E-011</v>
       </c>
       <c r="O20" s="1" t="n">
         <v>24.707347173049</v>
@@ -1585,7 +1616,9 @@
       <c r="G21" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="H21" s="1"/>
+      <c r="H21" s="1" t="n">
+        <v>30.2521803654474</v>
+      </c>
       <c r="I21" s="1" t="n">
         <v>35.0688671810033</v>
       </c>
@@ -1596,8 +1629,8 @@
       <c r="M21" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="N21" s="1" t="n">
-        <v>1.24344978758018E-014</v>
+      <c r="N21" s="3" t="n">
+        <v>7.49977857594786E-012</v>
       </c>
       <c r="O21" s="1" t="n">
         <v>19.9796925947625</v>
@@ -1663,7 +1696,9 @@
       <c r="G22" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="H22" s="1"/>
+      <c r="H22" s="1" t="n">
+        <v>30.1877102265675</v>
+      </c>
       <c r="I22" s="1" t="n">
         <v>35.1875366164269</v>
       </c>
@@ -1674,8 +1709,8 @@
       <c r="M22" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="N22" s="1" t="n">
-        <v>1.15463194561016E-014</v>
+      <c r="N22" s="3" t="n">
+        <v>1.59783297704053E-012</v>
       </c>
       <c r="O22" s="1" t="n">
         <v>22.5982308625973</v>
@@ -1741,7 +1776,9 @@
       <c r="G23" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="H23" s="1"/>
+      <c r="H23" s="1" t="n">
+        <v>28.5642747144664</v>
+      </c>
       <c r="I23" s="1" t="n">
         <v>35.4622261840293</v>
       </c>
@@ -1752,8 +1789,8 @@
       <c r="M23" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="N23" s="1" t="n">
-        <v>6.21724893790088E-015</v>
+      <c r="N23" s="3" t="n">
+        <v>4.9560355819267E-013</v>
       </c>
       <c r="O23" s="1" t="n">
         <v>25.1315089560829</v>
@@ -1819,7 +1856,9 @@
       <c r="G24" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="H24" s="1"/>
+      <c r="H24" s="1" t="n">
+        <v>29.6216439791358</v>
+      </c>
       <c r="I24" s="1" t="n">
         <v>35.947208224593</v>
       </c>
@@ -1830,8 +1869,8 @@
       <c r="M24" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="N24" s="1" t="n">
-        <v>5.32907051820075E-015</v>
+      <c r="N24" s="3" t="n">
+        <v>2.73558953267639E-013</v>
       </c>
       <c r="O24" s="1" t="n">
         <v>24.2484226559774</v>
@@ -1897,7 +1936,9 @@
       <c r="G25" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="H25" s="1"/>
+      <c r="H25" s="1" t="n">
+        <v>29.6530372129567</v>
+      </c>
       <c r="I25" s="1" t="n">
         <v>34.4108797884256</v>
       </c>
@@ -1908,8 +1949,8 @@
       <c r="M25" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="N25" s="1" t="n">
-        <v>1.24344978758018E-014</v>
+      <c r="N25" s="3" t="n">
+        <v>2.26485497023532E-013</v>
       </c>
       <c r="O25" s="1" t="n">
         <v>20.2278918741496</v>
@@ -1975,7 +2016,9 @@
       <c r="G26" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="H26" s="1"/>
+      <c r="H26" s="1" t="n">
+        <v>29.7613094675712</v>
+      </c>
       <c r="I26" s="1" t="n">
         <v>35.3213147442848</v>
       </c>
@@ -1986,8 +2029,8 @@
       <c r="M26" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="N26" s="1" t="n">
-        <v>1.33226762955019E-014</v>
+      <c r="N26" s="3" t="n">
+        <v>2.06057393370429E-013</v>
       </c>
       <c r="O26" s="1" t="n">
         <v>20.9701913726153</v>
@@ -2053,7 +2096,9 @@
       <c r="G27" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="H27" s="1"/>
+      <c r="H27" s="1" t="n">
+        <v>29.5541901787599</v>
+      </c>
       <c r="I27" s="1" t="n">
         <v>34.3480095058536</v>
       </c>
@@ -2064,8 +2109,8 @@
       <c r="M27" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="N27" s="1" t="n">
-        <v>1.06581410364015E-014</v>
+      <c r="N27" s="3" t="n">
+        <v>2.20268248085631E-013</v>
       </c>
       <c r="O27" s="1" t="n">
         <v>23.7337886223427</v>
@@ -2131,7 +2176,9 @@
       <c r="G28" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="H28" s="1"/>
+      <c r="H28" s="1" t="n">
+        <v>29.1730661578799</v>
+      </c>
       <c r="I28" s="1" t="n">
         <v>34.4748268551547</v>
       </c>
@@ -2142,8 +2189,8 @@
       <c r="M28" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="N28" s="1" t="n">
-        <v>1.24344978758018E-014</v>
+      <c r="N28" s="3" t="n">
+        <v>2.16715534406831E-013</v>
       </c>
       <c r="O28" s="1" t="n">
         <v>20.4610814381992</v>
@@ -2209,7 +2256,9 @@
       <c r="G29" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="H29" s="1"/>
+      <c r="H29" s="1" t="n">
+        <v>29.4309417509426</v>
+      </c>
       <c r="I29" s="1" t="n">
         <v>33.9131388982046</v>
       </c>
@@ -2220,8 +2269,8 @@
       <c r="M29" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="N29" s="1" t="n">
-        <v>1.06581410364015E-014</v>
+      <c r="N29" s="3" t="n">
+        <v>2.24709140184132E-013</v>
       </c>
       <c r="O29" s="1" t="n">
         <v>19.559688451556</v>
@@ -2287,7 +2336,9 @@
       <c r="G30" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="H30" s="1"/>
+      <c r="H30" s="1" t="n">
+        <v>30.094744245254</v>
+      </c>
       <c r="I30" s="1" t="n">
         <v>34.7557694386958</v>
       </c>
@@ -2298,8 +2349,8 @@
       <c r="M30" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="N30" s="1" t="n">
-        <v>1.24344978758018E-014</v>
+      <c r="N30" s="3" t="n">
+        <v>1.98951966012828E-013</v>
       </c>
       <c r="O30" s="1" t="n">
         <v>24.4744641965594</v>
@@ -2365,7 +2416,9 @@
       <c r="G31" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="H31" s="1"/>
+      <c r="H31" s="1" t="n">
+        <v>29.6558143729426</v>
+      </c>
       <c r="I31" s="1" t="n">
         <v>34.5109314671724</v>
       </c>
@@ -2376,8 +2429,8 @@
       <c r="M31" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="N31" s="1" t="n">
-        <v>1.15463194561016E-014</v>
+      <c r="N31" s="3" t="n">
+        <v>2.1405099914773E-013</v>
       </c>
       <c r="O31" s="1" t="n">
         <v>24.3470559435627</v>
@@ -2443,7 +2496,9 @@
       <c r="G32" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="H32" s="1"/>
+      <c r="H32" s="1" t="n">
+        <v>29.4844096757333</v>
+      </c>
       <c r="I32" s="1" t="n">
         <v>35.0137690559623</v>
       </c>
@@ -2454,8 +2509,8 @@
       <c r="M32" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="N32" s="1" t="n">
-        <v>1.06581410364015E-014</v>
+      <c r="N32" s="3" t="n">
+        <v>2.05169214950729E-013</v>
       </c>
       <c r="O32" s="1" t="n">
         <v>23.8953978235021</v>
@@ -2521,7 +2576,9 @@
       <c r="G33" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="H33" s="1"/>
+      <c r="H33" s="1" t="n">
+        <v>29.8039560314033</v>
+      </c>
       <c r="I33" s="1" t="n">
         <v>34.862596235722</v>
       </c>
@@ -2532,8 +2589,8 @@
       <c r="M33" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="N33" s="1" t="n">
-        <v>6.21724893790088E-015</v>
+      <c r="N33" s="3" t="n">
+        <v>2.22044604925031E-013</v>
       </c>
       <c r="O33" s="1" t="n">
         <v>18.3310554019384</v>
@@ -2599,7 +2656,9 @@
       <c r="G34" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="H34" s="1"/>
+      <c r="H34" s="1" t="n">
+        <v>28.6471187932084</v>
+      </c>
       <c r="I34" s="1" t="n">
         <v>35.2360195900296</v>
       </c>
@@ -2610,8 +2669,8 @@
       <c r="M34" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="N34" s="1" t="n">
-        <v>5.32907051820075E-015</v>
+      <c r="N34" s="3" t="n">
+        <v>2.04281036531029E-013</v>
       </c>
       <c r="O34" s="1" t="n">
         <v>20.1209404187791</v>
@@ -2686,8 +2745,8 @@
   </sheetPr>
   <dimension ref="A3:AI34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AH5" activeCellId="1" sqref="Y6 AH5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N23" activeCellId="0" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2849,7 +2908,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>8.19229951690228E+102</v>
+        <v>7.85099296157476</v>
       </c>
       <c r="I5" s="1" t="n">
         <v>8.3318691318503</v>
@@ -2862,7 +2921,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="1" t="n">
-        <v>1.64112276284101E-005</v>
+        <v>0.0698297677761</v>
       </c>
       <c r="O5" s="1" t="n">
         <v>4.71437682598315</v>
@@ -2911,7 +2970,7 @@
       </c>
       <c r="AI5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>2</v>
       </c>
@@ -2929,7 +2988,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>1.74897075717899E+204</v>
+        <v>8.59487820222737</v>
       </c>
       <c r="I6" s="1" t="n">
         <v>9.9055743149702</v>
@@ -2942,7 +3001,7 @@
         <v>2</v>
       </c>
       <c r="N6" s="1" t="n">
-        <v>4.47383818880098E-009</v>
+        <v>0.0395742304616809</v>
       </c>
       <c r="O6" s="1" t="n">
         <v>9.41242255660137</v>
@@ -2991,7 +3050,7 @@
       </c>
       <c r="AI6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>3</v>
       </c>
@@ -3009,7 +3068,7 @@
         <v>3</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>3.78766062357267E+305</v>
+        <v>7.30210105256202</v>
       </c>
       <c r="I7" s="1" t="n">
         <v>10.7243457883257</v>
@@ -3022,7 +3081,7 @@
         <v>3</v>
       </c>
       <c r="N7" s="1" t="n">
-        <v>2.19380069665931E-013</v>
+        <v>0.00415413238048856</v>
       </c>
       <c r="O7" s="1" t="n">
         <v>6.62185199525127</v>
@@ -3071,7 +3130,7 @@
       </c>
       <c r="AI7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>4</v>
       </c>
@@ -3088,7 +3147,9 @@
       <c r="G8" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1" t="n">
+        <v>8.32918925696465</v>
+      </c>
       <c r="I8" s="1" t="n">
         <v>8.14049034728243</v>
       </c>
@@ -3100,7 +3161,7 @@
         <v>4</v>
       </c>
       <c r="N8" s="1" t="n">
-        <v>8.88178419700125E-016</v>
+        <v>0.000772699850613456</v>
       </c>
       <c r="O8" s="1" t="n">
         <v>11.0552724612042</v>
@@ -3149,7 +3210,7 @@
       </c>
       <c r="AI8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>5</v>
       </c>
@@ -3166,7 +3227,9 @@
       <c r="G9" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1" t="n">
+        <v>6.76573561029311</v>
+      </c>
       <c r="I9" s="1" t="n">
         <v>9.65254972323569</v>
       </c>
@@ -3178,7 +3241,7 @@
         <v>5</v>
       </c>
       <c r="N9" s="1" t="n">
-        <v>2.66453525910038E-015</v>
+        <v>0.00022887748046152</v>
       </c>
       <c r="O9" s="1" t="n">
         <v>7.99666238200577</v>
@@ -3227,7 +3290,7 @@
       </c>
       <c r="AI9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>6</v>
       </c>
@@ -3244,7 +3307,9 @@
       <c r="G10" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1" t="n">
+        <v>6.3450001861118</v>
+      </c>
       <c r="I10" s="1" t="n">
         <v>9.5431094062838</v>
       </c>
@@ -3255,8 +3320,8 @@
       <c r="M10" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="N10" s="1" t="n">
-        <v>8.88178419700125E-016</v>
+      <c r="N10" s="3" t="n">
+        <v>3.79001378023602E-005</v>
       </c>
       <c r="O10" s="1" t="n">
         <v>8.54044597243349</v>
@@ -3305,7 +3370,7 @@
       </c>
       <c r="AI10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>7</v>
       </c>
@@ -3322,7 +3387,9 @@
       <c r="G11" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1" t="n">
+        <v>6.41770641164737</v>
+      </c>
       <c r="I11" s="1" t="n">
         <v>7.97944033383945</v>
       </c>
@@ -3333,8 +3400,8 @@
       <c r="M11" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="N11" s="1" t="n">
-        <v>8.88178419700125E-016</v>
+      <c r="N11" s="3" t="n">
+        <v>8.83752065750088E-006</v>
       </c>
       <c r="O11" s="1" t="n">
         <v>3.25034558912472</v>
@@ -3383,7 +3450,7 @@
       </c>
       <c r="AI11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>8</v>
       </c>
@@ -3400,7 +3467,9 @@
       <c r="G12" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1" t="n">
+        <v>5.84779194758769</v>
+      </c>
       <c r="I12" s="1" t="n">
         <v>9.32935018516199</v>
       </c>
@@ -3411,8 +3480,8 @@
       <c r="M12" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="N12" s="1" t="n">
-        <v>8.88178419700125E-016</v>
+      <c r="N12" s="3" t="n">
+        <v>1.86441844007845E-006</v>
       </c>
       <c r="O12" s="1" t="n">
         <v>7.1672572560075</v>
@@ -3461,7 +3530,7 @@
       </c>
       <c r="AI12" s="1"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>9</v>
       </c>
@@ -3478,7 +3547,9 @@
       <c r="G13" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="H13" s="1"/>
+      <c r="H13" s="1" t="n">
+        <v>6.85643416313127</v>
+      </c>
       <c r="I13" s="1" t="n">
         <v>8.70887912290166</v>
       </c>
@@ -3489,8 +3560,8 @@
       <c r="M13" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="N13" s="1" t="n">
-        <v>1.77635683940025E-015</v>
+      <c r="N13" s="3" t="n">
+        <v>2.50558188419348E-007</v>
       </c>
       <c r="O13" s="1" t="n">
         <v>4.67505880160087</v>
@@ -3539,7 +3610,7 @@
       </c>
       <c r="AI13" s="1"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>10</v>
       </c>
@@ -3556,7 +3627,9 @@
       <c r="G14" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="H14" s="1"/>
+      <c r="H14" s="1" t="n">
+        <v>7.71568112084078</v>
+      </c>
       <c r="I14" s="1" t="n">
         <v>9.14048757161958</v>
       </c>
@@ -3567,8 +3640,8 @@
       <c r="M14" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="N14" s="1" t="n">
-        <v>2.66453525910038E-015</v>
+      <c r="N14" s="3" t="n">
+        <v>6.39091846110773E-008</v>
       </c>
       <c r="O14" s="1" t="n">
         <v>7.76826410719756</v>
@@ -3617,7 +3690,7 @@
       </c>
       <c r="AI14" s="1"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>11</v>
       </c>
@@ -3634,7 +3707,9 @@
       <c r="G15" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="H15" s="1"/>
+      <c r="H15" s="1" t="n">
+        <v>7.40979235582417</v>
+      </c>
       <c r="I15" s="1" t="n">
         <v>9.30598091500411</v>
       </c>
@@ -3645,8 +3720,8 @@
       <c r="M15" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="N15" s="1" t="n">
-        <v>8.88178419700125E-016</v>
+      <c r="N15" s="3" t="n">
+        <v>1.68319420623675E-008</v>
       </c>
       <c r="O15" s="1" t="n">
         <v>7.86173588416561</v>
@@ -3695,7 +3770,7 @@
       </c>
       <c r="AI15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>12</v>
       </c>
@@ -3712,7 +3787,9 @@
       <c r="G16" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1" t="n">
+        <v>6.42090415100838</v>
+      </c>
       <c r="I16" s="1" t="n">
         <v>8.38881870586488</v>
       </c>
@@ -3723,8 +3800,8 @@
       <c r="M16" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="N16" s="1" t="n">
-        <v>0</v>
+      <c r="N16" s="3" t="n">
+        <v>3.93924270980506E-009</v>
       </c>
       <c r="O16" s="1" t="n">
         <v>7.25214098447091</v>
@@ -3773,7 +3850,7 @@
       </c>
       <c r="AI16" s="1"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>13</v>
       </c>
@@ -3790,7 +3867,9 @@
       <c r="G17" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="H17" s="1"/>
+      <c r="H17" s="1" t="n">
+        <v>7.93161617937519</v>
+      </c>
       <c r="I17" s="1" t="n">
         <v>8.93475577018844</v>
       </c>
@@ -3801,8 +3880,8 @@
       <c r="M17" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="N17" s="1" t="n">
-        <v>8.88178419700125E-016</v>
+      <c r="N17" s="3" t="n">
+        <v>2.6937829744611E-010</v>
       </c>
       <c r="O17" s="1" t="n">
         <v>4.86307193215853</v>
@@ -3851,7 +3930,7 @@
       </c>
       <c r="AI17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>14</v>
       </c>
@@ -3868,7 +3947,9 @@
       <c r="G18" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="H18" s="1"/>
+      <c r="H18" s="1" t="n">
+        <v>7.05616305824105</v>
+      </c>
       <c r="I18" s="1" t="n">
         <v>8.77141625316695</v>
       </c>
@@ -3879,8 +3960,8 @@
       <c r="M18" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="N18" s="1" t="n">
-        <v>2.66453525910038E-015</v>
+      <c r="N18" s="3" t="n">
+        <v>1.88010496060542E-010</v>
       </c>
       <c r="O18" s="1" t="n">
         <v>3.53881775358664</v>
@@ -3929,7 +4010,7 @@
       </c>
       <c r="AI18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>15</v>
       </c>
@@ -3946,7 +4027,9 @@
       <c r="G19" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="H19" s="1"/>
+      <c r="H19" s="1" t="n">
+        <v>6.77145494106795</v>
+      </c>
       <c r="I19" s="1" t="n">
         <v>8.6695442507979</v>
       </c>
@@ -3957,8 +4040,8 @@
       <c r="M19" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="N19" s="1" t="n">
-        <v>2.66453525910038E-015</v>
+      <c r="N19" s="3" t="n">
+        <v>2.10960138247174E-011</v>
       </c>
       <c r="O19" s="1" t="n">
         <v>7.02228611333286</v>
@@ -4007,7 +4090,7 @@
       </c>
       <c r="AI19" s="1"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>16</v>
       </c>
@@ -4024,7 +4107,9 @@
       <c r="G20" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="H20" s="1"/>
+      <c r="H20" s="1" t="n">
+        <v>6.70899043951548</v>
+      </c>
       <c r="I20" s="1" t="n">
         <v>8.83722540966896</v>
       </c>
@@ -4035,8 +4120,8 @@
       <c r="M20" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="N20" s="1" t="n">
-        <v>3.5527136788005E-015</v>
+      <c r="N20" s="3" t="n">
+        <v>4.19220214098459E-012</v>
       </c>
       <c r="O20" s="1" t="n">
         <v>4.91555783353421</v>
@@ -4085,7 +4170,7 @@
       </c>
       <c r="AI20" s="1"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>17</v>
       </c>
@@ -4102,7 +4187,9 @@
       <c r="G21" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="H21" s="1"/>
+      <c r="H21" s="1" t="n">
+        <v>6.52459519386047</v>
+      </c>
       <c r="I21" s="1" t="n">
         <v>8.60635931594838</v>
       </c>
@@ -4113,8 +4200,8 @@
       <c r="M21" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="N21" s="1" t="n">
-        <v>1.77635683940025E-015</v>
+      <c r="N21" s="3" t="n">
+        <v>1.55253587763582E-012</v>
       </c>
       <c r="O21" s="1" t="n">
         <v>8.81478449545319</v>
@@ -4163,7 +4250,7 @@
       </c>
       <c r="AI21" s="1"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>18</v>
       </c>
@@ -4180,7 +4267,9 @@
       <c r="G22" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="H22" s="1"/>
+      <c r="H22" s="1" t="n">
+        <v>6.58979453716593</v>
+      </c>
       <c r="I22" s="1" t="n">
         <v>9.72196413455355</v>
       </c>
@@ -4191,8 +4280,8 @@
       <c r="M22" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="N22" s="1" t="n">
-        <v>2.66453525910038E-015</v>
+      <c r="N22" s="3" t="n">
+        <v>3.5615954629975E-013</v>
       </c>
       <c r="O22" s="1" t="n">
         <v>6.62939618775199</v>
@@ -4241,7 +4330,7 @@
       </c>
       <c r="AI22" s="1"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>19</v>
       </c>
@@ -4258,7 +4347,9 @@
       <c r="G23" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="H23" s="1"/>
+      <c r="H23" s="1" t="n">
+        <v>8.21372409126069</v>
+      </c>
       <c r="I23" s="1" t="n">
         <v>7.99455265783832</v>
       </c>
@@ -4269,8 +4360,8 @@
       <c r="M23" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="N23" s="1" t="n">
-        <v>1.77635683940025E-015</v>
+      <c r="N23" s="3" t="n">
+        <v>3.64153152077051E-014</v>
       </c>
       <c r="O23" s="1" t="n">
         <v>3.75556060907889</v>
@@ -4319,7 +4410,7 @@
       </c>
       <c r="AI23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>20</v>
       </c>
@@ -4336,7 +4427,9 @@
       <c r="G24" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="H24" s="1"/>
+      <c r="H24" s="1" t="n">
+        <v>7.15668948291234</v>
+      </c>
       <c r="I24" s="1" t="n">
         <v>8.08366994456777</v>
       </c>
@@ -4347,8 +4440,8 @@
       <c r="M24" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="N24" s="1" t="n">
-        <v>2.66453525910038E-015</v>
+      <c r="N24" s="3" t="n">
+        <v>3.5527136788005E-014</v>
       </c>
       <c r="O24" s="1" t="n">
         <v>5.50369278205278</v>
@@ -4397,7 +4490,7 @@
       </c>
       <c r="AI24" s="1"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>21</v>
       </c>
@@ -4414,7 +4507,9 @@
       <c r="G25" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="H25" s="1"/>
+      <c r="H25" s="1" t="n">
+        <v>7.12552290155244</v>
+      </c>
       <c r="I25" s="1" t="n">
         <v>8.83082745302191</v>
       </c>
@@ -4425,8 +4520,8 @@
       <c r="M25" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="N25" s="1" t="n">
-        <v>8.88178419700125E-016</v>
+      <c r="N25" s="3" t="n">
+        <v>4.35207425653061E-014</v>
       </c>
       <c r="O25" s="1" t="n">
         <v>8.42338509143297</v>
@@ -4475,7 +4570,7 @@
       </c>
       <c r="AI25" s="1"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>22</v>
       </c>
@@ -4492,7 +4587,9 @@
       <c r="G26" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="H26" s="1"/>
+      <c r="H26" s="1" t="n">
+        <v>7.01740412774648</v>
+      </c>
       <c r="I26" s="1" t="n">
         <v>8.41059127270219</v>
       </c>
@@ -4503,8 +4600,8 @@
       <c r="M26" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="N26" s="1" t="n">
-        <v>8.88178419700125E-016</v>
+      <c r="N26" s="3" t="n">
+        <v>6.21724893790088E-014</v>
       </c>
       <c r="O26" s="1" t="n">
         <v>9.95001086765139</v>
@@ -4553,7 +4650,7 @@
       </c>
       <c r="AI26" s="1"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>23</v>
       </c>
@@ -4570,7 +4667,9 @@
       <c r="G27" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="H27" s="1"/>
+      <c r="H27" s="1" t="n">
+        <v>7.22462733339215</v>
+      </c>
       <c r="I27" s="1" t="n">
         <v>8.41416792036189</v>
       </c>
@@ -4581,8 +4680,8 @@
       <c r="M27" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="N27" s="1" t="n">
-        <v>2.66453525910038E-015</v>
+      <c r="N27" s="3" t="n">
+        <v>4.35207425653061E-014</v>
       </c>
       <c r="O27" s="1" t="n">
         <v>5.87173694004464</v>
@@ -4631,7 +4730,7 @@
       </c>
       <c r="AI27" s="1"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>24</v>
       </c>
@@ -4648,7 +4747,9 @@
       <c r="G28" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="H28" s="1"/>
+      <c r="H28" s="1" t="n">
+        <v>7.60582170387278</v>
+      </c>
       <c r="I28" s="1" t="n">
         <v>9.38024306412108</v>
       </c>
@@ -4659,8 +4760,8 @@
       <c r="M28" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="N28" s="1" t="n">
-        <v>1.77635683940025E-015</v>
+      <c r="N28" s="3" t="n">
+        <v>4.08562073062058E-014</v>
       </c>
       <c r="O28" s="1" t="n">
         <v>9.02658986457804</v>
@@ -4709,7 +4810,7 @@
       </c>
       <c r="AI28" s="1"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <v>25</v>
       </c>
@@ -4726,7 +4827,9 @@
       <c r="G29" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="H29" s="1"/>
+      <c r="H29" s="1" t="n">
+        <v>7.34799373050521</v>
+      </c>
       <c r="I29" s="1" t="n">
         <v>9.07053112554702</v>
       </c>
@@ -4737,8 +4840,8 @@
       <c r="M29" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="N29" s="1" t="n">
-        <v>3.5527136788005E-015</v>
+      <c r="N29" s="3" t="n">
+        <v>3.28626015289046E-014</v>
       </c>
       <c r="O29" s="1" t="n">
         <v>11.4697233823357</v>
@@ -4787,7 +4890,7 @@
       </c>
       <c r="AI29" s="1"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
         <v>26</v>
       </c>
@@ -4804,7 +4907,9 @@
       <c r="G30" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="H30" s="1"/>
+      <c r="H30" s="1" t="n">
+        <v>6.68422346659954</v>
+      </c>
       <c r="I30" s="1" t="n">
         <v>9.06318935254107</v>
       </c>
@@ -4815,8 +4920,8 @@
       <c r="M30" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="N30" s="1" t="n">
-        <v>1.77635683940025E-015</v>
+      <c r="N30" s="3" t="n">
+        <v>5.95079541199084E-014</v>
       </c>
       <c r="O30" s="1" t="n">
         <v>4.81664693591062</v>
@@ -4865,7 +4970,7 @@
       </c>
       <c r="AI30" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <v>27</v>
       </c>
@@ -4882,7 +4987,9 @@
       <c r="G31" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="H31" s="1"/>
+      <c r="H31" s="1" t="n">
+        <v>7.12317515132057</v>
+      </c>
       <c r="I31" s="1" t="n">
         <v>9.03673287957944</v>
       </c>
@@ -4893,8 +5000,8 @@
       <c r="M31" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="N31" s="1" t="n">
-        <v>2.66453525910038E-015</v>
+      <c r="N31" s="3" t="n">
+        <v>4.52970994047064E-014</v>
       </c>
       <c r="O31" s="1" t="n">
         <v>4.76752978486967</v>
@@ -4943,7 +5050,7 @@
       </c>
       <c r="AI31" s="1"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>28</v>
       </c>
@@ -4960,7 +5067,9 @@
       <c r="G32" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="H32" s="1"/>
+      <c r="H32" s="1" t="n">
+        <v>7.29459460914134</v>
+      </c>
       <c r="I32" s="1" t="n">
         <v>8.42732730679915</v>
       </c>
@@ -4971,8 +5080,8 @@
       <c r="M32" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="N32" s="1" t="n">
-        <v>4.44089209850063E-015</v>
+      <c r="N32" s="3" t="n">
+        <v>5.24025267623074E-014</v>
       </c>
       <c r="O32" s="1" t="n">
         <v>5.25798747480267</v>
@@ -5021,7 +5130,7 @@
       </c>
       <c r="AI32" s="1"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <v>29</v>
       </c>
@@ -5038,7 +5147,9 @@
       <c r="G33" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="H33" s="1"/>
+      <c r="H33" s="1" t="n">
+        <v>6.97505824131199</v>
+      </c>
       <c r="I33" s="1" t="n">
         <v>9.03998949351199</v>
       </c>
@@ -5049,8 +5160,8 @@
       <c r="M33" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="N33" s="1" t="n">
-        <v>1.77635683940025E-015</v>
+      <c r="N33" s="3" t="n">
+        <v>3.64153152077051E-014</v>
       </c>
       <c r="O33" s="1" t="n">
         <v>11.8413978213706</v>
@@ -5099,7 +5210,7 @@
       </c>
       <c r="AI33" s="1"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>30</v>
       </c>
@@ -5116,7 +5227,9 @@
       <c r="G34" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="H34" s="1"/>
+      <c r="H34" s="1" t="n">
+        <v>8.13190223736056</v>
+      </c>
       <c r="I34" s="1" t="n">
         <v>8.48947813852812</v>
       </c>
@@ -5127,8 +5240,8 @@
       <c r="M34" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="N34" s="1" t="n">
-        <v>2.66453525910038E-015</v>
+      <c r="N34" s="3" t="n">
+        <v>5.41788836017076E-014</v>
       </c>
       <c r="O34" s="1" t="n">
         <v>10.2551527680801</v>
@@ -5204,7 +5317,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="Y6 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Generate results of fireworks
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -174,13 +174,13 @@
   </sheetPr>
   <dimension ref="A3:AI34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AD20" activeCellId="0" sqref="AD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -332,7 +332,9 @@
       <c r="D5" s="1" t="n">
         <v>2.11432962548098</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="n">
+        <v>16.5030848698092</v>
+      </c>
       <c r="G5" s="1" t="n">
         <v>1</v>
       </c>
@@ -345,7 +347,9 @@
       <c r="J5" s="1" t="n">
         <v>30.2889633398914</v>
       </c>
-      <c r="K5" s="1"/>
+      <c r="K5" s="1" t="n">
+        <v>42.0063935101198</v>
+      </c>
       <c r="M5" s="1" t="n">
         <v>1</v>
       </c>
@@ -358,7 +362,9 @@
       <c r="P5" s="1" t="n">
         <v>0.0329999483896595</v>
       </c>
-      <c r="Q5" s="1"/>
+      <c r="Q5" s="1" t="n">
+        <v>56.021645021645</v>
+      </c>
       <c r="S5" s="1" t="n">
         <v>1</v>
       </c>
@@ -371,7 +377,9 @@
       <c r="V5" s="1" t="n">
         <v>85.6914805537944</v>
       </c>
-      <c r="W5" s="1"/>
+      <c r="W5" s="1" t="n">
+        <v>99.9700038297602</v>
+      </c>
       <c r="Y5" s="1" t="n">
         <v>1</v>
       </c>
@@ -384,7 +392,9 @@
       <c r="AB5" s="1" t="n">
         <v>192.865404529307</v>
       </c>
-      <c r="AC5" s="1"/>
+      <c r="AC5" s="1" t="n">
+        <v>137.848205525952</v>
+      </c>
       <c r="AE5" s="1" t="n">
         <v>1</v>
       </c>
@@ -397,9 +407,11 @@
       <c r="AH5" s="1" t="n">
         <v>411.956515041972</v>
       </c>
-      <c r="AI5" s="1"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI5" s="1" t="n">
+        <v>411.85958021772</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>2</v>
       </c>
@@ -412,7 +424,9 @@
       <c r="D6" s="1" t="n">
         <v>2.07873086465268</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1" t="n">
+        <v>16.3636548453399</v>
+      </c>
       <c r="G6" s="1" t="n">
         <v>2</v>
       </c>
@@ -425,7 +439,9 @@
       <c r="J6" s="1" t="n">
         <v>29.5736744328583</v>
       </c>
-      <c r="K6" s="1"/>
+      <c r="K6" s="1" t="n">
+        <v>42.298970116984</v>
+      </c>
       <c r="M6" s="1" t="n">
         <v>2</v>
       </c>
@@ -438,7 +454,9 @@
       <c r="P6" s="1" t="n">
         <v>0.0434526668178448</v>
       </c>
-      <c r="Q6" s="1"/>
+      <c r="Q6" s="1" t="n">
+        <v>55.4761904761905</v>
+      </c>
       <c r="S6" s="1" t="n">
         <v>2</v>
       </c>
@@ -451,7 +469,9 @@
       <c r="V6" s="1" t="n">
         <v>88.7292001831602</v>
       </c>
-      <c r="W6" s="1"/>
+      <c r="W6" s="1" t="n">
+        <v>92.9230553678904</v>
+      </c>
       <c r="Y6" s="1" t="n">
         <v>2</v>
       </c>
@@ -464,7 +484,9 @@
       <c r="AB6" s="1" t="n">
         <v>221.181865785075</v>
       </c>
-      <c r="AC6" s="1"/>
+      <c r="AC6" s="1" t="n">
+        <v>141.225493551861</v>
+      </c>
       <c r="AE6" s="1" t="n">
         <v>2</v>
       </c>
@@ -477,9 +499,11 @@
       <c r="AH6" s="1" t="n">
         <v>412.574711506663</v>
       </c>
-      <c r="AI6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI6" s="1" t="n">
+        <v>412.552844799927</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>3</v>
       </c>
@@ -492,7 +516,9 @@
       <c r="D7" s="1" t="n">
         <v>2.18384314869176</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1" t="n">
+        <v>15.7423748443529</v>
+      </c>
       <c r="G7" s="1" t="n">
         <v>3</v>
       </c>
@@ -505,7 +531,9 @@
       <c r="J7" s="1" t="n">
         <v>29.6839625645028</v>
       </c>
-      <c r="K7" s="1"/>
+      <c r="K7" s="1" t="n">
+        <v>49.0064771213432</v>
+      </c>
       <c r="M7" s="1" t="n">
         <v>3</v>
       </c>
@@ -518,7 +546,9 @@
       <c r="P7" s="1" t="n">
         <v>0.0550794360620053</v>
       </c>
-      <c r="Q7" s="1"/>
+      <c r="Q7" s="1" t="n">
+        <v>59.254329004329</v>
+      </c>
       <c r="S7" s="1" t="n">
         <v>3</v>
       </c>
@@ -531,7 +561,9 @@
       <c r="V7" s="1" t="n">
         <v>109.264173419045</v>
       </c>
-      <c r="W7" s="1"/>
+      <c r="W7" s="1" t="n">
+        <v>93.1287428395352</v>
+      </c>
       <c r="Y7" s="1" t="n">
         <v>3</v>
       </c>
@@ -544,7 +576,9 @@
       <c r="AB7" s="1" t="n">
         <v>175.51957673553</v>
       </c>
-      <c r="AC7" s="1"/>
+      <c r="AC7" s="1" t="n">
+        <v>135.85820190939</v>
+      </c>
       <c r="AE7" s="1" t="n">
         <v>3</v>
       </c>
@@ -557,9 +591,11 @@
       <c r="AH7" s="1" t="n">
         <v>440.296858559584</v>
       </c>
-      <c r="AI7" s="1"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI7" s="1" t="n">
+        <v>404.468482047801</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>4</v>
       </c>
@@ -572,7 +608,9 @@
       <c r="D8" s="1" t="n">
         <v>2.19530144732792</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1" t="n">
+        <v>16.5179160503601</v>
+      </c>
       <c r="G8" s="1" t="n">
         <v>4</v>
       </c>
@@ -585,7 +623,9 @@
       <c r="J8" s="1" t="n">
         <v>29.6915105975186</v>
       </c>
-      <c r="K8" s="1"/>
+      <c r="K8" s="1" t="n">
+        <v>48.6691594219696</v>
+      </c>
       <c r="M8" s="1" t="n">
         <v>4</v>
       </c>
@@ -598,7 +638,9 @@
       <c r="P8" s="1" t="n">
         <v>0.0289800781270291</v>
       </c>
-      <c r="Q8" s="1"/>
+      <c r="Q8" s="1" t="n">
+        <v>57.3484848484849</v>
+      </c>
       <c r="S8" s="1" t="n">
         <v>4</v>
       </c>
@@ -611,7 +653,9 @@
       <c r="V8" s="1" t="n">
         <v>89.5059930373964</v>
       </c>
-      <c r="W8" s="1"/>
+      <c r="W8" s="1" t="n">
+        <v>91.7026511561331</v>
+      </c>
       <c r="Y8" s="1" t="n">
         <v>4</v>
       </c>
@@ -624,7 +668,9 @@
       <c r="AB8" s="1" t="n">
         <v>182.931927177672</v>
       </c>
-      <c r="AC8" s="1"/>
+      <c r="AC8" s="1" t="n">
+        <v>144.401452845659</v>
+      </c>
       <c r="AE8" s="1" t="n">
         <v>4</v>
       </c>
@@ -637,9 +683,11 @@
       <c r="AH8" s="1" t="n">
         <v>455.64841468299</v>
       </c>
-      <c r="AI8" s="1"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI8" s="1" t="n">
+        <v>404.381547707255</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>5</v>
       </c>
@@ -652,7 +700,9 @@
       <c r="D9" s="1" t="n">
         <v>2.22755379109228</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1" t="n">
+        <v>16.5050264408329</v>
+      </c>
       <c r="G9" s="1" t="n">
         <v>5</v>
       </c>
@@ -665,7 +715,9 @@
       <c r="J9" s="1" t="n">
         <v>29.9061406476276</v>
       </c>
-      <c r="K9" s="1"/>
+      <c r="K9" s="1" t="n">
+        <v>48.7702764072189</v>
+      </c>
       <c r="M9" s="1" t="n">
         <v>5</v>
       </c>
@@ -678,7 +730,9 @@
       <c r="P9" s="1" t="n">
         <v>0.0358890748235963</v>
       </c>
-      <c r="Q9" s="1"/>
+      <c r="Q9" s="1" t="n">
+        <v>57.3917748917749</v>
+      </c>
       <c r="S9" s="1" t="n">
         <v>5</v>
       </c>
@@ -691,7 +745,9 @@
       <c r="V9" s="1" t="n">
         <v>94.2748591849073</v>
       </c>
-      <c r="W9" s="1"/>
+      <c r="W9" s="1" t="n">
+        <v>98.4799475171173</v>
+      </c>
       <c r="Y9" s="1" t="n">
         <v>5</v>
       </c>
@@ -704,7 +760,9 @@
       <c r="AB9" s="1" t="n">
         <v>163.672484524567</v>
       </c>
-      <c r="AC9" s="1"/>
+      <c r="AC9" s="1" t="n">
+        <v>142.506194837933</v>
+      </c>
       <c r="AE9" s="1" t="n">
         <v>5</v>
       </c>
@@ -717,9 +775,11 @@
       <c r="AH9" s="1" t="n">
         <v>463.009365914421</v>
       </c>
-      <c r="AI9" s="1"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI9" s="1" t="n">
+        <v>402.299435489111</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>6</v>
       </c>
@@ -732,7 +792,9 @@
       <c r="D10" s="1" t="n">
         <v>2.06816410733911</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1" t="n">
+        <v>15.5740604221762</v>
+      </c>
       <c r="G10" s="1" t="n">
         <v>6</v>
       </c>
@@ -745,7 +807,9 @@
       <c r="J10" s="1" t="n">
         <v>30.1671887072238</v>
       </c>
-      <c r="K10" s="1"/>
+      <c r="K10" s="1" t="n">
+        <v>40.9908960270192</v>
+      </c>
       <c r="M10" s="1" t="n">
         <v>6</v>
       </c>
@@ -758,7 +822,9 @@
       <c r="P10" s="1" t="n">
         <v>0.0346443586841643</v>
       </c>
-      <c r="Q10" s="1"/>
+      <c r="Q10" s="1" t="n">
+        <v>57.9231601731602</v>
+      </c>
       <c r="S10" s="1" t="n">
         <v>6</v>
       </c>
@@ -771,7 +837,9 @@
       <c r="V10" s="1" t="n">
         <v>126.854919663093</v>
       </c>
-      <c r="W10" s="1"/>
+      <c r="W10" s="1" t="n">
+        <v>96.110181003113</v>
+      </c>
       <c r="Y10" s="1" t="n">
         <v>6</v>
       </c>
@@ -784,7 +852,9 @@
       <c r="AB10" s="1" t="n">
         <v>159.293201425471</v>
       </c>
-      <c r="AC10" s="1"/>
+      <c r="AC10" s="1" t="n">
+        <v>140.161468920973</v>
+      </c>
       <c r="AE10" s="1" t="n">
         <v>6</v>
       </c>
@@ -797,9 +867,11 @@
       <c r="AH10" s="1" t="n">
         <v>424.819138159073</v>
       </c>
-      <c r="AI10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI10" s="1" t="n">
+        <v>408.908346271468</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>7</v>
       </c>
@@ -812,7 +884,9 @@
       <c r="D11" s="1" t="n">
         <v>1.98923382793467</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1" t="n">
+        <v>16.1820915635907</v>
+      </c>
       <c r="G11" s="1" t="n">
         <v>7</v>
       </c>
@@ -825,7 +899,9 @@
       <c r="J11" s="1" t="n">
         <v>27.8997059383328</v>
       </c>
-      <c r="K11" s="1"/>
+      <c r="K11" s="1" t="n">
+        <v>42.0334800901426</v>
+      </c>
       <c r="M11" s="1" t="n">
         <v>7</v>
       </c>
@@ -838,7 +914,9 @@
       <c r="P11" s="1" t="n">
         <v>0.0478499813532247</v>
       </c>
-      <c r="Q11" s="1"/>
+      <c r="Q11" s="1" t="n">
+        <v>58.0248917748918</v>
+      </c>
       <c r="S11" s="1" t="n">
         <v>7</v>
       </c>
@@ -851,7 +929,9 @@
       <c r="V11" s="1" t="n">
         <v>98.8561602597004</v>
       </c>
-      <c r="W11" s="1"/>
+      <c r="W11" s="1" t="n">
+        <v>96.4375038144246</v>
+      </c>
       <c r="Y11" s="1" t="n">
         <v>7</v>
       </c>
@@ -864,7 +944,9 @@
       <c r="AB11" s="1" t="n">
         <v>143.373799121494</v>
       </c>
-      <c r="AC11" s="1"/>
+      <c r="AC11" s="1" t="n">
+        <v>141.25501035956</v>
+      </c>
       <c r="AE11" s="1" t="n">
         <v>7</v>
       </c>
@@ -877,9 +959,11 @@
       <c r="AH11" s="1" t="n">
         <v>421.096420097035</v>
       </c>
-      <c r="AI11" s="1"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI11" s="1" t="n">
+        <v>400.897857438442</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>8</v>
       </c>
@@ -892,7 +976,9 @@
       <c r="D12" s="1" t="n">
         <v>2.13656560159711</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1" t="n">
+        <v>16.7319004646364</v>
+      </c>
       <c r="G12" s="1" t="n">
         <v>8</v>
       </c>
@@ -905,7 +991,9 @@
       <c r="J12" s="1" t="n">
         <v>30.1046770219229</v>
       </c>
-      <c r="K12" s="1"/>
+      <c r="K12" s="1" t="n">
+        <v>47.8166725636624</v>
+      </c>
       <c r="M12" s="1" t="n">
         <v>8</v>
       </c>
@@ -918,7 +1006,9 @@
       <c r="P12" s="1" t="n">
         <v>0.0318784808578769</v>
       </c>
-      <c r="Q12" s="1"/>
+      <c r="Q12" s="1" t="n">
+        <v>54.5075757575758</v>
+      </c>
       <c r="S12" s="1" t="n">
         <v>8</v>
       </c>
@@ -931,7 +1021,9 @@
       <c r="V12" s="1" t="n">
         <v>91.1271675080232</v>
       </c>
-      <c r="W12" s="1"/>
+      <c r="W12" s="1" t="n">
+        <v>95.517335662529</v>
+      </c>
       <c r="Y12" s="1" t="n">
         <v>8</v>
       </c>
@@ -944,7 +1036,9 @@
       <c r="AB12" s="1" t="n">
         <v>160.020940132229</v>
       </c>
-      <c r="AC12" s="1"/>
+      <c r="AC12" s="1" t="n">
+        <v>136.260311228425</v>
+      </c>
       <c r="AE12" s="1" t="n">
         <v>8</v>
       </c>
@@ -957,9 +1051,11 @@
       <c r="AH12" s="1" t="n">
         <v>467.731609288406</v>
       </c>
-      <c r="AI12" s="1"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI12" s="1" t="n">
+        <v>410.064977507151</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>9</v>
       </c>
@@ -972,7 +1068,9 @@
       <c r="D13" s="1" t="n">
         <v>2.20001463281431</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1" t="n">
+        <v>16.9288628351031</v>
+      </c>
       <c r="G13" s="1" t="n">
         <v>9</v>
       </c>
@@ -985,7 +1083,9 @@
       <c r="J13" s="1" t="n">
         <v>29.9044250956604</v>
       </c>
-      <c r="K13" s="1"/>
+      <c r="K13" s="1" t="n">
+        <v>49.9924987547251</v>
+      </c>
       <c r="M13" s="1" t="n">
         <v>9</v>
       </c>
@@ -998,7 +1098,9 @@
       <c r="P13" s="1" t="n">
         <v>0.0343964181010721</v>
       </c>
-      <c r="Q13" s="1"/>
+      <c r="Q13" s="1" t="n">
+        <v>58.1742424242424</v>
+      </c>
       <c r="S13" s="1" t="n">
         <v>9</v>
       </c>
@@ -1011,7 +1113,9 @@
       <c r="V13" s="1" t="n">
         <v>88.0382041398735</v>
       </c>
-      <c r="W13" s="1"/>
+      <c r="W13" s="1" t="n">
+        <v>92.6693493259238</v>
+      </c>
       <c r="Y13" s="1" t="n">
         <v>9</v>
       </c>
@@ -1024,7 +1128,9 @@
       <c r="AB13" s="1" t="n">
         <v>177.590362662413</v>
       </c>
-      <c r="AC13" s="1"/>
+      <c r="AC13" s="1" t="n">
+        <v>141.641622086995</v>
+      </c>
       <c r="AE13" s="1" t="n">
         <v>9</v>
       </c>
@@ -1037,9 +1143,11 @@
       <c r="AH13" s="1" t="n">
         <v>464.008438096092</v>
       </c>
-      <c r="AI13" s="1"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI13" s="1" t="n">
+        <v>408.260366886559</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>10</v>
       </c>
@@ -1052,7 +1160,9 @@
       <c r="D14" s="1" t="n">
         <v>2.0394233183169</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1" t="n">
+        <v>16.911568075489</v>
+      </c>
       <c r="G14" s="1" t="n">
         <v>10</v>
       </c>
@@ -1065,7 +1175,9 @@
       <c r="J14" s="1" t="n">
         <v>29.6205113976174</v>
       </c>
-      <c r="K14" s="1"/>
+      <c r="K14" s="1" t="n">
+        <v>39.759723613396</v>
+      </c>
       <c r="M14" s="1" t="n">
         <v>10</v>
       </c>
@@ -1078,7 +1190,9 @@
       <c r="P14" s="1" t="n">
         <v>0.0467217458742315</v>
       </c>
-      <c r="Q14" s="1"/>
+      <c r="Q14" s="1" t="n">
+        <v>56.3722943722944</v>
+      </c>
       <c r="S14" s="1" t="n">
         <v>10</v>
       </c>
@@ -1091,7 +1205,9 @@
       <c r="V14" s="1" t="n">
         <v>90.5192385752245</v>
       </c>
-      <c r="W14" s="1"/>
+      <c r="W14" s="1" t="n">
+        <v>88.648013391956</v>
+      </c>
       <c r="Y14" s="1" t="n">
         <v>10</v>
       </c>
@@ -1104,7 +1220,9 @@
       <c r="AB14" s="1" t="n">
         <v>140.580389917472</v>
       </c>
-      <c r="AC14" s="1"/>
+      <c r="AC14" s="1" t="n">
+        <v>144.098701003625</v>
+      </c>
       <c r="AE14" s="1" t="n">
         <v>10</v>
       </c>
@@ -1117,9 +1235,11 @@
       <c r="AH14" s="1" t="n">
         <v>435.649700319347</v>
       </c>
-      <c r="AI14" s="1"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI14" s="1" t="n">
+        <v>402.881200744287</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>11</v>
       </c>
@@ -1132,7 +1252,9 @@
       <c r="D15" s="1" t="n">
         <v>2.28348364030172</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1" t="n">
+        <v>16.7849264141599</v>
+      </c>
       <c r="G15" s="1" t="n">
         <v>11</v>
       </c>
@@ -1145,7 +1267,9 @@
       <c r="J15" s="1" t="n">
         <v>30.5596362242615</v>
       </c>
-      <c r="K15" s="1"/>
+      <c r="K15" s="1" t="n">
+        <v>46.976882552876</v>
+      </c>
       <c r="M15" s="1" t="n">
         <v>11</v>
       </c>
@@ -1158,7 +1282,9 @@
       <c r="P15" s="1" t="n">
         <v>0.073403757047279</v>
       </c>
-      <c r="Q15" s="1"/>
+      <c r="Q15" s="1" t="n">
+        <v>59.8008658008658</v>
+      </c>
       <c r="S15" s="1" t="n">
         <v>11</v>
       </c>
@@ -1171,7 +1297,9 @@
       <c r="V15" s="1" t="n">
         <v>91.375483394491</v>
       </c>
-      <c r="W15" s="1"/>
+      <c r="W15" s="1" t="n">
+        <v>91.6700747848336</v>
+      </c>
       <c r="Y15" s="1" t="n">
         <v>11</v>
       </c>
@@ -1184,7 +1312,9 @@
       <c r="AB15" s="1" t="n">
         <v>202.91530688522</v>
       </c>
-      <c r="AC15" s="1"/>
+      <c r="AC15" s="1" t="n">
+        <v>142.777771511148</v>
+      </c>
       <c r="AE15" s="1" t="n">
         <v>11</v>
       </c>
@@ -1197,9 +1327,11 @@
       <c r="AH15" s="1" t="n">
         <v>455.763539992615</v>
       </c>
-      <c r="AI15" s="1"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI15" s="1" t="n">
+        <v>406.099540654943</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>12</v>
       </c>
@@ -1212,7 +1344,9 @@
       <c r="D16" s="1" t="n">
         <v>2.20930198998859</v>
       </c>
-      <c r="E16" s="1"/>
+      <c r="E16" s="1" t="n">
+        <v>15.6749472497569</v>
+      </c>
       <c r="G16" s="1" t="n">
         <v>12</v>
       </c>
@@ -1225,7 +1359,9 @@
       <c r="J16" s="1" t="n">
         <v>29.1865348503694</v>
       </c>
-      <c r="K16" s="1"/>
+      <c r="K16" s="1" t="n">
+        <v>51.7745233807341</v>
+      </c>
       <c r="M16" s="1" t="n">
         <v>12</v>
       </c>
@@ -1238,7 +1374,9 @@
       <c r="P16" s="1" t="n">
         <v>0.0534843442136657</v>
       </c>
-      <c r="Q16" s="1"/>
+      <c r="Q16" s="1" t="n">
+        <v>55.2532467532468</v>
+      </c>
       <c r="S16" s="1" t="n">
         <v>12</v>
       </c>
@@ -1251,7 +1389,9 @@
       <c r="V16" s="1" t="n">
         <v>93.3771630804785</v>
       </c>
-      <c r="W16" s="1"/>
+      <c r="W16" s="1" t="n">
+        <v>91.8255311138901</v>
+      </c>
       <c r="Y16" s="1" t="n">
         <v>12</v>
       </c>
@@ -1264,7 +1404,9 @@
       <c r="AB16" s="1" t="n">
         <v>150.107504566011</v>
       </c>
-      <c r="AC16" s="1"/>
+      <c r="AC16" s="1" t="n">
+        <v>142.817849088031</v>
+      </c>
       <c r="AE16" s="1" t="n">
         <v>12</v>
       </c>
@@ -1277,9 +1419,11 @@
       <c r="AH16" s="1" t="n">
         <v>469.886399752747</v>
       </c>
-      <c r="AI16" s="1"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI16" s="1" t="n">
+        <v>406.747245826201</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>13</v>
       </c>
@@ -1292,7 +1436,9 @@
       <c r="D17" s="1" t="n">
         <v>2.13169717078861</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1" t="n">
+        <v>16.5665462238615</v>
+      </c>
       <c r="G17" s="1" t="n">
         <v>13</v>
       </c>
@@ -1305,7 +1451,9 @@
       <c r="J17" s="1" t="n">
         <v>31.2755215339957</v>
       </c>
-      <c r="K17" s="1"/>
+      <c r="K17" s="1" t="n">
+        <v>48.3859069546796</v>
+      </c>
       <c r="M17" s="1" t="n">
         <v>13</v>
       </c>
@@ -1318,7 +1466,9 @@
       <c r="P17" s="1" t="n">
         <v>0.0569409852516101</v>
       </c>
-      <c r="Q17" s="1"/>
+      <c r="Q17" s="1" t="n">
+        <v>56.1190476190476</v>
+      </c>
       <c r="S17" s="1" t="n">
         <v>13</v>
       </c>
@@ -1331,7 +1481,9 @@
       <c r="V17" s="1" t="n">
         <v>86.18801909808</v>
       </c>
-      <c r="W17" s="1"/>
+      <c r="W17" s="1" t="n">
+        <v>97.0782098573344</v>
+      </c>
       <c r="Y17" s="1" t="n">
         <v>13</v>
       </c>
@@ -1344,7 +1496,9 @@
       <c r="AB17" s="1" t="n">
         <v>163.133529842987</v>
       </c>
-      <c r="AC17" s="1"/>
+      <c r="AC17" s="1" t="n">
+        <v>141.26285648652</v>
+      </c>
       <c r="AE17" s="1" t="n">
         <v>13</v>
       </c>
@@ -1357,9 +1511,11 @@
       <c r="AH17" s="1" t="n">
         <v>454.398133067032</v>
       </c>
-      <c r="AI17" s="1"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI17" s="1" t="n">
+        <v>402.540866275494</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>14</v>
       </c>
@@ -1372,7 +1528,9 @@
       <c r="D18" s="1" t="n">
         <v>2.1792020827037</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="1" t="n">
+        <v>16.1628937071012</v>
+      </c>
       <c r="G18" s="1" t="n">
         <v>14</v>
       </c>
@@ -1385,7 +1543,9 @@
       <c r="J18" s="1" t="n">
         <v>29.6882690800628</v>
       </c>
-      <c r="K18" s="1"/>
+      <c r="K18" s="1" t="n">
+        <v>46.8831778915452</v>
+      </c>
       <c r="M18" s="1" t="n">
         <v>14</v>
       </c>
@@ -1398,7 +1558,9 @@
       <c r="P18" s="1" t="n">
         <v>0.016591991434229</v>
       </c>
-      <c r="Q18" s="1"/>
+      <c r="Q18" s="1" t="n">
+        <v>58.2034632034632</v>
+      </c>
       <c r="S18" s="1" t="n">
         <v>14</v>
       </c>
@@ -1411,7 +1573,9 @@
       <c r="V18" s="1" t="n">
         <v>87.1942892221527</v>
       </c>
-      <c r="W18" s="1"/>
+      <c r="W18" s="1" t="n">
+        <v>92.5112526904534</v>
+      </c>
       <c r="Y18" s="1" t="n">
         <v>14</v>
       </c>
@@ -1424,7 +1588,9 @@
       <c r="AB18" s="1" t="n">
         <v>151.352667503058</v>
       </c>
-      <c r="AC18" s="1"/>
+      <c r="AC18" s="1" t="n">
+        <v>144.948762230008</v>
+      </c>
       <c r="AE18" s="1" t="n">
         <v>14</v>
       </c>
@@ -1437,9 +1603,11 @@
       <c r="AH18" s="1" t="n">
         <v>461.287081628595</v>
       </c>
-      <c r="AI18" s="1"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI18" s="1" t="n">
+        <v>404.062974881537</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>15</v>
       </c>
@@ -1452,7 +1620,9 @@
       <c r="D19" s="1" t="n">
         <v>2.1553672295632</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1" t="n">
+        <v>15.8598167131258</v>
+      </c>
       <c r="G19" s="1" t="n">
         <v>15</v>
       </c>
@@ -1465,7 +1635,9 @@
       <c r="J19" s="1" t="n">
         <v>29.898270956051</v>
       </c>
-      <c r="K19" s="1"/>
+      <c r="K19" s="1" t="n">
+        <v>41.7456414357814</v>
+      </c>
       <c r="M19" s="1" t="n">
         <v>15</v>
       </c>
@@ -1478,7 +1650,9 @@
       <c r="P19" s="1" t="n">
         <v>0.0761302251022187</v>
       </c>
-      <c r="Q19" s="1"/>
+      <c r="Q19" s="1" t="n">
+        <v>56.1958874458875</v>
+      </c>
       <c r="S19" s="1" t="n">
         <v>15</v>
       </c>
@@ -1491,7 +1665,9 @@
       <c r="V19" s="1" t="n">
         <v>92.4438506337849</v>
       </c>
-      <c r="W19" s="1"/>
+      <c r="W19" s="1" t="n">
+        <v>94.5956904834498</v>
+      </c>
       <c r="Y19" s="1" t="n">
         <v>15</v>
       </c>
@@ -1504,7 +1680,9 @@
       <c r="AB19" s="1" t="n">
         <v>167.848728629209</v>
       </c>
-      <c r="AC19" s="1"/>
+      <c r="AC19" s="1" t="n">
+        <v>137.911932042558</v>
+      </c>
       <c r="AE19" s="1" t="n">
         <v>15</v>
       </c>
@@ -1517,9 +1695,11 @@
       <c r="AH19" s="1" t="n">
         <v>424.399719390843</v>
       </c>
-      <c r="AI19" s="1"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI19" s="1" t="n">
+        <v>403.268490756218</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>16</v>
       </c>
@@ -1532,7 +1712,9 @@
       <c r="D20" s="1" t="n">
         <v>2.09871507658777</v>
       </c>
-      <c r="E20" s="1"/>
+      <c r="E20" s="1" t="n">
+        <v>16.9970942420082</v>
+      </c>
       <c r="G20" s="1" t="n">
         <v>16</v>
       </c>
@@ -1545,7 +1727,9 @@
       <c r="J20" s="1" t="n">
         <v>29.8877348624323</v>
       </c>
-      <c r="K20" s="1"/>
+      <c r="K20" s="1" t="n">
+        <v>42.3935034579994</v>
+      </c>
       <c r="M20" s="1" t="n">
         <v>16</v>
       </c>
@@ -1558,7 +1742,9 @@
       <c r="P20" s="1" t="n">
         <v>0.0368488550372481</v>
       </c>
-      <c r="Q20" s="1"/>
+      <c r="Q20" s="1" t="n">
+        <v>57.4274891774892</v>
+      </c>
       <c r="S20" s="1" t="n">
         <v>16</v>
       </c>
@@ -1571,7 +1757,9 @@
       <c r="V20" s="1" t="n">
         <v>89.387245781072</v>
       </c>
-      <c r="W20" s="1"/>
+      <c r="W20" s="1" t="n">
+        <v>95.6969981487667</v>
+      </c>
       <c r="Y20" s="1" t="n">
         <v>16</v>
       </c>
@@ -1584,7 +1772,9 @@
       <c r="AB20" s="1" t="n">
         <v>178.393379322147</v>
       </c>
-      <c r="AC20" s="1"/>
+      <c r="AC20" s="1" t="n">
+        <v>144.358475421358</v>
+      </c>
       <c r="AE20" s="1" t="n">
         <v>16</v>
       </c>
@@ -1597,9 +1787,11 @@
       <c r="AH20" s="1" t="n">
         <v>530.471137577906</v>
       </c>
-      <c r="AI20" s="1"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI20" s="1" t="n">
+        <v>404.645127972948</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>17</v>
       </c>
@@ -1612,7 +1804,9 @@
       <c r="D21" s="1" t="n">
         <v>2.28108854414253</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="1" t="n">
+        <v>16.1110690533809</v>
+      </c>
       <c r="G21" s="1" t="n">
         <v>17</v>
       </c>
@@ -1625,7 +1819,9 @@
       <c r="J21" s="1" t="n">
         <v>28.7522717455451</v>
       </c>
-      <c r="K21" s="1"/>
+      <c r="K21" s="1" t="n">
+        <v>39.99342590521</v>
+      </c>
       <c r="M21" s="1" t="n">
         <v>17</v>
       </c>
@@ -1638,7 +1834,9 @@
       <c r="P21" s="1" t="n">
         <v>0.0244690919146722</v>
       </c>
-      <c r="Q21" s="1"/>
+      <c r="Q21" s="1" t="n">
+        <v>57.7813852813853</v>
+      </c>
       <c r="S21" s="1" t="n">
         <v>17</v>
       </c>
@@ -1651,7 +1849,9 @@
       <c r="V21" s="1" t="n">
         <v>100.508763350986</v>
       </c>
-      <c r="W21" s="1"/>
+      <c r="W21" s="1" t="n">
+        <v>100.404388667312</v>
+      </c>
       <c r="Y21" s="1" t="n">
         <v>17</v>
       </c>
@@ -1664,7 +1864,9 @@
       <c r="AB21" s="1" t="n">
         <v>192.110545499621</v>
       </c>
-      <c r="AC21" s="1"/>
+      <c r="AC21" s="1" t="n">
+        <v>142.617405244438</v>
+      </c>
       <c r="AE21" s="1" t="n">
         <v>17</v>
       </c>
@@ -1677,9 +1879,11 @@
       <c r="AH21" s="1" t="n">
         <v>443.040099534508</v>
       </c>
-      <c r="AI21" s="1"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI21" s="1" t="n">
+        <v>405.18327757672</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>18</v>
       </c>
@@ -1692,7 +1896,9 @@
       <c r="D22" s="1" t="n">
         <v>2.14020686231014</v>
       </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="1" t="n">
+        <v>15.9728262051465</v>
+      </c>
       <c r="G22" s="1" t="n">
         <v>18</v>
       </c>
@@ -1705,7 +1911,9 @@
       <c r="J22" s="1" t="n">
         <v>30.7437455712668</v>
       </c>
-      <c r="K22" s="1"/>
+      <c r="K22" s="1" t="n">
+        <v>45.8211486892593</v>
+      </c>
       <c r="M22" s="1" t="n">
         <v>18</v>
       </c>
@@ -1718,7 +1926,9 @@
       <c r="P22" s="1" t="n">
         <v>0.0405507343298508</v>
       </c>
-      <c r="Q22" s="1"/>
+      <c r="Q22" s="1" t="n">
+        <v>58.8982683982684</v>
+      </c>
       <c r="S22" s="1" t="n">
         <v>18</v>
       </c>
@@ -1731,7 +1941,9 @@
       <c r="V22" s="1" t="n">
         <v>100.43562704588</v>
       </c>
-      <c r="W22" s="1"/>
+      <c r="W22" s="1" t="n">
+        <v>90.4923046312075</v>
+      </c>
       <c r="Y22" s="1" t="n">
         <v>18</v>
       </c>
@@ -1744,7 +1956,9 @@
       <c r="AB22" s="1" t="n">
         <v>186.540915574456</v>
       </c>
-      <c r="AC22" s="1"/>
+      <c r="AC22" s="1" t="n">
+        <v>144.423294096891</v>
+      </c>
       <c r="AE22" s="1" t="n">
         <v>18</v>
       </c>
@@ -1757,9 +1971,11 @@
       <c r="AH22" s="1" t="n">
         <v>522.693220424006</v>
       </c>
-      <c r="AI22" s="1"/>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI22" s="1" t="n">
+        <v>406.184259998031</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>19</v>
       </c>
@@ -1772,7 +1988,9 @@
       <c r="D23" s="1" t="n">
         <v>2.15332505257297</v>
       </c>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1" t="n">
+        <v>16.6886452264954</v>
+      </c>
       <c r="G23" s="1" t="n">
         <v>19</v>
       </c>
@@ -1785,7 +2003,9 @@
       <c r="J23" s="1" t="n">
         <v>30.0795986268523</v>
       </c>
-      <c r="K23" s="1"/>
+      <c r="K23" s="1" t="n">
+        <v>47.8368219848362</v>
+      </c>
       <c r="M23" s="1" t="n">
         <v>19</v>
       </c>
@@ -1798,7 +2018,9 @@
       <c r="P23" s="1" t="n">
         <v>0.0599148120374942</v>
       </c>
-      <c r="Q23" s="1"/>
+      <c r="Q23" s="1" t="n">
+        <v>56.4621212121212</v>
+      </c>
       <c r="S23" s="1" t="n">
         <v>19</v>
       </c>
@@ -1811,7 +2033,9 @@
       <c r="V23" s="1" t="n">
         <v>99.1430436670135</v>
       </c>
-      <c r="W23" s="1"/>
+      <c r="W23" s="1" t="n">
+        <v>93.6504311445545</v>
+      </c>
       <c r="Y23" s="1" t="n">
         <v>19</v>
       </c>
@@ -1824,7 +2048,9 @@
       <c r="AB23" s="1" t="n">
         <v>164.790749510731</v>
       </c>
-      <c r="AC23" s="1"/>
+      <c r="AC23" s="1" t="n">
+        <v>133.930225530648</v>
+      </c>
       <c r="AE23" s="1" t="n">
         <v>19</v>
       </c>
@@ -1837,9 +2063,11 @@
       <c r="AH23" s="1" t="n">
         <v>513.113869059612</v>
       </c>
-      <c r="AI23" s="1"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI23" s="1" t="n">
+        <v>405.579361143406</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>20</v>
       </c>
@@ -1852,7 +2080,9 @@
       <c r="D24" s="1" t="n">
         <v>2.16598414494164</v>
       </c>
-      <c r="E24" s="1"/>
+      <c r="E24" s="1" t="n">
+        <v>16.6679461232927</v>
+      </c>
       <c r="G24" s="1" t="n">
         <v>20</v>
       </c>
@@ -1865,7 +2095,9 @@
       <c r="J24" s="1" t="n">
         <v>30.932781309876</v>
       </c>
-      <c r="K24" s="1"/>
+      <c r="K24" s="1" t="n">
+        <v>43.2020148249544</v>
+      </c>
       <c r="M24" s="1" t="n">
         <v>20</v>
       </c>
@@ -1878,7 +2110,9 @@
       <c r="P24" s="1" t="n">
         <v>0.0358625967427519</v>
       </c>
-      <c r="Q24" s="1"/>
+      <c r="Q24" s="1" t="n">
+        <v>57.3917748917749</v>
+      </c>
       <c r="S24" s="1" t="n">
         <v>20</v>
       </c>
@@ -1891,7 +2125,9 @@
       <c r="V24" s="1" t="n">
         <v>109.905736050215</v>
       </c>
-      <c r="W24" s="1"/>
+      <c r="W24" s="1" t="n">
+        <v>92.6047937925229</v>
+      </c>
       <c r="Y24" s="1" t="n">
         <v>20</v>
       </c>
@@ -1904,7 +2140,9 @@
       <c r="AB24" s="1" t="n">
         <v>179.368574855131</v>
       </c>
-      <c r="AC24" s="1"/>
+      <c r="AC24" s="1" t="n">
+        <v>137.295466458176</v>
+      </c>
       <c r="AE24" s="1" t="n">
         <v>20</v>
       </c>
@@ -1917,9 +2155,11 @@
       <c r="AH24" s="1" t="n">
         <v>473.634732445762</v>
       </c>
-      <c r="AI24" s="1"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI24" s="1" t="n">
+        <v>414.694937397284</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>21</v>
       </c>
@@ -1932,7 +2172,9 @@
       <c r="D25" s="1" t="n">
         <v>2.0906138760934</v>
       </c>
-      <c r="E25" s="1"/>
+      <c r="E25" s="1" t="n">
+        <v>16.0403320815211</v>
+      </c>
       <c r="G25" s="1" t="n">
         <v>21</v>
       </c>
@@ -1945,7 +2187,9 @@
       <c r="J25" s="1" t="n">
         <v>30.1049116928948</v>
       </c>
-      <c r="K25" s="1"/>
+      <c r="K25" s="1" t="n">
+        <v>43.7020414250727</v>
+      </c>
       <c r="M25" s="1" t="n">
         <v>21</v>
       </c>
@@ -1958,7 +2202,9 @@
       <c r="P25" s="1" t="n">
         <v>0.0963838619091568</v>
       </c>
-      <c r="Q25" s="1"/>
+      <c r="Q25" s="1" t="n">
+        <v>59.7132034632035</v>
+      </c>
       <c r="S25" s="1" t="n">
         <v>21</v>
       </c>
@@ -1971,7 +2217,9 @@
       <c r="V25" s="1" t="n">
         <v>92.844204747552</v>
       </c>
-      <c r="W25" s="1"/>
+      <c r="W25" s="1" t="n">
+        <v>98.5391709867703</v>
+      </c>
       <c r="Y25" s="1" t="n">
         <v>21</v>
       </c>
@@ -1984,7 +2232,9 @@
       <c r="AB25" s="1" t="n">
         <v>238.95710586703</v>
       </c>
-      <c r="AC25" s="1"/>
+      <c r="AC25" s="1" t="n">
+        <v>142.829942650777</v>
+      </c>
       <c r="AE25" s="1" t="n">
         <v>21</v>
       </c>
@@ -1997,9 +2247,11 @@
       <c r="AH25" s="1" t="n">
         <v>394.604559579722</v>
       </c>
-      <c r="AI25" s="1"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI25" s="1" t="n">
+        <v>406.50763399597</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>22</v>
       </c>
@@ -2012,7 +2264,9 @@
       <c r="D26" s="1" t="n">
         <v>1.96448885741852</v>
       </c>
-      <c r="E26" s="1"/>
+      <c r="E26" s="1" t="n">
+        <v>16.8069187553004</v>
+      </c>
       <c r="G26" s="1" t="n">
         <v>22</v>
       </c>
@@ -2025,7 +2279,9 @@
       <c r="J26" s="1" t="n">
         <v>29.3125826933575</v>
       </c>
-      <c r="K26" s="1"/>
+      <c r="K26" s="1" t="n">
+        <v>48.5816855635012</v>
+      </c>
       <c r="M26" s="1" t="n">
         <v>22</v>
       </c>
@@ -2038,7 +2294,9 @@
       <c r="P26" s="1" t="n">
         <v>0.0247895069037307</v>
       </c>
-      <c r="Q26" s="1"/>
+      <c r="Q26" s="1" t="n">
+        <v>56.2803030303031</v>
+      </c>
       <c r="S26" s="1" t="n">
         <v>22</v>
       </c>
@@ -2051,7 +2309,9 @@
       <c r="V26" s="1" t="n">
         <v>99.5297253216319</v>
       </c>
-      <c r="W26" s="1"/>
+      <c r="W26" s="1" t="n">
+        <v>94.5708014131303</v>
+      </c>
       <c r="Y26" s="1" t="n">
         <v>22</v>
       </c>
@@ -2064,7 +2324,9 @@
       <c r="AB26" s="1" t="n">
         <v>166.878417544009</v>
       </c>
-      <c r="AC26" s="1"/>
+      <c r="AC26" s="1" t="n">
+        <v>142.891905884991</v>
+      </c>
       <c r="AE26" s="1" t="n">
         <v>22</v>
       </c>
@@ -2077,9 +2339,11 @@
       <c r="AH26" s="1" t="n">
         <v>496.12612378681</v>
       </c>
-      <c r="AI26" s="1"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI26" s="1" t="n">
+        <v>409.239865012197</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>23</v>
       </c>
@@ -2092,7 +2356,9 @@
       <c r="D27" s="1" t="n">
         <v>2.10870545876739</v>
       </c>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1" t="n">
+        <v>16.6686484421241</v>
+      </c>
       <c r="G27" s="1" t="n">
         <v>23</v>
       </c>
@@ -2105,7 +2371,9 @@
       <c r="J27" s="1" t="n">
         <v>30.0989143729499</v>
       </c>
-      <c r="K27" s="1"/>
+      <c r="K27" s="1" t="n">
+        <v>40.8921173524655</v>
+      </c>
       <c r="M27" s="1" t="n">
         <v>23</v>
       </c>
@@ -2118,7 +2386,9 @@
       <c r="P27" s="1" t="n">
         <v>0.0716693656880416</v>
       </c>
-      <c r="Q27" s="1"/>
+      <c r="Q27" s="1" t="n">
+        <v>54.965367965368</v>
+      </c>
       <c r="S27" s="1" t="n">
         <v>23</v>
       </c>
@@ -2131,7 +2401,9 @@
       <c r="V27" s="1" t="n">
         <v>89.3738902185386</v>
       </c>
-      <c r="W27" s="1"/>
+      <c r="W27" s="1" t="n">
+        <v>92.8942508123728</v>
+      </c>
       <c r="Y27" s="1" t="n">
         <v>23</v>
       </c>
@@ -2144,7 +2416,9 @@
       <c r="AB27" s="1" t="n">
         <v>183.695344187029</v>
       </c>
-      <c r="AC27" s="1"/>
+      <c r="AC27" s="1" t="n">
+        <v>140.217774122437</v>
+      </c>
       <c r="AE27" s="1" t="n">
         <v>23</v>
       </c>
@@ -2157,9 +2431,11 @@
       <c r="AH27" s="1" t="n">
         <v>505.335740978045</v>
       </c>
-      <c r="AI27" s="1"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI27" s="1" t="n">
+        <v>404.993288576092</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>24</v>
       </c>
@@ -2172,7 +2448,9 @@
       <c r="D28" s="1" t="n">
         <v>2.15161741106677</v>
       </c>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1" t="n">
+        <v>16.0687452967842</v>
+      </c>
       <c r="G28" s="1" t="n">
         <v>24</v>
       </c>
@@ -2185,7 +2463,9 @@
       <c r="J28" s="1" t="n">
         <v>30.4667887715565</v>
       </c>
-      <c r="K28" s="1"/>
+      <c r="K28" s="1" t="n">
+        <v>48.1948592970781</v>
+      </c>
       <c r="M28" s="1" t="n">
         <v>24</v>
       </c>
@@ -2198,7 +2478,9 @@
       <c r="P28" s="1" t="n">
         <v>0.0562036634609218</v>
       </c>
-      <c r="Q28" s="1"/>
+      <c r="Q28" s="1" t="n">
+        <v>57.6352813852814</v>
+      </c>
       <c r="S28" s="1" t="n">
         <v>24</v>
       </c>
@@ -2211,7 +2493,9 @@
       <c r="V28" s="1" t="n">
         <v>124.334324660311</v>
       </c>
-      <c r="W28" s="1"/>
+      <c r="W28" s="1" t="n">
+        <v>89.7008084292804</v>
+      </c>
       <c r="Y28" s="1" t="n">
         <v>24</v>
       </c>
@@ -2224,7 +2508,9 @@
       <c r="AB28" s="1" t="n">
         <v>152.611634596184</v>
       </c>
-      <c r="AC28" s="1"/>
+      <c r="AC28" s="1" t="n">
+        <v>150.886051866749</v>
+      </c>
       <c r="AE28" s="1" t="n">
         <v>24</v>
       </c>
@@ -2237,9 +2523,11 @@
       <c r="AH28" s="1" t="n">
         <v>557.998667283165</v>
       </c>
-      <c r="AI28" s="1"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI28" s="1" t="n">
+        <v>404.812790300472</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <v>25</v>
       </c>
@@ -2252,7 +2540,9 @@
       <c r="D29" s="1" t="n">
         <v>2.16010645096121</v>
       </c>
-      <c r="E29" s="1"/>
+      <c r="E29" s="1" t="n">
+        <v>16.3090608621218</v>
+      </c>
       <c r="G29" s="1" t="n">
         <v>25</v>
       </c>
@@ -2265,7 +2555,9 @@
       <c r="J29" s="1" t="n">
         <v>29.9042971021688</v>
       </c>
-      <c r="K29" s="1"/>
+      <c r="K29" s="1" t="n">
+        <v>43.7818925757286</v>
+      </c>
       <c r="M29" s="1" t="n">
         <v>25</v>
       </c>
@@ -2278,7 +2570,9 @@
       <c r="P29" s="1" t="n">
         <v>0.0427148738349503</v>
       </c>
-      <c r="Q29" s="1"/>
+      <c r="Q29" s="1" t="n">
+        <v>58.2683982683983</v>
+      </c>
       <c r="S29" s="1" t="n">
         <v>25</v>
       </c>
@@ -2291,7 +2585,9 @@
       <c r="V29" s="1" t="n">
         <v>108.619409973546</v>
       </c>
-      <c r="W29" s="1"/>
+      <c r="W29" s="1" t="n">
+        <v>93.5422846048359</v>
+      </c>
       <c r="Y29" s="1" t="n">
         <v>25</v>
       </c>
@@ -2304,7 +2600,9 @@
       <c r="AB29" s="1" t="n">
         <v>181.169269023103</v>
       </c>
-      <c r="AC29" s="1"/>
+      <c r="AC29" s="1" t="n">
+        <v>142.729010941633</v>
+      </c>
       <c r="AE29" s="1" t="n">
         <v>25</v>
       </c>
@@ -2317,9 +2615,11 @@
       <c r="AH29" s="1" t="n">
         <v>413.995028444263</v>
       </c>
-      <c r="AI29" s="1"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI29" s="1" t="n">
+        <v>405.053863126803</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
         <v>26</v>
       </c>
@@ -2332,7 +2632,9 @@
       <c r="D30" s="1" t="n">
         <v>2.17410796953207</v>
       </c>
-      <c r="E30" s="1"/>
+      <c r="E30" s="1" t="n">
+        <v>16.6295191077311</v>
+      </c>
       <c r="G30" s="1" t="n">
         <v>26</v>
       </c>
@@ -2345,7 +2647,9 @@
       <c r="J30" s="1" t="n">
         <v>30.8090212319255</v>
       </c>
-      <c r="K30" s="1"/>
+      <c r="K30" s="1" t="n">
+        <v>42.5321915865216</v>
+      </c>
       <c r="M30" s="1" t="n">
         <v>26</v>
       </c>
@@ -2358,7 +2662,9 @@
       <c r="P30" s="1" t="n">
         <v>0.188462012695992</v>
       </c>
-      <c r="Q30" s="1"/>
+      <c r="Q30" s="1" t="n">
+        <v>56.9945887445888</v>
+      </c>
       <c r="S30" s="1" t="n">
         <v>26</v>
       </c>
@@ -2371,7 +2677,9 @@
       <c r="V30" s="1" t="n">
         <v>103.323809511203</v>
       </c>
-      <c r="W30" s="1"/>
+      <c r="W30" s="1" t="n">
+        <v>94.9168474169478</v>
+      </c>
       <c r="Y30" s="1" t="n">
         <v>26</v>
       </c>
@@ -2384,7 +2692,9 @@
       <c r="AB30" s="1" t="n">
         <v>191.558734542178</v>
       </c>
-      <c r="AC30" s="1"/>
+      <c r="AC30" s="1" t="n">
+        <v>134.874444612782</v>
+      </c>
       <c r="AE30" s="1" t="n">
         <v>26</v>
       </c>
@@ -2397,9 +2707,11 @@
       <c r="AH30" s="1" t="n">
         <v>461.532212642829</v>
       </c>
-      <c r="AI30" s="1"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI30" s="1" t="n">
+        <v>409.503295883759</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <v>27</v>
       </c>
@@ -2412,7 +2724,9 @@
       <c r="D31" s="1" t="n">
         <v>2.11036226236928</v>
       </c>
-      <c r="E31" s="1"/>
+      <c r="E31" s="1" t="n">
+        <v>16.9968317206617</v>
+      </c>
       <c r="G31" s="1" t="n">
         <v>27</v>
       </c>
@@ -2425,7 +2739,9 @@
       <c r="J31" s="1" t="n">
         <v>29.8909710863541</v>
       </c>
-      <c r="K31" s="1"/>
+      <c r="K31" s="1" t="n">
+        <v>43.5373782736802</v>
+      </c>
       <c r="M31" s="1" t="n">
         <v>27</v>
       </c>
@@ -2438,7 +2754,9 @@
       <c r="P31" s="1" t="n">
         <v>0.0917038511809212</v>
       </c>
-      <c r="Q31" s="1"/>
+      <c r="Q31" s="1" t="n">
+        <v>56.6969696969697</v>
+      </c>
       <c r="S31" s="1" t="n">
         <v>27</v>
       </c>
@@ -2451,7 +2769,9 @@
       <c r="V31" s="1" t="n">
         <v>92.3008658138341</v>
       </c>
-      <c r="W31" s="1"/>
+      <c r="W31" s="1" t="n">
+        <v>93.3612658390862</v>
+      </c>
       <c r="Y31" s="1" t="n">
         <v>27</v>
       </c>
@@ -2464,7 +2784,9 @@
       <c r="AB31" s="1" t="n">
         <v>142.92510813089</v>
       </c>
-      <c r="AC31" s="1"/>
+      <c r="AC31" s="1" t="n">
+        <v>147.05080753875</v>
+      </c>
       <c r="AE31" s="1" t="n">
         <v>27</v>
       </c>
@@ -2477,9 +2799,11 @@
       <c r="AH31" s="1" t="n">
         <v>584.263583586501</v>
       </c>
-      <c r="AI31" s="1"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI31" s="1" t="n">
+        <v>402.12342338378</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>28</v>
       </c>
@@ -2492,7 +2816,9 @@
       <c r="D32" s="1" t="n">
         <v>2.12723645104282</v>
       </c>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1" t="n">
+        <v>15.8612237151837</v>
+      </c>
       <c r="G32" s="1" t="n">
         <v>28</v>
       </c>
@@ -2505,7 +2831,9 @@
       <c r="J32" s="1" t="n">
         <v>29.6381679024587</v>
       </c>
-      <c r="K32" s="1"/>
+      <c r="K32" s="1" t="n">
+        <v>52.3051554791584</v>
+      </c>
       <c r="M32" s="1" t="n">
         <v>28</v>
       </c>
@@ -2518,7 +2846,9 @@
       <c r="P32" s="1" t="n">
         <v>0.0357764774913996</v>
       </c>
-      <c r="Q32" s="1"/>
+      <c r="Q32" s="1" t="n">
+        <v>61.3235930735931</v>
+      </c>
       <c r="S32" s="1" t="n">
         <v>28</v>
       </c>
@@ -2531,7 +2861,9 @@
       <c r="V32" s="1" t="n">
         <v>112.134242214121</v>
       </c>
-      <c r="W32" s="1"/>
+      <c r="W32" s="1" t="n">
+        <v>92.4965574582937</v>
+      </c>
       <c r="Y32" s="1" t="n">
         <v>28</v>
       </c>
@@ -2544,7 +2876,9 @@
       <c r="AB32" s="1" t="n">
         <v>197.274642970565</v>
       </c>
-      <c r="AC32" s="1"/>
+      <c r="AC32" s="1" t="n">
+        <v>141.452862734252</v>
+      </c>
       <c r="AE32" s="1" t="n">
         <v>28</v>
       </c>
@@ -2557,9 +2891,11 @@
       <c r="AH32" s="1" t="n">
         <v>456.889405059886</v>
       </c>
-      <c r="AI32" s="1"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI32" s="1" t="n">
+        <v>406.168532360845</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <v>29</v>
       </c>
@@ -2572,7 +2908,9 @@
       <c r="D33" s="1" t="n">
         <v>2.24881320986901</v>
       </c>
-      <c r="E33" s="1"/>
+      <c r="E33" s="1" t="n">
+        <v>16.5675270470185</v>
+      </c>
       <c r="G33" s="1" t="n">
         <v>29</v>
       </c>
@@ -2585,7 +2923,9 @@
       <c r="J33" s="1" t="n">
         <v>30.0048806242813</v>
       </c>
-      <c r="K33" s="1"/>
+      <c r="K33" s="1" t="n">
+        <v>42.0014533510607</v>
+      </c>
       <c r="M33" s="1" t="n">
         <v>29</v>
       </c>
@@ -2598,7 +2938,9 @@
       <c r="P33" s="1" t="n">
         <v>0.178901290438311</v>
       </c>
-      <c r="Q33" s="1"/>
+      <c r="Q33" s="1" t="n">
+        <v>60.0919913419913</v>
+      </c>
       <c r="S33" s="1" t="n">
         <v>29</v>
       </c>
@@ -2611,7 +2953,9 @@
       <c r="V33" s="1" t="n">
         <v>88.7729929828239</v>
       </c>
-      <c r="W33" s="1"/>
+      <c r="W33" s="1" t="n">
+        <v>93.1924393454548</v>
+      </c>
       <c r="Y33" s="1" t="n">
         <v>29</v>
       </c>
@@ -2624,7 +2968,9 @@
       <c r="AB33" s="1" t="n">
         <v>191.083731786491</v>
       </c>
-      <c r="AC33" s="1"/>
+      <c r="AC33" s="1" t="n">
+        <v>136.793138425808</v>
+      </c>
       <c r="AE33" s="1" t="n">
         <v>29</v>
       </c>
@@ -2637,9 +2983,11 @@
       <c r="AH33" s="1" t="n">
         <v>429.964037660764</v>
       </c>
-      <c r="AI33" s="1"/>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI33" s="1" t="n">
+        <v>401.117168664786</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>30</v>
       </c>
@@ -2652,7 +3000,9 @@
       <c r="D34" s="1" t="n">
         <v>2.14781278443396</v>
       </c>
-      <c r="E34" s="1"/>
+      <c r="E34" s="1" t="n">
+        <v>17.3659586272926</v>
+      </c>
       <c r="G34" s="1" t="n">
         <v>30</v>
       </c>
@@ -2665,7 +3015,9 @@
       <c r="J34" s="1" t="n">
         <v>29.592604022237</v>
       </c>
-      <c r="K34" s="1"/>
+      <c r="K34" s="1" t="n">
+        <v>45.574698741645</v>
+      </c>
       <c r="M34" s="1" t="n">
         <v>30</v>
       </c>
@@ -2678,7 +3030,9 @@
       <c r="P34" s="1" t="n">
         <v>0.0520740754601601</v>
       </c>
-      <c r="Q34" s="1"/>
+      <c r="Q34" s="1" t="n">
+        <v>60.284632034632</v>
+      </c>
       <c r="S34" s="1" t="n">
         <v>30</v>
       </c>
@@ -2691,7 +3045,9 @@
       <c r="V34" s="1" t="n">
         <v>95.9538106943383</v>
       </c>
-      <c r="W34" s="1"/>
+      <c r="W34" s="1" t="n">
+        <v>91.3762199408743</v>
+      </c>
       <c r="Y34" s="1" t="n">
         <v>30</v>
       </c>
@@ -2704,7 +3060,9 @@
       <c r="AB34" s="1" t="n">
         <v>180.54433986072</v>
       </c>
-      <c r="AC34" s="1"/>
+      <c r="AC34" s="1" t="n">
+        <v>141.819182221541</v>
+      </c>
       <c r="AE34" s="1" t="n">
         <v>30</v>
       </c>
@@ -2717,7 +3075,9 @@
       <c r="AH34" s="1" t="n">
         <v>541.49841483463</v>
       </c>
-      <c r="AI34" s="1"/>
+      <c r="AI34" s="1" t="n">
+        <v>405.537358310829</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2745,13 +3105,13 @@
   </sheetPr>
   <dimension ref="A3:AI34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N23" activeCellId="0" sqref="N23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AI5" activeCellId="0" sqref="AI5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2903,7 +3263,9 @@
       <c r="D5" s="1" t="n">
         <v>0.550826217428903</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="n">
+        <v>3.79444909199248</v>
+      </c>
       <c r="G5" s="1" t="n">
         <v>1</v>
       </c>
@@ -2916,7 +3278,9 @@
       <c r="J5" s="1" t="n">
         <v>6.62990989221775</v>
       </c>
-      <c r="K5" s="1"/>
+      <c r="K5" s="1" t="n">
+        <v>9.93397176136495</v>
+      </c>
       <c r="M5" s="1" t="n">
         <v>1</v>
       </c>
@@ -2929,7 +3293,9 @@
       <c r="P5" s="1" t="n">
         <v>0.00906417468399567</v>
       </c>
-      <c r="Q5" s="1"/>
+      <c r="Q5" s="1" t="n">
+        <v>13.7045454545455</v>
+      </c>
       <c r="S5" s="1" t="n">
         <v>1</v>
       </c>
@@ -2942,7 +3308,9 @@
       <c r="V5" s="1" t="n">
         <v>21.4581887086803</v>
       </c>
-      <c r="W5" s="1"/>
+      <c r="W5" s="1" t="n">
+        <v>23.2822504664432</v>
+      </c>
       <c r="Y5" s="1" t="n">
         <v>1</v>
       </c>
@@ -2955,7 +3323,9 @@
       <c r="AB5" s="1" t="n">
         <v>47.6008014912786</v>
       </c>
-      <c r="AC5" s="1"/>
+      <c r="AC5" s="1" t="n">
+        <v>35.1886955580126</v>
+      </c>
       <c r="AE5" s="1" t="n">
         <v>1</v>
       </c>
@@ -2968,7 +3338,9 @@
       <c r="AH5" s="1" t="n">
         <v>105.484708358061</v>
       </c>
-      <c r="AI5" s="1"/>
+      <c r="AI5" s="1" t="n">
+        <v>98.8231142350022</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -2983,7 +3355,9 @@
       <c r="D6" s="1" t="n">
         <v>0.586321323568484</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1" t="n">
+        <v>3.94922495655017</v>
+      </c>
       <c r="G6" s="1" t="n">
         <v>2</v>
       </c>
@@ -2996,7 +3370,9 @@
       <c r="J6" s="1" t="n">
         <v>7.15785631757336</v>
       </c>
-      <c r="K6" s="1"/>
+      <c r="K6" s="1" t="n">
+        <v>10.4988761205449</v>
+      </c>
       <c r="M6" s="1" t="n">
         <v>2</v>
       </c>
@@ -3009,7 +3385,9 @@
       <c r="P6" s="1" t="n">
         <v>0.0147347388165739</v>
       </c>
-      <c r="Q6" s="1"/>
+      <c r="Q6" s="1" t="n">
+        <v>14.25</v>
+      </c>
       <c r="S6" s="1" t="n">
         <v>2</v>
       </c>
@@ -3022,7 +3400,9 @@
       <c r="V6" s="1" t="n">
         <v>22.2696691206159</v>
       </c>
-      <c r="W6" s="1"/>
+      <c r="W6" s="1" t="n">
+        <v>20.8494148952502</v>
+      </c>
       <c r="Y6" s="1" t="n">
         <v>2</v>
       </c>
@@ -3035,7 +3415,9 @@
       <c r="AB6" s="1" t="n">
         <v>56.8791963881628</v>
       </c>
-      <c r="AC6" s="1"/>
+      <c r="AC6" s="1" t="n">
+        <v>34.2267395010717</v>
+      </c>
       <c r="AE6" s="1" t="n">
         <v>2</v>
       </c>
@@ -3048,7 +3430,9 @@
       <c r="AH6" s="1" t="n">
         <v>100.645138272345</v>
       </c>
-      <c r="AI6" s="1"/>
+      <c r="AI6" s="1" t="n">
+        <v>99.3541384814229</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -3063,7 +3447,9 @@
       <c r="D7" s="1" t="n">
         <v>0.481408702746925</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1" t="n">
+        <v>4.65107028542448</v>
+      </c>
       <c r="G7" s="1" t="n">
         <v>3</v>
       </c>
@@ -3076,7 +3462,9 @@
       <c r="J7" s="1" t="n">
         <v>8.72027586987487</v>
       </c>
-      <c r="K7" s="1"/>
+      <c r="K7" s="1" t="n">
+        <v>10.3894495177343</v>
+      </c>
       <c r="M7" s="1" t="n">
         <v>3</v>
       </c>
@@ -3089,7 +3477,9 @@
       <c r="P7" s="1" t="n">
         <v>0.00954222522006987</v>
       </c>
-      <c r="Q7" s="1"/>
+      <c r="Q7" s="1" t="n">
+        <v>10.4718614718615</v>
+      </c>
       <c r="S7" s="1" t="n">
         <v>3</v>
       </c>
@@ -3102,7 +3492,9 @@
       <c r="V7" s="1" t="n">
         <v>25.214903509635</v>
       </c>
-      <c r="W7" s="1"/>
+      <c r="W7" s="1" t="n">
+        <v>24.913891238825</v>
+      </c>
       <c r="Y7" s="1" t="n">
         <v>3</v>
       </c>
@@ -3115,7 +3507,9 @@
       <c r="AB7" s="1" t="n">
         <v>43.5115946070976</v>
       </c>
-      <c r="AC7" s="1"/>
+      <c r="AC7" s="1" t="n">
+        <v>35.7021759371363</v>
+      </c>
       <c r="AE7" s="1" t="n">
         <v>3</v>
       </c>
@@ -3128,7 +3522,9 @@
       <c r="AH7" s="1" t="n">
         <v>109.534647516568</v>
       </c>
-      <c r="AI7" s="1"/>
+      <c r="AI7" s="1" t="n">
+        <v>100.829629833458</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -3143,7 +3539,9 @@
       <c r="D8" s="1" t="n">
         <v>0.468870662844844</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1" t="n">
+        <v>3.82931928996756</v>
+      </c>
       <c r="G8" s="1" t="n">
         <v>4</v>
       </c>
@@ -3156,7 +3554,9 @@
       <c r="J8" s="1" t="n">
         <v>7.02223709287943</v>
       </c>
-      <c r="K8" s="1"/>
+      <c r="K8" s="1" t="n">
+        <v>13.3438129915241</v>
+      </c>
       <c r="M8" s="1" t="n">
         <v>4</v>
       </c>
@@ -3169,7 +3569,9 @@
       <c r="P8" s="1" t="n">
         <v>0.00658909134258057</v>
       </c>
-      <c r="Q8" s="1"/>
+      <c r="Q8" s="1" t="n">
+        <v>12.3777056277056</v>
+      </c>
       <c r="S8" s="1" t="n">
         <v>4</v>
       </c>
@@ -3182,7 +3584,9 @@
       <c r="V8" s="1" t="n">
         <v>23.344328381004</v>
       </c>
-      <c r="W8" s="1"/>
+      <c r="W8" s="1" t="n">
+        <v>23.1938098293613</v>
+      </c>
       <c r="Y8" s="1" t="n">
         <v>4</v>
       </c>
@@ -3195,7 +3599,9 @@
       <c r="AB8" s="1" t="n">
         <v>44.3546965713396</v>
       </c>
-      <c r="AC8" s="1"/>
+      <c r="AC8" s="1" t="n">
+        <v>34.0174226317887</v>
+      </c>
       <c r="AE8" s="1" t="n">
         <v>4</v>
       </c>
@@ -3208,7 +3614,9 @@
       <c r="AH8" s="1" t="n">
         <v>111.330072987575</v>
       </c>
-      <c r="AI8" s="1"/>
+      <c r="AI8" s="1" t="n">
+        <v>97.8740999775604</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -3223,7 +3631,9 @@
       <c r="D9" s="1" t="n">
         <v>0.427575784302547</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1" t="n">
+        <v>3.81418034113879</v>
+      </c>
       <c r="G9" s="1" t="n">
         <v>5</v>
       </c>
@@ -3236,7 +3646,9 @@
       <c r="J9" s="1" t="n">
         <v>6.66694197740062</v>
       </c>
-      <c r="K9" s="1"/>
+      <c r="K9" s="1" t="n">
+        <v>11.8160971055406</v>
+      </c>
       <c r="M9" s="1" t="n">
         <v>5</v>
       </c>
@@ -3249,7 +3661,9 @@
       <c r="P9" s="1" t="n">
         <v>0.00998655896829703</v>
       </c>
-      <c r="Q9" s="1"/>
+      <c r="Q9" s="1" t="n">
+        <v>12.3344155844156</v>
+      </c>
       <c r="S9" s="1" t="n">
         <v>5</v>
       </c>
@@ -3262,7 +3676,9 @@
       <c r="V9" s="1" t="n">
         <v>21.3600573163621</v>
       </c>
-      <c r="W9" s="1"/>
+      <c r="W9" s="1" t="n">
+        <v>25.2387139070958</v>
+      </c>
       <c r="Y9" s="1" t="n">
         <v>5</v>
       </c>
@@ -3275,7 +3691,9 @@
       <c r="AB9" s="1" t="n">
         <v>39.9608424153256</v>
       </c>
-      <c r="AC9" s="1"/>
+      <c r="AC9" s="1" t="n">
+        <v>33.8301733255812</v>
+      </c>
       <c r="AE9" s="1" t="n">
         <v>5</v>
       </c>
@@ -3288,7 +3706,9 @@
       <c r="AH9" s="1" t="n">
         <v>115.482260099676</v>
       </c>
-      <c r="AI9" s="1"/>
+      <c r="AI9" s="1" t="n">
+        <v>102.903595886471</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -3303,7 +3723,9 @@
       <c r="D10" s="1" t="n">
         <v>0.592937381169602</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1" t="n">
+        <v>4.76013420097486</v>
+      </c>
       <c r="G10" s="1" t="n">
         <v>6</v>
       </c>
@@ -3316,7 +3738,9 @@
       <c r="J10" s="1" t="n">
         <v>7.22082879357438</v>
       </c>
-      <c r="K10" s="1"/>
+      <c r="K10" s="1" t="n">
+        <v>11.2317336002836</v>
+      </c>
       <c r="M10" s="1" t="n">
         <v>6</v>
       </c>
@@ -3329,7 +3753,9 @@
       <c r="P10" s="1" t="n">
         <v>0.0126120199306419</v>
       </c>
-      <c r="Q10" s="1"/>
+      <c r="Q10" s="1" t="n">
+        <v>11.8030303030303</v>
+      </c>
       <c r="S10" s="1" t="n">
         <v>6</v>
       </c>
@@ -3342,7 +3768,9 @@
       <c r="V10" s="1" t="n">
         <v>31.9749734404252</v>
       </c>
-      <c r="W10" s="1"/>
+      <c r="W10" s="1" t="n">
+        <v>24.0671993292773</v>
+      </c>
       <c r="Y10" s="1" t="n">
         <v>6</v>
       </c>
@@ -3355,7 +3783,9 @@
       <c r="AB10" s="1" t="n">
         <v>42.5361701756123</v>
       </c>
-      <c r="AC10" s="1"/>
+      <c r="AC10" s="1" t="n">
+        <v>39.1827619462851</v>
+      </c>
       <c r="AE10" s="1" t="n">
         <v>6</v>
       </c>
@@ -3368,7 +3798,9 @@
       <c r="AH10" s="1" t="n">
         <v>104.549662565679</v>
       </c>
-      <c r="AI10" s="1"/>
+      <c r="AI10" s="1" t="n">
+        <v>101.434701585534</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -3383,7 +3815,9 @@
       <c r="D11" s="1" t="n">
         <v>0.658855462240024</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1" t="n">
+        <v>4.11185946179996</v>
+      </c>
       <c r="G11" s="1" t="n">
         <v>7</v>
       </c>
@@ -3396,7 +3830,9 @@
       <c r="J11" s="1" t="n">
         <v>8.9024903826171</v>
       </c>
-      <c r="K11" s="1"/>
+      <c r="K11" s="1" t="n">
+        <v>10.3002926304806</v>
+      </c>
       <c r="M11" s="1" t="n">
         <v>7</v>
       </c>
@@ -3409,7 +3845,9 @@
       <c r="P11" s="1" t="n">
         <v>0.00912041201031855</v>
       </c>
-      <c r="Q11" s="1"/>
+      <c r="Q11" s="1" t="n">
+        <v>11.7012987012987</v>
+      </c>
       <c r="S11" s="1" t="n">
         <v>7</v>
       </c>
@@ -3422,7 +3860,9 @@
       <c r="V11" s="1" t="n">
         <v>25.083752108097</v>
       </c>
-      <c r="W11" s="1"/>
+      <c r="W11" s="1" t="n">
+        <v>25.1376584798296</v>
+      </c>
       <c r="Y11" s="1" t="n">
         <v>7</v>
       </c>
@@ -3435,7 +3875,9 @@
       <c r="AB11" s="1" t="n">
         <v>34.7211164462704</v>
       </c>
-      <c r="AC11" s="1"/>
+      <c r="AC11" s="1" t="n">
+        <v>33.5158397194745</v>
+      </c>
       <c r="AE11" s="1" t="n">
         <v>7</v>
       </c>
@@ -3448,7 +3890,9 @@
       <c r="AH11" s="1" t="n">
         <v>108.787106598399</v>
       </c>
-      <c r="AI11" s="1"/>
+      <c r="AI11" s="1" t="n">
+        <v>101.865263382158</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -3463,7 +3907,9 @@
       <c r="D12" s="1" t="n">
         <v>0.548885819149942</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1" t="n">
+        <v>3.56610497237953</v>
+      </c>
       <c r="G12" s="1" t="n">
         <v>8</v>
       </c>
@@ -3476,7 +3922,9 @@
       <c r="J12" s="1" t="n">
         <v>7.15807556304447</v>
       </c>
-      <c r="K12" s="1"/>
+      <c r="K12" s="1" t="n">
+        <v>12.2435633282995</v>
+      </c>
       <c r="M12" s="1" t="n">
         <v>8</v>
       </c>
@@ -3489,7 +3937,9 @@
       <c r="P12" s="1" t="n">
         <v>0.0132962081619628</v>
       </c>
-      <c r="Q12" s="1"/>
+      <c r="Q12" s="1" t="n">
+        <v>15.2186147186147</v>
+      </c>
       <c r="S12" s="1" t="n">
         <v>8</v>
       </c>
@@ -3502,7 +3952,9 @@
       <c r="V12" s="1" t="n">
         <v>23.7863577302495</v>
       </c>
-      <c r="W12" s="1"/>
+      <c r="W12" s="1" t="n">
+        <v>23.638813785823</v>
+      </c>
       <c r="Y12" s="1" t="n">
         <v>8</v>
       </c>
@@ -3515,7 +3967,9 @@
       <c r="AB12" s="1" t="n">
         <v>43.1612783271953</v>
       </c>
-      <c r="AC12" s="1"/>
+      <c r="AC12" s="1" t="n">
+        <v>33.7741337605056</v>
+      </c>
       <c r="AE12" s="1" t="n">
         <v>8</v>
       </c>
@@ -3528,7 +3982,9 @@
       <c r="AH12" s="1" t="n">
         <v>115.240928735789</v>
       </c>
-      <c r="AI12" s="1"/>
+      <c r="AI12" s="1" t="n">
+        <v>95.8880302155511</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -3543,7 +3999,9 @@
       <c r="D13" s="1" t="n">
         <v>0.472507916571237</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1" t="n">
+        <v>3.37457920226511</v>
+      </c>
       <c r="G13" s="1" t="n">
         <v>9</v>
       </c>
@@ -3556,7 +4014,9 @@
       <c r="J13" s="1" t="n">
         <v>7.20351347440833</v>
       </c>
-      <c r="K13" s="1"/>
+      <c r="K13" s="1" t="n">
+        <v>10.2132493922338</v>
+      </c>
       <c r="M13" s="1" t="n">
         <v>9</v>
       </c>
@@ -3569,7 +4029,9 @@
       <c r="P13" s="1" t="n">
         <v>0.00582272964296315</v>
       </c>
-      <c r="Q13" s="1"/>
+      <c r="Q13" s="1" t="n">
+        <v>11.5519480519481</v>
+      </c>
       <c r="S13" s="1" t="n">
         <v>9</v>
       </c>
@@ -3582,7 +4044,9 @@
       <c r="V13" s="1" t="n">
         <v>20.4737858219265</v>
       </c>
-      <c r="W13" s="1"/>
+      <c r="W13" s="1" t="n">
+        <v>22.3095693108681</v>
+      </c>
       <c r="Y13" s="1" t="n">
         <v>9</v>
       </c>
@@ -3595,7 +4059,9 @@
       <c r="AB13" s="1" t="n">
         <v>39.8741511411412</v>
       </c>
-      <c r="AC13" s="1"/>
+      <c r="AC13" s="1" t="n">
+        <v>33.5777765007468</v>
+      </c>
       <c r="AE13" s="1" t="n">
         <v>9</v>
       </c>
@@ -3608,7 +4074,9 @@
       <c r="AH13" s="1" t="n">
         <v>114.988021728419</v>
       </c>
-      <c r="AI13" s="1"/>
+      <c r="AI13" s="1" t="n">
+        <v>96.4092145921906</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -3623,7 +4091,9 @@
       <c r="D14" s="1" t="n">
         <v>0.618019705253307</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1" t="n">
+        <v>3.35681575810996</v>
+      </c>
       <c r="G14" s="1" t="n">
         <v>10</v>
       </c>
@@ -3636,7 +4106,9 @@
       <c r="J14" s="1" t="n">
         <v>6.90733866961143</v>
       </c>
-      <c r="K14" s="1"/>
+      <c r="K14" s="1" t="n">
+        <v>12.4819152203576</v>
+      </c>
       <c r="M14" s="1" t="n">
         <v>10</v>
       </c>
@@ -3649,7 +4121,9 @@
       <c r="P14" s="1" t="n">
         <v>0.0120178890807425</v>
       </c>
-      <c r="Q14" s="1"/>
+      <c r="Q14" s="1" t="n">
+        <v>13.3538961038961</v>
+      </c>
       <c r="S14" s="1" t="n">
         <v>10</v>
       </c>
@@ -3662,7 +4136,9 @@
       <c r="V14" s="1" t="n">
         <v>24.2813841050712</v>
       </c>
-      <c r="W14" s="1"/>
+      <c r="W14" s="1" t="n">
+        <v>23.7344500224541</v>
+      </c>
       <c r="Y14" s="1" t="n">
         <v>10</v>
       </c>
@@ -3675,7 +4151,9 @@
       <c r="AB14" s="1" t="n">
         <v>35.2461489306278</v>
       </c>
-      <c r="AC14" s="1"/>
+      <c r="AC14" s="1" t="n">
+        <v>35.3933899935883</v>
+      </c>
       <c r="AE14" s="1" t="n">
         <v>10</v>
       </c>
@@ -3688,7 +4166,9 @@
       <c r="AH14" s="1" t="n">
         <v>110.249513161671</v>
       </c>
-      <c r="AI14" s="1"/>
+      <c r="AI14" s="1" t="n">
+        <v>100.458940540052</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -3703,7 +4183,9 @@
       <c r="D15" s="1" t="n">
         <v>0.379187144395741</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1" t="n">
+        <v>3.71418779222245</v>
+      </c>
       <c r="G15" s="1" t="n">
         <v>11</v>
       </c>
@@ -3716,7 +4198,9 @@
       <c r="J15" s="1" t="n">
         <v>6.71754839110247</v>
       </c>
-      <c r="K15" s="1"/>
+      <c r="K15" s="1" t="n">
+        <v>12.6063468936234</v>
+      </c>
       <c r="M15" s="1" t="n">
         <v>11</v>
       </c>
@@ -3729,7 +4213,9 @@
       <c r="P15" s="1" t="n">
         <v>0.0145563733152976</v>
       </c>
-      <c r="Q15" s="1"/>
+      <c r="Q15" s="1" t="n">
+        <v>9.92532467532468</v>
+      </c>
       <c r="S15" s="1" t="n">
         <v>11</v>
       </c>
@@ -3742,7 +4228,9 @@
       <c r="V15" s="1" t="n">
         <v>21.9475105413206</v>
       </c>
-      <c r="W15" s="1"/>
+      <c r="W15" s="1" t="n">
+        <v>22.5567491285329</v>
+      </c>
       <c r="Y15" s="1" t="n">
         <v>11</v>
       </c>
@@ -3755,7 +4243,9 @@
       <c r="AB15" s="1" t="n">
         <v>49.4064588342828</v>
       </c>
-      <c r="AC15" s="1"/>
+      <c r="AC15" s="1" t="n">
+        <v>34.3802670955847</v>
+      </c>
       <c r="AE15" s="1" t="n">
         <v>11</v>
       </c>
@@ -3768,7 +4258,9 @@
       <c r="AH15" s="1" t="n">
         <v>113.121856131613</v>
       </c>
-      <c r="AI15" s="1"/>
+      <c r="AI15" s="1" t="n">
+        <v>100.312339551001</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -3783,7 +4275,9 @@
       <c r="D16" s="1" t="n">
         <v>0.455424492108553</v>
       </c>
-      <c r="E16" s="1"/>
+      <c r="E16" s="1" t="n">
+        <v>4.60320819017459</v>
+      </c>
       <c r="G16" s="1" t="n">
         <v>12</v>
       </c>
@@ -3796,7 +4290,9 @@
       <c r="J16" s="1" t="n">
         <v>7.88893413668511</v>
       </c>
-      <c r="K16" s="1"/>
+      <c r="K16" s="1" t="n">
+        <v>10.2624626581717</v>
+      </c>
       <c r="M16" s="1" t="n">
         <v>12</v>
       </c>
@@ -3809,7 +4305,9 @@
       <c r="P16" s="1" t="n">
         <v>0.0159035195835857</v>
       </c>
-      <c r="Q16" s="1"/>
+      <c r="Q16" s="1" t="n">
+        <v>14.4729437229437</v>
+      </c>
       <c r="S16" s="1" t="n">
         <v>12</v>
       </c>
@@ -3822,7 +4320,9 @@
       <c r="V16" s="1" t="n">
         <v>23.1770918839151</v>
       </c>
-      <c r="W16" s="1"/>
+      <c r="W16" s="1" t="n">
+        <v>22.0719436260236</v>
+      </c>
       <c r="Y16" s="1" t="n">
         <v>12</v>
       </c>
@@ -3835,7 +4335,9 @@
       <c r="AB16" s="1" t="n">
         <v>34.1356068723382</v>
       </c>
-      <c r="AC16" s="1"/>
+      <c r="AC16" s="1" t="n">
+        <v>35.9397031311104</v>
+      </c>
       <c r="AE16" s="1" t="n">
         <v>12</v>
       </c>
@@ -3848,7 +4350,9 @@
       <c r="AH16" s="1" t="n">
         <v>118.11538578629</v>
       </c>
-      <c r="AI16" s="1"/>
+      <c r="AI16" s="1" t="n">
+        <v>99.5527768185965</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -3863,7 +4367,9 @@
       <c r="D17" s="1" t="n">
         <v>0.52765246383826</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1" t="n">
+        <v>3.9866507961255</v>
+      </c>
       <c r="G17" s="1" t="n">
         <v>13</v>
       </c>
@@ -3876,7 +4382,9 @@
       <c r="J17" s="1" t="n">
         <v>7.23451975460391</v>
       </c>
-      <c r="K17" s="1"/>
+      <c r="K17" s="1" t="n">
+        <v>12.9495553540881</v>
+      </c>
       <c r="M17" s="1" t="n">
         <v>13</v>
       </c>
@@ -3889,7 +4397,9 @@
       <c r="P17" s="1" t="n">
         <v>0.00710278339438819</v>
       </c>
-      <c r="Q17" s="1"/>
+      <c r="Q17" s="1" t="n">
+        <v>13.6071428571429</v>
+      </c>
       <c r="S17" s="1" t="n">
         <v>13</v>
       </c>
@@ -3902,7 +4412,9 @@
       <c r="V17" s="1" t="n">
         <v>20.6270540795013</v>
       </c>
-      <c r="W17" s="1"/>
+      <c r="W17" s="1" t="n">
+        <v>23.1784876765705</v>
+      </c>
       <c r="Y17" s="1" t="n">
         <v>13</v>
       </c>
@@ -3915,7 +4427,9 @@
       <c r="AB17" s="1" t="n">
         <v>42.5225745143925</v>
       </c>
-      <c r="AC17" s="1"/>
+      <c r="AC17" s="1" t="n">
+        <v>34.2228498419607</v>
+      </c>
       <c r="AE17" s="1" t="n">
         <v>13</v>
       </c>
@@ -3928,7 +4442,9 @@
       <c r="AH17" s="1" t="n">
         <v>113.564014814867</v>
       </c>
-      <c r="AI17" s="1"/>
+      <c r="AI17" s="1" t="n">
+        <v>104.440388193721</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -3943,7 +4459,9 @@
       <c r="D18" s="1" t="n">
         <v>0.483422218770095</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="1" t="n">
+        <v>4.1233905697312</v>
+      </c>
       <c r="G18" s="1" t="n">
         <v>14</v>
       </c>
@@ -3956,7 +4474,9 @@
       <c r="J18" s="1" t="n">
         <v>7.97081184677852</v>
       </c>
-      <c r="K18" s="1"/>
+      <c r="K18" s="1" t="n">
+        <v>11.6291672215298</v>
+      </c>
       <c r="M18" s="1" t="n">
         <v>14</v>
       </c>
@@ -3969,7 +4489,9 @@
       <c r="P18" s="1" t="n">
         <v>0.00441509811785146</v>
       </c>
-      <c r="Q18" s="1"/>
+      <c r="Q18" s="1" t="n">
+        <v>11.5227272727273</v>
+      </c>
       <c r="S18" s="1" t="n">
         <v>14</v>
       </c>
@@ -3982,7 +4504,9 @@
       <c r="V18" s="1" t="n">
         <v>23.0466107895804</v>
       </c>
-      <c r="W18" s="1"/>
+      <c r="W18" s="1" t="n">
+        <v>20.1144145143151</v>
+      </c>
       <c r="Y18" s="1" t="n">
         <v>14</v>
       </c>
@@ -3995,7 +4519,9 @@
       <c r="AB18" s="1" t="n">
         <v>35.9292099112492</v>
       </c>
-      <c r="AC18" s="1"/>
+      <c r="AC18" s="1" t="n">
+        <v>35.2889269293415</v>
+      </c>
       <c r="AE18" s="1" t="n">
         <v>14</v>
       </c>
@@ -4008,7 +4534,9 @@
       <c r="AH18" s="1" t="n">
         <v>108.855288013744</v>
       </c>
-      <c r="AI18" s="1"/>
+      <c r="AI18" s="1" t="n">
+        <v>98.2196691087821</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -4023,7 +4551,9 @@
       <c r="D19" s="1" t="n">
         <v>0.500511677445584</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1" t="n">
+        <v>4.3777220644171</v>
+      </c>
       <c r="G19" s="1" t="n">
         <v>15</v>
       </c>
@@ -4036,7 +4566,9 @@
       <c r="J19" s="1" t="n">
         <v>7.18214154009277</v>
       </c>
-      <c r="K19" s="1"/>
+      <c r="K19" s="1" t="n">
+        <v>11.106290021226</v>
+      </c>
       <c r="M19" s="1" t="n">
         <v>15</v>
       </c>
@@ -4049,7 +4581,9 @@
       <c r="P19" s="1" t="n">
         <v>0.01818648106594</v>
       </c>
-      <c r="Q19" s="1"/>
+      <c r="Q19" s="1" t="n">
+        <v>13.530303030303</v>
+      </c>
       <c r="S19" s="1" t="n">
         <v>15</v>
       </c>
@@ -4062,7 +4596,9 @@
       <c r="V19" s="1" t="n">
         <v>23.6854662287309</v>
       </c>
-      <c r="W19" s="1"/>
+      <c r="W19" s="1" t="n">
+        <v>22.8249340695551</v>
+      </c>
       <c r="Y19" s="1" t="n">
         <v>15</v>
       </c>
@@ -4075,7 +4611,9 @@
       <c r="AB19" s="1" t="n">
         <v>40.706165479993</v>
       </c>
-      <c r="AC19" s="1"/>
+      <c r="AC19" s="1" t="n">
+        <v>35.6583529210787</v>
+      </c>
       <c r="AE19" s="1" t="n">
         <v>15</v>
       </c>
@@ -4088,7 +4626,9 @@
       <c r="AH19" s="1" t="n">
         <v>101.749295674199</v>
       </c>
-      <c r="AI19" s="1"/>
+      <c r="AI19" s="1" t="n">
+        <v>98.619781441511</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -4103,7 +4643,9 @@
       <c r="D20" s="1" t="n">
         <v>0.557703435069758</v>
       </c>
-      <c r="E20" s="1"/>
+      <c r="E20" s="1" t="n">
+        <v>3.31006540509852</v>
+      </c>
       <c r="G20" s="1" t="n">
         <v>16</v>
       </c>
@@ -4116,7 +4658,9 @@
       <c r="J20" s="1" t="n">
         <v>7.03579431960793</v>
       </c>
-      <c r="K20" s="1"/>
+      <c r="K20" s="1" t="n">
+        <v>10.0699775653025</v>
+      </c>
       <c r="M20" s="1" t="n">
         <v>16</v>
       </c>
@@ -4129,7 +4673,9 @@
       <c r="P20" s="1" t="n">
         <v>0.0108448323485213</v>
       </c>
-      <c r="Q20" s="1"/>
+      <c r="Q20" s="1" t="n">
+        <v>12.2987012987013</v>
+      </c>
       <c r="S20" s="1" t="n">
         <v>16</v>
       </c>
@@ -4142,7 +4688,9 @@
       <c r="V20" s="1" t="n">
         <v>22.703099598005</v>
       </c>
-      <c r="W20" s="1"/>
+      <c r="W20" s="1" t="n">
+        <v>22.8747205309333</v>
+      </c>
       <c r="Y20" s="1" t="n">
         <v>16</v>
       </c>
@@ -4155,7 +4703,9 @@
       <c r="AB20" s="1" t="n">
         <v>46.7805609020679</v>
       </c>
-      <c r="AC20" s="1"/>
+      <c r="AC20" s="1" t="n">
+        <v>36.2495599027907</v>
+      </c>
       <c r="AE20" s="1" t="n">
         <v>16</v>
       </c>
@@ -4168,7 +4718,9 @@
       <c r="AH20" s="1" t="n">
         <v>132.73772096689</v>
       </c>
-      <c r="AI20" s="1"/>
+      <c r="AI20" s="1" t="n">
+        <v>99.4626657399853</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
@@ -4183,7 +4735,9 @@
       <c r="D21" s="1" t="n">
         <v>0.400846765841117</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="1" t="n">
+        <v>4.27092982551891</v>
+      </c>
       <c r="G21" s="1" t="n">
         <v>17</v>
       </c>
@@ -4196,7 +4750,9 @@
       <c r="J21" s="1" t="n">
         <v>8.9697148101102</v>
       </c>
-      <c r="K21" s="1"/>
+      <c r="K21" s="1" t="n">
+        <v>11.8830997021792</v>
+      </c>
       <c r="M21" s="1" t="n">
         <v>17</v>
       </c>
@@ -4209,7 +4765,9 @@
       <c r="P21" s="1" t="n">
         <v>0.00557332778673203</v>
       </c>
-      <c r="Q21" s="1"/>
+      <c r="Q21" s="1" t="n">
+        <v>11.9448051948052</v>
+      </c>
       <c r="S21" s="1" t="n">
         <v>17</v>
       </c>
@@ -4222,7 +4780,9 @@
       <c r="V21" s="1" t="n">
         <v>25.7831564234683</v>
       </c>
-      <c r="W21" s="1"/>
+      <c r="W21" s="1" t="n">
+        <v>24.4279113185608</v>
+      </c>
       <c r="Y21" s="1" t="n">
         <v>17</v>
       </c>
@@ -4235,7 +4795,9 @@
       <c r="AB21" s="1" t="n">
         <v>50.0458679202596</v>
       </c>
-      <c r="AC21" s="1"/>
+      <c r="AC21" s="1" t="n">
+        <v>36.2335149381236</v>
+      </c>
       <c r="AE21" s="1" t="n">
         <v>17</v>
       </c>
@@ -4248,7 +4810,9 @@
       <c r="AH21" s="1" t="n">
         <v>111.342476915484</v>
       </c>
-      <c r="AI21" s="1"/>
+      <c r="AI21" s="1" t="n">
+        <v>103.389682395308</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
@@ -4263,7 +4827,9 @@
       <c r="D22" s="1" t="n">
         <v>0.519790381479749</v>
       </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="1" t="n">
+        <v>4.37944535884647</v>
+      </c>
       <c r="G22" s="1" t="n">
         <v>18</v>
       </c>
@@ -4276,7 +4842,9 @@
       <c r="J22" s="1" t="n">
         <v>6.15081395526995</v>
       </c>
-      <c r="K22" s="1"/>
+      <c r="K22" s="1" t="n">
+        <v>11.0413357706442</v>
+      </c>
       <c r="M22" s="1" t="n">
         <v>18</v>
       </c>
@@ -4289,7 +4857,9 @@
       <c r="P22" s="1" t="n">
         <v>0.00863334036598307</v>
       </c>
-      <c r="Q22" s="1"/>
+      <c r="Q22" s="1" t="n">
+        <v>10.8279220779221</v>
+      </c>
       <c r="S22" s="1" t="n">
         <v>18</v>
       </c>
@@ -4302,7 +4872,9 @@
       <c r="V22" s="1" t="n">
         <v>24.9684056893444</v>
       </c>
-      <c r="W22" s="1"/>
+      <c r="W22" s="1" t="n">
+        <v>23.370587628067</v>
+      </c>
       <c r="Y22" s="1" t="n">
         <v>18</v>
       </c>
@@ -4315,7 +4887,9 @@
       <c r="AB22" s="1" t="n">
         <v>47.6054804547907</v>
       </c>
-      <c r="AC22" s="1"/>
+      <c r="AC22" s="1" t="n">
+        <v>32.9958719990987</v>
+      </c>
       <c r="AE22" s="1" t="n">
         <v>18</v>
       </c>
@@ -4328,7 +4902,9 @@
       <c r="AH22" s="1" t="n">
         <v>134.200437377642</v>
       </c>
-      <c r="AI22" s="1"/>
+      <c r="AI22" s="1" t="n">
+        <v>96.2887845221689</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
@@ -4343,7 +4919,9 @@
       <c r="D23" s="1" t="n">
         <v>0.51020726490002</v>
       </c>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1" t="n">
+        <v>3.63079728526111</v>
+      </c>
       <c r="G23" s="1" t="n">
         <v>19</v>
       </c>
@@ -4356,7 +4934,9 @@
       <c r="J23" s="1" t="n">
         <v>7.252785136916</v>
       </c>
-      <c r="K23" s="1"/>
+      <c r="K23" s="1" t="n">
+        <v>10.1515491767327</v>
+      </c>
       <c r="M23" s="1" t="n">
         <v>19</v>
       </c>
@@ -4369,7 +4949,9 @@
       <c r="P23" s="1" t="n">
         <v>0.00950000095646431</v>
       </c>
-      <c r="Q23" s="1"/>
+      <c r="Q23" s="1" t="n">
+        <v>13.2640692640693</v>
+      </c>
       <c r="S23" s="1" t="n">
         <v>19</v>
       </c>
@@ -4382,7 +4964,9 @@
       <c r="V23" s="1" t="n">
         <v>23.5152168609544</v>
       </c>
-      <c r="W23" s="1"/>
+      <c r="W23" s="1" t="n">
+        <v>21.553645460912</v>
+      </c>
       <c r="Y23" s="1" t="n">
         <v>19</v>
       </c>
@@ -4395,7 +4979,9 @@
       <c r="AB23" s="1" t="n">
         <v>45.8929889621378</v>
       </c>
-      <c r="AC23" s="1"/>
+      <c r="AC23" s="1" t="n">
+        <v>34.2355586957329</v>
+      </c>
       <c r="AE23" s="1" t="n">
         <v>19</v>
       </c>
@@ -4408,7 +4994,9 @@
       <c r="AH23" s="1" t="n">
         <v>129.708701350182</v>
       </c>
-      <c r="AI23" s="1"/>
+      <c r="AI23" s="1" t="n">
+        <v>100.076055180818</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
@@ -4423,7 +5011,9 @@
       <c r="D24" s="1" t="n">
         <v>0.492844970287169</v>
       </c>
-      <c r="E24" s="1"/>
+      <c r="E24" s="1" t="n">
+        <v>3.62237728913438</v>
+      </c>
       <c r="G24" s="1" t="n">
         <v>20</v>
       </c>
@@ -4436,7 +5026,9 @@
       <c r="J24" s="1" t="n">
         <v>7.53468933832323</v>
       </c>
-      <c r="K24" s="1"/>
+      <c r="K24" s="1" t="n">
+        <v>10.1925113790138</v>
+      </c>
       <c r="M24" s="1" t="n">
         <v>20</v>
       </c>
@@ -4449,7 +5041,9 @@
       <c r="P24" s="1" t="n">
         <v>0.0110566258988491</v>
       </c>
-      <c r="Q24" s="1"/>
+      <c r="Q24" s="1" t="n">
+        <v>12.3344155844156</v>
+      </c>
       <c r="S24" s="1" t="n">
         <v>20</v>
       </c>
@@ -4462,7 +5056,9 @@
       <c r="V24" s="1" t="n">
         <v>27.4052607206466</v>
       </c>
-      <c r="W24" s="1"/>
+      <c r="W24" s="1" t="n">
+        <v>22.0030776442519</v>
+      </c>
       <c r="Y24" s="1" t="n">
         <v>20</v>
       </c>
@@ -4475,7 +5071,9 @@
       <c r="AB24" s="1" t="n">
         <v>44.7308485654494</v>
       </c>
-      <c r="AC24" s="1"/>
+      <c r="AC24" s="1" t="n">
+        <v>32.0071390588696</v>
+      </c>
       <c r="AE24" s="1" t="n">
         <v>20</v>
       </c>
@@ -4488,7 +5086,9 @@
       <c r="AH24" s="1" t="n">
         <v>113.188766927363</v>
       </c>
-      <c r="AI24" s="1"/>
+      <c r="AI24" s="1" t="n">
+        <v>103.684155380959</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
@@ -4503,7 +5103,9 @@
       <c r="D25" s="1" t="n">
         <v>0.57329346653479</v>
       </c>
-      <c r="E25" s="1"/>
+      <c r="E25" s="1" t="n">
+        <v>4.50541280527137</v>
+      </c>
       <c r="G25" s="1" t="n">
         <v>21</v>
       </c>
@@ -4516,7 +5118,9 @@
       <c r="J25" s="1" t="n">
         <v>6.88799630069767</v>
       </c>
-      <c r="K25" s="1"/>
+      <c r="K25" s="1" t="n">
+        <v>10.8169845010569</v>
+      </c>
       <c r="M25" s="1" t="n">
         <v>21</v>
       </c>
@@ -4529,7 +5133,9 @@
       <c r="P25" s="1" t="n">
         <v>0.0132762132207471</v>
       </c>
-      <c r="Q25" s="1"/>
+      <c r="Q25" s="1" t="n">
+        <v>10.012987012987</v>
+      </c>
       <c r="S25" s="1" t="n">
         <v>21</v>
       </c>
@@ -4542,7 +5148,9 @@
       <c r="V25" s="1" t="n">
         <v>25.3490399637717</v>
       </c>
-      <c r="W25" s="1"/>
+      <c r="W25" s="1" t="n">
+        <v>24.4343266669266</v>
+      </c>
       <c r="Y25" s="1" t="n">
         <v>21</v>
       </c>
@@ -4555,7 +5163,9 @@
       <c r="AB25" s="1" t="n">
         <v>54.2897477531678</v>
       </c>
-      <c r="AC25" s="1"/>
+      <c r="AC25" s="1" t="n">
+        <v>34.3446986415347</v>
+      </c>
       <c r="AE25" s="1" t="n">
         <v>21</v>
       </c>
@@ -4568,7 +5178,9 @@
       <c r="AH25" s="1" t="n">
         <v>106.724272707764</v>
       </c>
-      <c r="AI25" s="1"/>
+      <c r="AI25" s="1" t="n">
+        <v>98.6922171613267</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
@@ -4583,7 +5195,9 @@
       <c r="D26" s="1" t="n">
         <v>0.67172379446274</v>
       </c>
-      <c r="E26" s="1"/>
+      <c r="E26" s="1" t="n">
+        <v>3.46284913101637</v>
+      </c>
       <c r="G26" s="1" t="n">
         <v>22</v>
       </c>
@@ -4596,7 +5210,9 @@
       <c r="J26" s="1" t="n">
         <v>7.27163870535051</v>
       </c>
-      <c r="K26" s="1"/>
+      <c r="K26" s="1" t="n">
+        <v>11.2054252634828</v>
+      </c>
       <c r="M26" s="1" t="n">
         <v>22</v>
       </c>
@@ -4609,7 +5225,9 @@
       <c r="P26" s="1" t="n">
         <v>0.00613231345941223</v>
       </c>
-      <c r="Q26" s="1"/>
+      <c r="Q26" s="1" t="n">
+        <v>13.4458874458874</v>
+      </c>
       <c r="S26" s="1" t="n">
         <v>22</v>
       </c>
@@ -4622,7 +5240,9 @@
       <c r="V26" s="1" t="n">
         <v>24.2493731476316</v>
       </c>
-      <c r="W26" s="1"/>
+      <c r="W26" s="1" t="n">
+        <v>22.4246039876242</v>
+      </c>
       <c r="Y26" s="1" t="n">
         <v>22</v>
       </c>
@@ -4635,7 +5255,9 @@
       <c r="AB26" s="1" t="n">
         <v>38.6803327402936</v>
       </c>
-      <c r="AC26" s="1"/>
+      <c r="AC26" s="1" t="n">
+        <v>35.9678778584726</v>
+      </c>
       <c r="AE26" s="1" t="n">
         <v>22</v>
       </c>
@@ -4648,7 +5270,9 @@
       <c r="AH26" s="1" t="n">
         <v>124.215519526913</v>
       </c>
-      <c r="AI26" s="1"/>
+      <c r="AI26" s="1" t="n">
+        <v>98.8762733303166</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
@@ -4663,7 +5287,9 @@
       <c r="D27" s="1" t="n">
         <v>0.550732469384134</v>
       </c>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1" t="n">
+        <v>3.63029115695811</v>
+      </c>
       <c r="G27" s="1" t="n">
         <v>23</v>
       </c>
@@ -4676,7 +5302,9 @@
       <c r="J27" s="1" t="n">
         <v>7.6762199954275</v>
       </c>
-      <c r="K27" s="1"/>
+      <c r="K27" s="1" t="n">
+        <v>11.9839172731469</v>
+      </c>
       <c r="M27" s="1" t="n">
         <v>23</v>
       </c>
@@ -4689,7 +5317,9 @@
       <c r="P27" s="1" t="n">
         <v>0.0108204275576114</v>
       </c>
-      <c r="Q27" s="1"/>
+      <c r="Q27" s="1" t="n">
+        <v>14.7608225108225</v>
+      </c>
       <c r="S27" s="1" t="n">
         <v>23</v>
       </c>
@@ -4702,7 +5332,9 @@
       <c r="V27" s="1" t="n">
         <v>22.5899776159737</v>
       </c>
-      <c r="W27" s="1"/>
+      <c r="W27" s="1" t="n">
+        <v>24.2955217409372</v>
+      </c>
       <c r="Y27" s="1" t="n">
         <v>23</v>
       </c>
@@ -4715,7 +5347,9 @@
       <c r="AB27" s="1" t="n">
         <v>45.508844490579</v>
       </c>
-      <c r="AC27" s="1"/>
+      <c r="AC27" s="1" t="n">
+        <v>34.5722070481246</v>
+      </c>
       <c r="AE27" s="1" t="n">
         <v>23</v>
       </c>
@@ -4728,7 +5362,9 @@
       <c r="AH27" s="1" t="n">
         <v>125.152625973855</v>
       </c>
-      <c r="AI27" s="1"/>
+      <c r="AI27" s="1" t="n">
+        <v>97.8809758875043</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
@@ -4743,7 +5379,9 @@
       <c r="D28" s="1" t="n">
         <v>0.511558599338394</v>
       </c>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1" t="n">
+        <v>4.32056584180893</v>
+      </c>
       <c r="G28" s="1" t="n">
         <v>24</v>
       </c>
@@ -4756,7 +5394,9 @@
       <c r="J28" s="1" t="n">
         <v>6.73057577183308</v>
       </c>
-      <c r="K28" s="1"/>
+      <c r="K28" s="1" t="n">
+        <v>11.7873788419151</v>
+      </c>
       <c r="M28" s="1" t="n">
         <v>24</v>
       </c>
@@ -4769,7 +5409,9 @@
       <c r="P28" s="1" t="n">
         <v>0.0086252976754464</v>
       </c>
-      <c r="Q28" s="1"/>
+      <c r="Q28" s="1" t="n">
+        <v>12.0909090909091</v>
+      </c>
       <c r="S28" s="1" t="n">
         <v>24</v>
       </c>
@@ -4782,7 +5424,9 @@
       <c r="V28" s="1" t="n">
         <v>28.1405354385361</v>
       </c>
-      <c r="W28" s="1"/>
+      <c r="W28" s="1" t="n">
+        <v>23.3844539546584</v>
+      </c>
       <c r="Y28" s="1" t="n">
         <v>24</v>
       </c>
@@ -4795,7 +5439,9 @@
       <c r="AB28" s="1" t="n">
         <v>38.025350453156</v>
       </c>
-      <c r="AC28" s="1"/>
+      <c r="AC28" s="1" t="n">
+        <v>36.3779001456479</v>
+      </c>
       <c r="AE28" s="1" t="n">
         <v>24</v>
       </c>
@@ -4808,7 +5454,9 @@
       <c r="AH28" s="1" t="n">
         <v>144.314019364</v>
       </c>
-      <c r="AI28" s="1"/>
+      <c r="AI28" s="1" t="n">
+        <v>100.678611793917</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
@@ -4823,7 +5471,9 @@
       <c r="D29" s="1" t="n">
         <v>0.514110922764676</v>
       </c>
-      <c r="E29" s="1"/>
+      <c r="E29" s="1" t="n">
+        <v>4.01893349681224</v>
+      </c>
       <c r="G29" s="1" t="n">
         <v>25</v>
       </c>
@@ -4836,7 +5486,9 @@
       <c r="J29" s="1" t="n">
         <v>6.971452557242</v>
       </c>
-      <c r="K29" s="1"/>
+      <c r="K29" s="1" t="n">
+        <v>8.95520059179743</v>
+      </c>
       <c r="M29" s="1" t="n">
         <v>25</v>
       </c>
@@ -4849,7 +5501,9 @@
       <c r="P29" s="1" t="n">
         <v>0.0116228370113118</v>
       </c>
-      <c r="Q29" s="1"/>
+      <c r="Q29" s="1" t="n">
+        <v>11.4577922077922</v>
+      </c>
       <c r="S29" s="1" t="n">
         <v>25</v>
       </c>
@@ -4862,7 +5516,9 @@
       <c r="V29" s="1" t="n">
         <v>28.9297378983193</v>
       </c>
-      <c r="W29" s="1"/>
+      <c r="W29" s="1" t="n">
+        <v>23.6822545699977</v>
+      </c>
       <c r="Y29" s="1" t="n">
         <v>25</v>
       </c>
@@ -4875,7 +5531,9 @@
       <c r="AB29" s="1" t="n">
         <v>44.5264298591248</v>
       </c>
-      <c r="AC29" s="1"/>
+      <c r="AC29" s="1" t="n">
+        <v>35.3893750552639</v>
+      </c>
       <c r="AE29" s="1" t="n">
         <v>25</v>
       </c>
@@ -4888,7 +5546,9 @@
       <c r="AH29" s="1" t="n">
         <v>106.898216840556</v>
       </c>
-      <c r="AI29" s="1"/>
+      <c r="AI29" s="1" t="n">
+        <v>98.4497456605905</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
@@ -4903,7 +5563,9 @@
       <c r="D30" s="1" t="n">
         <v>0.491304844510723</v>
       </c>
-      <c r="E30" s="1"/>
+      <c r="E30" s="1" t="n">
+        <v>3.82886623439362</v>
+      </c>
       <c r="G30" s="1" t="n">
         <v>26</v>
       </c>
@@ -4916,7 +5578,9 @@
       <c r="J30" s="1" t="n">
         <v>7.72027464620142</v>
       </c>
-      <c r="K30" s="1"/>
+      <c r="K30" s="1" t="n">
+        <v>9.7143150974153</v>
+      </c>
       <c r="M30" s="1" t="n">
         <v>26</v>
       </c>
@@ -4929,7 +5593,9 @@
       <c r="P30" s="1" t="n">
         <v>0.0185635060062133</v>
       </c>
-      <c r="Q30" s="1"/>
+      <c r="Q30" s="1" t="n">
+        <v>12.7316017316017</v>
+      </c>
       <c r="S30" s="1" t="n">
         <v>26</v>
       </c>
@@ -4942,7 +5608,9 @@
       <c r="V30" s="1" t="n">
         <v>25.7735078421167</v>
       </c>
-      <c r="W30" s="1"/>
+      <c r="W30" s="1" t="n">
+        <v>23.6224639504399</v>
+      </c>
       <c r="Y30" s="1" t="n">
         <v>26</v>
       </c>
@@ -4955,7 +5623,9 @@
       <c r="AB30" s="1" t="n">
         <v>43.6493520685917</v>
       </c>
-      <c r="AC30" s="1"/>
+      <c r="AC30" s="1" t="n">
+        <v>35.2323883933084</v>
+      </c>
       <c r="AE30" s="1" t="n">
         <v>26</v>
       </c>
@@ -4968,7 +5638,9 @@
       <c r="AH30" s="1" t="n">
         <v>113.986305574276</v>
       </c>
-      <c r="AI30" s="1"/>
+      <c r="AI30" s="1" t="n">
+        <v>102.040415228321</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
@@ -4983,7 +5655,9 @@
       <c r="D31" s="1" t="n">
         <v>0.557897558867958</v>
       </c>
-      <c r="E31" s="1"/>
+      <c r="E31" s="1" t="n">
+        <v>3.3814124996716</v>
+      </c>
       <c r="G31" s="1" t="n">
         <v>27</v>
       </c>
@@ -4996,7 +5670,9 @@
       <c r="J31" s="1" t="n">
         <v>7.21770899284721</v>
       </c>
-      <c r="K31" s="1"/>
+      <c r="K31" s="1" t="n">
+        <v>9.63861779835719</v>
+      </c>
       <c r="M31" s="1" t="n">
         <v>27</v>
       </c>
@@ -5009,7 +5685,9 @@
       <c r="P31" s="1" t="n">
         <v>0.0143283532712006</v>
       </c>
-      <c r="Q31" s="1"/>
+      <c r="Q31" s="1" t="n">
+        <v>13.0292207792208</v>
+      </c>
       <c r="S31" s="1" t="n">
         <v>27</v>
       </c>
@@ -5022,7 +5700,9 @@
       <c r="V31" s="1" t="n">
         <v>21.8906597981547</v>
       </c>
-      <c r="W31" s="1"/>
+      <c r="W31" s="1" t="n">
+        <v>23.7018903735823</v>
+      </c>
       <c r="Y31" s="1" t="n">
         <v>27</v>
       </c>
@@ -5035,7 +5715,9 @@
       <c r="AB31" s="1" t="n">
         <v>37.1795758511458</v>
       </c>
-      <c r="AC31" s="1"/>
+      <c r="AC31" s="1" t="n">
+        <v>36.4909285987837</v>
+      </c>
       <c r="AE31" s="1" t="n">
         <v>27</v>
       </c>
@@ -5048,7 +5730,9 @@
       <c r="AH31" s="1" t="n">
         <v>139.602033533277</v>
       </c>
-      <c r="AI31" s="1"/>
+      <c r="AI31" s="1" t="n">
+        <v>99.778513962564</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
@@ -5063,7 +5747,9 @@
       <c r="D32" s="1" t="n">
         <v>0.540789091588485</v>
       </c>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1" t="n">
+        <v>4.43227702626672</v>
+      </c>
       <c r="G32" s="1" t="n">
         <v>28</v>
       </c>
@@ -5076,7 +5762,9 @@
       <c r="J32" s="1" t="n">
         <v>7.87065050479848</v>
       </c>
-      <c r="K32" s="1"/>
+      <c r="K32" s="1" t="n">
+        <v>11.3799922455231</v>
+      </c>
       <c r="M32" s="1" t="n">
         <v>28</v>
       </c>
@@ -5089,7 +5777,9 @@
       <c r="P32" s="1" t="n">
         <v>0.0112803570007092</v>
       </c>
-      <c r="Q32" s="1"/>
+      <c r="Q32" s="1" t="n">
+        <v>8.40259740259741</v>
+      </c>
       <c r="S32" s="1" t="n">
         <v>28</v>
       </c>
@@ -5102,7 +5792,9 @@
       <c r="V32" s="1" t="n">
         <v>29.8088519373981</v>
       </c>
-      <c r="W32" s="1"/>
+      <c r="W32" s="1" t="n">
+        <v>23.1938885960891</v>
+      </c>
       <c r="Y32" s="1" t="n">
         <v>28</v>
       </c>
@@ -5115,7 +5807,9 @@
       <c r="AB32" s="1" t="n">
         <v>54.4257689630271</v>
       </c>
-      <c r="AC32" s="1"/>
+      <c r="AC32" s="1" t="n">
+        <v>37.738865363785</v>
+      </c>
       <c r="AE32" s="1" t="n">
         <v>28</v>
       </c>
@@ -5128,7 +5822,9 @@
       <c r="AH32" s="1" t="n">
         <v>114.068169690309</v>
       </c>
-      <c r="AI32" s="1"/>
+      <c r="AI32" s="1" t="n">
+        <v>98.7215913904853</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
@@ -5143,7 +5839,9 @@
       <c r="D33" s="1" t="n">
         <v>0.405036976645196</v>
       </c>
-      <c r="E33" s="1"/>
+      <c r="E33" s="1" t="n">
+        <v>3.68922706061437</v>
+      </c>
       <c r="G33" s="1" t="n">
         <v>29</v>
       </c>
@@ -5156,7 +5854,9 @@
       <c r="J33" s="1" t="n">
         <v>6.43597627472405</v>
       </c>
-      <c r="K33" s="1"/>
+      <c r="K33" s="1" t="n">
+        <v>12.4973866856755</v>
+      </c>
       <c r="M33" s="1" t="n">
         <v>29</v>
       </c>
@@ -5169,7 +5869,9 @@
       <c r="P33" s="1" t="n">
         <v>0.0303242024448904</v>
       </c>
-      <c r="Q33" s="1"/>
+      <c r="Q33" s="1" t="n">
+        <v>9.63419913419913</v>
+      </c>
       <c r="S33" s="1" t="n">
         <v>29</v>
       </c>
@@ -5182,7 +5884,9 @@
       <c r="V33" s="1" t="n">
         <v>22.7931274597943</v>
       </c>
-      <c r="W33" s="1"/>
+      <c r="W33" s="1" t="n">
+        <v>23.9283365825517</v>
+      </c>
       <c r="Y33" s="1" t="n">
         <v>29</v>
       </c>
@@ -5195,7 +5899,9 @@
       <c r="AB33" s="1" t="n">
         <v>49.6941146048501</v>
       </c>
-      <c r="AC33" s="1"/>
+      <c r="AC33" s="1" t="n">
+        <v>35.3247233114784</v>
+      </c>
       <c r="AE33" s="1" t="n">
         <v>29</v>
       </c>
@@ -5208,7 +5914,9 @@
       <c r="AH33" s="1" t="n">
         <v>103.237406530062</v>
       </c>
-      <c r="AI33" s="1"/>
+      <c r="AI33" s="1" t="n">
+        <v>106.388833962106</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
@@ -5223,7 +5931,9 @@
       <c r="D34" s="1" t="n">
         <v>0.526559880376022</v>
       </c>
-      <c r="E34" s="1"/>
+      <c r="E34" s="1" t="n">
+        <v>2.92768173629888</v>
+      </c>
       <c r="G34" s="1" t="n">
         <v>30</v>
       </c>
@@ -5236,7 +5946,9 @@
       <c r="J34" s="1" t="n">
         <v>7.27534935236467</v>
       </c>
-      <c r="K34" s="1"/>
+      <c r="K34" s="1" t="n">
+        <v>10.8845205895149</v>
+      </c>
       <c r="M34" s="1" t="n">
         <v>30</v>
       </c>
@@ -5249,7 +5961,9 @@
       <c r="P34" s="1" t="n">
         <v>0.0104826124108159</v>
       </c>
-      <c r="Q34" s="1"/>
+      <c r="Q34" s="1" t="n">
+        <v>9.44155844155844</v>
+      </c>
       <c r="S34" s="1" t="n">
         <v>30</v>
       </c>
@@ -5262,7 +5976,9 @@
       <c r="V34" s="1" t="n">
         <v>22.2229967953584</v>
       </c>
-      <c r="W34" s="1"/>
+      <c r="W34" s="1" t="n">
+        <v>22.3449782210613</v>
+      </c>
       <c r="Y34" s="1" t="n">
         <v>30</v>
       </c>
@@ -5275,7 +5991,9 @@
       <c r="AB34" s="1" t="n">
         <v>44.2559530231769</v>
       </c>
-      <c r="AC34" s="1"/>
+      <c r="AC34" s="1" t="n">
+        <v>34.5809786478987</v>
+      </c>
       <c r="AE34" s="1" t="n">
         <v>30</v>
       </c>
@@ -5288,7 +6006,9 @@
       <c r="AH34" s="1" t="n">
         <v>142.444408944977</v>
       </c>
-      <c r="AI34" s="1"/>
+      <c r="AI34" s="1" t="n">
+        <v>105.887536795916</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -5322,7 +6042,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Generate results of Improved FWA
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="12">
   <si>
     <t xml:space="preserve">Slump Test</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t xml:space="preserve">FWA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IFWA</t>
   </si>
 </sst>
 </file>
@@ -138,7 +141,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -153,6 +156,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -172,10 +179,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:AI34"/>
+  <dimension ref="A3:AJ34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AD20" activeCellId="0" sqref="AD20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AJ5" activeCellId="0" sqref="AJ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -335,6 +342,9 @@
       <c r="E5" s="1" t="n">
         <v>16.5030848698092</v>
       </c>
+      <c r="F5" s="0" t="n">
+        <v>16.3325383103567</v>
+      </c>
       <c r="G5" s="1" t="n">
         <v>1</v>
       </c>
@@ -350,6 +360,9 @@
       <c r="K5" s="1" t="n">
         <v>42.0063935101198</v>
       </c>
+      <c r="L5" s="0" t="n">
+        <v>45.1048892814417</v>
+      </c>
       <c r="M5" s="1" t="n">
         <v>1</v>
       </c>
@@ -365,6 +378,9 @@
       <c r="Q5" s="1" t="n">
         <v>56.021645021645</v>
       </c>
+      <c r="R5" s="0" t="n">
+        <v>57.9192681122316</v>
+      </c>
       <c r="S5" s="1" t="n">
         <v>1</v>
       </c>
@@ -380,6 +396,9 @@
       <c r="W5" s="1" t="n">
         <v>99.9700038297602</v>
       </c>
+      <c r="X5" s="0" t="n">
+        <v>98.7038274976786</v>
+      </c>
       <c r="Y5" s="1" t="n">
         <v>1</v>
       </c>
@@ -395,6 +414,9 @@
       <c r="AC5" s="1" t="n">
         <v>137.848205525952</v>
       </c>
+      <c r="AD5" s="0" t="n">
+        <v>145.19993302948</v>
+      </c>
       <c r="AE5" s="1" t="n">
         <v>1</v>
       </c>
@@ -409,6 +431,9 @@
       </c>
       <c r="AI5" s="1" t="n">
         <v>411.85958021772</v>
+      </c>
+      <c r="AJ5" s="0" t="n">
+        <v>421.751312193383</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -427,6 +452,9 @@
       <c r="E6" s="1" t="n">
         <v>16.3636548453399</v>
       </c>
+      <c r="F6" s="0" t="n">
+        <v>17.0849082755987</v>
+      </c>
       <c r="G6" s="1" t="n">
         <v>2</v>
       </c>
@@ -442,6 +470,9 @@
       <c r="K6" s="1" t="n">
         <v>42.298970116984</v>
       </c>
+      <c r="L6" s="0" t="n">
+        <v>52.0574103387868</v>
+      </c>
       <c r="M6" s="1" t="n">
         <v>2</v>
       </c>
@@ -457,6 +488,9 @@
       <c r="Q6" s="1" t="n">
         <v>55.4761904761905</v>
       </c>
+      <c r="R6" s="0" t="n">
+        <v>59.5371714794982</v>
+      </c>
       <c r="S6" s="1" t="n">
         <v>2</v>
       </c>
@@ -472,6 +506,9 @@
       <c r="W6" s="1" t="n">
         <v>92.9230553678904</v>
       </c>
+      <c r="X6" s="0" t="n">
+        <v>102.217822005731</v>
+      </c>
       <c r="Y6" s="1" t="n">
         <v>2</v>
       </c>
@@ -487,6 +524,9 @@
       <c r="AC6" s="1" t="n">
         <v>141.225493551861</v>
       </c>
+      <c r="AD6" s="0" t="n">
+        <v>151.432461473046</v>
+      </c>
       <c r="AE6" s="1" t="n">
         <v>2</v>
       </c>
@@ -501,6 +541,9 @@
       </c>
       <c r="AI6" s="1" t="n">
         <v>412.552844799927</v>
+      </c>
+      <c r="AJ6" s="0" t="n">
+        <v>405.51875951572</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -519,6 +562,9 @@
       <c r="E7" s="1" t="n">
         <v>15.7423748443529</v>
       </c>
+      <c r="F7" s="0" t="n">
+        <v>16.6706688214643</v>
+      </c>
       <c r="G7" s="1" t="n">
         <v>3</v>
       </c>
@@ -534,6 +580,9 @@
       <c r="K7" s="1" t="n">
         <v>49.0064771213432</v>
       </c>
+      <c r="L7" s="0" t="n">
+        <v>53.1117601036745</v>
+      </c>
       <c r="M7" s="1" t="n">
         <v>3</v>
       </c>
@@ -549,6 +598,9 @@
       <c r="Q7" s="1" t="n">
         <v>59.254329004329</v>
       </c>
+      <c r="R7" s="0" t="n">
+        <v>61.0266838304414</v>
+      </c>
       <c r="S7" s="1" t="n">
         <v>3</v>
       </c>
@@ -564,6 +616,9 @@
       <c r="W7" s="1" t="n">
         <v>93.1287428395352</v>
       </c>
+      <c r="X7" s="0" t="n">
+        <v>105.317454641669</v>
+      </c>
       <c r="Y7" s="1" t="n">
         <v>3</v>
       </c>
@@ -579,6 +634,9 @@
       <c r="AC7" s="1" t="n">
         <v>135.85820190939</v>
       </c>
+      <c r="AD7" s="0" t="n">
+        <v>143.977858031483</v>
+      </c>
       <c r="AE7" s="1" t="n">
         <v>3</v>
       </c>
@@ -593,6 +651,9 @@
       </c>
       <c r="AI7" s="1" t="n">
         <v>404.468482047801</v>
+      </c>
+      <c r="AJ7" s="0" t="n">
+        <v>405.974324227987</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -611,6 +672,9 @@
       <c r="E8" s="1" t="n">
         <v>16.5179160503601</v>
       </c>
+      <c r="F8" s="0" t="n">
+        <v>16.7964583141245</v>
+      </c>
       <c r="G8" s="1" t="n">
         <v>4</v>
       </c>
@@ -626,6 +690,9 @@
       <c r="K8" s="1" t="n">
         <v>48.6691594219696</v>
       </c>
+      <c r="L8" s="0" t="n">
+        <v>51.0629461908936</v>
+      </c>
       <c r="M8" s="1" t="n">
         <v>4</v>
       </c>
@@ -641,6 +708,9 @@
       <c r="Q8" s="1" t="n">
         <v>57.3484848484849</v>
       </c>
+      <c r="R8" s="0" t="n">
+        <v>55.2306928348189</v>
+      </c>
       <c r="S8" s="1" t="n">
         <v>4</v>
       </c>
@@ -656,6 +726,9 @@
       <c r="W8" s="1" t="n">
         <v>91.7026511561331</v>
       </c>
+      <c r="X8" s="0" t="n">
+        <v>93.5124606877489</v>
+      </c>
       <c r="Y8" s="1" t="n">
         <v>4</v>
       </c>
@@ -671,6 +744,9 @@
       <c r="AC8" s="1" t="n">
         <v>144.401452845659</v>
       </c>
+      <c r="AD8" s="0" t="n">
+        <v>138.139329938364</v>
+      </c>
       <c r="AE8" s="1" t="n">
         <v>4</v>
       </c>
@@ -685,6 +761,9 @@
       </c>
       <c r="AI8" s="1" t="n">
         <v>404.381547707255</v>
+      </c>
+      <c r="AJ8" s="0" t="n">
+        <v>410.355876443291</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -703,6 +782,9 @@
       <c r="E9" s="1" t="n">
         <v>16.5050264408329</v>
       </c>
+      <c r="F9" s="0" t="n">
+        <v>15.5299701915389</v>
+      </c>
       <c r="G9" s="1" t="n">
         <v>5</v>
       </c>
@@ -718,6 +800,9 @@
       <c r="K9" s="1" t="n">
         <v>48.7702764072189</v>
       </c>
+      <c r="L9" s="0" t="n">
+        <v>53.3629902064208</v>
+      </c>
       <c r="M9" s="1" t="n">
         <v>5</v>
       </c>
@@ -733,6 +818,9 @@
       <c r="Q9" s="1" t="n">
         <v>57.3917748917749</v>
       </c>
+      <c r="R9" s="0" t="n">
+        <v>60.4337490245505</v>
+      </c>
       <c r="S9" s="1" t="n">
         <v>5</v>
       </c>
@@ -748,6 +836,9 @@
       <c r="W9" s="1" t="n">
         <v>98.4799475171173</v>
       </c>
+      <c r="X9" s="0" t="n">
+        <v>93.9056105523152</v>
+      </c>
       <c r="Y9" s="1" t="n">
         <v>5</v>
       </c>
@@ -763,6 +854,9 @@
       <c r="AC9" s="1" t="n">
         <v>142.506194837933</v>
       </c>
+      <c r="AD9" s="0" t="n">
+        <v>146.49035508776</v>
+      </c>
       <c r="AE9" s="1" t="n">
         <v>5</v>
       </c>
@@ -777,6 +871,9 @@
       </c>
       <c r="AI9" s="1" t="n">
         <v>402.299435489111</v>
+      </c>
+      <c r="AJ9" s="0" t="n">
+        <v>420.433760539637</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -795,6 +892,9 @@
       <c r="E10" s="1" t="n">
         <v>15.5740604221762</v>
       </c>
+      <c r="F10" s="0" t="n">
+        <v>16.3218491072746</v>
+      </c>
       <c r="G10" s="1" t="n">
         <v>6</v>
       </c>
@@ -810,6 +910,9 @@
       <c r="K10" s="1" t="n">
         <v>40.9908960270192</v>
       </c>
+      <c r="L10" s="0" t="n">
+        <v>50.9138023975579</v>
+      </c>
       <c r="M10" s="1" t="n">
         <v>6</v>
       </c>
@@ -825,6 +928,9 @@
       <c r="Q10" s="1" t="n">
         <v>57.9231601731602</v>
       </c>
+      <c r="R10" s="0" t="n">
+        <v>56.4451749220518</v>
+      </c>
       <c r="S10" s="1" t="n">
         <v>6</v>
       </c>
@@ -840,6 +946,9 @@
       <c r="W10" s="1" t="n">
         <v>96.110181003113</v>
       </c>
+      <c r="X10" s="0" t="n">
+        <v>93.2535405001406</v>
+      </c>
       <c r="Y10" s="1" t="n">
         <v>6</v>
       </c>
@@ -855,6 +964,9 @@
       <c r="AC10" s="1" t="n">
         <v>140.161468920973</v>
       </c>
+      <c r="AD10" s="0" t="n">
+        <v>140.957658927892</v>
+      </c>
       <c r="AE10" s="1" t="n">
         <v>6</v>
       </c>
@@ -869,6 +981,9 @@
       </c>
       <c r="AI10" s="1" t="n">
         <v>408.908346271468</v>
+      </c>
+      <c r="AJ10" s="0" t="n">
+        <v>416.488139471733</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -887,6 +1002,9 @@
       <c r="E11" s="1" t="n">
         <v>16.1820915635907</v>
       </c>
+      <c r="F11" s="0" t="n">
+        <v>15.9677986626871</v>
+      </c>
       <c r="G11" s="1" t="n">
         <v>7</v>
       </c>
@@ -902,6 +1020,9 @@
       <c r="K11" s="1" t="n">
         <v>42.0334800901426</v>
       </c>
+      <c r="L11" s="0" t="n">
+        <v>53.0611441498496</v>
+      </c>
       <c r="M11" s="1" t="n">
         <v>7</v>
       </c>
@@ -917,6 +1038,9 @@
       <c r="Q11" s="1" t="n">
         <v>58.0248917748918</v>
       </c>
+      <c r="R11" s="0" t="n">
+        <v>56.9067014939054</v>
+      </c>
       <c r="S11" s="1" t="n">
         <v>7</v>
       </c>
@@ -932,6 +1056,9 @@
       <c r="W11" s="1" t="n">
         <v>96.4375038144246</v>
       </c>
+      <c r="X11" s="0" t="n">
+        <v>101.574274337409</v>
+      </c>
       <c r="Y11" s="1" t="n">
         <v>7</v>
       </c>
@@ -947,6 +1074,9 @@
       <c r="AC11" s="1" t="n">
         <v>141.25501035956</v>
       </c>
+      <c r="AD11" s="0" t="n">
+        <v>143.266479479298</v>
+      </c>
       <c r="AE11" s="1" t="n">
         <v>7</v>
       </c>
@@ -961,6 +1091,9 @@
       </c>
       <c r="AI11" s="1" t="n">
         <v>400.897857438442</v>
+      </c>
+      <c r="AJ11" s="0" t="n">
+        <v>406.209435678826</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -979,6 +1112,9 @@
       <c r="E12" s="1" t="n">
         <v>16.7319004646364</v>
       </c>
+      <c r="F12" s="0" t="n">
+        <v>16.3507972732355</v>
+      </c>
       <c r="G12" s="1" t="n">
         <v>8</v>
       </c>
@@ -994,6 +1130,9 @@
       <c r="K12" s="1" t="n">
         <v>47.8166725636624</v>
       </c>
+      <c r="L12" s="0" t="n">
+        <v>55.871848587368</v>
+      </c>
       <c r="M12" s="1" t="n">
         <v>8</v>
       </c>
@@ -1009,6 +1148,9 @@
       <c r="Q12" s="1" t="n">
         <v>54.5075757575758</v>
       </c>
+      <c r="R12" s="0" t="n">
+        <v>57.7621035582966</v>
+      </c>
       <c r="S12" s="1" t="n">
         <v>8</v>
       </c>
@@ -1024,6 +1166,9 @@
       <c r="W12" s="1" t="n">
         <v>95.517335662529</v>
       </c>
+      <c r="X12" s="0" t="n">
+        <v>92.759185026295</v>
+      </c>
       <c r="Y12" s="1" t="n">
         <v>8</v>
       </c>
@@ -1039,6 +1184,9 @@
       <c r="AC12" s="1" t="n">
         <v>136.260311228425</v>
       </c>
+      <c r="AD12" s="0" t="n">
+        <v>140.071352720745</v>
+      </c>
       <c r="AE12" s="1" t="n">
         <v>8</v>
       </c>
@@ -1053,6 +1201,9 @@
       </c>
       <c r="AI12" s="1" t="n">
         <v>410.064977507151</v>
+      </c>
+      <c r="AJ12" s="0" t="n">
+        <v>407.647110510839</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1071,6 +1222,9 @@
       <c r="E13" s="1" t="n">
         <v>16.9288628351031</v>
       </c>
+      <c r="F13" s="0" t="n">
+        <v>16.7798856016198</v>
+      </c>
       <c r="G13" s="1" t="n">
         <v>9</v>
       </c>
@@ -1086,6 +1240,9 @@
       <c r="K13" s="1" t="n">
         <v>49.9924987547251</v>
       </c>
+      <c r="L13" s="0" t="n">
+        <v>43.8780433179959</v>
+      </c>
       <c r="M13" s="1" t="n">
         <v>9</v>
       </c>
@@ -1101,6 +1258,9 @@
       <c r="Q13" s="1" t="n">
         <v>58.1742424242424</v>
       </c>
+      <c r="R13" s="0" t="n">
+        <v>55.5545602405037</v>
+      </c>
       <c r="S13" s="1" t="n">
         <v>9</v>
       </c>
@@ -1116,6 +1276,9 @@
       <c r="W13" s="1" t="n">
         <v>92.6693493259238</v>
       </c>
+      <c r="X13" s="0" t="n">
+        <v>95.7943922925706</v>
+      </c>
       <c r="Y13" s="1" t="n">
         <v>9</v>
       </c>
@@ -1131,6 +1294,9 @@
       <c r="AC13" s="1" t="n">
         <v>141.641622086995</v>
       </c>
+      <c r="AD13" s="0" t="n">
+        <v>141.244883473383</v>
+      </c>
       <c r="AE13" s="1" t="n">
         <v>9</v>
       </c>
@@ -1145,6 +1311,9 @@
       </c>
       <c r="AI13" s="1" t="n">
         <v>408.260366886559</v>
+      </c>
+      <c r="AJ13" s="0" t="n">
+        <v>415.805905089662</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1163,6 +1332,9 @@
       <c r="E14" s="1" t="n">
         <v>16.911568075489</v>
       </c>
+      <c r="F14" s="0" t="n">
+        <v>16.4954445020065</v>
+      </c>
       <c r="G14" s="1" t="n">
         <v>10</v>
       </c>
@@ -1178,6 +1350,9 @@
       <c r="K14" s="1" t="n">
         <v>39.759723613396</v>
       </c>
+      <c r="L14" s="0" t="n">
+        <v>47.3463737114752</v>
+      </c>
       <c r="M14" s="1" t="n">
         <v>10</v>
       </c>
@@ -1193,6 +1368,9 @@
       <c r="Q14" s="1" t="n">
         <v>56.3722943722944</v>
       </c>
+      <c r="R14" s="0" t="n">
+        <v>59.3879472248264</v>
+      </c>
       <c r="S14" s="1" t="n">
         <v>10</v>
       </c>
@@ -1208,6 +1386,9 @@
       <c r="W14" s="1" t="n">
         <v>88.648013391956</v>
       </c>
+      <c r="X14" s="0" t="n">
+        <v>91.9643322124583</v>
+      </c>
       <c r="Y14" s="1" t="n">
         <v>10</v>
       </c>
@@ -1223,6 +1404,9 @@
       <c r="AC14" s="1" t="n">
         <v>144.098701003625</v>
       </c>
+      <c r="AD14" s="0" t="n">
+        <v>155.546407298707</v>
+      </c>
       <c r="AE14" s="1" t="n">
         <v>10</v>
       </c>
@@ -1237,6 +1421,9 @@
       </c>
       <c r="AI14" s="1" t="n">
         <v>402.881200744287</v>
+      </c>
+      <c r="AJ14" s="0" t="n">
+        <v>400.876175242336</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1255,6 +1442,9 @@
       <c r="E15" s="1" t="n">
         <v>16.7849264141599</v>
       </c>
+      <c r="F15" s="0" t="n">
+        <v>17.2738466411454</v>
+      </c>
       <c r="G15" s="1" t="n">
         <v>11</v>
       </c>
@@ -1270,6 +1460,9 @@
       <c r="K15" s="1" t="n">
         <v>46.976882552876</v>
       </c>
+      <c r="L15" s="0" t="n">
+        <v>52.4311335685765</v>
+      </c>
       <c r="M15" s="1" t="n">
         <v>11</v>
       </c>
@@ -1285,6 +1478,9 @@
       <c r="Q15" s="1" t="n">
         <v>59.8008658008658</v>
       </c>
+      <c r="R15" s="0" t="n">
+        <v>57.3017931507866</v>
+      </c>
       <c r="S15" s="1" t="n">
         <v>11</v>
       </c>
@@ -1300,6 +1496,9 @@
       <c r="W15" s="1" t="n">
         <v>91.6700747848336</v>
       </c>
+      <c r="X15" s="0" t="n">
+        <v>93.1952749528969</v>
+      </c>
       <c r="Y15" s="1" t="n">
         <v>11</v>
       </c>
@@ -1315,6 +1514,9 @@
       <c r="AC15" s="1" t="n">
         <v>142.777771511148</v>
       </c>
+      <c r="AD15" s="0" t="n">
+        <v>145.946174904208</v>
+      </c>
       <c r="AE15" s="1" t="n">
         <v>11</v>
       </c>
@@ -1329,6 +1531,9 @@
       </c>
       <c r="AI15" s="1" t="n">
         <v>406.099540654943</v>
+      </c>
+      <c r="AJ15" s="0" t="n">
+        <v>411.445847493356</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1347,6 +1552,9 @@
       <c r="E16" s="1" t="n">
         <v>15.6749472497569</v>
       </c>
+      <c r="F16" s="0" t="n">
+        <v>16.7633852596219</v>
+      </c>
       <c r="G16" s="1" t="n">
         <v>12</v>
       </c>
@@ -1362,6 +1570,9 @@
       <c r="K16" s="1" t="n">
         <v>51.7745233807341</v>
       </c>
+      <c r="L16" s="0" t="n">
+        <v>49.1799197705609</v>
+      </c>
       <c r="M16" s="1" t="n">
         <v>12</v>
       </c>
@@ -1377,6 +1588,9 @@
       <c r="Q16" s="1" t="n">
         <v>55.2532467532468</v>
       </c>
+      <c r="R16" s="0" t="n">
+        <v>58.4087772260198</v>
+      </c>
       <c r="S16" s="1" t="n">
         <v>12</v>
       </c>
@@ -1392,6 +1606,9 @@
       <c r="W16" s="1" t="n">
         <v>91.8255311138901</v>
       </c>
+      <c r="X16" s="0" t="n">
+        <v>105.84956065751</v>
+      </c>
       <c r="Y16" s="1" t="n">
         <v>12</v>
       </c>
@@ -1407,6 +1624,9 @@
       <c r="AC16" s="1" t="n">
         <v>142.817849088031</v>
       </c>
+      <c r="AD16" s="0" t="n">
+        <v>143.047463827957</v>
+      </c>
       <c r="AE16" s="1" t="n">
         <v>12</v>
       </c>
@@ -1421,6 +1641,9 @@
       </c>
       <c r="AI16" s="1" t="n">
         <v>406.747245826201</v>
+      </c>
+      <c r="AJ16" s="0" t="n">
+        <v>411.085245794968</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1439,6 +1662,9 @@
       <c r="E17" s="1" t="n">
         <v>16.5665462238615</v>
       </c>
+      <c r="F17" s="0" t="n">
+        <v>16.5749456445098</v>
+      </c>
       <c r="G17" s="1" t="n">
         <v>13</v>
       </c>
@@ -1454,6 +1680,9 @@
       <c r="K17" s="1" t="n">
         <v>48.3859069546796</v>
       </c>
+      <c r="L17" s="0" t="n">
+        <v>52.4010684292365</v>
+      </c>
       <c r="M17" s="1" t="n">
         <v>13</v>
       </c>
@@ -1469,6 +1698,9 @@
       <c r="Q17" s="1" t="n">
         <v>56.1190476190476</v>
       </c>
+      <c r="R17" s="0" t="n">
+        <v>57.3884423170586</v>
+      </c>
       <c r="S17" s="1" t="n">
         <v>13</v>
       </c>
@@ -1484,6 +1716,9 @@
       <c r="W17" s="1" t="n">
         <v>97.0782098573344</v>
       </c>
+      <c r="X17" s="0" t="n">
+        <v>92.14031964826</v>
+      </c>
       <c r="Y17" s="1" t="n">
         <v>13</v>
       </c>
@@ -1499,6 +1734,9 @@
       <c r="AC17" s="1" t="n">
         <v>141.26285648652</v>
       </c>
+      <c r="AD17" s="0" t="n">
+        <v>151.405618260606</v>
+      </c>
       <c r="AE17" s="1" t="n">
         <v>13</v>
       </c>
@@ -1513,6 +1751,9 @@
       </c>
       <c r="AI17" s="1" t="n">
         <v>402.540866275494</v>
+      </c>
+      <c r="AJ17" s="0" t="n">
+        <v>406.645292016447</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1531,6 +1772,9 @@
       <c r="E18" s="1" t="n">
         <v>16.1628937071012</v>
       </c>
+      <c r="F18" s="0" t="n">
+        <v>16.288581545864</v>
+      </c>
       <c r="G18" s="1" t="n">
         <v>14</v>
       </c>
@@ -1546,6 +1790,9 @@
       <c r="K18" s="1" t="n">
         <v>46.8831778915452</v>
       </c>
+      <c r="L18" s="0" t="n">
+        <v>52.2919185304945</v>
+      </c>
       <c r="M18" s="1" t="n">
         <v>14</v>
       </c>
@@ -1561,6 +1808,9 @@
       <c r="Q18" s="1" t="n">
         <v>58.2034632034632</v>
       </c>
+      <c r="R18" s="0" t="n">
+        <v>57.177033052845</v>
+      </c>
       <c r="S18" s="1" t="n">
         <v>14</v>
       </c>
@@ -1576,6 +1826,9 @@
       <c r="W18" s="1" t="n">
         <v>92.5112526904534</v>
       </c>
+      <c r="X18" s="0" t="n">
+        <v>101.092808603485</v>
+      </c>
       <c r="Y18" s="1" t="n">
         <v>14</v>
       </c>
@@ -1591,6 +1844,9 @@
       <c r="AC18" s="1" t="n">
         <v>144.948762230008</v>
       </c>
+      <c r="AD18" s="0" t="n">
+        <v>142.234999404134</v>
+      </c>
       <c r="AE18" s="1" t="n">
         <v>14</v>
       </c>
@@ -1605,6 +1861,9 @@
       </c>
       <c r="AI18" s="1" t="n">
         <v>404.062974881537</v>
+      </c>
+      <c r="AJ18" s="0" t="n">
+        <v>409.028870029143</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1623,6 +1882,9 @@
       <c r="E19" s="1" t="n">
         <v>15.8598167131258</v>
       </c>
+      <c r="F19" s="0" t="n">
+        <v>16.1061685883576</v>
+      </c>
       <c r="G19" s="1" t="n">
         <v>15</v>
       </c>
@@ -1638,6 +1900,9 @@
       <c r="K19" s="1" t="n">
         <v>41.7456414357814</v>
       </c>
+      <c r="L19" s="0" t="n">
+        <v>54.5906716531789</v>
+      </c>
       <c r="M19" s="1" t="n">
         <v>15</v>
       </c>
@@ -1653,6 +1918,9 @@
       <c r="Q19" s="1" t="n">
         <v>56.1958874458875</v>
       </c>
+      <c r="R19" s="0" t="n">
+        <v>60.177213534649</v>
+      </c>
       <c r="S19" s="1" t="n">
         <v>15</v>
       </c>
@@ -1668,6 +1936,9 @@
       <c r="W19" s="1" t="n">
         <v>94.5956904834498</v>
       </c>
+      <c r="X19" s="0" t="n">
+        <v>100.351846382332</v>
+      </c>
       <c r="Y19" s="1" t="n">
         <v>15</v>
       </c>
@@ -1683,6 +1954,9 @@
       <c r="AC19" s="1" t="n">
         <v>137.911932042558</v>
       </c>
+      <c r="AD19" s="0" t="n">
+        <v>152.329214752354</v>
+      </c>
       <c r="AE19" s="1" t="n">
         <v>15</v>
       </c>
@@ -1697,6 +1971,9 @@
       </c>
       <c r="AI19" s="1" t="n">
         <v>403.268490756218</v>
+      </c>
+      <c r="AJ19" s="0" t="n">
+        <v>411.71762858644</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1715,6 +1992,9 @@
       <c r="E20" s="1" t="n">
         <v>16.9970942420082</v>
       </c>
+      <c r="F20" s="0" t="n">
+        <v>16.7400864453445</v>
+      </c>
       <c r="G20" s="1" t="n">
         <v>16</v>
       </c>
@@ -1730,6 +2010,9 @@
       <c r="K20" s="1" t="n">
         <v>42.3935034579994</v>
       </c>
+      <c r="L20" s="0" t="n">
+        <v>43.5438063365121</v>
+      </c>
       <c r="M20" s="1" t="n">
         <v>16</v>
       </c>
@@ -1745,6 +2028,9 @@
       <c r="Q20" s="1" t="n">
         <v>57.4274891774892</v>
       </c>
+      <c r="R20" s="0" t="n">
+        <v>60.2185235807032</v>
+      </c>
       <c r="S20" s="1" t="n">
         <v>16</v>
       </c>
@@ -1760,6 +2046,9 @@
       <c r="W20" s="1" t="n">
         <v>95.6969981487667</v>
       </c>
+      <c r="X20" s="0" t="n">
+        <v>95.5556556624275</v>
+      </c>
       <c r="Y20" s="1" t="n">
         <v>16</v>
       </c>
@@ -1775,6 +2064,9 @@
       <c r="AC20" s="1" t="n">
         <v>144.358475421358</v>
       </c>
+      <c r="AD20" s="0" t="n">
+        <v>149.312774696448</v>
+      </c>
       <c r="AE20" s="1" t="n">
         <v>16</v>
       </c>
@@ -1789,6 +2081,9 @@
       </c>
       <c r="AI20" s="1" t="n">
         <v>404.645127972948</v>
+      </c>
+      <c r="AJ20" s="0" t="n">
+        <v>419.10269793902</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1807,6 +2102,9 @@
       <c r="E21" s="1" t="n">
         <v>16.1110690533809</v>
       </c>
+      <c r="F21" s="0" t="n">
+        <v>17.6786904474092</v>
+      </c>
       <c r="G21" s="1" t="n">
         <v>17</v>
       </c>
@@ -1822,6 +2120,9 @@
       <c r="K21" s="1" t="n">
         <v>39.99342590521</v>
       </c>
+      <c r="L21" s="0" t="n">
+        <v>57.2986408610424</v>
+      </c>
       <c r="M21" s="1" t="n">
         <v>17</v>
       </c>
@@ -1837,6 +2138,9 @@
       <c r="Q21" s="1" t="n">
         <v>57.7813852813853</v>
       </c>
+      <c r="R21" s="0" t="n">
+        <v>57.940516190306</v>
+      </c>
       <c r="S21" s="1" t="n">
         <v>17</v>
       </c>
@@ -1852,6 +2156,9 @@
       <c r="W21" s="1" t="n">
         <v>100.404388667312</v>
       </c>
+      <c r="X21" s="0" t="n">
+        <v>101.897875695908</v>
+      </c>
       <c r="Y21" s="1" t="n">
         <v>17</v>
       </c>
@@ -1867,6 +2174,9 @@
       <c r="AC21" s="1" t="n">
         <v>142.617405244438</v>
       </c>
+      <c r="AD21" s="0" t="n">
+        <v>145.120184270581</v>
+      </c>
       <c r="AE21" s="1" t="n">
         <v>17</v>
       </c>
@@ -1881,6 +2191,9 @@
       </c>
       <c r="AI21" s="1" t="n">
         <v>405.18327757672</v>
+      </c>
+      <c r="AJ21" s="0" t="n">
+        <v>417.479044266336</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1899,6 +2212,9 @@
       <c r="E22" s="1" t="n">
         <v>15.9728262051465</v>
       </c>
+      <c r="F22" s="0" t="n">
+        <v>16.8438720901158</v>
+      </c>
       <c r="G22" s="1" t="n">
         <v>18</v>
       </c>
@@ -1914,6 +2230,9 @@
       <c r="K22" s="1" t="n">
         <v>45.8211486892593</v>
       </c>
+      <c r="L22" s="0" t="n">
+        <v>49.2710081445473</v>
+      </c>
       <c r="M22" s="1" t="n">
         <v>18</v>
       </c>
@@ -1929,6 +2248,9 @@
       <c r="Q22" s="1" t="n">
         <v>58.8982683982684</v>
       </c>
+      <c r="R22" s="0" t="n">
+        <v>61.6479516383529</v>
+      </c>
       <c r="S22" s="1" t="n">
         <v>18</v>
       </c>
@@ -1944,6 +2266,9 @@
       <c r="W22" s="1" t="n">
         <v>90.4923046312075</v>
       </c>
+      <c r="X22" s="0" t="n">
+        <v>94.7650077568909</v>
+      </c>
       <c r="Y22" s="1" t="n">
         <v>18</v>
       </c>
@@ -1959,6 +2284,9 @@
       <c r="AC22" s="1" t="n">
         <v>144.423294096891</v>
       </c>
+      <c r="AD22" s="0" t="n">
+        <v>145.353629194475</v>
+      </c>
       <c r="AE22" s="1" t="n">
         <v>18</v>
       </c>
@@ -1973,6 +2301,9 @@
       </c>
       <c r="AI22" s="1" t="n">
         <v>406.184259998031</v>
+      </c>
+      <c r="AJ22" s="0" t="n">
+        <v>413.480486731452</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1991,6 +2322,9 @@
       <c r="E23" s="1" t="n">
         <v>16.6886452264954</v>
       </c>
+      <c r="F23" s="0" t="n">
+        <v>16.2969445804419</v>
+      </c>
       <c r="G23" s="1" t="n">
         <v>19</v>
       </c>
@@ -2006,6 +2340,9 @@
       <c r="K23" s="1" t="n">
         <v>47.8368219848362</v>
       </c>
+      <c r="L23" s="0" t="n">
+        <v>48.9886177220259</v>
+      </c>
       <c r="M23" s="1" t="n">
         <v>19</v>
       </c>
@@ -2021,6 +2358,9 @@
       <c r="Q23" s="1" t="n">
         <v>56.4621212121212</v>
       </c>
+      <c r="R23" s="0" t="n">
+        <v>57.6679508309225</v>
+      </c>
       <c r="S23" s="1" t="n">
         <v>19</v>
       </c>
@@ -2036,6 +2376,9 @@
       <c r="W23" s="1" t="n">
         <v>93.6504311445545</v>
       </c>
+      <c r="X23" s="0" t="n">
+        <v>94.2248992710727</v>
+      </c>
       <c r="Y23" s="1" t="n">
         <v>19</v>
       </c>
@@ -2051,6 +2394,9 @@
       <c r="AC23" s="1" t="n">
         <v>133.930225530648</v>
       </c>
+      <c r="AD23" s="0" t="n">
+        <v>144.992144958017</v>
+      </c>
       <c r="AE23" s="1" t="n">
         <v>19</v>
       </c>
@@ -2065,6 +2411,9 @@
       </c>
       <c r="AI23" s="1" t="n">
         <v>405.579361143406</v>
+      </c>
+      <c r="AJ23" s="0" t="n">
+        <v>420.604143636762</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2083,6 +2432,9 @@
       <c r="E24" s="1" t="n">
         <v>16.6679461232927</v>
       </c>
+      <c r="F24" s="0" t="n">
+        <v>17.4752586372412</v>
+      </c>
       <c r="G24" s="1" t="n">
         <v>20</v>
       </c>
@@ -2098,6 +2450,9 @@
       <c r="K24" s="1" t="n">
         <v>43.2020148249544</v>
       </c>
+      <c r="L24" s="0" t="n">
+        <v>52.1999220014213</v>
+      </c>
       <c r="M24" s="1" t="n">
         <v>20</v>
       </c>
@@ -2113,6 +2468,9 @@
       <c r="Q24" s="1" t="n">
         <v>57.3917748917749</v>
       </c>
+      <c r="R24" s="0" t="n">
+        <v>53.7095673475176</v>
+      </c>
       <c r="S24" s="1" t="n">
         <v>20</v>
       </c>
@@ -2128,6 +2486,9 @@
       <c r="W24" s="1" t="n">
         <v>92.6047937925229</v>
       </c>
+      <c r="X24" s="0" t="n">
+        <v>107.602962343052</v>
+      </c>
       <c r="Y24" s="1" t="n">
         <v>20</v>
       </c>
@@ -2143,6 +2504,9 @@
       <c r="AC24" s="1" t="n">
         <v>137.295466458176</v>
       </c>
+      <c r="AD24" s="0" t="n">
+        <v>146.764406939074</v>
+      </c>
       <c r="AE24" s="1" t="n">
         <v>20</v>
       </c>
@@ -2157,6 +2521,9 @@
       </c>
       <c r="AI24" s="1" t="n">
         <v>414.694937397284</v>
+      </c>
+      <c r="AJ24" s="0" t="n">
+        <v>408.02611408608</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2175,6 +2542,9 @@
       <c r="E25" s="1" t="n">
         <v>16.0403320815211</v>
       </c>
+      <c r="F25" s="0" t="n">
+        <v>16.8198568359504</v>
+      </c>
       <c r="G25" s="1" t="n">
         <v>21</v>
       </c>
@@ -2190,6 +2560,9 @@
       <c r="K25" s="1" t="n">
         <v>43.7020414250727</v>
       </c>
+      <c r="L25" s="0" t="n">
+        <v>46.6792019947478</v>
+      </c>
       <c r="M25" s="1" t="n">
         <v>21</v>
       </c>
@@ -2205,6 +2578,9 @@
       <c r="Q25" s="1" t="n">
         <v>59.7132034632035</v>
       </c>
+      <c r="R25" s="0" t="n">
+        <v>58.0693914269817</v>
+      </c>
       <c r="S25" s="1" t="n">
         <v>21</v>
       </c>
@@ -2220,6 +2596,9 @@
       <c r="W25" s="1" t="n">
         <v>98.5391709867703</v>
       </c>
+      <c r="X25" s="0" t="n">
+        <v>93.5278073363832</v>
+      </c>
       <c r="Y25" s="1" t="n">
         <v>21</v>
       </c>
@@ -2235,6 +2614,9 @@
       <c r="AC25" s="1" t="n">
         <v>142.829942650777</v>
       </c>
+      <c r="AD25" s="0" t="n">
+        <v>151.772469958349</v>
+      </c>
       <c r="AE25" s="1" t="n">
         <v>21</v>
       </c>
@@ -2249,6 +2631,9 @@
       </c>
       <c r="AI25" s="1" t="n">
         <v>406.50763399597</v>
+      </c>
+      <c r="AJ25" s="0" t="n">
+        <v>412.931660617666</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2267,6 +2652,9 @@
       <c r="E26" s="1" t="n">
         <v>16.8069187553004</v>
       </c>
+      <c r="F26" s="0" t="n">
+        <v>16.4264927362955</v>
+      </c>
       <c r="G26" s="1" t="n">
         <v>22</v>
       </c>
@@ -2282,6 +2670,9 @@
       <c r="K26" s="1" t="n">
         <v>48.5816855635012</v>
       </c>
+      <c r="L26" s="0" t="n">
+        <v>45.283219707153</v>
+      </c>
       <c r="M26" s="1" t="n">
         <v>22</v>
       </c>
@@ -2297,6 +2688,9 @@
       <c r="Q26" s="1" t="n">
         <v>56.2803030303031</v>
       </c>
+      <c r="R26" s="0" t="n">
+        <v>56.4062758035942</v>
+      </c>
       <c r="S26" s="1" t="n">
         <v>22</v>
       </c>
@@ -2312,6 +2706,9 @@
       <c r="W26" s="1" t="n">
         <v>94.5708014131303</v>
       </c>
+      <c r="X26" s="0" t="n">
+        <v>97.2344448225683</v>
+      </c>
       <c r="Y26" s="1" t="n">
         <v>22</v>
       </c>
@@ -2327,6 +2724,9 @@
       <c r="AC26" s="1" t="n">
         <v>142.891905884991</v>
       </c>
+      <c r="AD26" s="0" t="n">
+        <v>146.554901406837</v>
+      </c>
       <c r="AE26" s="1" t="n">
         <v>22</v>
       </c>
@@ -2341,6 +2741,9 @@
       </c>
       <c r="AI26" s="1" t="n">
         <v>409.239865012197</v>
+      </c>
+      <c r="AJ26" s="0" t="n">
+        <v>414.492608306322</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2359,6 +2762,9 @@
       <c r="E27" s="1" t="n">
         <v>16.6686484421241</v>
       </c>
+      <c r="F27" s="0" t="n">
+        <v>17.0580183393566</v>
+      </c>
       <c r="G27" s="1" t="n">
         <v>23</v>
       </c>
@@ -2374,6 +2780,9 @@
       <c r="K27" s="1" t="n">
         <v>40.8921173524655</v>
       </c>
+      <c r="L27" s="0" t="n">
+        <v>51.0228309954178</v>
+      </c>
       <c r="M27" s="1" t="n">
         <v>23</v>
       </c>
@@ -2389,6 +2798,9 @@
       <c r="Q27" s="1" t="n">
         <v>54.965367965368</v>
       </c>
+      <c r="R27" s="0" t="n">
+        <v>55.9753061569875</v>
+      </c>
       <c r="S27" s="1" t="n">
         <v>23</v>
       </c>
@@ -2404,6 +2816,9 @@
       <c r="W27" s="1" t="n">
         <v>92.8942508123728</v>
       </c>
+      <c r="X27" s="0" t="n">
+        <v>100.956022113259</v>
+      </c>
       <c r="Y27" s="1" t="n">
         <v>23</v>
       </c>
@@ -2419,6 +2834,9 @@
       <c r="AC27" s="1" t="n">
         <v>140.217774122437</v>
       </c>
+      <c r="AD27" s="0" t="n">
+        <v>143.798542318076</v>
+      </c>
       <c r="AE27" s="1" t="n">
         <v>23</v>
       </c>
@@ -2433,6 +2851,9 @@
       </c>
       <c r="AI27" s="1" t="n">
         <v>404.993288576092</v>
+      </c>
+      <c r="AJ27" s="0" t="n">
+        <v>400.945255543971</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2451,6 +2872,9 @@
       <c r="E28" s="1" t="n">
         <v>16.0687452967842</v>
       </c>
+      <c r="F28" s="0" t="n">
+        <v>17.3440465478817</v>
+      </c>
       <c r="G28" s="1" t="n">
         <v>24</v>
       </c>
@@ -2466,6 +2890,9 @@
       <c r="K28" s="1" t="n">
         <v>48.1948592970781</v>
       </c>
+      <c r="L28" s="0" t="n">
+        <v>53.1489178806454</v>
+      </c>
       <c r="M28" s="1" t="n">
         <v>24</v>
       </c>
@@ -2481,6 +2908,9 @@
       <c r="Q28" s="1" t="n">
         <v>57.6352813852814</v>
       </c>
+      <c r="R28" s="0" t="n">
+        <v>56.4408684909584</v>
+      </c>
       <c r="S28" s="1" t="n">
         <v>24</v>
       </c>
@@ -2496,6 +2926,9 @@
       <c r="W28" s="1" t="n">
         <v>89.7008084292804</v>
       </c>
+      <c r="X28" s="0" t="n">
+        <v>93.0117437160441</v>
+      </c>
       <c r="Y28" s="1" t="n">
         <v>24</v>
       </c>
@@ -2511,6 +2944,9 @@
       <c r="AC28" s="1" t="n">
         <v>150.886051866749</v>
       </c>
+      <c r="AD28" s="0" t="n">
+        <v>144.253299679939</v>
+      </c>
       <c r="AE28" s="1" t="n">
         <v>24</v>
       </c>
@@ -2525,6 +2961,9 @@
       </c>
       <c r="AI28" s="1" t="n">
         <v>404.812790300472</v>
+      </c>
+      <c r="AJ28" s="0" t="n">
+        <v>417.300029092399</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2543,6 +2982,9 @@
       <c r="E29" s="1" t="n">
         <v>16.3090608621218</v>
       </c>
+      <c r="F29" s="0" t="n">
+        <v>16.2988057815579</v>
+      </c>
       <c r="G29" s="1" t="n">
         <v>25</v>
       </c>
@@ -2558,6 +3000,9 @@
       <c r="K29" s="1" t="n">
         <v>43.7818925757286</v>
       </c>
+      <c r="L29" s="0" t="n">
+        <v>43.440328988291</v>
+      </c>
       <c r="M29" s="1" t="n">
         <v>25</v>
       </c>
@@ -2573,6 +3018,9 @@
       <c r="Q29" s="1" t="n">
         <v>58.2683982683983</v>
       </c>
+      <c r="R29" s="0" t="n">
+        <v>57.0443510563242</v>
+      </c>
       <c r="S29" s="1" t="n">
         <v>25</v>
       </c>
@@ -2588,6 +3036,9 @@
       <c r="W29" s="1" t="n">
         <v>93.5422846048359</v>
       </c>
+      <c r="X29" s="0" t="n">
+        <v>96.93224569283</v>
+      </c>
       <c r="Y29" s="1" t="n">
         <v>25</v>
       </c>
@@ -2603,6 +3054,9 @@
       <c r="AC29" s="1" t="n">
         <v>142.729010941633</v>
       </c>
+      <c r="AD29" s="0" t="n">
+        <v>148.156836075273</v>
+      </c>
       <c r="AE29" s="1" t="n">
         <v>25</v>
       </c>
@@ -2617,6 +3071,9 @@
       </c>
       <c r="AI29" s="1" t="n">
         <v>405.053863126803</v>
+      </c>
+      <c r="AJ29" s="0" t="n">
+        <v>412.144792980638</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2635,6 +3092,9 @@
       <c r="E30" s="1" t="n">
         <v>16.6295191077311</v>
       </c>
+      <c r="F30" s="0" t="n">
+        <v>15.6022455301257</v>
+      </c>
       <c r="G30" s="1" t="n">
         <v>26</v>
       </c>
@@ -2650,6 +3110,9 @@
       <c r="K30" s="1" t="n">
         <v>42.5321915865216</v>
       </c>
+      <c r="L30" s="0" t="n">
+        <v>53.9588348584036</v>
+      </c>
       <c r="M30" s="1" t="n">
         <v>26</v>
       </c>
@@ -2665,6 +3128,9 @@
       <c r="Q30" s="1" t="n">
         <v>56.9945887445888</v>
       </c>
+      <c r="R30" s="0" t="n">
+        <v>57.618067414753</v>
+      </c>
       <c r="S30" s="1" t="n">
         <v>26</v>
       </c>
@@ -2680,6 +3146,9 @@
       <c r="W30" s="1" t="n">
         <v>94.9168474169478</v>
       </c>
+      <c r="X30" s="0" t="n">
+        <v>93.2664916612522</v>
+      </c>
       <c r="Y30" s="1" t="n">
         <v>26</v>
       </c>
@@ -2695,6 +3164,9 @@
       <c r="AC30" s="1" t="n">
         <v>134.874444612782</v>
       </c>
+      <c r="AD30" s="0" t="n">
+        <v>157.585162530893</v>
+      </c>
       <c r="AE30" s="1" t="n">
         <v>26</v>
       </c>
@@ -2709,6 +3181,9 @@
       </c>
       <c r="AI30" s="1" t="n">
         <v>409.503295883759</v>
+      </c>
+      <c r="AJ30" s="0" t="n">
+        <v>403.968273567921</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2727,6 +3202,9 @@
       <c r="E31" s="1" t="n">
         <v>16.9968317206617</v>
       </c>
+      <c r="F31" s="0" t="n">
+        <v>17.3152746473606</v>
+      </c>
       <c r="G31" s="1" t="n">
         <v>27</v>
       </c>
@@ -2742,6 +3220,9 @@
       <c r="K31" s="1" t="n">
         <v>43.5373782736802</v>
       </c>
+      <c r="L31" s="0" t="n">
+        <v>43.6636076625071</v>
+      </c>
       <c r="M31" s="1" t="n">
         <v>27</v>
       </c>
@@ -2757,6 +3238,9 @@
       <c r="Q31" s="1" t="n">
         <v>56.6969696969697</v>
       </c>
+      <c r="R31" s="0" t="n">
+        <v>56.6334909320822</v>
+      </c>
       <c r="S31" s="1" t="n">
         <v>27</v>
       </c>
@@ -2772,6 +3256,9 @@
       <c r="W31" s="1" t="n">
         <v>93.3612658390862</v>
       </c>
+      <c r="X31" s="0" t="n">
+        <v>106.622133207648</v>
+      </c>
       <c r="Y31" s="1" t="n">
         <v>27</v>
       </c>
@@ -2787,6 +3274,9 @@
       <c r="AC31" s="1" t="n">
         <v>147.05080753875</v>
       </c>
+      <c r="AD31" s="0" t="n">
+        <v>147.223684325873</v>
+      </c>
       <c r="AE31" s="1" t="n">
         <v>27</v>
       </c>
@@ -2801,6 +3291,9 @@
       </c>
       <c r="AI31" s="1" t="n">
         <v>402.12342338378</v>
+      </c>
+      <c r="AJ31" s="0" t="n">
+        <v>412.787945800732</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2819,6 +3312,9 @@
       <c r="E32" s="1" t="n">
         <v>15.8612237151837</v>
       </c>
+      <c r="F32" s="0" t="n">
+        <v>16.5015334724443</v>
+      </c>
       <c r="G32" s="1" t="n">
         <v>28</v>
       </c>
@@ -2834,6 +3330,9 @@
       <c r="K32" s="1" t="n">
         <v>52.3051554791584</v>
       </c>
+      <c r="L32" s="0" t="n">
+        <v>48.5083346913836</v>
+      </c>
       <c r="M32" s="1" t="n">
         <v>28</v>
       </c>
@@ -2849,6 +3348,9 @@
       <c r="Q32" s="1" t="n">
         <v>61.3235930735931</v>
       </c>
+      <c r="R32" s="0" t="n">
+        <v>58.3842467337601</v>
+      </c>
       <c r="S32" s="1" t="n">
         <v>28</v>
       </c>
@@ -2864,6 +3366,9 @@
       <c r="W32" s="1" t="n">
         <v>92.4965574582937</v>
       </c>
+      <c r="X32" s="0" t="n">
+        <v>91.4638084837643</v>
+      </c>
       <c r="Y32" s="1" t="n">
         <v>28</v>
       </c>
@@ -2879,6 +3384,9 @@
       <c r="AC32" s="1" t="n">
         <v>141.452862734252</v>
       </c>
+      <c r="AD32" s="0" t="n">
+        <v>143.85740184766</v>
+      </c>
       <c r="AE32" s="1" t="n">
         <v>28</v>
       </c>
@@ -2893,6 +3401,9 @@
       </c>
       <c r="AI32" s="1" t="n">
         <v>406.168532360845</v>
+      </c>
+      <c r="AJ32" s="0" t="n">
+        <v>404.126701857956</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2911,6 +3422,9 @@
       <c r="E33" s="1" t="n">
         <v>16.5675270470185</v>
       </c>
+      <c r="F33" s="0" t="n">
+        <v>16.7657823313522</v>
+      </c>
       <c r="G33" s="1" t="n">
         <v>29</v>
       </c>
@@ -2926,6 +3440,9 @@
       <c r="K33" s="1" t="n">
         <v>42.0014533510607</v>
       </c>
+      <c r="L33" s="0" t="n">
+        <v>51.6676879012013</v>
+      </c>
       <c r="M33" s="1" t="n">
         <v>29</v>
       </c>
@@ -2941,6 +3458,9 @@
       <c r="Q33" s="1" t="n">
         <v>60.0919913419913</v>
       </c>
+      <c r="R33" s="0" t="n">
+        <v>59.671498510448</v>
+      </c>
       <c r="S33" s="1" t="n">
         <v>29</v>
       </c>
@@ -2956,6 +3476,9 @@
       <c r="W33" s="1" t="n">
         <v>93.1924393454548</v>
       </c>
+      <c r="X33" s="0" t="n">
+        <v>96.0943881615749</v>
+      </c>
       <c r="Y33" s="1" t="n">
         <v>29</v>
       </c>
@@ -2971,6 +3494,9 @@
       <c r="AC33" s="1" t="n">
         <v>136.793138425808</v>
       </c>
+      <c r="AD33" s="0" t="n">
+        <v>138.635762384215</v>
+      </c>
       <c r="AE33" s="1" t="n">
         <v>29</v>
       </c>
@@ -2985,6 +3511,9 @@
       </c>
       <c r="AI33" s="1" t="n">
         <v>401.117168664786</v>
+      </c>
+      <c r="AJ33" s="0" t="n">
+        <v>405.773095950942</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3003,6 +3532,9 @@
       <c r="E34" s="1" t="n">
         <v>17.3659586272926</v>
       </c>
+      <c r="F34" s="0" t="n">
+        <v>15.9732153942818</v>
+      </c>
       <c r="G34" s="1" t="n">
         <v>30</v>
       </c>
@@ -3018,6 +3550,9 @@
       <c r="K34" s="1" t="n">
         <v>45.574698741645</v>
       </c>
+      <c r="L34" s="0" t="n">
+        <v>47.1201027097357</v>
+      </c>
       <c r="M34" s="1" t="n">
         <v>30</v>
       </c>
@@ -3033,6 +3568,9 @@
       <c r="Q34" s="1" t="n">
         <v>60.284632034632</v>
       </c>
+      <c r="R34" s="0" t="n">
+        <v>59.1930449124927</v>
+      </c>
       <c r="S34" s="1" t="n">
         <v>30</v>
       </c>
@@ -3048,6 +3586,9 @@
       <c r="W34" s="1" t="n">
         <v>91.3762199408743</v>
       </c>
+      <c r="X34" s="0" t="n">
+        <v>91.0447390611901</v>
+      </c>
       <c r="Y34" s="1" t="n">
         <v>30</v>
       </c>
@@ -3063,6 +3604,9 @@
       <c r="AC34" s="1" t="n">
         <v>141.819182221541</v>
       </c>
+      <c r="AD34" s="0" t="n">
+        <v>139.876023615784</v>
+      </c>
       <c r="AE34" s="1" t="n">
         <v>30</v>
       </c>
@@ -3077,6 +3621,9 @@
       </c>
       <c r="AI34" s="1" t="n">
         <v>405.537358310829</v>
+      </c>
+      <c r="AJ34" s="0" t="n">
+        <v>407.805522659397</v>
       </c>
     </row>
   </sheetData>
@@ -3103,10 +3650,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:AI34"/>
+  <dimension ref="A3:AJ34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AI5" activeCellId="0" sqref="AI5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AJ4" activeCellId="0" sqref="AJ4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3158,7 +3705,7 @@
       <c r="AH3" s="2"/>
       <c r="AI3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -3174,6 +3721,9 @@
       <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="F4" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
@@ -3248,6 +3798,9 @@
       </c>
       <c r="AI4" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="AJ4" s="0" t="n">
+        <v>106.552534120526</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3266,6 +3819,9 @@
       <c r="E5" s="1" t="n">
         <v>3.79444909199248</v>
       </c>
+      <c r="F5" s="0" t="n">
+        <v>4.2487552536555</v>
+      </c>
       <c r="G5" s="1" t="n">
         <v>1</v>
       </c>
@@ -3281,6 +3837,9 @@
       <c r="K5" s="1" t="n">
         <v>9.93397176136495</v>
       </c>
+      <c r="L5" s="0" t="n">
+        <v>10.5804275363094</v>
+      </c>
       <c r="M5" s="1" t="n">
         <v>1</v>
       </c>
@@ -3296,6 +3855,9 @@
       <c r="Q5" s="1" t="n">
         <v>13.7045454545455</v>
       </c>
+      <c r="R5" s="0" t="n">
+        <v>12.0136229130628</v>
+      </c>
       <c r="S5" s="1" t="n">
         <v>1</v>
       </c>
@@ -3311,6 +3873,9 @@
       <c r="W5" s="1" t="n">
         <v>23.2822504664432</v>
       </c>
+      <c r="X5" s="0" t="n">
+        <v>23.3604227368954</v>
+      </c>
       <c r="Y5" s="1" t="n">
         <v>1</v>
       </c>
@@ -3326,6 +3891,9 @@
       <c r="AC5" s="1" t="n">
         <v>35.1886955580126</v>
       </c>
+      <c r="AD5" s="0" t="n">
+        <v>31.9635989619083</v>
+      </c>
       <c r="AE5" s="1" t="n">
         <v>1</v>
       </c>
@@ -3340,6 +3908,9 @@
       </c>
       <c r="AI5" s="1" t="n">
         <v>98.8231142350022</v>
+      </c>
+      <c r="AJ5" s="0" t="n">
+        <v>104.781711331082</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3358,6 +3929,9 @@
       <c r="E6" s="1" t="n">
         <v>3.94922495655017</v>
       </c>
+      <c r="F6" s="0" t="n">
+        <v>3.56994399136473</v>
+      </c>
       <c r="G6" s="1" t="n">
         <v>2</v>
       </c>
@@ -3373,6 +3947,9 @@
       <c r="K6" s="1" t="n">
         <v>10.4988761205449</v>
       </c>
+      <c r="L6" s="0" t="n">
+        <v>12.0111860641946</v>
+      </c>
       <c r="M6" s="1" t="n">
         <v>2</v>
       </c>
@@ -3388,6 +3965,9 @@
       <c r="Q6" s="1" t="n">
         <v>14.25</v>
       </c>
+      <c r="R6" s="0" t="n">
+        <v>10.4090399626059</v>
+      </c>
       <c r="S6" s="1" t="n">
         <v>2</v>
       </c>
@@ -3403,6 +3983,9 @@
       <c r="W6" s="1" t="n">
         <v>20.8494148952502</v>
       </c>
+      <c r="X6" s="0" t="n">
+        <v>25.2937221034628</v>
+      </c>
       <c r="Y6" s="1" t="n">
         <v>2</v>
       </c>
@@ -3418,6 +4001,9 @@
       <c r="AC6" s="1" t="n">
         <v>34.2267395010717</v>
       </c>
+      <c r="AD6" s="0" t="n">
+        <v>35.052431234102</v>
+      </c>
       <c r="AE6" s="1" t="n">
         <v>2</v>
       </c>
@@ -3432,6 +4018,9 @@
       </c>
       <c r="AI6" s="1" t="n">
         <v>99.3541384814229</v>
+      </c>
+      <c r="AJ6" s="0" t="n">
+        <v>99.1221337299265</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3450,6 +4039,9 @@
       <c r="E7" s="1" t="n">
         <v>4.65107028542448</v>
       </c>
+      <c r="F7" s="0" t="n">
+        <v>3.88500325178857</v>
+      </c>
       <c r="G7" s="1" t="n">
         <v>3</v>
       </c>
@@ -3465,6 +4057,9 @@
       <c r="K7" s="1" t="n">
         <v>10.3894495177343</v>
       </c>
+      <c r="L7" s="0" t="n">
+        <v>13.028409273463</v>
+      </c>
       <c r="M7" s="1" t="n">
         <v>3</v>
       </c>
@@ -3480,6 +4075,9 @@
       <c r="Q7" s="1" t="n">
         <v>10.4718614718615</v>
       </c>
+      <c r="R7" s="0" t="n">
+        <v>8.8779210593647</v>
+      </c>
       <c r="S7" s="1" t="n">
         <v>3</v>
       </c>
@@ -3495,6 +4093,9 @@
       <c r="W7" s="1" t="n">
         <v>24.913891238825</v>
       </c>
+      <c r="X7" s="0" t="n">
+        <v>23.7002526595269</v>
+      </c>
       <c r="Y7" s="1" t="n">
         <v>3</v>
       </c>
@@ -3510,6 +4111,9 @@
       <c r="AC7" s="1" t="n">
         <v>35.7021759371363</v>
       </c>
+      <c r="AD7" s="0" t="n">
+        <v>35.4464097874194</v>
+      </c>
       <c r="AE7" s="1" t="n">
         <v>3</v>
       </c>
@@ -3524,6 +4128,9 @@
       </c>
       <c r="AI7" s="1" t="n">
         <v>100.829629833458</v>
+      </c>
+      <c r="AJ7" s="0" t="n">
+        <v>103.687247405535</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3542,6 +4149,9 @@
       <c r="E8" s="1" t="n">
         <v>3.82931928996756</v>
       </c>
+      <c r="F8" s="0" t="n">
+        <v>3.73184115110462</v>
+      </c>
       <c r="G8" s="1" t="n">
         <v>4</v>
       </c>
@@ -3557,6 +4167,9 @@
       <c r="K8" s="1" t="n">
         <v>13.3438129915241</v>
       </c>
+      <c r="L8" s="0" t="n">
+        <v>12.7495057926044</v>
+      </c>
       <c r="M8" s="1" t="n">
         <v>4</v>
       </c>
@@ -3572,6 +4185,9 @@
       <c r="Q8" s="1" t="n">
         <v>12.3777056277056</v>
       </c>
+      <c r="R8" s="0" t="n">
+        <v>14.6431929146662</v>
+      </c>
       <c r="S8" s="1" t="n">
         <v>4</v>
       </c>
@@ -3587,6 +4203,9 @@
       <c r="W8" s="1" t="n">
         <v>23.1938098293613</v>
       </c>
+      <c r="X8" s="0" t="n">
+        <v>25.6362649849664</v>
+      </c>
       <c r="Y8" s="1" t="n">
         <v>4</v>
       </c>
@@ -3602,6 +4221,9 @@
       <c r="AC8" s="1" t="n">
         <v>34.0174226317887</v>
       </c>
+      <c r="AD8" s="0" t="n">
+        <v>37.0379756349189</v>
+      </c>
       <c r="AE8" s="1" t="n">
         <v>4</v>
       </c>
@@ -3616,6 +4238,9 @@
       </c>
       <c r="AI8" s="1" t="n">
         <v>97.8740999775604</v>
+      </c>
+      <c r="AJ8" s="0" t="n">
+        <v>102.652109367771</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3634,6 +4259,9 @@
       <c r="E9" s="1" t="n">
         <v>3.81418034113879</v>
       </c>
+      <c r="F9" s="0" t="n">
+        <v>5.23173998538864</v>
+      </c>
       <c r="G9" s="1" t="n">
         <v>5</v>
       </c>
@@ -3649,6 +4277,9 @@
       <c r="K9" s="1" t="n">
         <v>11.8160971055406</v>
       </c>
+      <c r="L9" s="0" t="n">
+        <v>12.6175644106273</v>
+      </c>
       <c r="M9" s="1" t="n">
         <v>5</v>
       </c>
@@ -3664,6 +4295,9 @@
       <c r="Q9" s="1" t="n">
         <v>12.3344155844156</v>
       </c>
+      <c r="R9" s="0" t="n">
+        <v>9.47065386320831</v>
+      </c>
       <c r="S9" s="1" t="n">
         <v>5</v>
       </c>
@@ -3679,6 +4313,9 @@
       <c r="W9" s="1" t="n">
         <v>25.2387139070958</v>
       </c>
+      <c r="X9" s="0" t="n">
+        <v>22.250031716052</v>
+      </c>
       <c r="Y9" s="1" t="n">
         <v>5</v>
       </c>
@@ -3694,6 +4331,9 @@
       <c r="AC9" s="1" t="n">
         <v>33.8301733255812</v>
       </c>
+      <c r="AD9" s="0" t="n">
+        <v>36.0898981583601</v>
+      </c>
       <c r="AE9" s="1" t="n">
         <v>5</v>
       </c>
@@ -3708,6 +4348,9 @@
       </c>
       <c r="AI9" s="1" t="n">
         <v>102.903595886471</v>
+      </c>
+      <c r="AJ9" s="0" t="n">
+        <v>108.226911289459</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3726,6 +4369,9 @@
       <c r="E10" s="1" t="n">
         <v>4.76013420097486</v>
       </c>
+      <c r="F10" s="0" t="n">
+        <v>4.40926635323458</v>
+      </c>
       <c r="G10" s="1" t="n">
         <v>6</v>
       </c>
@@ -3741,6 +4387,9 @@
       <c r="K10" s="1" t="n">
         <v>11.2317336002836</v>
       </c>
+      <c r="L10" s="0" t="n">
+        <v>14.2687228085226</v>
+      </c>
       <c r="M10" s="1" t="n">
         <v>6</v>
       </c>
@@ -3756,6 +4405,9 @@
       <c r="Q10" s="1" t="n">
         <v>11.8030303030303</v>
       </c>
+      <c r="R10" s="0" t="n">
+        <v>13.4110688265592</v>
+      </c>
       <c r="S10" s="1" t="n">
         <v>6</v>
       </c>
@@ -3771,6 +4423,9 @@
       <c r="W10" s="1" t="n">
         <v>24.0671993292773</v>
       </c>
+      <c r="X10" s="0" t="n">
+        <v>21.9471419650445</v>
+      </c>
       <c r="Y10" s="1" t="n">
         <v>6</v>
       </c>
@@ -3786,6 +4441,9 @@
       <c r="AC10" s="1" t="n">
         <v>39.1827619462851</v>
       </c>
+      <c r="AD10" s="0" t="n">
+        <v>36.7064957588213</v>
+      </c>
       <c r="AE10" s="1" t="n">
         <v>6</v>
       </c>
@@ -3800,6 +4458,9 @@
       </c>
       <c r="AI10" s="1" t="n">
         <v>101.434701585534</v>
+      </c>
+      <c r="AJ10" s="0" t="n">
+        <v>104.804115042683</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3818,6 +4479,9 @@
       <c r="E11" s="1" t="n">
         <v>4.11185946179996</v>
       </c>
+      <c r="F11" s="0" t="n">
+        <v>4.67220434784893</v>
+      </c>
       <c r="G11" s="1" t="n">
         <v>7</v>
       </c>
@@ -3833,6 +4497,9 @@
       <c r="K11" s="1" t="n">
         <v>10.3002926304806</v>
       </c>
+      <c r="L11" s="0" t="n">
+        <v>11.7563878077226</v>
+      </c>
       <c r="M11" s="1" t="n">
         <v>7</v>
       </c>
@@ -3848,6 +4515,9 @@
       <c r="Q11" s="1" t="n">
         <v>11.7012987012987</v>
       </c>
+      <c r="R11" s="0" t="n">
+        <v>13.0270198132201</v>
+      </c>
       <c r="S11" s="1" t="n">
         <v>7</v>
       </c>
@@ -3863,6 +4533,9 @@
       <c r="W11" s="1" t="n">
         <v>25.1376584798296</v>
       </c>
+      <c r="X11" s="0" t="n">
+        <v>25.37112310755</v>
+      </c>
       <c r="Y11" s="1" t="n">
         <v>7</v>
       </c>
@@ -3878,6 +4551,9 @@
       <c r="AC11" s="1" t="n">
         <v>33.5158397194745</v>
       </c>
+      <c r="AD11" s="0" t="n">
+        <v>32.2043745360498</v>
+      </c>
       <c r="AE11" s="1" t="n">
         <v>7</v>
       </c>
@@ -3892,6 +4568,9 @@
       </c>
       <c r="AI11" s="1" t="n">
         <v>101.865263382158</v>
+      </c>
+      <c r="AJ11" s="0" t="n">
+        <v>103.64972910697</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3910,6 +4589,9 @@
       <c r="E12" s="1" t="n">
         <v>3.56610497237953</v>
       </c>
+      <c r="F12" s="0" t="n">
+        <v>4.36932522884975</v>
+      </c>
       <c r="G12" s="1" t="n">
         <v>8</v>
       </c>
@@ -3925,6 +4607,9 @@
       <c r="K12" s="1" t="n">
         <v>12.2435633282995</v>
       </c>
+      <c r="L12" s="0" t="n">
+        <v>16.0216571115028</v>
+      </c>
       <c r="M12" s="1" t="n">
         <v>8</v>
       </c>
@@ -3940,6 +4625,9 @@
       <c r="Q12" s="1" t="n">
         <v>15.2186147186147</v>
       </c>
+      <c r="R12" s="0" t="n">
+        <v>12.1533011413897</v>
+      </c>
       <c r="S12" s="1" t="n">
         <v>8</v>
       </c>
@@ -3955,6 +4643,9 @@
       <c r="W12" s="1" t="n">
         <v>23.638813785823</v>
       </c>
+      <c r="X12" s="0" t="n">
+        <v>23.9333930982052</v>
+      </c>
       <c r="Y12" s="1" t="n">
         <v>8</v>
       </c>
@@ -3970,6 +4661,9 @@
       <c r="AC12" s="1" t="n">
         <v>33.7741337605056</v>
       </c>
+      <c r="AD12" s="0" t="n">
+        <v>37.060296526342</v>
+      </c>
       <c r="AE12" s="1" t="n">
         <v>8</v>
       </c>
@@ -3984,6 +4678,9 @@
       </c>
       <c r="AI12" s="1" t="n">
         <v>95.8880302155511</v>
+      </c>
+      <c r="AJ12" s="0" t="n">
+        <v>100.974551869814</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4002,6 +4699,9 @@
       <c r="E13" s="1" t="n">
         <v>3.37457920226511</v>
       </c>
+      <c r="F13" s="0" t="n">
+        <v>3.84457644825661</v>
+      </c>
       <c r="G13" s="1" t="n">
         <v>9</v>
       </c>
@@ -4017,6 +4717,9 @@
       <c r="K13" s="1" t="n">
         <v>10.2132493922338</v>
       </c>
+      <c r="L13" s="0" t="n">
+        <v>10.9850030349745</v>
+      </c>
       <c r="M13" s="1" t="n">
         <v>9</v>
       </c>
@@ -4032,6 +4735,9 @@
       <c r="Q13" s="1" t="n">
         <v>11.5519480519481</v>
       </c>
+      <c r="R13" s="0" t="n">
+        <v>14.3638303387089</v>
+      </c>
       <c r="S13" s="1" t="n">
         <v>9</v>
       </c>
@@ -4047,6 +4753,9 @@
       <c r="W13" s="1" t="n">
         <v>22.3095693108681</v>
       </c>
+      <c r="X13" s="0" t="n">
+        <v>21.9298759294002</v>
+      </c>
       <c r="Y13" s="1" t="n">
         <v>9</v>
       </c>
@@ -4062,6 +4771,9 @@
       <c r="AC13" s="1" t="n">
         <v>33.5777765007468</v>
       </c>
+      <c r="AD13" s="0" t="n">
+        <v>34.9226456705233</v>
+      </c>
       <c r="AE13" s="1" t="n">
         <v>9</v>
       </c>
@@ -4076,6 +4788,9 @@
       </c>
       <c r="AI13" s="1" t="n">
         <v>96.4092145921906</v>
+      </c>
+      <c r="AJ13" s="0" t="n">
+        <v>108.09538772369</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4094,6 +4809,9 @@
       <c r="E14" s="1" t="n">
         <v>3.35681575810996</v>
       </c>
+      <c r="F14" s="0" t="n">
+        <v>4.13162123117499</v>
+      </c>
       <c r="G14" s="1" t="n">
         <v>10</v>
       </c>
@@ -4109,6 +4827,9 @@
       <c r="K14" s="1" t="n">
         <v>12.4819152203576</v>
       </c>
+      <c r="L14" s="0" t="n">
+        <v>12.4827327162313</v>
+      </c>
       <c r="M14" s="1" t="n">
         <v>10</v>
       </c>
@@ -4124,6 +4845,9 @@
       <c r="Q14" s="1" t="n">
         <v>13.3538961038961</v>
       </c>
+      <c r="R14" s="0" t="n">
+        <v>10.5399415939274</v>
+      </c>
       <c r="S14" s="1" t="n">
         <v>10</v>
       </c>
@@ -4139,6 +4863,9 @@
       <c r="W14" s="1" t="n">
         <v>23.7344500224541</v>
       </c>
+      <c r="X14" s="0" t="n">
+        <v>23.3785432587946</v>
+      </c>
       <c r="Y14" s="1" t="n">
         <v>10</v>
       </c>
@@ -4154,6 +4881,9 @@
       <c r="AC14" s="1" t="n">
         <v>35.3933899935883</v>
       </c>
+      <c r="AD14" s="0" t="n">
+        <v>36.4605546422447</v>
+      </c>
       <c r="AE14" s="1" t="n">
         <v>10</v>
       </c>
@@ -4168,6 +4898,9 @@
       </c>
       <c r="AI14" s="1" t="n">
         <v>100.458940540052</v>
+      </c>
+      <c r="AJ14" s="0" t="n">
+        <v>103.369294623957</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4186,6 +4919,9 @@
       <c r="E15" s="1" t="n">
         <v>3.71418779222245</v>
       </c>
+      <c r="F15" s="0" t="n">
+        <v>3.56517377896168</v>
+      </c>
       <c r="G15" s="1" t="n">
         <v>11</v>
       </c>
@@ -4201,6 +4937,9 @@
       <c r="K15" s="1" t="n">
         <v>12.6063468936234</v>
       </c>
+      <c r="L15" s="0" t="n">
+        <v>13.4265659417132</v>
+      </c>
       <c r="M15" s="1" t="n">
         <v>11</v>
       </c>
@@ -4216,6 +4955,9 @@
       <c r="Q15" s="1" t="n">
         <v>9.92532467532468</v>
       </c>
+      <c r="R15" s="0" t="n">
+        <v>12.6354658340702</v>
+      </c>
       <c r="S15" s="1" t="n">
         <v>11</v>
       </c>
@@ -4231,6 +4973,9 @@
       <c r="W15" s="1" t="n">
         <v>22.5567491285329</v>
       </c>
+      <c r="X15" s="0" t="n">
+        <v>22.8149325730167</v>
+      </c>
       <c r="Y15" s="1" t="n">
         <v>11</v>
       </c>
@@ -4246,6 +4991,9 @@
       <c r="AC15" s="1" t="n">
         <v>34.3802670955847</v>
       </c>
+      <c r="AD15" s="0" t="n">
+        <v>35.2181597905977</v>
+      </c>
       <c r="AE15" s="1" t="n">
         <v>11</v>
       </c>
@@ -4260,6 +5008,9 @@
       </c>
       <c r="AI15" s="1" t="n">
         <v>100.312339551001</v>
+      </c>
+      <c r="AJ15" s="0" t="n">
+        <v>100.989883480683</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4278,6 +5029,9 @@
       <c r="E16" s="1" t="n">
         <v>4.60320819017459</v>
       </c>
+      <c r="F16" s="0" t="n">
+        <v>3.9973553964694</v>
+      </c>
       <c r="G16" s="1" t="n">
         <v>12</v>
       </c>
@@ -4293,6 +5047,9 @@
       <c r="K16" s="1" t="n">
         <v>10.2624626581717</v>
       </c>
+      <c r="L16" s="0" t="n">
+        <v>12.1674998696762</v>
+      </c>
       <c r="M16" s="1" t="n">
         <v>12</v>
       </c>
@@ -4308,6 +5065,9 @@
       <c r="Q16" s="1" t="n">
         <v>14.4729437229437</v>
       </c>
+      <c r="R16" s="0" t="n">
+        <v>11.5116649653986</v>
+      </c>
       <c r="S16" s="1" t="n">
         <v>12</v>
       </c>
@@ -4323,6 +5083,9 @@
       <c r="W16" s="1" t="n">
         <v>22.0719436260236</v>
       </c>
+      <c r="X16" s="0" t="n">
+        <v>23.4867282669799</v>
+      </c>
       <c r="Y16" s="1" t="n">
         <v>12</v>
       </c>
@@ -4338,6 +5101,9 @@
       <c r="AC16" s="1" t="n">
         <v>35.9397031311104</v>
       </c>
+      <c r="AD16" s="0" t="n">
+        <v>35.8368512621518</v>
+      </c>
       <c r="AE16" s="1" t="n">
         <v>12</v>
       </c>
@@ -4352,6 +5118,9 @@
       </c>
       <c r="AI16" s="1" t="n">
         <v>99.5527768185965</v>
+      </c>
+      <c r="AJ16" s="0" t="n">
+        <v>100.908475504901</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4370,6 +5139,9 @@
       <c r="E17" s="1" t="n">
         <v>3.9866507961255</v>
       </c>
+      <c r="F17" s="0" t="n">
+        <v>4.12979190960978</v>
+      </c>
       <c r="G17" s="1" t="n">
         <v>13</v>
       </c>
@@ -4385,6 +5157,9 @@
       <c r="K17" s="1" t="n">
         <v>12.9495553540881</v>
       </c>
+      <c r="L17" s="0" t="n">
+        <v>13.5657295352949</v>
+      </c>
       <c r="M17" s="1" t="n">
         <v>13</v>
       </c>
@@ -4400,6 +5175,9 @@
       <c r="Q17" s="1" t="n">
         <v>13.6071428571429</v>
       </c>
+      <c r="R17" s="0" t="n">
+        <v>12.5562077897178</v>
+      </c>
       <c r="S17" s="1" t="n">
         <v>13</v>
       </c>
@@ -4415,6 +5193,9 @@
       <c r="W17" s="1" t="n">
         <v>23.1784876765705</v>
       </c>
+      <c r="X17" s="0" t="n">
+        <v>23.5754053456381</v>
+      </c>
       <c r="Y17" s="1" t="n">
         <v>13</v>
       </c>
@@ -4430,6 +5211,9 @@
       <c r="AC17" s="1" t="n">
         <v>34.2228498419607</v>
       </c>
+      <c r="AD17" s="0" t="n">
+        <v>36.7051014338156</v>
+      </c>
       <c r="AE17" s="1" t="n">
         <v>13</v>
       </c>
@@ -4444,6 +5228,9 @@
       </c>
       <c r="AI17" s="1" t="n">
         <v>104.440388193721</v>
+      </c>
+      <c r="AJ17" s="0" t="n">
+        <v>103.34888069048</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4462,6 +5249,9 @@
       <c r="E18" s="1" t="n">
         <v>4.1233905697312</v>
       </c>
+      <c r="F18" s="0" t="n">
+        <v>4.45705290462529</v>
+      </c>
       <c r="G18" s="1" t="n">
         <v>14</v>
       </c>
@@ -4477,6 +5267,9 @@
       <c r="K18" s="1" t="n">
         <v>11.6291672215298</v>
       </c>
+      <c r="L18" s="0" t="n">
+        <v>12.6476567815866</v>
+      </c>
       <c r="M18" s="1" t="n">
         <v>14</v>
       </c>
@@ -4492,6 +5285,9 @@
       <c r="Q18" s="1" t="n">
         <v>11.5227272727273</v>
       </c>
+      <c r="R18" s="0" t="n">
+        <v>12.7135541503659</v>
+      </c>
       <c r="S18" s="1" t="n">
         <v>14</v>
       </c>
@@ -4507,6 +5303,9 @@
       <c r="W18" s="1" t="n">
         <v>20.1144145143151</v>
       </c>
+      <c r="X18" s="0" t="n">
+        <v>22.6645199649674</v>
+      </c>
       <c r="Y18" s="1" t="n">
         <v>14</v>
       </c>
@@ -4522,6 +5321,9 @@
       <c r="AC18" s="1" t="n">
         <v>35.2889269293415</v>
       </c>
+      <c r="AD18" s="0" t="n">
+        <v>34.0338112324602</v>
+      </c>
       <c r="AE18" s="1" t="n">
         <v>14</v>
       </c>
@@ -4536,6 +5338,9 @@
       </c>
       <c r="AI18" s="1" t="n">
         <v>98.2196691087821</v>
+      </c>
+      <c r="AJ18" s="0" t="n">
+        <v>101.669660812278</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4554,6 +5359,9 @@
       <c r="E19" s="1" t="n">
         <v>4.3777220644171</v>
       </c>
+      <c r="F19" s="0" t="n">
+        <v>4.63582905001935</v>
+      </c>
       <c r="G19" s="1" t="n">
         <v>15</v>
       </c>
@@ -4569,6 +5377,9 @@
       <c r="K19" s="1" t="n">
         <v>11.106290021226</v>
       </c>
+      <c r="L19" s="0" t="n">
+        <v>10.9071409846253</v>
+      </c>
       <c r="M19" s="1" t="n">
         <v>15</v>
       </c>
@@ -4584,6 +5395,9 @@
       <c r="Q19" s="1" t="n">
         <v>13.530303030303</v>
       </c>
+      <c r="R19" s="0" t="n">
+        <v>9.73799579615823</v>
+      </c>
       <c r="S19" s="1" t="n">
         <v>15</v>
       </c>
@@ -4599,6 +5413,9 @@
       <c r="W19" s="1" t="n">
         <v>22.8249340695551</v>
       </c>
+      <c r="X19" s="0" t="n">
+        <v>21.8411501224598</v>
+      </c>
       <c r="Y19" s="1" t="n">
         <v>15</v>
       </c>
@@ -4614,6 +5431,9 @@
       <c r="AC19" s="1" t="n">
         <v>35.6583529210787</v>
       </c>
+      <c r="AD19" s="0" t="n">
+        <v>35.559044734269</v>
+      </c>
       <c r="AE19" s="1" t="n">
         <v>15</v>
       </c>
@@ -4628,6 +5448,9 @@
       </c>
       <c r="AI19" s="1" t="n">
         <v>98.619781441511</v>
+      </c>
+      <c r="AJ19" s="0" t="n">
+        <v>101.999180030824</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4646,6 +5469,9 @@
       <c r="E20" s="1" t="n">
         <v>3.31006540509852</v>
       </c>
+      <c r="F20" s="0" t="n">
+        <v>3.99746750341822</v>
+      </c>
       <c r="G20" s="1" t="n">
         <v>16</v>
       </c>
@@ -4661,6 +5487,9 @@
       <c r="K20" s="1" t="n">
         <v>10.0699775653025</v>
       </c>
+      <c r="L20" s="0" t="n">
+        <v>12.9769962911401</v>
+      </c>
       <c r="M20" s="1" t="n">
         <v>16</v>
       </c>
@@ -4676,6 +5505,9 @@
       <c r="Q20" s="1" t="n">
         <v>12.2987012987013</v>
       </c>
+      <c r="R20" s="0" t="n">
+        <v>9.7372072435122</v>
+      </c>
       <c r="S20" s="1" t="n">
         <v>16</v>
       </c>
@@ -4691,6 +5523,9 @@
       <c r="W20" s="1" t="n">
         <v>22.8747205309333</v>
       </c>
+      <c r="X20" s="0" t="n">
+        <v>25.7784228633955</v>
+      </c>
       <c r="Y20" s="1" t="n">
         <v>16</v>
       </c>
@@ -4706,6 +5541,9 @@
       <c r="AC20" s="1" t="n">
         <v>36.2495599027907</v>
       </c>
+      <c r="AD20" s="0" t="n">
+        <v>38.8617953073769</v>
+      </c>
       <c r="AE20" s="1" t="n">
         <v>16</v>
       </c>
@@ -4720,6 +5558,9 @@
       </c>
       <c r="AI20" s="1" t="n">
         <v>99.4626657399853</v>
+      </c>
+      <c r="AJ20" s="0" t="n">
+        <v>99.5712601615613</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4738,6 +5579,9 @@
       <c r="E21" s="1" t="n">
         <v>4.27092982551891</v>
       </c>
+      <c r="F21" s="0" t="n">
+        <v>3.0547625051681</v>
+      </c>
       <c r="G21" s="1" t="n">
         <v>17</v>
       </c>
@@ -4753,6 +5597,9 @@
       <c r="K21" s="1" t="n">
         <v>11.8830997021792</v>
       </c>
+      <c r="L21" s="0" t="n">
+        <v>11.7334372045444</v>
+      </c>
       <c r="M21" s="1" t="n">
         <v>17</v>
       </c>
@@ -4768,6 +5615,9 @@
       <c r="Q21" s="1" t="n">
         <v>11.9448051948052</v>
       </c>
+      <c r="R21" s="0" t="n">
+        <v>11.9809128889974</v>
+      </c>
       <c r="S21" s="1" t="n">
         <v>17</v>
       </c>
@@ -4783,6 +5633,9 @@
       <c r="W21" s="1" t="n">
         <v>24.4279113185608</v>
       </c>
+      <c r="X21" s="0" t="n">
+        <v>27.5503701815952</v>
+      </c>
       <c r="Y21" s="1" t="n">
         <v>17</v>
       </c>
@@ -4798,6 +5651,9 @@
       <c r="AC21" s="1" t="n">
         <v>36.2335149381236</v>
       </c>
+      <c r="AD21" s="0" t="n">
+        <v>37.396895186666</v>
+      </c>
       <c r="AE21" s="1" t="n">
         <v>17</v>
       </c>
@@ -4812,6 +5668,9 @@
       </c>
       <c r="AI21" s="1" t="n">
         <v>103.389682395308</v>
+      </c>
+      <c r="AJ21" s="0" t="n">
+        <v>103.357433545115</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4830,6 +5689,9 @@
       <c r="E22" s="1" t="n">
         <v>4.37944535884647</v>
       </c>
+      <c r="F22" s="0" t="n">
+        <v>3.76278287973869</v>
+      </c>
       <c r="G22" s="1" t="n">
         <v>18</v>
       </c>
@@ -4845,6 +5707,9 @@
       <c r="K22" s="1" t="n">
         <v>11.0413357706442</v>
       </c>
+      <c r="L22" s="0" t="n">
+        <v>10.4109859510503</v>
+      </c>
       <c r="M22" s="1" t="n">
         <v>18</v>
       </c>
@@ -4860,6 +5725,9 @@
       <c r="Q22" s="1" t="n">
         <v>10.8279220779221</v>
       </c>
+      <c r="R22" s="0" t="n">
+        <v>8.26607558085626</v>
+      </c>
       <c r="S22" s="1" t="n">
         <v>18</v>
       </c>
@@ -4875,6 +5743,9 @@
       <c r="W22" s="1" t="n">
         <v>23.370587628067</v>
       </c>
+      <c r="X22" s="0" t="n">
+        <v>23.0064361875287</v>
+      </c>
       <c r="Y22" s="1" t="n">
         <v>18</v>
       </c>
@@ -4890,6 +5761,9 @@
       <c r="AC22" s="1" t="n">
         <v>32.9958719990987</v>
       </c>
+      <c r="AD22" s="0" t="n">
+        <v>38.1744220673334</v>
+      </c>
       <c r="AE22" s="1" t="n">
         <v>18</v>
       </c>
@@ -4904,6 +5778,9 @@
       </c>
       <c r="AI22" s="1" t="n">
         <v>96.2887845221689</v>
+      </c>
+      <c r="AJ22" s="0" t="n">
+        <v>98.036186486855</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4922,6 +5799,9 @@
       <c r="E23" s="1" t="n">
         <v>3.63079728526111</v>
       </c>
+      <c r="F23" s="0" t="n">
+        <v>4.32220228701213</v>
+      </c>
       <c r="G23" s="1" t="n">
         <v>19</v>
       </c>
@@ -4937,6 +5817,9 @@
       <c r="K23" s="1" t="n">
         <v>10.1515491767327</v>
       </c>
+      <c r="L23" s="0" t="n">
+        <v>12.6186710588752</v>
+      </c>
       <c r="M23" s="1" t="n">
         <v>19</v>
       </c>
@@ -4952,6 +5835,9 @@
       <c r="Q23" s="1" t="n">
         <v>13.2640692640693</v>
       </c>
+      <c r="R23" s="0" t="n">
+        <v>12.2617524615282</v>
+      </c>
       <c r="S23" s="1" t="n">
         <v>19</v>
       </c>
@@ -4967,6 +5853,9 @@
       <c r="W23" s="1" t="n">
         <v>21.553645460912</v>
       </c>
+      <c r="X23" s="0" t="n">
+        <v>25.0689696412277</v>
+      </c>
       <c r="Y23" s="1" t="n">
         <v>19</v>
       </c>
@@ -4982,6 +5871,9 @@
       <c r="AC23" s="1" t="n">
         <v>34.2355586957329</v>
       </c>
+      <c r="AD23" s="0" t="n">
+        <v>35.6475389773434</v>
+      </c>
       <c r="AE23" s="1" t="n">
         <v>19</v>
       </c>
@@ -4996,6 +5888,9 @@
       </c>
       <c r="AI23" s="1" t="n">
         <v>100.076055180818</v>
+      </c>
+      <c r="AJ23" s="0" t="n">
+        <v>103.675549170129</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5014,6 +5909,9 @@
       <c r="E24" s="1" t="n">
         <v>3.62237728913438</v>
       </c>
+      <c r="F24" s="0" t="n">
+        <v>3.35930486648195</v>
+      </c>
       <c r="G24" s="1" t="n">
         <v>20</v>
       </c>
@@ -5029,6 +5927,9 @@
       <c r="K24" s="1" t="n">
         <v>10.1925113790138</v>
       </c>
+      <c r="L24" s="0" t="n">
+        <v>12.9454171681682</v>
+      </c>
       <c r="M24" s="1" t="n">
         <v>20</v>
       </c>
@@ -5044,6 +5945,9 @@
       <c r="Q24" s="1" t="n">
         <v>12.3344155844156</v>
       </c>
+      <c r="R24" s="0" t="n">
+        <v>16.2058350777416</v>
+      </c>
       <c r="S24" s="1" t="n">
         <v>20</v>
       </c>
@@ -5059,6 +5963,9 @@
       <c r="W24" s="1" t="n">
         <v>22.0030776442519</v>
       </c>
+      <c r="X24" s="0" t="n">
+        <v>26.2286783069326</v>
+      </c>
       <c r="Y24" s="1" t="n">
         <v>20</v>
       </c>
@@ -5074,6 +5981,9 @@
       <c r="AC24" s="1" t="n">
         <v>32.0071390588696</v>
       </c>
+      <c r="AD24" s="0" t="n">
+        <v>34.0423004999749</v>
+      </c>
       <c r="AE24" s="1" t="n">
         <v>20</v>
       </c>
@@ -5088,6 +5998,9 @@
       </c>
       <c r="AI24" s="1" t="n">
         <v>103.684155380959</v>
+      </c>
+      <c r="AJ24" s="0" t="n">
+        <v>104.090969577048</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5106,6 +6019,9 @@
       <c r="E25" s="1" t="n">
         <v>4.50541280527137</v>
       </c>
+      <c r="F25" s="0" t="n">
+        <v>3.61445993711194</v>
+      </c>
       <c r="G25" s="1" t="n">
         <v>21</v>
       </c>
@@ -5121,6 +6037,9 @@
       <c r="K25" s="1" t="n">
         <v>10.8169845010569</v>
       </c>
+      <c r="L25" s="0" t="n">
+        <v>12.913364033922</v>
+      </c>
       <c r="M25" s="1" t="n">
         <v>21</v>
       </c>
@@ -5136,6 +6055,9 @@
       <c r="Q25" s="1" t="n">
         <v>10.012987012987</v>
       </c>
+      <c r="R25" s="0" t="n">
+        <v>11.8769203612647</v>
+      </c>
       <c r="S25" s="1" t="n">
         <v>21</v>
       </c>
@@ -5151,6 +6073,9 @@
       <c r="W25" s="1" t="n">
         <v>24.4343266669266</v>
       </c>
+      <c r="X25" s="0" t="n">
+        <v>23.4493268312795</v>
+      </c>
       <c r="Y25" s="1" t="n">
         <v>21</v>
       </c>
@@ -5166,6 +6091,9 @@
       <c r="AC25" s="1" t="n">
         <v>34.3446986415347</v>
       </c>
+      <c r="AD25" s="0" t="n">
+        <v>35.8573958422427</v>
+      </c>
       <c r="AE25" s="1" t="n">
         <v>21</v>
       </c>
@@ -5180,6 +6108,9 @@
       </c>
       <c r="AI25" s="1" t="n">
         <v>98.6922171613267</v>
+      </c>
+      <c r="AJ25" s="0" t="n">
+        <v>105.697999260475</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5198,6 +6129,9 @@
       <c r="E26" s="1" t="n">
         <v>3.46284913101637</v>
       </c>
+      <c r="F26" s="0" t="n">
+        <v>4.22169186906857</v>
+      </c>
       <c r="G26" s="1" t="n">
         <v>22</v>
       </c>
@@ -5213,6 +6147,9 @@
       <c r="K26" s="1" t="n">
         <v>11.2054252634828</v>
       </c>
+      <c r="L26" s="0" t="n">
+        <v>12.5507777817646</v>
+      </c>
       <c r="M26" s="1" t="n">
         <v>22</v>
       </c>
@@ -5228,6 +6165,9 @@
       <c r="Q26" s="1" t="n">
         <v>13.4458874458874</v>
       </c>
+      <c r="R26" s="0" t="n">
+        <v>13.5329653312453</v>
+      </c>
       <c r="S26" s="1" t="n">
         <v>22</v>
       </c>
@@ -5243,6 +6183,9 @@
       <c r="W26" s="1" t="n">
         <v>22.4246039876242</v>
       </c>
+      <c r="X26" s="0" t="n">
+        <v>24.1749224279521</v>
+      </c>
       <c r="Y26" s="1" t="n">
         <v>22</v>
       </c>
@@ -5258,6 +6201,9 @@
       <c r="AC26" s="1" t="n">
         <v>35.9678778584726</v>
       </c>
+      <c r="AD26" s="0" t="n">
+        <v>35.876165671648</v>
+      </c>
       <c r="AE26" s="1" t="n">
         <v>22</v>
       </c>
@@ -5272,6 +6218,9 @@
       </c>
       <c r="AI26" s="1" t="n">
         <v>98.8762733303166</v>
+      </c>
+      <c r="AJ26" s="0" t="n">
+        <v>104.806362272589</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5290,6 +6239,9 @@
       <c r="E27" s="1" t="n">
         <v>3.63029115695811</v>
       </c>
+      <c r="F27" s="0" t="n">
+        <v>3.63800280888157</v>
+      </c>
       <c r="G27" s="1" t="n">
         <v>23</v>
       </c>
@@ -5305,6 +6257,9 @@
       <c r="K27" s="1" t="n">
         <v>11.9839172731469</v>
       </c>
+      <c r="L27" s="0" t="n">
+        <v>13.9894507865909</v>
+      </c>
       <c r="M27" s="1" t="n">
         <v>23</v>
       </c>
@@ -5320,6 +6275,9 @@
       <c r="Q27" s="1" t="n">
         <v>14.7608225108225</v>
       </c>
+      <c r="R27" s="0" t="n">
+        <v>14.002100512776</v>
+      </c>
       <c r="S27" s="1" t="n">
         <v>23</v>
       </c>
@@ -5335,6 +6293,9 @@
       <c r="W27" s="1" t="n">
         <v>24.2955217409372</v>
       </c>
+      <c r="X27" s="0" t="n">
+        <v>25.3922536278268</v>
+      </c>
       <c r="Y27" s="1" t="n">
         <v>23</v>
       </c>
@@ -5350,6 +6311,9 @@
       <c r="AC27" s="1" t="n">
         <v>34.5722070481246</v>
       </c>
+      <c r="AD27" s="0" t="n">
+        <v>31.4034069904402</v>
+      </c>
       <c r="AE27" s="1" t="n">
         <v>23</v>
       </c>
@@ -5364,6 +6328,9 @@
       </c>
       <c r="AI27" s="1" t="n">
         <v>97.8809758875043</v>
+      </c>
+      <c r="AJ27" s="0" t="n">
+        <v>104.464413025222</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5382,6 +6349,9 @@
       <c r="E28" s="1" t="n">
         <v>4.32056584180893</v>
       </c>
+      <c r="F28" s="0" t="n">
+        <v>3.61165692682433</v>
+      </c>
       <c r="G28" s="1" t="n">
         <v>24</v>
       </c>
@@ -5397,6 +6367,9 @@
       <c r="K28" s="1" t="n">
         <v>11.7873788419151</v>
       </c>
+      <c r="L28" s="0" t="n">
+        <v>12.8163711694564</v>
+      </c>
       <c r="M28" s="1" t="n">
         <v>24</v>
       </c>
@@ -5412,6 +6385,9 @@
       <c r="Q28" s="1" t="n">
         <v>12.0909090909091</v>
       </c>
+      <c r="R28" s="0" t="n">
+        <v>13.5291538038532</v>
+      </c>
       <c r="S28" s="1" t="n">
         <v>24</v>
       </c>
@@ -5427,6 +6403,9 @@
       <c r="W28" s="1" t="n">
         <v>23.3844539546584</v>
       </c>
+      <c r="X28" s="0" t="n">
+        <v>24.2179938412773</v>
+      </c>
       <c r="Y28" s="1" t="n">
         <v>24</v>
       </c>
@@ -5442,6 +6421,9 @@
       <c r="AC28" s="1" t="n">
         <v>36.3779001456479</v>
       </c>
+      <c r="AD28" s="0" t="n">
+        <v>35.7976689502891</v>
+      </c>
       <c r="AE28" s="1" t="n">
         <v>24</v>
       </c>
@@ -5456,6 +6438,9 @@
       </c>
       <c r="AI28" s="1" t="n">
         <v>100.678611793917</v>
+      </c>
+      <c r="AJ28" s="0" t="n">
+        <v>99.3127755103743</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5474,6 +6459,9 @@
       <c r="E29" s="1" t="n">
         <v>4.01893349681224</v>
       </c>
+      <c r="F29" s="0" t="n">
+        <v>4.50858789882697</v>
+      </c>
       <c r="G29" s="1" t="n">
         <v>25</v>
       </c>
@@ -5489,6 +6477,9 @@
       <c r="K29" s="1" t="n">
         <v>8.95520059179743</v>
       </c>
+      <c r="L29" s="0" t="n">
+        <v>9.76878342927149</v>
+      </c>
       <c r="M29" s="1" t="n">
         <v>25</v>
       </c>
@@ -5504,6 +6495,9 @@
       <c r="Q29" s="1" t="n">
         <v>11.4577922077922</v>
       </c>
+      <c r="R29" s="0" t="n">
+        <v>12.8636850837875</v>
+      </c>
       <c r="S29" s="1" t="n">
         <v>25</v>
       </c>
@@ -5519,6 +6513,9 @@
       <c r="W29" s="1" t="n">
         <v>23.6822545699977</v>
       </c>
+      <c r="X29" s="0" t="n">
+        <v>25.0522648062273</v>
+      </c>
       <c r="Y29" s="1" t="n">
         <v>25</v>
       </c>
@@ -5534,6 +6531,9 @@
       <c r="AC29" s="1" t="n">
         <v>35.3893750552639</v>
       </c>
+      <c r="AD29" s="0" t="n">
+        <v>36.5098973298358</v>
+      </c>
       <c r="AE29" s="1" t="n">
         <v>25</v>
       </c>
@@ -5548,6 +6548,9 @@
       </c>
       <c r="AI29" s="1" t="n">
         <v>98.4497456605905</v>
+      </c>
+      <c r="AJ29" s="0" t="n">
+        <v>106.204406061914</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5566,6 +6569,9 @@
       <c r="E30" s="1" t="n">
         <v>3.82886623439362</v>
       </c>
+      <c r="F30" s="0" t="n">
+        <v>5.19674169822789</v>
+      </c>
       <c r="G30" s="1" t="n">
         <v>26</v>
       </c>
@@ -5581,6 +6587,9 @@
       <c r="K30" s="1" t="n">
         <v>9.7143150974153</v>
       </c>
+      <c r="L30" s="0" t="n">
+        <v>12.1787040016894</v>
+      </c>
       <c r="M30" s="1" t="n">
         <v>26</v>
       </c>
@@ -5596,6 +6605,9 @@
       <c r="Q30" s="1" t="n">
         <v>12.7316017316017</v>
       </c>
+      <c r="R30" s="0" t="n">
+        <v>12.3249289384559</v>
+      </c>
       <c r="S30" s="1" t="n">
         <v>26</v>
       </c>
@@ -5611,6 +6623,9 @@
       <c r="W30" s="1" t="n">
         <v>23.6224639504399</v>
       </c>
+      <c r="X30" s="0" t="n">
+        <v>22.7428134831703</v>
+      </c>
       <c r="Y30" s="1" t="n">
         <v>26</v>
       </c>
@@ -5626,6 +6641,9 @@
       <c r="AC30" s="1" t="n">
         <v>35.2323883933084</v>
       </c>
+      <c r="AD30" s="0" t="n">
+        <v>36.7511276740196</v>
+      </c>
       <c r="AE30" s="1" t="n">
         <v>26</v>
       </c>
@@ -5640,6 +6658,9 @@
       </c>
       <c r="AI30" s="1" t="n">
         <v>102.040415228321</v>
+      </c>
+      <c r="AJ30" s="0" t="n">
+        <v>103.437589264419</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5658,6 +6679,9 @@
       <c r="E31" s="1" t="n">
         <v>3.3814124996716</v>
       </c>
+      <c r="F31" s="0" t="n">
+        <v>3.39532543890559</v>
+      </c>
       <c r="G31" s="1" t="n">
         <v>27</v>
       </c>
@@ -5673,6 +6697,9 @@
       <c r="K31" s="1" t="n">
         <v>9.63861779835719</v>
       </c>
+      <c r="L31" s="0" t="n">
+        <v>12.5369990877499</v>
+      </c>
       <c r="M31" s="1" t="n">
         <v>27</v>
       </c>
@@ -5688,6 +6715,9 @@
       <c r="Q31" s="1" t="n">
         <v>13.0292207792208</v>
       </c>
+      <c r="R31" s="0" t="n">
+        <v>13.2637934573373</v>
+      </c>
       <c r="S31" s="1" t="n">
         <v>27</v>
       </c>
@@ -5703,6 +6733,9 @@
       <c r="W31" s="1" t="n">
         <v>23.7018903735823</v>
       </c>
+      <c r="X31" s="0" t="n">
+        <v>25.2097053940015</v>
+      </c>
       <c r="Y31" s="1" t="n">
         <v>27</v>
       </c>
@@ -5718,6 +6751,9 @@
       <c r="AC31" s="1" t="n">
         <v>36.4909285987837</v>
       </c>
+      <c r="AD31" s="0" t="n">
+        <v>37.0742501080117</v>
+      </c>
       <c r="AE31" s="1" t="n">
         <v>27</v>
       </c>
@@ -5732,6 +6768,9 @@
       </c>
       <c r="AI31" s="1" t="n">
         <v>99.778513962564</v>
+      </c>
+      <c r="AJ31" s="0" t="n">
+        <v>103.742581291385</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5750,6 +6789,9 @@
       <c r="E32" s="1" t="n">
         <v>4.43227702626672</v>
       </c>
+      <c r="F32" s="0" t="n">
+        <v>4.11367291472995</v>
+      </c>
       <c r="G32" s="1" t="n">
         <v>28</v>
       </c>
@@ -5765,6 +6807,9 @@
       <c r="K32" s="1" t="n">
         <v>11.3799922455231</v>
       </c>
+      <c r="L32" s="0" t="n">
+        <v>11.1810509275943</v>
+      </c>
       <c r="M32" s="1" t="n">
         <v>28</v>
       </c>
@@ -5780,6 +6825,9 @@
       <c r="Q32" s="1" t="n">
         <v>8.40259740259741</v>
       </c>
+      <c r="R32" s="0" t="n">
+        <v>11.5635057967269</v>
+      </c>
       <c r="S32" s="1" t="n">
         <v>28</v>
       </c>
@@ -5795,6 +6843,9 @@
       <c r="W32" s="1" t="n">
         <v>23.1938885960891</v>
       </c>
+      <c r="X32" s="0" t="n">
+        <v>25.0381489713494</v>
+      </c>
       <c r="Y32" s="1" t="n">
         <v>28</v>
       </c>
@@ -5810,6 +6861,9 @@
       <c r="AC32" s="1" t="n">
         <v>37.738865363785</v>
       </c>
+      <c r="AD32" s="0" t="n">
+        <v>34.8635700599355</v>
+      </c>
       <c r="AE32" s="1" t="n">
         <v>28</v>
       </c>
@@ -5824,6 +6878,9 @@
       </c>
       <c r="AI32" s="1" t="n">
         <v>98.7215913904853</v>
+      </c>
+      <c r="AJ32" s="0" t="n">
+        <v>101.706363411039</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5842,6 +6899,9 @@
       <c r="E33" s="1" t="n">
         <v>3.68922706061437</v>
       </c>
+      <c r="F33" s="0" t="n">
+        <v>4.02373799514301</v>
+      </c>
       <c r="G33" s="1" t="n">
         <v>29</v>
       </c>
@@ -5857,6 +6917,9 @@
       <c r="K33" s="1" t="n">
         <v>12.4973866856755</v>
       </c>
+      <c r="L33" s="0" t="n">
+        <v>13.0894233889364</v>
+      </c>
       <c r="M33" s="1" t="n">
         <v>29</v>
       </c>
@@ -5872,6 +6935,9 @@
       <c r="Q33" s="1" t="n">
         <v>9.63419913419913</v>
       </c>
+      <c r="R33" s="0" t="n">
+        <v>10.2516158832248</v>
+      </c>
       <c r="S33" s="1" t="n">
         <v>29</v>
       </c>
@@ -5887,6 +6953,9 @@
       <c r="W33" s="1" t="n">
         <v>23.9283365825517</v>
       </c>
+      <c r="X33" s="0" t="n">
+        <v>24.5204188935599</v>
+      </c>
       <c r="Y33" s="1" t="n">
         <v>29</v>
       </c>
@@ -5902,6 +6971,9 @@
       <c r="AC33" s="1" t="n">
         <v>35.3247233114784</v>
       </c>
+      <c r="AD33" s="0" t="n">
+        <v>33.6440614916068</v>
+      </c>
       <c r="AE33" s="1" t="n">
         <v>29</v>
       </c>
@@ -5916,6 +6988,9 @@
       </c>
       <c r="AI33" s="1" t="n">
         <v>106.388833962106</v>
+      </c>
+      <c r="AJ33" s="0" t="n">
+        <v>103.490537833095</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5934,6 +7009,9 @@
       <c r="E34" s="1" t="n">
         <v>2.92768173629888</v>
       </c>
+      <c r="F34" s="0" t="n">
+        <v>4.60193481012546</v>
+      </c>
       <c r="G34" s="1" t="n">
         <v>30</v>
       </c>
@@ -5949,6 +7027,9 @@
       <c r="K34" s="1" t="n">
         <v>10.8845205895149</v>
       </c>
+      <c r="L34" s="0" t="n">
+        <v>12.9885609030208</v>
+      </c>
       <c r="M34" s="1" t="n">
         <v>30</v>
       </c>
@@ -5964,6 +7045,9 @@
       <c r="Q34" s="1" t="n">
         <v>9.44155844155844</v>
       </c>
+      <c r="R34" s="0" t="n">
+        <v>10.7412436511312</v>
+      </c>
       <c r="S34" s="1" t="n">
         <v>30</v>
       </c>
@@ -5979,6 +7063,9 @@
       <c r="W34" s="1" t="n">
         <v>22.3449782210613</v>
       </c>
+      <c r="X34" s="0" t="n">
+        <v>23.3594903410467</v>
+      </c>
       <c r="Y34" s="1" t="n">
         <v>30</v>
       </c>
@@ -5993,6 +7080,9 @@
       </c>
       <c r="AC34" s="1" t="n">
         <v>34.5809786478987</v>
+      </c>
+      <c r="AD34" s="0" t="n">
+        <v>34.5086130588105</v>
       </c>
       <c r="AE34" s="1" t="n">
         <v>30</v>

</xml_diff>